<commit_message>
updated the equipment list
</commit_message>
<xml_diff>
--- a/Kilroy Equipment List 2016.xlsx
+++ b/Kilroy Equipment List 2016.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Robotics\2016\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Robotics\2016\Kilroy\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -897,8 +897,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H236"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A94" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" sqref="A1:E1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added more print statements to the print()
</commit_message>
<xml_diff>
--- a/Kilroy Equipment List 2016.xlsx
+++ b/Kilroy Equipment List 2016.xlsx
@@ -163,9 +163,6 @@
     <t>CAN 15</t>
   </si>
   <si>
-    <t>Left Motor Motor Controller</t>
-  </si>
-  <si>
     <t>Right Front Motor Controller</t>
   </si>
   <si>
@@ -296,6 +293,9 @@
   </si>
   <si>
     <t>errorMessage</t>
+  </si>
+  <si>
+    <t>Left Rear Motor Controller</t>
   </si>
 </sst>
 </file>
@@ -1040,8 +1040,8 @@
   <dimension ref="A1:H238"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A90" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C106" sqref="C106"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -1111,7 +1111,7 @@
       <c r="A5" s="68"/>
       <c r="B5" s="68"/>
       <c r="C5" s="31" t="s">
-        <v>48</v>
+        <v>92</v>
       </c>
       <c r="D5" s="34" t="s">
         <v>43</v>
@@ -1124,23 +1124,23 @@
       <c r="A6" s="8"/>
       <c r="B6" s="8"/>
       <c r="C6" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="D6" s="29" t="s">
+      <c r="E6" s="30" t="s">
         <v>50</v>
-      </c>
-      <c r="E6" s="30" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="37" customFormat="1">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" s="34" t="s">
         <v>52</v>
-      </c>
-      <c r="D7" s="34" t="s">
-        <v>53</v>
       </c>
       <c r="E7" s="35" t="s">
         <v>44</v>
@@ -1205,26 +1205,26 @@
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="31" t="s">
+        <v>74</v>
+      </c>
+      <c r="D14" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="D14" s="34" t="s">
-        <v>76</v>
-      </c>
       <c r="E14" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:8" s="1" customFormat="1">
       <c r="A15" s="54"/>
       <c r="B15" s="54"/>
       <c r="C15" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="D15" s="29" t="s">
         <v>77</v>
       </c>
-      <c r="D15" s="29" t="s">
+      <c r="E15" s="46" t="s">
         <v>78</v>
-      </c>
-      <c r="E15" s="46" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="16" spans="1:8" s="1" customFormat="1">
@@ -1336,65 +1336,65 @@
       <c r="A27" s="45"/>
       <c r="B27" s="45"/>
       <c r="C27" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="D27" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="D27" s="34" t="s">
-        <v>55</v>
-      </c>
       <c r="E27" s="35" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="28" spans="1:8" s="1" customFormat="1">
       <c r="A28" s="13"/>
       <c r="B28" s="13"/>
       <c r="C28" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="D28" s="47" t="s">
         <v>56</v>
       </c>
-      <c r="D28" s="47" t="s">
+      <c r="E28" s="46" t="s">
         <v>57</v>
-      </c>
-      <c r="E28" s="46" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="29" spans="1:8" s="1" customFormat="1">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="31" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D29" s="34" t="s">
+        <v>59</v>
+      </c>
+      <c r="E29" s="35" t="s">
         <v>60</v>
-      </c>
-      <c r="E29" s="35" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="30" spans="1:8" s="1" customFormat="1">
       <c r="A30" s="13"/>
       <c r="B30" s="13"/>
       <c r="C30" s="25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D30" s="47" t="s">
+        <v>62</v>
+      </c>
+      <c r="E30" s="46" t="s">
         <v>63</v>
-      </c>
-      <c r="E30" s="46" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="31" spans="1:8" s="1" customFormat="1">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="D31" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="D31" s="34" t="s">
+      <c r="E31" s="35" t="s">
         <v>70</v>
-      </c>
-      <c r="E31" s="35" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="32" spans="1:8" s="1" customFormat="1">
@@ -1536,13 +1536,13 @@
       <c r="A49" s="20"/>
       <c r="B49" s="20"/>
       <c r="C49" s="48" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D49" s="27" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E49" s="49" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="50" spans="1:8" s="1" customFormat="1">
@@ -1685,13 +1685,13 @@
       <c r="A67" s="8"/>
       <c r="B67" s="8"/>
       <c r="C67" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="D67" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="D67" s="29" t="s">
-        <v>82</v>
-      </c>
       <c r="E67" s="30" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G67" s="23"/>
     </row>
@@ -1699,13 +1699,13 @@
       <c r="A68" s="4"/>
       <c r="B68" s="4"/>
       <c r="C68" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="D68" s="34" t="s">
         <v>83</v>
       </c>
-      <c r="D68" s="34" t="s">
-        <v>84</v>
-      </c>
       <c r="E68" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G68" s="23"/>
     </row>
@@ -1713,13 +1713,13 @@
       <c r="A69" s="8"/>
       <c r="B69" s="8"/>
       <c r="C69" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="D69" s="47" t="s">
         <v>85</v>
       </c>
-      <c r="D69" s="47" t="s">
+      <c r="E69" s="46" t="s">
         <v>86</v>
-      </c>
-      <c r="E69" s="46" t="s">
-        <v>87</v>
       </c>
       <c r="G69" s="23"/>
     </row>
@@ -1727,13 +1727,13 @@
       <c r="A70" s="4"/>
       <c r="B70" s="4"/>
       <c r="C70" s="31" t="s">
+        <v>87</v>
+      </c>
+      <c r="D70" s="34" t="s">
         <v>88</v>
       </c>
-      <c r="D70" s="34" t="s">
-        <v>89</v>
-      </c>
       <c r="E70" s="35" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G70" s="23"/>
     </row>
@@ -2005,7 +2005,7 @@
         <v>22</v>
       </c>
       <c r="D104" s="29" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E104" s="46" t="s">
         <v>24</v>
@@ -2028,10 +2028,10 @@
       <c r="A106" s="13"/>
       <c r="B106" s="13"/>
       <c r="C106" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="D106" s="29" t="s">
         <v>66</v>
-      </c>
-      <c r="D106" s="29" t="s">
-        <v>67</v>
       </c>
       <c r="E106" s="46" t="s">
         <v>20</v>
@@ -2067,7 +2067,7 @@
       <c r="A109" s="4"/>
       <c r="B109" s="4"/>
       <c r="C109" s="31" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D109" s="6" t="s">
         <v>8</v>
@@ -2106,10 +2106,10 @@
       <c r="A112" s="13"/>
       <c r="B112" s="13"/>
       <c r="C112" s="25" t="s">
+        <v>90</v>
+      </c>
+      <c r="D112" s="47" t="s">
         <v>91</v>
-      </c>
-      <c r="D112" s="47" t="s">
-        <v>92</v>
       </c>
       <c r="E112" s="25" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
Fixed problem with conflicting IR sensors and encoders on the same IO port and updated equipment list
</commit_message>
<xml_diff>
--- a/Kilroy Equipment List 2016.xlsx
+++ b/Kilroy Equipment List 2016.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="11625" windowHeight="3150"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="10590" windowHeight="5790"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,12 +12,13 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$E$102</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="95">
   <si>
     <t>Code Written/Tested</t>
   </si>
@@ -296,6 +297,12 @@
   </si>
   <si>
     <t>Left Rear Motor Controller</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>22</t>
   </si>
 </sst>
 </file>
@@ -1039,9 +1046,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H238"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -1211,7 +1218,7 @@
         <v>75</v>
       </c>
       <c r="E14" s="35" t="s">
-        <v>72</v>
+        <v>93</v>
       </c>
     </row>
     <row r="15" spans="1:8" s="1" customFormat="1">
@@ -1224,7 +1231,7 @@
         <v>77</v>
       </c>
       <c r="E15" s="46" t="s">
-        <v>78</v>
+        <v>94</v>
       </c>
     </row>
     <row r="16" spans="1:8" s="1" customFormat="1">

</xml_diff>

<commit_message>
Added more functionality to the CAN network system so that we can create a list of objects and test them for faults
</commit_message>
<xml_diff>
--- a/Kilroy Equipment List 2016.xlsx
+++ b/Kilroy Equipment List 2016.xlsx
@@ -13,12 +13,11 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$E$102</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="96">
   <si>
     <t>Code Written/Tested</t>
   </si>
@@ -110,9 +109,6 @@
     <t>CAN Port</t>
   </si>
   <si>
-    <t>PDB (Power Distribution Board)</t>
-  </si>
-  <si>
     <t>roboRIO</t>
   </si>
   <si>
@@ -303,6 +299,12 @@
   </si>
   <si>
     <t>22</t>
+  </si>
+  <si>
+    <t>PDP (Power Distribution Panel)</t>
+  </si>
+  <si>
+    <t>pdp</t>
   </si>
 </sst>
 </file>
@@ -464,7 +466,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -677,6 +679,9 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1046,9 +1051,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H238"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F60" sqref="F60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -1066,7 +1071,7 @@
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1">
       <c r="A1" s="70" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B1" s="70"/>
       <c r="C1" s="70"/>
@@ -1098,59 +1103,59 @@
       </c>
       <c r="D3" s="69"/>
       <c r="E3" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="1" customFormat="1" ht="12.75" customHeight="1">
       <c r="A4" s="67"/>
       <c r="B4" s="67"/>
       <c r="C4" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" s="52" t="s">
         <v>46</v>
-      </c>
-      <c r="D4" s="33" t="s">
-        <v>42</v>
-      </c>
-      <c r="E4" s="52" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="1" customFormat="1" ht="12.75" customHeight="1">
       <c r="A5" s="68"/>
       <c r="B5" s="68"/>
       <c r="C5" s="31" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D5" s="34" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E5" s="35" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="1" customFormat="1" ht="12.75" customHeight="1">
       <c r="A6" s="8"/>
       <c r="B6" s="8"/>
       <c r="C6" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="D6" s="29" t="s">
+      <c r="E6" s="30" t="s">
         <v>49</v>
-      </c>
-      <c r="E6" s="30" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="37" customFormat="1">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" s="34" t="s">
         <v>51</v>
       </c>
-      <c r="D7" s="34" t="s">
-        <v>52</v>
-      </c>
       <c r="E7" s="35" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="1" customFormat="1">
@@ -1212,26 +1217,26 @@
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="31" t="s">
+        <v>73</v>
+      </c>
+      <c r="D14" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="D14" s="34" t="s">
-        <v>75</v>
-      </c>
       <c r="E14" s="35" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="15" spans="1:8" s="1" customFormat="1">
       <c r="A15" s="54"/>
       <c r="B15" s="54"/>
       <c r="C15" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="D15" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="D15" s="29" t="s">
-        <v>77</v>
-      </c>
       <c r="E15" s="46" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="16" spans="1:8" s="1" customFormat="1">
@@ -1343,65 +1348,65 @@
       <c r="A27" s="45"/>
       <c r="B27" s="45"/>
       <c r="C27" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="D27" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="D27" s="34" t="s">
-        <v>54</v>
-      </c>
       <c r="E27" s="35" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="28" spans="1:8" s="1" customFormat="1">
       <c r="A28" s="13"/>
       <c r="B28" s="13"/>
       <c r="C28" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="D28" s="47" t="s">
         <v>55</v>
       </c>
-      <c r="D28" s="47" t="s">
+      <c r="E28" s="46" t="s">
         <v>56</v>
-      </c>
-      <c r="E28" s="46" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="29" spans="1:8" s="1" customFormat="1">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="31" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D29" s="34" t="s">
+        <v>58</v>
+      </c>
+      <c r="E29" s="35" t="s">
         <v>59</v>
-      </c>
-      <c r="E29" s="35" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="30" spans="1:8" s="1" customFormat="1">
       <c r="A30" s="13"/>
       <c r="B30" s="13"/>
       <c r="C30" s="25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D30" s="47" t="s">
+        <v>61</v>
+      </c>
+      <c r="E30" s="46" t="s">
         <v>62</v>
-      </c>
-      <c r="E30" s="46" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="31" spans="1:8" s="1" customFormat="1">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="D31" s="34" t="s">
         <v>68</v>
       </c>
-      <c r="D31" s="34" t="s">
+      <c r="E31" s="35" t="s">
         <v>69</v>
-      </c>
-      <c r="E31" s="35" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="32" spans="1:8" s="1" customFormat="1">
@@ -1543,13 +1548,13 @@
       <c r="A49" s="20"/>
       <c r="B49" s="20"/>
       <c r="C49" s="48" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D49" s="27" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E49" s="49" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="50" spans="1:8" s="1" customFormat="1">
@@ -1638,8 +1643,8 @@
     <row r="61" spans="1:8" s="1" customFormat="1" ht="13.35" customHeight="1">
       <c r="A61" s="17"/>
       <c r="B61" s="17"/>
-      <c r="C61" s="69" t="s">
-        <v>30</v>
+      <c r="C61" s="72" t="s">
+        <v>94</v>
       </c>
       <c r="D61" s="69"/>
       <c r="E61" s="3" t="s">
@@ -1649,9 +1654,15 @@
     <row r="62" spans="1:8" s="1" customFormat="1">
       <c r="A62" s="8"/>
       <c r="B62" s="8"/>
-      <c r="C62" s="9"/>
-      <c r="D62" s="10"/>
-      <c r="E62" s="11"/>
+      <c r="C62" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="D62" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="E62" s="30" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="63" spans="1:8" s="1" customFormat="1">
       <c r="A63" s="4"/>
@@ -1692,13 +1703,13 @@
       <c r="A67" s="8"/>
       <c r="B67" s="8"/>
       <c r="C67" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="D67" s="29" t="s">
         <v>80</v>
       </c>
-      <c r="D67" s="29" t="s">
-        <v>81</v>
-      </c>
       <c r="E67" s="30" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G67" s="23"/>
     </row>
@@ -1706,13 +1717,13 @@
       <c r="A68" s="4"/>
       <c r="B68" s="4"/>
       <c r="C68" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="D68" s="34" t="s">
         <v>82</v>
       </c>
-      <c r="D68" s="34" t="s">
-        <v>83</v>
-      </c>
       <c r="E68" s="35" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G68" s="23"/>
     </row>
@@ -1720,13 +1731,13 @@
       <c r="A69" s="8"/>
       <c r="B69" s="8"/>
       <c r="C69" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="D69" s="47" t="s">
         <v>84</v>
       </c>
-      <c r="D69" s="47" t="s">
+      <c r="E69" s="46" t="s">
         <v>85</v>
-      </c>
-      <c r="E69" s="46" t="s">
-        <v>86</v>
       </c>
       <c r="G69" s="23"/>
     </row>
@@ -1734,13 +1745,13 @@
       <c r="A70" s="4"/>
       <c r="B70" s="4"/>
       <c r="C70" s="31" t="s">
+        <v>86</v>
+      </c>
+      <c r="D70" s="34" t="s">
         <v>87</v>
       </c>
-      <c r="D70" s="34" t="s">
-        <v>88</v>
-      </c>
       <c r="E70" s="35" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G70" s="23"/>
     </row>
@@ -2012,7 +2023,7 @@
         <v>22</v>
       </c>
       <c r="D104" s="29" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E104" s="46" t="s">
         <v>24</v>
@@ -2028,17 +2039,17 @@
         <v>8</v>
       </c>
       <c r="E105" s="35" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="106" spans="1:6" s="1" customFormat="1">
       <c r="A106" s="13"/>
       <c r="B106" s="13"/>
       <c r="C106" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="D106" s="29" t="s">
         <v>65</v>
-      </c>
-      <c r="D106" s="29" t="s">
-        <v>66</v>
       </c>
       <c r="E106" s="46" t="s">
         <v>20</v>
@@ -2048,10 +2059,10 @@
       <c r="A107" s="4"/>
       <c r="B107" s="4"/>
       <c r="C107" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="D107" s="34" t="s">
         <v>38</v>
-      </c>
-      <c r="D107" s="34" t="s">
-        <v>39</v>
       </c>
       <c r="E107" s="35" t="s">
         <v>20</v>
@@ -2061,36 +2072,36 @@
       <c r="A108" s="13"/>
       <c r="B108" s="13"/>
       <c r="C108" s="25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D108" s="15" t="s">
         <v>8</v>
       </c>
       <c r="E108" s="16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="109" spans="1:6" s="1" customFormat="1">
       <c r="A109" s="4"/>
       <c r="B109" s="4"/>
       <c r="C109" s="31" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D109" s="6" t="s">
         <v>8</v>
       </c>
       <c r="E109" s="35" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="110" spans="1:6" s="1" customFormat="1">
       <c r="A110" s="13"/>
       <c r="B110" s="13"/>
       <c r="C110" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="D110" s="47" t="s">
         <v>36</v>
-      </c>
-      <c r="D110" s="47" t="s">
-        <v>37</v>
       </c>
       <c r="E110" s="25" t="s">
         <v>20</v>
@@ -2100,23 +2111,23 @@
       <c r="A111" s="4"/>
       <c r="B111" s="4"/>
       <c r="C111" s="31" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D111" s="6" t="s">
         <v>8</v>
       </c>
       <c r="E111" s="35" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="112" spans="1:6" s="1" customFormat="1">
       <c r="A112" s="13"/>
       <c r="B112" s="13"/>
       <c r="C112" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="D112" s="47" t="s">
         <v>90</v>
-      </c>
-      <c r="D112" s="47" t="s">
-        <v>91</v>
       </c>
       <c r="E112" s="25" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
Declared certain hardware components, and added print statements for them also wrote code for the solenoids
</commit_message>
<xml_diff>
--- a/Kilroy Equipment List 2016.xlsx
+++ b/Kilroy Equipment List 2016.xlsx
@@ -13,12 +13,11 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$E$102</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="112">
   <si>
     <t>Code Written/Tested</t>
   </si>
@@ -303,6 +302,57 @@
   </si>
   <si>
     <t>22</t>
+  </si>
+  <si>
+    <t>Compressor Relay</t>
+  </si>
+  <si>
+    <t>compressorRelay</t>
+  </si>
+  <si>
+    <t>Ring Light Relay</t>
+  </si>
+  <si>
+    <t>ringLightRelay</t>
+  </si>
+  <si>
+    <t>Six Position Switch</t>
+  </si>
+  <si>
+    <t>sixPositionDial</t>
+  </si>
+  <si>
+    <t>14,15,16,17,18,21</t>
+  </si>
+  <si>
+    <t>Transducer - (range 130)</t>
+  </si>
+  <si>
+    <t>transducer</t>
+  </si>
+  <si>
+    <t>Double Solenoid</t>
+  </si>
+  <si>
+    <t>cameraSolenoid</t>
+  </si>
+  <si>
+    <t>PCM Port</t>
+  </si>
+  <si>
+    <t>3,4</t>
+  </si>
+  <si>
+    <t>Single Solenoid</t>
+  </si>
+  <si>
+    <t>catapultSolenoid0</t>
+  </si>
+  <si>
+    <t>catapultSolenoid1</t>
+  </si>
+  <si>
+    <t>catapultSolenoid2</t>
   </si>
 </sst>
 </file>
@@ -464,7 +514,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -524,12 +574,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1046,32 +1090,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H238"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E63" sqref="E63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" style="63" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" style="63" customWidth="1"/>
-    <col min="3" max="3" width="70.5703125" style="63" customWidth="1"/>
-    <col min="4" max="4" width="21" style="64" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" style="66" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" style="63" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" style="63"/>
-    <col min="8" max="8" width="11.140625" style="63" customWidth="1"/>
-    <col min="9" max="16384" width="8.85546875" style="63"/>
+    <col min="1" max="1" width="14.7109375" style="61" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" style="61" customWidth="1"/>
+    <col min="3" max="3" width="70.5703125" style="61" customWidth="1"/>
+    <col min="4" max="4" width="21" style="62" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" style="64" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" style="61" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" style="61"/>
+    <col min="8" max="8" width="11.140625" style="61" customWidth="1"/>
+    <col min="9" max="16384" width="8.85546875" style="61"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="68" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
     </row>
     <row r="2" spans="1:8" s="1" customFormat="1" ht="25.5">
       <c r="A2" s="13" t="s">
@@ -1080,85 +1124,85 @@
       <c r="B2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="40" t="s">
+      <c r="C2" s="38" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="41" t="s">
+      <c r="E2" s="39" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="1" customFormat="1" ht="13.15" customHeight="1">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
-      <c r="C3" s="69" t="s">
+      <c r="C3" s="67" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="69"/>
+      <c r="D3" s="67"/>
       <c r="E3" s="3" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="1" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A4" s="67"/>
-      <c r="B4" s="67"/>
-      <c r="C4" s="32" t="s">
+      <c r="A4" s="65"/>
+      <c r="B4" s="65"/>
+      <c r="C4" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="D4" s="33" t="s">
+      <c r="D4" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="E4" s="52" t="s">
+      <c r="E4" s="50" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="1" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A5" s="68"/>
-      <c r="B5" s="68"/>
-      <c r="C5" s="31" t="s">
+      <c r="A5" s="66"/>
+      <c r="B5" s="66"/>
+      <c r="C5" s="29" t="s">
         <v>92</v>
       </c>
-      <c r="D5" s="34" t="s">
+      <c r="D5" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="E5" s="35" t="s">
+      <c r="E5" s="33" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="1" customFormat="1" ht="12.75" customHeight="1">
       <c r="A6" s="8"/>
       <c r="B6" s="8"/>
-      <c r="C6" s="28" t="s">
+      <c r="C6" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="D6" s="29" t="s">
+      <c r="D6" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="E6" s="30" t="s">
+      <c r="E6" s="28" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="37" customFormat="1">
+    <row r="7" spans="1:8" s="35" customFormat="1">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
-      <c r="C7" s="31" t="s">
+      <c r="C7" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="D7" s="34" t="s">
+      <c r="D7" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="E7" s="35" t="s">
+      <c r="E7" s="33" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="1" customFormat="1">
-      <c r="A8" s="36"/>
-      <c r="B8" s="36"/>
-      <c r="C8" s="51"/>
-      <c r="D8" s="58"/>
-      <c r="E8" s="53"/>
+      <c r="A8" s="34"/>
+      <c r="B8" s="34"/>
+      <c r="C8" s="49"/>
+      <c r="D8" s="56"/>
+      <c r="E8" s="51"/>
       <c r="F8" s="12"/>
       <c r="G8" s="12"/>
       <c r="H8" s="12"/>
@@ -1166,9 +1210,9 @@
     <row r="9" spans="1:8" s="1" customFormat="1">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
-      <c r="C9" s="31"/>
-      <c r="D9" s="34"/>
-      <c r="E9" s="35"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="33"/>
       <c r="F9" s="12"/>
       <c r="G9" s="12"/>
       <c r="H9" s="12"/>
@@ -1176,9 +1220,9 @@
     <row r="10" spans="1:8" s="1" customFormat="1">
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
-      <c r="C10" s="28"/>
-      <c r="D10" s="29"/>
-      <c r="E10" s="30"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="28"/>
       <c r="F10" s="12"/>
       <c r="G10" s="12"/>
       <c r="H10" s="12"/>
@@ -1200,46 +1244,46 @@
     <row r="13" spans="1:8" s="1" customFormat="1" ht="13.15" customHeight="1">
       <c r="A13" s="17"/>
       <c r="B13" s="17"/>
-      <c r="C13" s="71" t="s">
+      <c r="C13" s="69" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="71"/>
-      <c r="E13" s="62" t="s">
+      <c r="D13" s="69"/>
+      <c r="E13" s="60" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:8" s="1" customFormat="1">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
-      <c r="C14" s="31" t="s">
+      <c r="C14" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="D14" s="34" t="s">
+      <c r="D14" s="32" t="s">
         <v>75</v>
       </c>
-      <c r="E14" s="35" t="s">
+      <c r="E14" s="33" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="15" spans="1:8" s="1" customFormat="1">
-      <c r="A15" s="54"/>
-      <c r="B15" s="54"/>
-      <c r="C15" s="28" t="s">
+      <c r="A15" s="52"/>
+      <c r="B15" s="52"/>
+      <c r="C15" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="D15" s="29" t="s">
+      <c r="D15" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="E15" s="46" t="s">
+      <c r="E15" s="44" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="16" spans="1:8" s="1" customFormat="1">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
-      <c r="C16" s="31"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="35"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="33"/>
       <c r="F16" s="12"/>
       <c r="G16" s="12"/>
       <c r="H16" s="12"/>
@@ -1247,16 +1291,16 @@
     <row r="17" spans="1:8" s="1" customFormat="1">
       <c r="A17" s="8"/>
       <c r="B17" s="8"/>
-      <c r="C17" s="28"/>
-      <c r="D17" s="29"/>
-      <c r="E17" s="30"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="28"/>
       <c r="F17" s="12"/>
       <c r="G17" s="12"/>
       <c r="H17" s="12"/>
     </row>
     <row r="18" spans="1:8" s="1" customFormat="1">
-      <c r="A18" s="45"/>
-      <c r="B18" s="45"/>
+      <c r="A18" s="43"/>
+      <c r="B18" s="43"/>
       <c r="C18" s="5"/>
       <c r="D18" s="6"/>
       <c r="E18" s="7"/>
@@ -1331,134 +1375,140 @@
     <row r="26" spans="1:8" s="1" customFormat="1" ht="13.35" customHeight="1">
       <c r="A26" s="17"/>
       <c r="B26" s="17"/>
-      <c r="C26" s="69" t="s">
+      <c r="C26" s="67" t="s">
         <v>7</v>
       </c>
-      <c r="D26" s="69"/>
+      <c r="D26" s="67"/>
       <c r="E26" s="3" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="27" spans="1:8" s="1" customFormat="1">
-      <c r="A27" s="45"/>
-      <c r="B27" s="45"/>
-      <c r="C27" s="31" t="s">
+      <c r="A27" s="43"/>
+      <c r="B27" s="43"/>
+      <c r="C27" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="D27" s="34" t="s">
+      <c r="D27" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="E27" s="35" t="s">
+      <c r="E27" s="33" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="28" spans="1:8" s="1" customFormat="1">
       <c r="A28" s="13"/>
       <c r="B28" s="13"/>
-      <c r="C28" s="25" t="s">
+      <c r="C28" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="D28" s="47" t="s">
+      <c r="D28" s="45" t="s">
         <v>56</v>
       </c>
-      <c r="E28" s="46" t="s">
+      <c r="E28" s="44" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="29" spans="1:8" s="1" customFormat="1">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
-      <c r="C29" s="31" t="s">
+      <c r="C29" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="D29" s="34" t="s">
+      <c r="D29" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="E29" s="35" t="s">
+      <c r="E29" s="33" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="30" spans="1:8" s="1" customFormat="1">
       <c r="A30" s="13"/>
       <c r="B30" s="13"/>
-      <c r="C30" s="25" t="s">
+      <c r="C30" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="D30" s="47" t="s">
+      <c r="D30" s="45" t="s">
         <v>62</v>
       </c>
-      <c r="E30" s="46" t="s">
+      <c r="E30" s="44" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="31" spans="1:8" s="1" customFormat="1">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
-      <c r="C31" s="31" t="s">
+      <c r="C31" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="D31" s="34" t="s">
+      <c r="D31" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="E31" s="35" t="s">
+      <c r="E31" s="33" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="32" spans="1:8" s="1" customFormat="1">
       <c r="A32" s="13"/>
       <c r="B32" s="13"/>
-      <c r="C32" s="25"/>
-      <c r="D32" s="47"/>
-      <c r="E32" s="46"/>
+      <c r="C32" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="D32" s="45" t="s">
+        <v>100</v>
+      </c>
+      <c r="E32" s="44" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="33" spans="1:5" s="1" customFormat="1">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
-      <c r="C33" s="31"/>
-      <c r="D33" s="34"/>
-      <c r="E33" s="35"/>
+      <c r="C33" s="29"/>
+      <c r="D33" s="32"/>
+      <c r="E33" s="33"/>
     </row>
     <row r="34" spans="1:5" s="1" customFormat="1">
       <c r="A34" s="13"/>
       <c r="B34" s="13"/>
-      <c r="C34" s="25"/>
-      <c r="D34" s="47"/>
-      <c r="E34" s="46"/>
+      <c r="C34" s="23"/>
+      <c r="D34" s="45"/>
+      <c r="E34" s="44"/>
     </row>
     <row r="35" spans="1:5" s="1" customFormat="1">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
-      <c r="C35" s="31"/>
-      <c r="D35" s="34"/>
-      <c r="E35" s="35"/>
+      <c r="C35" s="29"/>
+      <c r="D35" s="32"/>
+      <c r="E35" s="33"/>
     </row>
     <row r="36" spans="1:5" s="1" customFormat="1">
       <c r="A36" s="8"/>
       <c r="B36" s="8"/>
-      <c r="C36" s="28"/>
+      <c r="C36" s="26"/>
       <c r="D36" s="18"/>
-      <c r="E36" s="59"/>
+      <c r="E36" s="57"/>
     </row>
     <row r="37" spans="1:5" s="1" customFormat="1">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
-      <c r="C37" s="31"/>
-      <c r="D37" s="34"/>
-      <c r="E37" s="35"/>
+      <c r="C37" s="29"/>
+      <c r="D37" s="32"/>
+      <c r="E37" s="33"/>
     </row>
     <row r="38" spans="1:5" s="1" customFormat="1" ht="13.35" customHeight="1">
       <c r="A38" s="13"/>
       <c r="B38" s="13"/>
-      <c r="C38" s="25"/>
-      <c r="D38" s="47"/>
-      <c r="E38" s="46"/>
+      <c r="C38" s="23"/>
+      <c r="D38" s="45"/>
+      <c r="E38" s="44"/>
     </row>
     <row r="39" spans="1:5" s="19" customFormat="1" ht="13.15" customHeight="1">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
-      <c r="C39" s="60"/>
-      <c r="D39" s="34"/>
-      <c r="E39" s="35"/>
+      <c r="C39" s="58"/>
+      <c r="D39" s="32"/>
+      <c r="E39" s="33"/>
     </row>
     <row r="40" spans="1:5" s="1" customFormat="1" ht="13.15" customHeight="1">
       <c r="A40" s="8"/>
@@ -1477,38 +1527,50 @@
     <row r="42" spans="1:5" s="19" customFormat="1" ht="13.15" customHeight="1">
       <c r="A42" s="13"/>
       <c r="B42" s="13"/>
-      <c r="C42" s="25"/>
-      <c r="D42" s="47"/>
-      <c r="E42" s="46"/>
+      <c r="C42" s="23"/>
+      <c r="D42" s="45"/>
+      <c r="E42" s="44"/>
     </row>
     <row r="43" spans="1:5" s="1" customFormat="1" ht="13.15" customHeight="1">
       <c r="A43" s="17"/>
       <c r="B43" s="17"/>
-      <c r="C43" s="69" t="s">
+      <c r="C43" s="67" t="s">
         <v>9</v>
       </c>
-      <c r="D43" s="69"/>
+      <c r="D43" s="67"/>
       <c r="E43" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="44" spans="1:5" s="1" customFormat="1">
-      <c r="A44" s="42" t="s">
+      <c r="A44" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="B44" s="42" t="s">
+      <c r="B44" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="C44" s="31"/>
-      <c r="D44" s="27"/>
-      <c r="E44" s="49"/>
+      <c r="C44" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="D44" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="E44" s="47" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="45" spans="1:5" s="1" customFormat="1">
-      <c r="A45" s="43"/>
+      <c r="A45" s="41"/>
       <c r="B45" s="14"/>
-      <c r="C45" s="44"/>
-      <c r="D45" s="47"/>
-      <c r="E45" s="14"/>
+      <c r="C45" s="42" t="s">
+        <v>97</v>
+      </c>
+      <c r="D45" s="45" t="s">
+        <v>98</v>
+      </c>
+      <c r="E45" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="46" spans="1:5" s="1" customFormat="1">
       <c r="A46" s="4" t="s">
@@ -1531,10 +1593,10 @@
     <row r="48" spans="1:5" s="1" customFormat="1" ht="13.15" customHeight="1">
       <c r="A48" s="17"/>
       <c r="B48" s="17"/>
-      <c r="C48" s="69" t="s">
+      <c r="C48" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="D48" s="69"/>
+      <c r="D48" s="67"/>
       <c r="E48" s="3" t="s">
         <v>12</v>
       </c>
@@ -1542,106 +1604,136 @@
     <row r="49" spans="1:8" s="19" customFormat="1" ht="13.15" customHeight="1">
       <c r="A49" s="20"/>
       <c r="B49" s="20"/>
-      <c r="C49" s="48" t="s">
+      <c r="C49" s="46" t="s">
         <v>73</v>
       </c>
-      <c r="D49" s="27" t="s">
+      <c r="D49" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="E49" s="49" t="s">
+      <c r="E49" s="47" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="50" spans="1:8" s="1" customFormat="1">
       <c r="A50" s="8"/>
       <c r="B50" s="8"/>
-      <c r="C50" s="28"/>
-      <c r="D50" s="29"/>
-      <c r="E50" s="30"/>
+      <c r="C50" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="D50" s="27" t="s">
+        <v>103</v>
+      </c>
+      <c r="E50" s="28" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="51" spans="1:8" s="1" customFormat="1">
       <c r="A51" s="4"/>
       <c r="B51" s="4"/>
-      <c r="C51" s="31"/>
-      <c r="D51" s="34"/>
-      <c r="E51" s="35"/>
+      <c r="C51" s="29"/>
+      <c r="D51" s="32"/>
+      <c r="E51" s="33"/>
     </row>
     <row r="52" spans="1:8" s="1" customFormat="1">
       <c r="A52" s="8"/>
       <c r="B52" s="8"/>
-      <c r="C52" s="28"/>
-      <c r="D52" s="29"/>
-      <c r="E52" s="30"/>
+      <c r="C52" s="26"/>
+      <c r="D52" s="27"/>
+      <c r="E52" s="28"/>
     </row>
     <row r="53" spans="1:8" s="1" customFormat="1">
       <c r="A53" s="4"/>
       <c r="B53" s="4"/>
-      <c r="C53" s="31"/>
-      <c r="D53" s="34"/>
-      <c r="E53" s="35"/>
+      <c r="C53" s="29"/>
+      <c r="D53" s="32"/>
+      <c r="E53" s="33"/>
     </row>
     <row r="54" spans="1:8" s="1" customFormat="1">
       <c r="A54" s="8"/>
       <c r="B54" s="8"/>
-      <c r="C54" s="28"/>
-      <c r="D54" s="29"/>
-      <c r="E54" s="30"/>
+      <c r="C54" s="26"/>
+      <c r="D54" s="27"/>
+      <c r="E54" s="28"/>
     </row>
     <row r="55" spans="1:8" s="1" customFormat="1" ht="13.35" customHeight="1">
       <c r="A55" s="17"/>
       <c r="B55" s="17"/>
-      <c r="C55" s="69" t="s">
+      <c r="C55" s="67" t="s">
         <v>13</v>
       </c>
-      <c r="D55" s="69"/>
+      <c r="D55" s="67"/>
       <c r="E55" s="3" t="s">
-        <v>29</v>
+        <v>106</v>
       </c>
     </row>
     <row r="56" spans="1:8" s="1" customFormat="1">
       <c r="A56" s="20"/>
       <c r="B56" s="20"/>
-      <c r="C56" s="21"/>
-      <c r="D56" s="22"/>
-      <c r="E56" s="7"/>
+      <c r="C56" s="46" t="s">
+        <v>104</v>
+      </c>
+      <c r="D56" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="E56" s="33" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="57" spans="1:8" s="1" customFormat="1">
       <c r="A57" s="8"/>
       <c r="B57" s="8"/>
-      <c r="C57" s="9"/>
-      <c r="D57" s="10"/>
-      <c r="E57" s="11"/>
+      <c r="C57" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="D57" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="E57" s="28" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="58" spans="1:8" s="1" customFormat="1">
       <c r="A58" s="4"/>
       <c r="B58" s="4"/>
-      <c r="C58" s="5"/>
-      <c r="D58" s="6"/>
-      <c r="E58" s="7"/>
+      <c r="C58" s="29" t="s">
+        <v>108</v>
+      </c>
+      <c r="D58" s="32" t="s">
+        <v>110</v>
+      </c>
+      <c r="E58" s="33" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="59" spans="1:8" s="1" customFormat="1">
       <c r="A59" s="8"/>
       <c r="B59" s="8"/>
-      <c r="C59" s="9"/>
-      <c r="D59" s="10"/>
-      <c r="E59" s="11"/>
-    </row>
-    <row r="60" spans="1:8" s="38" customFormat="1" ht="13.15" customHeight="1">
+      <c r="C59" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="D59" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="E59" s="28" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" s="36" customFormat="1" ht="13.15" customHeight="1">
       <c r="A60" s="4"/>
       <c r="B60" s="4"/>
       <c r="C60" s="5"/>
       <c r="D60" s="6"/>
       <c r="E60" s="7"/>
-      <c r="G60" s="39"/>
-      <c r="H60" s="39"/>
+      <c r="G60" s="37"/>
+      <c r="H60" s="37"/>
     </row>
     <row r="61" spans="1:8" s="1" customFormat="1" ht="13.35" customHeight="1">
       <c r="A61" s="17"/>
       <c r="B61" s="17"/>
-      <c r="C61" s="69" t="s">
+      <c r="C61" s="67" t="s">
         <v>30</v>
       </c>
-      <c r="D61" s="69"/>
+      <c r="D61" s="67"/>
       <c r="E61" s="3" t="s">
         <v>29</v>
       </c>
@@ -1667,260 +1759,260 @@
       <c r="D64" s="10"/>
       <c r="E64" s="11"/>
     </row>
-    <row r="65" spans="1:8" s="38" customFormat="1" ht="13.15" customHeight="1">
+    <row r="65" spans="1:8" s="36" customFormat="1" ht="13.15" customHeight="1">
       <c r="A65" s="4"/>
       <c r="B65" s="4"/>
       <c r="C65" s="5"/>
       <c r="D65" s="6"/>
       <c r="E65" s="7"/>
-      <c r="G65" s="39"/>
-      <c r="H65" s="39"/>
+      <c r="G65" s="37"/>
+      <c r="H65" s="37"/>
     </row>
     <row r="66" spans="1:8" s="1" customFormat="1" ht="13.35" customHeight="1">
       <c r="A66" s="17"/>
       <c r="B66" s="17"/>
-      <c r="C66" s="69" t="s">
+      <c r="C66" s="67" t="s">
         <v>14</v>
       </c>
-      <c r="D66" s="69"/>
+      <c r="D66" s="67"/>
       <c r="E66" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G66" s="23"/>
+      <c r="G66" s="21"/>
     </row>
     <row r="67" spans="1:8" s="1" customFormat="1">
       <c r="A67" s="8"/>
       <c r="B67" s="8"/>
-      <c r="C67" s="28" t="s">
+      <c r="C67" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="D67" s="29" t="s">
+      <c r="D67" s="27" t="s">
         <v>81</v>
       </c>
-      <c r="E67" s="30" t="s">
+      <c r="E67" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="G67" s="23"/>
+      <c r="G67" s="21"/>
     </row>
     <row r="68" spans="1:8" s="1" customFormat="1">
       <c r="A68" s="4"/>
       <c r="B68" s="4"/>
-      <c r="C68" s="31" t="s">
+      <c r="C68" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="D68" s="34" t="s">
+      <c r="D68" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="E68" s="35" t="s">
+      <c r="E68" s="33" t="s">
         <v>72</v>
       </c>
-      <c r="G68" s="23"/>
+      <c r="G68" s="21"/>
     </row>
     <row r="69" spans="1:8" s="1" customFormat="1">
       <c r="A69" s="8"/>
       <c r="B69" s="8"/>
-      <c r="C69" s="25" t="s">
+      <c r="C69" s="23" t="s">
         <v>84</v>
       </c>
-      <c r="D69" s="47" t="s">
+      <c r="D69" s="45" t="s">
         <v>85</v>
       </c>
-      <c r="E69" s="46" t="s">
+      <c r="E69" s="44" t="s">
         <v>86</v>
       </c>
-      <c r="G69" s="23"/>
+      <c r="G69" s="21"/>
     </row>
     <row r="70" spans="1:8" s="1" customFormat="1">
       <c r="A70" s="4"/>
       <c r="B70" s="4"/>
-      <c r="C70" s="31" t="s">
+      <c r="C70" s="29" t="s">
         <v>87</v>
       </c>
-      <c r="D70" s="34" t="s">
+      <c r="D70" s="32" t="s">
         <v>88</v>
       </c>
-      <c r="E70" s="35" t="s">
+      <c r="E70" s="33" t="s">
         <v>79</v>
       </c>
-      <c r="G70" s="23"/>
+      <c r="G70" s="21"/>
     </row>
     <row r="71" spans="1:8" s="1" customFormat="1" ht="13.35" customHeight="1">
       <c r="A71" s="17"/>
       <c r="B71" s="17"/>
-      <c r="C71" s="69" t="s">
+      <c r="C71" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="D71" s="69"/>
+      <c r="D71" s="67"/>
       <c r="E71" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G71" s="23"/>
+      <c r="G71" s="21"/>
     </row>
     <row r="72" spans="1:8" s="1" customFormat="1">
       <c r="A72" s="8"/>
       <c r="B72" s="8"/>
-      <c r="C72" s="26"/>
-      <c r="D72" s="29" t="s">
+      <c r="C72" s="24"/>
+      <c r="D72" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="E72" s="28"/>
-    </row>
-    <row r="73" spans="1:8" s="38" customFormat="1">
+      <c r="E72" s="26"/>
+    </row>
+    <row r="73" spans="1:8" s="36" customFormat="1">
       <c r="A73" s="4"/>
       <c r="B73" s="4"/>
-      <c r="C73" s="31"/>
-      <c r="D73" s="34"/>
-      <c r="E73" s="35"/>
+      <c r="C73" s="29"/>
+      <c r="D73" s="32"/>
+      <c r="E73" s="33"/>
     </row>
     <row r="74" spans="1:8" s="1" customFormat="1">
-      <c r="A74" s="50"/>
-      <c r="B74" s="50"/>
-      <c r="C74" s="25"/>
-      <c r="D74" s="25"/>
-      <c r="E74" s="25"/>
+      <c r="A74" s="48"/>
+      <c r="B74" s="48"/>
+      <c r="C74" s="23"/>
+      <c r="D74" s="23"/>
+      <c r="E74" s="23"/>
     </row>
     <row r="75" spans="1:8" s="1" customFormat="1">
       <c r="A75" s="4"/>
       <c r="B75" s="4"/>
-      <c r="C75" s="35"/>
-      <c r="D75" s="34"/>
-      <c r="E75" s="35"/>
+      <c r="C75" s="33"/>
+      <c r="D75" s="32"/>
+      <c r="E75" s="33"/>
     </row>
     <row r="76" spans="1:8" s="1" customFormat="1">
       <c r="A76" s="8"/>
       <c r="B76" s="8"/>
-      <c r="C76" s="55"/>
-      <c r="D76" s="56"/>
-      <c r="E76" s="57"/>
+      <c r="C76" s="53"/>
+      <c r="D76" s="54"/>
+      <c r="E76" s="55"/>
     </row>
     <row r="77" spans="1:8" s="1" customFormat="1">
       <c r="A77" s="4"/>
       <c r="B77" s="4"/>
-      <c r="C77" s="31"/>
-      <c r="D77" s="34"/>
-      <c r="E77" s="35"/>
+      <c r="C77" s="29"/>
+      <c r="D77" s="32"/>
+      <c r="E77" s="33"/>
     </row>
     <row r="78" spans="1:8" s="1" customFormat="1" ht="13.15" customHeight="1">
       <c r="A78" s="13"/>
       <c r="B78" s="8"/>
-      <c r="C78" s="32"/>
-      <c r="D78" s="47"/>
-      <c r="E78" s="46"/>
-      <c r="F78" s="23"/>
+      <c r="C78" s="30"/>
+      <c r="D78" s="45"/>
+      <c r="E78" s="44"/>
+      <c r="F78" s="21"/>
     </row>
     <row r="79" spans="1:8" s="1" customFormat="1">
       <c r="A79" s="4"/>
       <c r="B79" s="4"/>
-      <c r="C79" s="31"/>
-      <c r="D79" s="34"/>
-      <c r="E79" s="35"/>
+      <c r="C79" s="29"/>
+      <c r="D79" s="32"/>
+      <c r="E79" s="33"/>
     </row>
     <row r="80" spans="1:8" s="1" customFormat="1" ht="13.15" customHeight="1">
       <c r="A80" s="13"/>
       <c r="B80" s="8"/>
-      <c r="C80" s="25"/>
-      <c r="D80" s="47"/>
-      <c r="E80" s="46"/>
-      <c r="F80" s="23"/>
+      <c r="C80" s="23"/>
+      <c r="D80" s="45"/>
+      <c r="E80" s="44"/>
+      <c r="F80" s="21"/>
     </row>
     <row r="81" spans="1:7" s="1" customFormat="1">
       <c r="A81" s="4"/>
       <c r="B81" s="4"/>
-      <c r="C81" s="31"/>
-      <c r="D81" s="34"/>
-      <c r="E81" s="35"/>
+      <c r="C81" s="29"/>
+      <c r="D81" s="32"/>
+      <c r="E81" s="33"/>
     </row>
     <row r="82" spans="1:7" s="1" customFormat="1" ht="12.75" customHeight="1">
       <c r="A82" s="13"/>
       <c r="B82" s="8"/>
-      <c r="C82" s="25"/>
-      <c r="D82" s="47"/>
-      <c r="E82" s="61"/>
-      <c r="F82" s="23"/>
+      <c r="C82" s="23"/>
+      <c r="D82" s="45"/>
+      <c r="E82" s="59"/>
+      <c r="F82" s="21"/>
     </row>
     <row r="83" spans="1:7" s="1" customFormat="1">
       <c r="A83" s="4"/>
       <c r="B83" s="4"/>
-      <c r="C83" s="31"/>
-      <c r="D83" s="34"/>
-      <c r="E83" s="46"/>
+      <c r="C83" s="29"/>
+      <c r="D83" s="32"/>
+      <c r="E83" s="44"/>
     </row>
     <row r="84" spans="1:7" s="1" customFormat="1" ht="13.15" customHeight="1">
       <c r="A84" s="13"/>
       <c r="B84" s="8"/>
-      <c r="C84" s="25"/>
-      <c r="D84" s="47"/>
-      <c r="E84" s="46"/>
-      <c r="F84" s="23"/>
+      <c r="C84" s="23"/>
+      <c r="D84" s="45"/>
+      <c r="E84" s="44"/>
+      <c r="F84" s="21"/>
     </row>
     <row r="85" spans="1:7" s="1" customFormat="1">
       <c r="A85" s="4"/>
       <c r="B85" s="4"/>
-      <c r="C85" s="31"/>
+      <c r="C85" s="29"/>
       <c r="D85" s="6"/>
-      <c r="E85" s="35"/>
+      <c r="E85" s="33"/>
     </row>
     <row r="86" spans="1:7" s="1" customFormat="1" ht="13.15" customHeight="1">
       <c r="A86" s="13"/>
       <c r="B86" s="8"/>
-      <c r="C86" s="25"/>
-      <c r="D86" s="47"/>
-      <c r="E86" s="46"/>
-      <c r="F86" s="23"/>
+      <c r="C86" s="23"/>
+      <c r="D86" s="45"/>
+      <c r="E86" s="44"/>
+      <c r="F86" s="21"/>
     </row>
     <row r="87" spans="1:7" s="1" customFormat="1">
       <c r="A87" s="4"/>
       <c r="B87" s="4"/>
-      <c r="C87" s="31"/>
-      <c r="D87" s="34"/>
-      <c r="E87" s="35"/>
+      <c r="C87" s="29"/>
+      <c r="D87" s="32"/>
+      <c r="E87" s="33"/>
     </row>
     <row r="88" spans="1:7" s="1" customFormat="1" ht="12.75" customHeight="1">
       <c r="A88" s="13"/>
       <c r="B88" s="8"/>
-      <c r="C88" s="25"/>
+      <c r="C88" s="23"/>
       <c r="D88" s="15"/>
-      <c r="E88" s="46"/>
-      <c r="F88" s="23"/>
+      <c r="E88" s="44"/>
+      <c r="F88" s="21"/>
     </row>
     <row r="89" spans="1:7" s="1" customFormat="1" ht="13.5" customHeight="1">
       <c r="A89" s="4"/>
       <c r="B89" s="4"/>
-      <c r="C89" s="31"/>
-      <c r="D89" s="34"/>
-      <c r="E89" s="35"/>
+      <c r="C89" s="29"/>
+      <c r="D89" s="32"/>
+      <c r="E89" s="33"/>
     </row>
     <row r="90" spans="1:7" s="1" customFormat="1" ht="13.15" customHeight="1">
       <c r="A90" s="13"/>
       <c r="B90" s="8"/>
-      <c r="C90" s="25"/>
-      <c r="D90" s="47"/>
-      <c r="E90" s="46"/>
-      <c r="F90" s="23"/>
+      <c r="C90" s="23"/>
+      <c r="D90" s="45"/>
+      <c r="E90" s="44"/>
+      <c r="F90" s="21"/>
     </row>
     <row r="91" spans="1:7" s="1" customFormat="1">
       <c r="A91" s="4"/>
       <c r="B91" s="4"/>
-      <c r="C91" s="31"/>
-      <c r="D91" s="34"/>
-      <c r="E91" s="35"/>
+      <c r="C91" s="29"/>
+      <c r="D91" s="32"/>
+      <c r="E91" s="33"/>
     </row>
     <row r="92" spans="1:7" s="1" customFormat="1" ht="13.35" customHeight="1">
       <c r="A92" s="17"/>
       <c r="B92" s="17"/>
-      <c r="C92" s="69" t="s">
+      <c r="C92" s="67" t="s">
         <v>18</v>
       </c>
-      <c r="D92" s="69"/>
+      <c r="D92" s="67"/>
       <c r="E92" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G92" s="23"/>
+      <c r="G92" s="21"/>
     </row>
     <row r="93" spans="1:7" s="1" customFormat="1">
       <c r="A93" s="8"/>
       <c r="B93" s="8"/>
-      <c r="C93" s="26" t="s">
+      <c r="C93" s="24" t="s">
         <v>23</v>
       </c>
       <c r="D93" s="10" t="s">
@@ -1940,7 +2032,7 @@
     <row r="95" spans="1:7" s="1" customFormat="1">
       <c r="A95" s="8"/>
       <c r="B95" s="8"/>
-      <c r="C95" s="25"/>
+      <c r="C95" s="23"/>
       <c r="D95" s="15"/>
       <c r="E95" s="16"/>
     </row>
@@ -1954,7 +2046,7 @@
     <row r="97" spans="1:6" s="1" customFormat="1" ht="13.35" customHeight="1">
       <c r="A97" s="8"/>
       <c r="B97" s="8"/>
-      <c r="C97" s="23"/>
+      <c r="C97" s="21"/>
       <c r="D97" s="15"/>
       <c r="E97" s="16"/>
     </row>
@@ -1978,7 +2070,7 @@
       <c r="C100" s="5"/>
       <c r="D100" s="6"/>
       <c r="E100" s="7"/>
-      <c r="F100" s="23"/>
+      <c r="F100" s="21"/>
     </row>
     <row r="101" spans="1:6" s="1" customFormat="1">
       <c r="A101" s="13"/>
@@ -1997,11 +2089,11 @@
     <row r="103" spans="1:6" s="1" customFormat="1">
       <c r="A103" s="17"/>
       <c r="B103" s="17"/>
-      <c r="C103" s="62" t="s">
+      <c r="C103" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="D103" s="24"/>
-      <c r="E103" s="62" t="s">
+      <c r="D103" s="22"/>
+      <c r="E103" s="60" t="s">
         <v>26</v>
       </c>
     </row>
@@ -2011,10 +2103,10 @@
       <c r="C104" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D104" s="29" t="s">
+      <c r="D104" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="E104" s="46" t="s">
+      <c r="E104" s="44" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2027,40 +2119,40 @@
       <c r="D105" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E105" s="35" t="s">
+      <c r="E105" s="33" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="106" spans="1:6" s="1" customFormat="1">
       <c r="A106" s="13"/>
       <c r="B106" s="13"/>
-      <c r="C106" s="28" t="s">
+      <c r="C106" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="D106" s="29" t="s">
+      <c r="D106" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="E106" s="46" t="s">
+      <c r="E106" s="44" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="107" spans="1:6" s="1" customFormat="1">
       <c r="A107" s="4"/>
       <c r="B107" s="4"/>
-      <c r="C107" s="31" t="s">
+      <c r="C107" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="D107" s="34" t="s">
+      <c r="D107" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="E107" s="35" t="s">
+      <c r="E107" s="33" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="108" spans="1:6" s="1" customFormat="1">
       <c r="A108" s="13"/>
       <c r="B108" s="13"/>
-      <c r="C108" s="25" t="s">
+      <c r="C108" s="23" t="s">
         <v>31</v>
       </c>
       <c r="D108" s="15" t="s">
@@ -2073,936 +2165,936 @@
     <row r="109" spans="1:6" s="1" customFormat="1">
       <c r="A109" s="4"/>
       <c r="B109" s="4"/>
-      <c r="C109" s="31" t="s">
+      <c r="C109" s="29" t="s">
         <v>89</v>
       </c>
       <c r="D109" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E109" s="35" t="s">
+      <c r="E109" s="33" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="110" spans="1:6" s="1" customFormat="1">
       <c r="A110" s="13"/>
       <c r="B110" s="13"/>
-      <c r="C110" s="25" t="s">
+      <c r="C110" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="D110" s="47" t="s">
+      <c r="D110" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="E110" s="25" t="s">
+      <c r="E110" s="23" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="111" spans="1:6" s="1" customFormat="1">
       <c r="A111" s="4"/>
       <c r="B111" s="4"/>
-      <c r="C111" s="31" t="s">
+      <c r="C111" s="29" t="s">
         <v>35</v>
       </c>
       <c r="D111" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E111" s="35" t="s">
+      <c r="E111" s="33" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="112" spans="1:6" s="1" customFormat="1">
       <c r="A112" s="13"/>
       <c r="B112" s="13"/>
-      <c r="C112" s="25" t="s">
+      <c r="C112" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="D112" s="47" t="s">
+      <c r="D112" s="45" t="s">
         <v>91</v>
       </c>
-      <c r="E112" s="25" t="s">
+      <c r="E112" s="23" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="113" spans="1:5" s="1" customFormat="1">
       <c r="A113" s="4"/>
       <c r="B113" s="4"/>
-      <c r="C113" s="31"/>
-      <c r="D113" s="6"/>
-      <c r="E113" s="35"/>
+      <c r="C113" s="29"/>
+      <c r="D113" s="32"/>
+      <c r="E113" s="33"/>
     </row>
     <row r="114" spans="1:5" s="1" customFormat="1">
-      <c r="A114" s="63"/>
-      <c r="B114" s="63"/>
-      <c r="C114" s="63"/>
-      <c r="D114" s="64"/>
-      <c r="E114" s="65"/>
+      <c r="A114" s="61"/>
+      <c r="B114" s="61"/>
+      <c r="C114" s="61"/>
+      <c r="D114" s="62"/>
+      <c r="E114" s="63"/>
     </row>
     <row r="115" spans="1:5" s="1" customFormat="1">
-      <c r="A115" s="63"/>
-      <c r="B115" s="63"/>
-      <c r="C115" s="63"/>
-      <c r="D115" s="64"/>
-      <c r="E115" s="65"/>
+      <c r="A115" s="61"/>
+      <c r="B115" s="61"/>
+      <c r="C115" s="61"/>
+      <c r="D115" s="62"/>
+      <c r="E115" s="63"/>
     </row>
     <row r="116" spans="1:5" s="1" customFormat="1">
-      <c r="A116" s="63"/>
-      <c r="B116" s="63"/>
-      <c r="C116" s="63"/>
-      <c r="D116" s="64"/>
-      <c r="E116" s="65"/>
+      <c r="A116" s="61"/>
+      <c r="B116" s="61"/>
+      <c r="C116" s="61"/>
+      <c r="D116" s="62"/>
+      <c r="E116" s="63"/>
     </row>
     <row r="117" spans="1:5" s="1" customFormat="1">
-      <c r="A117" s="63"/>
-      <c r="B117" s="63"/>
-      <c r="C117" s="63"/>
-      <c r="D117" s="64"/>
-      <c r="E117" s="65"/>
+      <c r="A117" s="61"/>
+      <c r="B117" s="61"/>
+      <c r="C117" s="61"/>
+      <c r="D117" s="62"/>
+      <c r="E117" s="63"/>
     </row>
     <row r="118" spans="1:5" s="1" customFormat="1">
-      <c r="A118" s="63"/>
-      <c r="B118" s="63"/>
-      <c r="C118" s="63"/>
-      <c r="D118" s="64"/>
-      <c r="E118" s="65"/>
+      <c r="A118" s="61"/>
+      <c r="B118" s="61"/>
+      <c r="C118" s="61"/>
+      <c r="D118" s="62"/>
+      <c r="E118" s="63"/>
     </row>
     <row r="119" spans="1:5" s="1" customFormat="1">
-      <c r="A119" s="63"/>
-      <c r="B119" s="63"/>
-      <c r="C119" s="63"/>
-      <c r="D119" s="64"/>
-      <c r="E119" s="65"/>
+      <c r="A119" s="61"/>
+      <c r="B119" s="61"/>
+      <c r="C119" s="61"/>
+      <c r="D119" s="62"/>
+      <c r="E119" s="63"/>
     </row>
     <row r="120" spans="1:5" s="1" customFormat="1">
-      <c r="A120" s="63"/>
-      <c r="B120" s="63"/>
-      <c r="C120" s="63"/>
-      <c r="D120" s="64"/>
-      <c r="E120" s="65"/>
+      <c r="A120" s="61"/>
+      <c r="B120" s="61"/>
+      <c r="C120" s="61"/>
+      <c r="D120" s="62"/>
+      <c r="E120" s="63"/>
     </row>
     <row r="121" spans="1:5" s="1" customFormat="1">
-      <c r="A121" s="63"/>
-      <c r="B121" s="63"/>
-      <c r="C121" s="63"/>
-      <c r="D121" s="64"/>
-      <c r="E121" s="65"/>
+      <c r="A121" s="61"/>
+      <c r="B121" s="61"/>
+      <c r="C121" s="61"/>
+      <c r="D121" s="62"/>
+      <c r="E121" s="63"/>
     </row>
     <row r="122" spans="1:5" s="1" customFormat="1">
-      <c r="A122" s="63"/>
-      <c r="B122" s="63"/>
-      <c r="C122" s="63"/>
-      <c r="D122" s="64"/>
-      <c r="E122" s="65"/>
+      <c r="A122" s="61"/>
+      <c r="B122" s="61"/>
+      <c r="C122" s="61"/>
+      <c r="D122" s="62"/>
+      <c r="E122" s="63"/>
     </row>
     <row r="123" spans="1:5" s="1" customFormat="1">
-      <c r="A123" s="63"/>
-      <c r="B123" s="63"/>
-      <c r="C123" s="63"/>
-      <c r="D123" s="64"/>
-      <c r="E123" s="65"/>
+      <c r="A123" s="61"/>
+      <c r="B123" s="61"/>
+      <c r="C123" s="61"/>
+      <c r="D123" s="62"/>
+      <c r="E123" s="63"/>
     </row>
     <row r="124" spans="1:5" s="1" customFormat="1">
-      <c r="A124" s="63"/>
-      <c r="B124" s="63"/>
-      <c r="C124" s="63"/>
-      <c r="D124" s="64"/>
-      <c r="E124" s="65"/>
+      <c r="A124" s="61"/>
+      <c r="B124" s="61"/>
+      <c r="C124" s="61"/>
+      <c r="D124" s="62"/>
+      <c r="E124" s="63"/>
     </row>
     <row r="125" spans="1:5" s="1" customFormat="1">
-      <c r="A125" s="63"/>
-      <c r="B125" s="63"/>
-      <c r="C125" s="63"/>
-      <c r="D125" s="64"/>
-      <c r="E125" s="65"/>
+      <c r="A125" s="61"/>
+      <c r="B125" s="61"/>
+      <c r="C125" s="61"/>
+      <c r="D125" s="62"/>
+      <c r="E125" s="63"/>
     </row>
     <row r="126" spans="1:5" s="1" customFormat="1">
-      <c r="A126" s="63"/>
-      <c r="B126" s="63"/>
-      <c r="C126" s="63"/>
-      <c r="D126" s="64"/>
-      <c r="E126" s="65"/>
+      <c r="A126" s="61"/>
+      <c r="B126" s="61"/>
+      <c r="C126" s="61"/>
+      <c r="D126" s="62"/>
+      <c r="E126" s="63"/>
     </row>
     <row r="127" spans="1:5" s="1" customFormat="1">
-      <c r="A127" s="63"/>
-      <c r="B127" s="63"/>
-      <c r="C127" s="63"/>
-      <c r="D127" s="64"/>
-      <c r="E127" s="65"/>
+      <c r="A127" s="61"/>
+      <c r="B127" s="61"/>
+      <c r="C127" s="61"/>
+      <c r="D127" s="62"/>
+      <c r="E127" s="63"/>
     </row>
     <row r="128" spans="1:5" s="1" customFormat="1">
-      <c r="A128" s="63"/>
-      <c r="B128" s="63"/>
-      <c r="C128" s="63"/>
-      <c r="D128" s="64"/>
-      <c r="E128" s="65"/>
+      <c r="A128" s="61"/>
+      <c r="B128" s="61"/>
+      <c r="C128" s="61"/>
+      <c r="D128" s="62"/>
+      <c r="E128" s="63"/>
     </row>
     <row r="129" spans="1:5" s="1" customFormat="1">
-      <c r="A129" s="63"/>
-      <c r="B129" s="63"/>
-      <c r="C129" s="63"/>
-      <c r="D129" s="64"/>
-      <c r="E129" s="65"/>
+      <c r="A129" s="61"/>
+      <c r="B129" s="61"/>
+      <c r="C129" s="61"/>
+      <c r="D129" s="62"/>
+      <c r="E129" s="63"/>
     </row>
     <row r="130" spans="1:5" s="1" customFormat="1">
-      <c r="A130" s="63"/>
-      <c r="B130" s="63"/>
-      <c r="C130" s="63"/>
-      <c r="D130" s="64"/>
-      <c r="E130" s="65"/>
+      <c r="A130" s="61"/>
+      <c r="B130" s="61"/>
+      <c r="C130" s="61"/>
+      <c r="D130" s="62"/>
+      <c r="E130" s="63"/>
     </row>
     <row r="131" spans="1:5" s="1" customFormat="1">
-      <c r="A131" s="63"/>
-      <c r="B131" s="63"/>
-      <c r="C131" s="63"/>
-      <c r="D131" s="64"/>
-      <c r="E131" s="65"/>
+      <c r="A131" s="61"/>
+      <c r="B131" s="61"/>
+      <c r="C131" s="61"/>
+      <c r="D131" s="62"/>
+      <c r="E131" s="63"/>
     </row>
     <row r="132" spans="1:5" s="1" customFormat="1">
-      <c r="A132" s="63"/>
-      <c r="B132" s="63"/>
-      <c r="C132" s="63"/>
-      <c r="D132" s="64"/>
-      <c r="E132" s="65"/>
+      <c r="A132" s="61"/>
+      <c r="B132" s="61"/>
+      <c r="C132" s="61"/>
+      <c r="D132" s="62"/>
+      <c r="E132" s="63"/>
     </row>
     <row r="133" spans="1:5" s="1" customFormat="1">
-      <c r="A133" s="63"/>
-      <c r="B133" s="63"/>
-      <c r="C133" s="63"/>
-      <c r="D133" s="64"/>
-      <c r="E133" s="65"/>
+      <c r="A133" s="61"/>
+      <c r="B133" s="61"/>
+      <c r="C133" s="61"/>
+      <c r="D133" s="62"/>
+      <c r="E133" s="63"/>
     </row>
     <row r="134" spans="1:5" s="1" customFormat="1">
-      <c r="A134" s="63"/>
-      <c r="B134" s="63"/>
-      <c r="C134" s="63"/>
-      <c r="D134" s="64"/>
-      <c r="E134" s="65"/>
+      <c r="A134" s="61"/>
+      <c r="B134" s="61"/>
+      <c r="C134" s="61"/>
+      <c r="D134" s="62"/>
+      <c r="E134" s="63"/>
     </row>
     <row r="135" spans="1:5" s="1" customFormat="1">
-      <c r="A135" s="63"/>
-      <c r="B135" s="63"/>
-      <c r="C135" s="63"/>
-      <c r="D135" s="64"/>
-      <c r="E135" s="65"/>
+      <c r="A135" s="61"/>
+      <c r="B135" s="61"/>
+      <c r="C135" s="61"/>
+      <c r="D135" s="62"/>
+      <c r="E135" s="63"/>
     </row>
     <row r="136" spans="1:5" s="1" customFormat="1">
-      <c r="A136" s="63"/>
-      <c r="B136" s="63"/>
-      <c r="C136" s="63"/>
-      <c r="D136" s="64"/>
-      <c r="E136" s="65"/>
+      <c r="A136" s="61"/>
+      <c r="B136" s="61"/>
+      <c r="C136" s="61"/>
+      <c r="D136" s="62"/>
+      <c r="E136" s="63"/>
     </row>
     <row r="137" spans="1:5" s="1" customFormat="1">
-      <c r="A137" s="63"/>
-      <c r="B137" s="63"/>
-      <c r="C137" s="63"/>
-      <c r="D137" s="64"/>
-      <c r="E137" s="65"/>
+      <c r="A137" s="61"/>
+      <c r="B137" s="61"/>
+      <c r="C137" s="61"/>
+      <c r="D137" s="62"/>
+      <c r="E137" s="63"/>
     </row>
     <row r="138" spans="1:5" s="1" customFormat="1">
-      <c r="A138" s="63"/>
-      <c r="B138" s="63"/>
-      <c r="C138" s="63"/>
-      <c r="D138" s="64"/>
-      <c r="E138" s="65"/>
+      <c r="A138" s="61"/>
+      <c r="B138" s="61"/>
+      <c r="C138" s="61"/>
+      <c r="D138" s="62"/>
+      <c r="E138" s="63"/>
     </row>
     <row r="139" spans="1:5" s="1" customFormat="1">
-      <c r="A139" s="63"/>
-      <c r="B139" s="63"/>
-      <c r="C139" s="63"/>
-      <c r="D139" s="64"/>
-      <c r="E139" s="65"/>
+      <c r="A139" s="61"/>
+      <c r="B139" s="61"/>
+      <c r="C139" s="61"/>
+      <c r="D139" s="62"/>
+      <c r="E139" s="63"/>
     </row>
     <row r="140" spans="1:5" s="1" customFormat="1">
-      <c r="A140" s="63"/>
-      <c r="B140" s="63"/>
-      <c r="C140" s="63"/>
-      <c r="D140" s="64"/>
-      <c r="E140" s="65"/>
+      <c r="A140" s="61"/>
+      <c r="B140" s="61"/>
+      <c r="C140" s="61"/>
+      <c r="D140" s="62"/>
+      <c r="E140" s="63"/>
     </row>
     <row r="141" spans="1:5" s="1" customFormat="1">
-      <c r="A141" s="63"/>
-      <c r="B141" s="63"/>
-      <c r="C141" s="63"/>
-      <c r="D141" s="64"/>
-      <c r="E141" s="65"/>
+      <c r="A141" s="61"/>
+      <c r="B141" s="61"/>
+      <c r="C141" s="61"/>
+      <c r="D141" s="62"/>
+      <c r="E141" s="63"/>
     </row>
     <row r="142" spans="1:5" s="1" customFormat="1">
-      <c r="A142" s="63"/>
-      <c r="B142" s="63"/>
-      <c r="C142" s="63"/>
-      <c r="D142" s="64"/>
-      <c r="E142" s="65"/>
+      <c r="A142" s="61"/>
+      <c r="B142" s="61"/>
+      <c r="C142" s="61"/>
+      <c r="D142" s="62"/>
+      <c r="E142" s="63"/>
     </row>
     <row r="143" spans="1:5" s="1" customFormat="1">
-      <c r="A143" s="63"/>
-      <c r="B143" s="63"/>
-      <c r="C143" s="63"/>
-      <c r="D143" s="64"/>
-      <c r="E143" s="65"/>
+      <c r="A143" s="61"/>
+      <c r="B143" s="61"/>
+      <c r="C143" s="61"/>
+      <c r="D143" s="62"/>
+      <c r="E143" s="63"/>
     </row>
     <row r="144" spans="1:5" s="1" customFormat="1">
-      <c r="A144" s="63"/>
-      <c r="B144" s="63"/>
-      <c r="C144" s="63"/>
-      <c r="D144" s="64"/>
-      <c r="E144" s="65"/>
+      <c r="A144" s="61"/>
+      <c r="B144" s="61"/>
+      <c r="C144" s="61"/>
+      <c r="D144" s="62"/>
+      <c r="E144" s="63"/>
     </row>
     <row r="145" spans="1:5" s="1" customFormat="1">
-      <c r="A145" s="63"/>
-      <c r="B145" s="63"/>
-      <c r="C145" s="63"/>
-      <c r="D145" s="64"/>
-      <c r="E145" s="65"/>
+      <c r="A145" s="61"/>
+      <c r="B145" s="61"/>
+      <c r="C145" s="61"/>
+      <c r="D145" s="62"/>
+      <c r="E145" s="63"/>
     </row>
     <row r="146" spans="1:5" s="1" customFormat="1">
-      <c r="A146" s="63"/>
-      <c r="B146" s="63"/>
-      <c r="C146" s="63"/>
-      <c r="D146" s="64"/>
-      <c r="E146" s="65"/>
+      <c r="A146" s="61"/>
+      <c r="B146" s="61"/>
+      <c r="C146" s="61"/>
+      <c r="D146" s="62"/>
+      <c r="E146" s="63"/>
     </row>
     <row r="147" spans="1:5" s="1" customFormat="1">
-      <c r="A147" s="63"/>
-      <c r="B147" s="63"/>
-      <c r="C147" s="63"/>
-      <c r="D147" s="64"/>
-      <c r="E147" s="65"/>
+      <c r="A147" s="61"/>
+      <c r="B147" s="61"/>
+      <c r="C147" s="61"/>
+      <c r="D147" s="62"/>
+      <c r="E147" s="63"/>
     </row>
     <row r="148" spans="1:5" s="1" customFormat="1">
-      <c r="A148" s="63"/>
-      <c r="B148" s="63"/>
-      <c r="C148" s="63"/>
-      <c r="D148" s="64"/>
-      <c r="E148" s="65"/>
+      <c r="A148" s="61"/>
+      <c r="B148" s="61"/>
+      <c r="C148" s="61"/>
+      <c r="D148" s="62"/>
+      <c r="E148" s="63"/>
     </row>
     <row r="149" spans="1:5" s="1" customFormat="1">
-      <c r="A149" s="63"/>
-      <c r="B149" s="63"/>
-      <c r="C149" s="63"/>
-      <c r="D149" s="64"/>
-      <c r="E149" s="65"/>
+      <c r="A149" s="61"/>
+      <c r="B149" s="61"/>
+      <c r="C149" s="61"/>
+      <c r="D149" s="62"/>
+      <c r="E149" s="63"/>
     </row>
     <row r="150" spans="1:5" s="1" customFormat="1">
-      <c r="A150" s="63"/>
-      <c r="B150" s="63"/>
-      <c r="C150" s="63"/>
-      <c r="D150" s="64"/>
-      <c r="E150" s="65"/>
+      <c r="A150" s="61"/>
+      <c r="B150" s="61"/>
+      <c r="C150" s="61"/>
+      <c r="D150" s="62"/>
+      <c r="E150" s="63"/>
     </row>
     <row r="151" spans="1:5" s="1" customFormat="1">
-      <c r="A151" s="63"/>
-      <c r="B151" s="63"/>
-      <c r="C151" s="63"/>
-      <c r="D151" s="64"/>
-      <c r="E151" s="65"/>
+      <c r="A151" s="61"/>
+      <c r="B151" s="61"/>
+      <c r="C151" s="61"/>
+      <c r="D151" s="62"/>
+      <c r="E151" s="63"/>
     </row>
     <row r="152" spans="1:5" s="1" customFormat="1">
-      <c r="A152" s="63"/>
-      <c r="B152" s="63"/>
-      <c r="C152" s="63"/>
-      <c r="D152" s="64"/>
-      <c r="E152" s="65"/>
+      <c r="A152" s="61"/>
+      <c r="B152" s="61"/>
+      <c r="C152" s="61"/>
+      <c r="D152" s="62"/>
+      <c r="E152" s="63"/>
     </row>
     <row r="153" spans="1:5" s="1" customFormat="1">
-      <c r="A153" s="63"/>
-      <c r="B153" s="63"/>
-      <c r="C153" s="63"/>
-      <c r="D153" s="64"/>
-      <c r="E153" s="65"/>
+      <c r="A153" s="61"/>
+      <c r="B153" s="61"/>
+      <c r="C153" s="61"/>
+      <c r="D153" s="62"/>
+      <c r="E153" s="63"/>
     </row>
     <row r="154" spans="1:5" s="1" customFormat="1">
-      <c r="A154" s="63"/>
-      <c r="B154" s="63"/>
-      <c r="C154" s="63"/>
-      <c r="D154" s="64"/>
-      <c r="E154" s="65"/>
+      <c r="A154" s="61"/>
+      <c r="B154" s="61"/>
+      <c r="C154" s="61"/>
+      <c r="D154" s="62"/>
+      <c r="E154" s="63"/>
     </row>
     <row r="155" spans="1:5" s="1" customFormat="1">
-      <c r="A155" s="63"/>
-      <c r="B155" s="63"/>
-      <c r="C155" s="63"/>
-      <c r="D155" s="64"/>
-      <c r="E155" s="65"/>
+      <c r="A155" s="61"/>
+      <c r="B155" s="61"/>
+      <c r="C155" s="61"/>
+      <c r="D155" s="62"/>
+      <c r="E155" s="63"/>
     </row>
     <row r="156" spans="1:5" s="1" customFormat="1">
-      <c r="A156" s="63"/>
-      <c r="B156" s="63"/>
-      <c r="C156" s="63"/>
-      <c r="D156" s="64"/>
-      <c r="E156" s="65"/>
+      <c r="A156" s="61"/>
+      <c r="B156" s="61"/>
+      <c r="C156" s="61"/>
+      <c r="D156" s="62"/>
+      <c r="E156" s="63"/>
     </row>
     <row r="157" spans="1:5" s="1" customFormat="1">
-      <c r="A157" s="63"/>
-      <c r="B157" s="63"/>
-      <c r="C157" s="63"/>
-      <c r="D157" s="64"/>
-      <c r="E157" s="65"/>
+      <c r="A157" s="61"/>
+      <c r="B157" s="61"/>
+      <c r="C157" s="61"/>
+      <c r="D157" s="62"/>
+      <c r="E157" s="63"/>
     </row>
     <row r="158" spans="1:5" s="1" customFormat="1">
-      <c r="A158" s="63"/>
-      <c r="B158" s="63"/>
-      <c r="C158" s="63"/>
-      <c r="D158" s="64"/>
-      <c r="E158" s="65"/>
+      <c r="A158" s="61"/>
+      <c r="B158" s="61"/>
+      <c r="C158" s="61"/>
+      <c r="D158" s="62"/>
+      <c r="E158" s="63"/>
     </row>
     <row r="159" spans="1:5" s="1" customFormat="1">
-      <c r="A159" s="63"/>
-      <c r="B159" s="63"/>
-      <c r="C159" s="63"/>
-      <c r="D159" s="64"/>
-      <c r="E159" s="65"/>
+      <c r="A159" s="61"/>
+      <c r="B159" s="61"/>
+      <c r="C159" s="61"/>
+      <c r="D159" s="62"/>
+      <c r="E159" s="63"/>
     </row>
     <row r="160" spans="1:5" s="1" customFormat="1">
-      <c r="A160" s="63"/>
-      <c r="B160" s="63"/>
-      <c r="C160" s="63"/>
-      <c r="D160" s="64"/>
-      <c r="E160" s="65"/>
+      <c r="A160" s="61"/>
+      <c r="B160" s="61"/>
+      <c r="C160" s="61"/>
+      <c r="D160" s="62"/>
+      <c r="E160" s="63"/>
     </row>
     <row r="161" spans="1:5" s="1" customFormat="1">
-      <c r="A161" s="63"/>
-      <c r="B161" s="63"/>
-      <c r="C161" s="63"/>
-      <c r="D161" s="64"/>
-      <c r="E161" s="65"/>
+      <c r="A161" s="61"/>
+      <c r="B161" s="61"/>
+      <c r="C161" s="61"/>
+      <c r="D161" s="62"/>
+      <c r="E161" s="63"/>
     </row>
     <row r="162" spans="1:5" s="1" customFormat="1">
-      <c r="A162" s="63"/>
-      <c r="B162" s="63"/>
-      <c r="C162" s="63"/>
-      <c r="D162" s="64"/>
-      <c r="E162" s="65"/>
+      <c r="A162" s="61"/>
+      <c r="B162" s="61"/>
+      <c r="C162" s="61"/>
+      <c r="D162" s="62"/>
+      <c r="E162" s="63"/>
     </row>
     <row r="163" spans="1:5" s="1" customFormat="1">
-      <c r="A163" s="63"/>
-      <c r="B163" s="63"/>
-      <c r="C163" s="63"/>
-      <c r="D163" s="64"/>
-      <c r="E163" s="65"/>
+      <c r="A163" s="61"/>
+      <c r="B163" s="61"/>
+      <c r="C163" s="61"/>
+      <c r="D163" s="62"/>
+      <c r="E163" s="63"/>
     </row>
     <row r="164" spans="1:5" s="1" customFormat="1">
-      <c r="A164" s="63"/>
-      <c r="B164" s="63"/>
-      <c r="C164" s="63"/>
-      <c r="D164" s="64"/>
-      <c r="E164" s="65"/>
+      <c r="A164" s="61"/>
+      <c r="B164" s="61"/>
+      <c r="C164" s="61"/>
+      <c r="D164" s="62"/>
+      <c r="E164" s="63"/>
     </row>
     <row r="165" spans="1:5" s="1" customFormat="1">
-      <c r="A165" s="63"/>
-      <c r="B165" s="63"/>
-      <c r="C165" s="63"/>
-      <c r="D165" s="64"/>
-      <c r="E165" s="65"/>
+      <c r="A165" s="61"/>
+      <c r="B165" s="61"/>
+      <c r="C165" s="61"/>
+      <c r="D165" s="62"/>
+      <c r="E165" s="63"/>
     </row>
     <row r="166" spans="1:5" s="1" customFormat="1">
-      <c r="A166" s="63"/>
-      <c r="B166" s="63"/>
-      <c r="C166" s="63"/>
-      <c r="D166" s="64"/>
-      <c r="E166" s="65"/>
+      <c r="A166" s="61"/>
+      <c r="B166" s="61"/>
+      <c r="C166" s="61"/>
+      <c r="D166" s="62"/>
+      <c r="E166" s="63"/>
     </row>
     <row r="167" spans="1:5" s="1" customFormat="1">
-      <c r="A167" s="63"/>
-      <c r="B167" s="63"/>
-      <c r="C167" s="63"/>
-      <c r="D167" s="64"/>
-      <c r="E167" s="65"/>
+      <c r="A167" s="61"/>
+      <c r="B167" s="61"/>
+      <c r="C167" s="61"/>
+      <c r="D167" s="62"/>
+      <c r="E167" s="63"/>
     </row>
     <row r="168" spans="1:5" s="1" customFormat="1">
-      <c r="A168" s="63"/>
-      <c r="B168" s="63"/>
-      <c r="C168" s="63"/>
-      <c r="D168" s="64"/>
-      <c r="E168" s="65"/>
+      <c r="A168" s="61"/>
+      <c r="B168" s="61"/>
+      <c r="C168" s="61"/>
+      <c r="D168" s="62"/>
+      <c r="E168" s="63"/>
     </row>
     <row r="169" spans="1:5" s="1" customFormat="1">
-      <c r="A169" s="63"/>
-      <c r="B169" s="63"/>
-      <c r="C169" s="63"/>
-      <c r="D169" s="64"/>
-      <c r="E169" s="65"/>
+      <c r="A169" s="61"/>
+      <c r="B169" s="61"/>
+      <c r="C169" s="61"/>
+      <c r="D169" s="62"/>
+      <c r="E169" s="63"/>
     </row>
     <row r="170" spans="1:5" s="1" customFormat="1">
-      <c r="A170" s="63"/>
-      <c r="B170" s="63"/>
-      <c r="C170" s="63"/>
-      <c r="D170" s="64"/>
-      <c r="E170" s="65"/>
+      <c r="A170" s="61"/>
+      <c r="B170" s="61"/>
+      <c r="C170" s="61"/>
+      <c r="D170" s="62"/>
+      <c r="E170" s="63"/>
     </row>
     <row r="171" spans="1:5" s="1" customFormat="1">
-      <c r="A171" s="63"/>
-      <c r="B171" s="63"/>
-      <c r="C171" s="63"/>
-      <c r="D171" s="64"/>
-      <c r="E171" s="65"/>
+      <c r="A171" s="61"/>
+      <c r="B171" s="61"/>
+      <c r="C171" s="61"/>
+      <c r="D171" s="62"/>
+      <c r="E171" s="63"/>
     </row>
     <row r="172" spans="1:5" s="1" customFormat="1">
-      <c r="A172" s="63"/>
-      <c r="B172" s="63"/>
-      <c r="C172" s="63"/>
-      <c r="D172" s="64"/>
-      <c r="E172" s="65"/>
+      <c r="A172" s="61"/>
+      <c r="B172" s="61"/>
+      <c r="C172" s="61"/>
+      <c r="D172" s="62"/>
+      <c r="E172" s="63"/>
     </row>
     <row r="173" spans="1:5" s="1" customFormat="1">
-      <c r="A173" s="63"/>
-      <c r="B173" s="63"/>
-      <c r="C173" s="63"/>
-      <c r="D173" s="64"/>
-      <c r="E173" s="65"/>
+      <c r="A173" s="61"/>
+      <c r="B173" s="61"/>
+      <c r="C173" s="61"/>
+      <c r="D173" s="62"/>
+      <c r="E173" s="63"/>
     </row>
     <row r="174" spans="1:5" s="1" customFormat="1">
-      <c r="A174" s="63"/>
-      <c r="B174" s="63"/>
-      <c r="C174" s="63"/>
-      <c r="D174" s="64"/>
-      <c r="E174" s="65"/>
+      <c r="A174" s="61"/>
+      <c r="B174" s="61"/>
+      <c r="C174" s="61"/>
+      <c r="D174" s="62"/>
+      <c r="E174" s="63"/>
     </row>
     <row r="175" spans="1:5" s="1" customFormat="1">
-      <c r="A175" s="63"/>
-      <c r="B175" s="63"/>
-      <c r="C175" s="63"/>
-      <c r="D175" s="64"/>
-      <c r="E175" s="65"/>
+      <c r="A175" s="61"/>
+      <c r="B175" s="61"/>
+      <c r="C175" s="61"/>
+      <c r="D175" s="62"/>
+      <c r="E175" s="63"/>
     </row>
     <row r="176" spans="1:5" s="1" customFormat="1">
-      <c r="A176" s="63"/>
-      <c r="B176" s="63"/>
-      <c r="C176" s="63"/>
-      <c r="D176" s="64"/>
-      <c r="E176" s="65"/>
+      <c r="A176" s="61"/>
+      <c r="B176" s="61"/>
+      <c r="C176" s="61"/>
+      <c r="D176" s="62"/>
+      <c r="E176" s="63"/>
     </row>
     <row r="177" spans="1:5" s="1" customFormat="1">
-      <c r="A177" s="63"/>
-      <c r="B177" s="63"/>
-      <c r="C177" s="63"/>
-      <c r="D177" s="64"/>
-      <c r="E177" s="65"/>
+      <c r="A177" s="61"/>
+      <c r="B177" s="61"/>
+      <c r="C177" s="61"/>
+      <c r="D177" s="62"/>
+      <c r="E177" s="63"/>
     </row>
     <row r="178" spans="1:5" s="1" customFormat="1">
-      <c r="A178" s="63"/>
-      <c r="B178" s="63"/>
-      <c r="C178" s="63"/>
-      <c r="D178" s="64"/>
-      <c r="E178" s="65"/>
+      <c r="A178" s="61"/>
+      <c r="B178" s="61"/>
+      <c r="C178" s="61"/>
+      <c r="D178" s="62"/>
+      <c r="E178" s="63"/>
     </row>
     <row r="179" spans="1:5" s="1" customFormat="1">
-      <c r="A179" s="63"/>
-      <c r="B179" s="63"/>
-      <c r="C179" s="63"/>
-      <c r="D179" s="64"/>
-      <c r="E179" s="65"/>
+      <c r="A179" s="61"/>
+      <c r="B179" s="61"/>
+      <c r="C179" s="61"/>
+      <c r="D179" s="62"/>
+      <c r="E179" s="63"/>
     </row>
     <row r="180" spans="1:5" s="1" customFormat="1">
-      <c r="A180" s="63"/>
-      <c r="B180" s="63"/>
-      <c r="C180" s="63"/>
-      <c r="D180" s="64"/>
-      <c r="E180" s="65"/>
+      <c r="A180" s="61"/>
+      <c r="B180" s="61"/>
+      <c r="C180" s="61"/>
+      <c r="D180" s="62"/>
+      <c r="E180" s="63"/>
     </row>
     <row r="181" spans="1:5" s="1" customFormat="1">
-      <c r="A181" s="63"/>
-      <c r="B181" s="63"/>
-      <c r="C181" s="63"/>
-      <c r="D181" s="64"/>
-      <c r="E181" s="65"/>
+      <c r="A181" s="61"/>
+      <c r="B181" s="61"/>
+      <c r="C181" s="61"/>
+      <c r="D181" s="62"/>
+      <c r="E181" s="63"/>
     </row>
     <row r="182" spans="1:5" s="1" customFormat="1">
-      <c r="A182" s="63"/>
-      <c r="B182" s="63"/>
-      <c r="C182" s="63"/>
-      <c r="D182" s="64"/>
-      <c r="E182" s="65"/>
+      <c r="A182" s="61"/>
+      <c r="B182" s="61"/>
+      <c r="C182" s="61"/>
+      <c r="D182" s="62"/>
+      <c r="E182" s="63"/>
     </row>
     <row r="183" spans="1:5" s="1" customFormat="1">
-      <c r="A183" s="63"/>
-      <c r="B183" s="63"/>
-      <c r="C183" s="63"/>
-      <c r="D183" s="64"/>
-      <c r="E183" s="65"/>
+      <c r="A183" s="61"/>
+      <c r="B183" s="61"/>
+      <c r="C183" s="61"/>
+      <c r="D183" s="62"/>
+      <c r="E183" s="63"/>
     </row>
     <row r="184" spans="1:5" s="1" customFormat="1">
-      <c r="A184" s="63"/>
-      <c r="B184" s="63"/>
-      <c r="C184" s="63"/>
-      <c r="D184" s="64"/>
-      <c r="E184" s="65"/>
+      <c r="A184" s="61"/>
+      <c r="B184" s="61"/>
+      <c r="C184" s="61"/>
+      <c r="D184" s="62"/>
+      <c r="E184" s="63"/>
     </row>
     <row r="185" spans="1:5" s="1" customFormat="1">
-      <c r="A185" s="63"/>
-      <c r="B185" s="63"/>
-      <c r="C185" s="63"/>
-      <c r="D185" s="64"/>
-      <c r="E185" s="65"/>
+      <c r="A185" s="61"/>
+      <c r="B185" s="61"/>
+      <c r="C185" s="61"/>
+      <c r="D185" s="62"/>
+      <c r="E185" s="63"/>
     </row>
     <row r="186" spans="1:5" s="1" customFormat="1">
-      <c r="A186" s="63"/>
-      <c r="B186" s="63"/>
-      <c r="C186" s="63"/>
-      <c r="D186" s="64"/>
-      <c r="E186" s="65"/>
+      <c r="A186" s="61"/>
+      <c r="B186" s="61"/>
+      <c r="C186" s="61"/>
+      <c r="D186" s="62"/>
+      <c r="E186" s="63"/>
     </row>
     <row r="187" spans="1:5" s="1" customFormat="1">
-      <c r="A187" s="63"/>
-      <c r="B187" s="63"/>
-      <c r="C187" s="63"/>
-      <c r="D187" s="64"/>
-      <c r="E187" s="65"/>
+      <c r="A187" s="61"/>
+      <c r="B187" s="61"/>
+      <c r="C187" s="61"/>
+      <c r="D187" s="62"/>
+      <c r="E187" s="63"/>
     </row>
     <row r="188" spans="1:5" s="1" customFormat="1">
-      <c r="A188" s="63"/>
-      <c r="B188" s="63"/>
-      <c r="C188" s="63"/>
-      <c r="D188" s="64"/>
-      <c r="E188" s="65"/>
+      <c r="A188" s="61"/>
+      <c r="B188" s="61"/>
+      <c r="C188" s="61"/>
+      <c r="D188" s="62"/>
+      <c r="E188" s="63"/>
     </row>
     <row r="189" spans="1:5" s="1" customFormat="1">
-      <c r="A189" s="63"/>
-      <c r="B189" s="63"/>
-      <c r="C189" s="63"/>
-      <c r="D189" s="64"/>
-      <c r="E189" s="65"/>
+      <c r="A189" s="61"/>
+      <c r="B189" s="61"/>
+      <c r="C189" s="61"/>
+      <c r="D189" s="62"/>
+      <c r="E189" s="63"/>
     </row>
     <row r="190" spans="1:5" s="1" customFormat="1">
-      <c r="A190" s="63"/>
-      <c r="B190" s="63"/>
-      <c r="C190" s="63"/>
-      <c r="D190" s="64"/>
-      <c r="E190" s="65"/>
+      <c r="A190" s="61"/>
+      <c r="B190" s="61"/>
+      <c r="C190" s="61"/>
+      <c r="D190" s="62"/>
+      <c r="E190" s="63"/>
     </row>
     <row r="191" spans="1:5" s="1" customFormat="1">
-      <c r="A191" s="63"/>
-      <c r="B191" s="63"/>
-      <c r="C191" s="63"/>
-      <c r="D191" s="64"/>
-      <c r="E191" s="65"/>
+      <c r="A191" s="61"/>
+      <c r="B191" s="61"/>
+      <c r="C191" s="61"/>
+      <c r="D191" s="62"/>
+      <c r="E191" s="63"/>
     </row>
     <row r="192" spans="1:5" s="1" customFormat="1">
-      <c r="A192" s="63"/>
-      <c r="B192" s="63"/>
-      <c r="C192" s="63"/>
-      <c r="D192" s="64"/>
-      <c r="E192" s="65"/>
+      <c r="A192" s="61"/>
+      <c r="B192" s="61"/>
+      <c r="C192" s="61"/>
+      <c r="D192" s="62"/>
+      <c r="E192" s="63"/>
     </row>
     <row r="193" spans="1:5" s="1" customFormat="1">
-      <c r="A193" s="63"/>
-      <c r="B193" s="63"/>
-      <c r="C193" s="63"/>
-      <c r="D193" s="64"/>
-      <c r="E193" s="65"/>
+      <c r="A193" s="61"/>
+      <c r="B193" s="61"/>
+      <c r="C193" s="61"/>
+      <c r="D193" s="62"/>
+      <c r="E193" s="63"/>
     </row>
     <row r="194" spans="1:5" s="1" customFormat="1">
-      <c r="A194" s="63"/>
-      <c r="B194" s="63"/>
-      <c r="C194" s="63"/>
-      <c r="D194" s="64"/>
-      <c r="E194" s="66"/>
+      <c r="A194" s="61"/>
+      <c r="B194" s="61"/>
+      <c r="C194" s="61"/>
+      <c r="D194" s="62"/>
+      <c r="E194" s="64"/>
     </row>
     <row r="195" spans="1:5" s="1" customFormat="1">
-      <c r="A195" s="63"/>
-      <c r="B195" s="63"/>
-      <c r="C195" s="63"/>
-      <c r="D195" s="64"/>
-      <c r="E195" s="66"/>
+      <c r="A195" s="61"/>
+      <c r="B195" s="61"/>
+      <c r="C195" s="61"/>
+      <c r="D195" s="62"/>
+      <c r="E195" s="64"/>
     </row>
     <row r="196" spans="1:5" s="1" customFormat="1">
-      <c r="A196" s="63"/>
-      <c r="B196" s="63"/>
-      <c r="C196" s="63"/>
-      <c r="D196" s="64"/>
-      <c r="E196" s="66"/>
+      <c r="A196" s="61"/>
+      <c r="B196" s="61"/>
+      <c r="C196" s="61"/>
+      <c r="D196" s="62"/>
+      <c r="E196" s="64"/>
     </row>
     <row r="197" spans="1:5" s="1" customFormat="1">
-      <c r="A197" s="63"/>
-      <c r="B197" s="63"/>
-      <c r="C197" s="63"/>
-      <c r="D197" s="64"/>
-      <c r="E197" s="66"/>
+      <c r="A197" s="61"/>
+      <c r="B197" s="61"/>
+      <c r="C197" s="61"/>
+      <c r="D197" s="62"/>
+      <c r="E197" s="64"/>
     </row>
     <row r="198" spans="1:5" s="1" customFormat="1">
-      <c r="A198" s="63"/>
-      <c r="B198" s="63"/>
-      <c r="C198" s="63"/>
-      <c r="D198" s="64"/>
-      <c r="E198" s="66"/>
+      <c r="A198" s="61"/>
+      <c r="B198" s="61"/>
+      <c r="C198" s="61"/>
+      <c r="D198" s="62"/>
+      <c r="E198" s="64"/>
     </row>
     <row r="199" spans="1:5" s="1" customFormat="1">
-      <c r="A199" s="63"/>
-      <c r="B199" s="63"/>
-      <c r="C199" s="63"/>
-      <c r="D199" s="64"/>
-      <c r="E199" s="66"/>
+      <c r="A199" s="61"/>
+      <c r="B199" s="61"/>
+      <c r="C199" s="61"/>
+      <c r="D199" s="62"/>
+      <c r="E199" s="64"/>
     </row>
     <row r="200" spans="1:5" s="1" customFormat="1">
-      <c r="A200" s="63"/>
-      <c r="B200" s="63"/>
-      <c r="C200" s="63"/>
-      <c r="D200" s="64"/>
-      <c r="E200" s="66"/>
+      <c r="A200" s="61"/>
+      <c r="B200" s="61"/>
+      <c r="C200" s="61"/>
+      <c r="D200" s="62"/>
+      <c r="E200" s="64"/>
     </row>
     <row r="201" spans="1:5" s="1" customFormat="1">
-      <c r="A201" s="63"/>
-      <c r="B201" s="63"/>
-      <c r="C201" s="63"/>
-      <c r="D201" s="64"/>
-      <c r="E201" s="66"/>
+      <c r="A201" s="61"/>
+      <c r="B201" s="61"/>
+      <c r="C201" s="61"/>
+      <c r="D201" s="62"/>
+      <c r="E201" s="64"/>
     </row>
     <row r="202" spans="1:5" s="1" customFormat="1">
-      <c r="A202" s="63"/>
-      <c r="B202" s="63"/>
-      <c r="C202" s="63"/>
-      <c r="D202" s="64"/>
-      <c r="E202" s="66"/>
+      <c r="A202" s="61"/>
+      <c r="B202" s="61"/>
+      <c r="C202" s="61"/>
+      <c r="D202" s="62"/>
+      <c r="E202" s="64"/>
     </row>
     <row r="203" spans="1:5" s="1" customFormat="1">
-      <c r="A203" s="63"/>
-      <c r="B203" s="63"/>
-      <c r="C203" s="63"/>
-      <c r="D203" s="64"/>
-      <c r="E203" s="66"/>
+      <c r="A203" s="61"/>
+      <c r="B203" s="61"/>
+      <c r="C203" s="61"/>
+      <c r="D203" s="62"/>
+      <c r="E203" s="64"/>
     </row>
     <row r="204" spans="1:5" s="1" customFormat="1">
-      <c r="A204" s="63"/>
-      <c r="B204" s="63"/>
-      <c r="C204" s="63"/>
-      <c r="D204" s="64"/>
-      <c r="E204" s="66"/>
+      <c r="A204" s="61"/>
+      <c r="B204" s="61"/>
+      <c r="C204" s="61"/>
+      <c r="D204" s="62"/>
+      <c r="E204" s="64"/>
     </row>
     <row r="205" spans="1:5" s="1" customFormat="1">
-      <c r="A205" s="63"/>
-      <c r="B205" s="63"/>
-      <c r="C205" s="63"/>
-      <c r="D205" s="64"/>
-      <c r="E205" s="66"/>
+      <c r="A205" s="61"/>
+      <c r="B205" s="61"/>
+      <c r="C205" s="61"/>
+      <c r="D205" s="62"/>
+      <c r="E205" s="64"/>
     </row>
     <row r="206" spans="1:5" s="1" customFormat="1">
-      <c r="A206" s="63"/>
-      <c r="B206" s="63"/>
-      <c r="C206" s="63"/>
-      <c r="D206" s="64"/>
-      <c r="E206" s="66"/>
+      <c r="A206" s="61"/>
+      <c r="B206" s="61"/>
+      <c r="C206" s="61"/>
+      <c r="D206" s="62"/>
+      <c r="E206" s="64"/>
     </row>
     <row r="207" spans="1:5" s="1" customFormat="1">
-      <c r="A207" s="63"/>
-      <c r="B207" s="63"/>
-      <c r="C207" s="63"/>
-      <c r="D207" s="64"/>
-      <c r="E207" s="66"/>
+      <c r="A207" s="61"/>
+      <c r="B207" s="61"/>
+      <c r="C207" s="61"/>
+      <c r="D207" s="62"/>
+      <c r="E207" s="64"/>
     </row>
     <row r="208" spans="1:5" s="1" customFormat="1">
-      <c r="A208" s="63"/>
-      <c r="B208" s="63"/>
-      <c r="C208" s="63"/>
-      <c r="D208" s="64"/>
-      <c r="E208" s="66"/>
+      <c r="A208" s="61"/>
+      <c r="B208" s="61"/>
+      <c r="C208" s="61"/>
+      <c r="D208" s="62"/>
+      <c r="E208" s="64"/>
     </row>
     <row r="209" spans="1:5" s="1" customFormat="1">
-      <c r="A209" s="63"/>
-      <c r="B209" s="63"/>
-      <c r="C209" s="63"/>
-      <c r="D209" s="64"/>
-      <c r="E209" s="66"/>
+      <c r="A209" s="61"/>
+      <c r="B209" s="61"/>
+      <c r="C209" s="61"/>
+      <c r="D209" s="62"/>
+      <c r="E209" s="64"/>
     </row>
     <row r="210" spans="1:5" s="1" customFormat="1">
-      <c r="A210" s="63"/>
-      <c r="B210" s="63"/>
-      <c r="C210" s="63"/>
-      <c r="D210" s="64"/>
-      <c r="E210" s="66"/>
+      <c r="A210" s="61"/>
+      <c r="B210" s="61"/>
+      <c r="C210" s="61"/>
+      <c r="D210" s="62"/>
+      <c r="E210" s="64"/>
     </row>
     <row r="211" spans="1:5" s="1" customFormat="1">
-      <c r="A211" s="63"/>
-      <c r="B211" s="63"/>
-      <c r="C211" s="63"/>
-      <c r="D211" s="64"/>
-      <c r="E211" s="66"/>
+      <c r="A211" s="61"/>
+      <c r="B211" s="61"/>
+      <c r="C211" s="61"/>
+      <c r="D211" s="62"/>
+      <c r="E211" s="64"/>
     </row>
     <row r="212" spans="1:5" s="1" customFormat="1">
-      <c r="A212" s="63"/>
-      <c r="B212" s="63"/>
-      <c r="C212" s="63"/>
-      <c r="D212" s="64"/>
-      <c r="E212" s="66"/>
+      <c r="A212" s="61"/>
+      <c r="B212" s="61"/>
+      <c r="C212" s="61"/>
+      <c r="D212" s="62"/>
+      <c r="E212" s="64"/>
     </row>
     <row r="213" spans="1:5" s="1" customFormat="1">
-      <c r="A213" s="63"/>
-      <c r="B213" s="63"/>
-      <c r="C213" s="63"/>
-      <c r="D213" s="64"/>
-      <c r="E213" s="66"/>
+      <c r="A213" s="61"/>
+      <c r="B213" s="61"/>
+      <c r="C213" s="61"/>
+      <c r="D213" s="62"/>
+      <c r="E213" s="64"/>
     </row>
     <row r="214" spans="1:5" s="1" customFormat="1">
-      <c r="A214" s="63"/>
-      <c r="B214" s="63"/>
-      <c r="C214" s="63"/>
-      <c r="D214" s="64"/>
-      <c r="E214" s="66"/>
+      <c r="A214" s="61"/>
+      <c r="B214" s="61"/>
+      <c r="C214" s="61"/>
+      <c r="D214" s="62"/>
+      <c r="E214" s="64"/>
     </row>
     <row r="215" spans="1:5" s="1" customFormat="1">
-      <c r="A215" s="63"/>
-      <c r="B215" s="63"/>
-      <c r="C215" s="63"/>
-      <c r="D215" s="64"/>
-      <c r="E215" s="66"/>
+      <c r="A215" s="61"/>
+      <c r="B215" s="61"/>
+      <c r="C215" s="61"/>
+      <c r="D215" s="62"/>
+      <c r="E215" s="64"/>
     </row>
     <row r="216" spans="1:5" s="1" customFormat="1">
-      <c r="A216" s="63"/>
-      <c r="B216" s="63"/>
-      <c r="C216" s="63"/>
-      <c r="D216" s="64"/>
-      <c r="E216" s="66"/>
+      <c r="A216" s="61"/>
+      <c r="B216" s="61"/>
+      <c r="C216" s="61"/>
+      <c r="D216" s="62"/>
+      <c r="E216" s="64"/>
     </row>
     <row r="217" spans="1:5" s="1" customFormat="1">
-      <c r="A217" s="63"/>
-      <c r="B217" s="63"/>
-      <c r="C217" s="63"/>
-      <c r="D217" s="64"/>
-      <c r="E217" s="66"/>
+      <c r="A217" s="61"/>
+      <c r="B217" s="61"/>
+      <c r="C217" s="61"/>
+      <c r="D217" s="62"/>
+      <c r="E217" s="64"/>
     </row>
     <row r="218" spans="1:5" s="1" customFormat="1">
-      <c r="A218" s="63"/>
-      <c r="B218" s="63"/>
-      <c r="C218" s="63"/>
-      <c r="D218" s="64"/>
-      <c r="E218" s="66"/>
+      <c r="A218" s="61"/>
+      <c r="B218" s="61"/>
+      <c r="C218" s="61"/>
+      <c r="D218" s="62"/>
+      <c r="E218" s="64"/>
     </row>
     <row r="219" spans="1:5" s="1" customFormat="1">
-      <c r="A219" s="63"/>
-      <c r="B219" s="63"/>
-      <c r="C219" s="63"/>
-      <c r="D219" s="64"/>
-      <c r="E219" s="66"/>
+      <c r="A219" s="61"/>
+      <c r="B219" s="61"/>
+      <c r="C219" s="61"/>
+      <c r="D219" s="62"/>
+      <c r="E219" s="64"/>
     </row>
     <row r="220" spans="1:5" s="1" customFormat="1">
-      <c r="A220" s="63"/>
-      <c r="B220" s="63"/>
-      <c r="C220" s="63"/>
-      <c r="D220" s="64"/>
-      <c r="E220" s="66"/>
+      <c r="A220" s="61"/>
+      <c r="B220" s="61"/>
+      <c r="C220" s="61"/>
+      <c r="D220" s="62"/>
+      <c r="E220" s="64"/>
     </row>
     <row r="221" spans="1:5" s="1" customFormat="1">
-      <c r="A221" s="63"/>
-      <c r="B221" s="63"/>
-      <c r="C221" s="63"/>
-      <c r="D221" s="64"/>
-      <c r="E221" s="66"/>
+      <c r="A221" s="61"/>
+      <c r="B221" s="61"/>
+      <c r="C221" s="61"/>
+      <c r="D221" s="62"/>
+      <c r="E221" s="64"/>
     </row>
     <row r="222" spans="1:5" s="1" customFormat="1">
-      <c r="A222" s="63"/>
-      <c r="B222" s="63"/>
-      <c r="C222" s="63"/>
-      <c r="D222" s="64"/>
-      <c r="E222" s="66"/>
+      <c r="A222" s="61"/>
+      <c r="B222" s="61"/>
+      <c r="C222" s="61"/>
+      <c r="D222" s="62"/>
+      <c r="E222" s="64"/>
     </row>
     <row r="223" spans="1:5" s="1" customFormat="1">
-      <c r="A223" s="63"/>
-      <c r="B223" s="63"/>
-      <c r="C223" s="63"/>
-      <c r="D223" s="64"/>
-      <c r="E223" s="66"/>
+      <c r="A223" s="61"/>
+      <c r="B223" s="61"/>
+      <c r="C223" s="61"/>
+      <c r="D223" s="62"/>
+      <c r="E223" s="64"/>
     </row>
     <row r="224" spans="1:5" s="1" customFormat="1">
-      <c r="A224" s="63"/>
-      <c r="B224" s="63"/>
-      <c r="C224" s="63"/>
-      <c r="D224" s="64"/>
-      <c r="E224" s="66"/>
+      <c r="A224" s="61"/>
+      <c r="B224" s="61"/>
+      <c r="C224" s="61"/>
+      <c r="D224" s="62"/>
+      <c r="E224" s="64"/>
     </row>
     <row r="225" spans="1:5" s="1" customFormat="1">
-      <c r="A225" s="63"/>
-      <c r="B225" s="63"/>
-      <c r="C225" s="63"/>
-      <c r="D225" s="64"/>
-      <c r="E225" s="66"/>
+      <c r="A225" s="61"/>
+      <c r="B225" s="61"/>
+      <c r="C225" s="61"/>
+      <c r="D225" s="62"/>
+      <c r="E225" s="64"/>
     </row>
     <row r="226" spans="1:5" s="1" customFormat="1">
-      <c r="A226" s="63"/>
-      <c r="B226" s="63"/>
-      <c r="C226" s="63"/>
-      <c r="D226" s="64"/>
-      <c r="E226" s="66"/>
+      <c r="A226" s="61"/>
+      <c r="B226" s="61"/>
+      <c r="C226" s="61"/>
+      <c r="D226" s="62"/>
+      <c r="E226" s="64"/>
     </row>
     <row r="227" spans="1:5" s="1" customFormat="1">
-      <c r="A227" s="63"/>
-      <c r="B227" s="63"/>
-      <c r="C227" s="63"/>
-      <c r="D227" s="64"/>
-      <c r="E227" s="66"/>
+      <c r="A227" s="61"/>
+      <c r="B227" s="61"/>
+      <c r="C227" s="61"/>
+      <c r="D227" s="62"/>
+      <c r="E227" s="64"/>
     </row>
     <row r="228" spans="1:5" s="1" customFormat="1">
-      <c r="A228" s="63"/>
-      <c r="B228" s="63"/>
-      <c r="C228" s="63"/>
-      <c r="D228" s="64"/>
-      <c r="E228" s="66"/>
+      <c r="A228" s="61"/>
+      <c r="B228" s="61"/>
+      <c r="C228" s="61"/>
+      <c r="D228" s="62"/>
+      <c r="E228" s="64"/>
     </row>
     <row r="229" spans="1:5" s="1" customFormat="1">
-      <c r="A229" s="63"/>
-      <c r="B229" s="63"/>
-      <c r="C229" s="63"/>
-      <c r="D229" s="64"/>
-      <c r="E229" s="66"/>
+      <c r="A229" s="61"/>
+      <c r="B229" s="61"/>
+      <c r="C229" s="61"/>
+      <c r="D229" s="62"/>
+      <c r="E229" s="64"/>
     </row>
     <row r="230" spans="1:5" s="1" customFormat="1">
-      <c r="A230" s="63"/>
-      <c r="B230" s="63"/>
-      <c r="C230" s="63"/>
-      <c r="D230" s="64"/>
-      <c r="E230" s="66"/>
+      <c r="A230" s="61"/>
+      <c r="B230" s="61"/>
+      <c r="C230" s="61"/>
+      <c r="D230" s="62"/>
+      <c r="E230" s="64"/>
     </row>
     <row r="231" spans="1:5" s="1" customFormat="1">
-      <c r="A231" s="63"/>
-      <c r="B231" s="63"/>
-      <c r="C231" s="63"/>
-      <c r="D231" s="64"/>
-      <c r="E231" s="66"/>
+      <c r="A231" s="61"/>
+      <c r="B231" s="61"/>
+      <c r="C231" s="61"/>
+      <c r="D231" s="62"/>
+      <c r="E231" s="64"/>
     </row>
     <row r="232" spans="1:5" s="1" customFormat="1">
-      <c r="A232" s="63"/>
-      <c r="B232" s="63"/>
-      <c r="C232" s="63"/>
-      <c r="D232" s="64"/>
-      <c r="E232" s="66"/>
+      <c r="A232" s="61"/>
+      <c r="B232" s="61"/>
+      <c r="C232" s="61"/>
+      <c r="D232" s="62"/>
+      <c r="E232" s="64"/>
     </row>
     <row r="233" spans="1:5" s="1" customFormat="1">
-      <c r="A233" s="63"/>
-      <c r="B233" s="63"/>
-      <c r="C233" s="63"/>
-      <c r="D233" s="64"/>
-      <c r="E233" s="66"/>
+      <c r="A233" s="61"/>
+      <c r="B233" s="61"/>
+      <c r="C233" s="61"/>
+      <c r="D233" s="62"/>
+      <c r="E233" s="64"/>
     </row>
     <row r="234" spans="1:5" s="1" customFormat="1">
-      <c r="A234" s="63"/>
-      <c r="B234" s="63"/>
-      <c r="C234" s="63"/>
-      <c r="D234" s="64"/>
-      <c r="E234" s="66"/>
+      <c r="A234" s="61"/>
+      <c r="B234" s="61"/>
+      <c r="C234" s="61"/>
+      <c r="D234" s="62"/>
+      <c r="E234" s="64"/>
     </row>
     <row r="235" spans="1:5" s="1" customFormat="1">
-      <c r="A235" s="63"/>
-      <c r="B235" s="63"/>
-      <c r="C235" s="63"/>
-      <c r="D235" s="64"/>
-      <c r="E235" s="66"/>
+      <c r="A235" s="61"/>
+      <c r="B235" s="61"/>
+      <c r="C235" s="61"/>
+      <c r="D235" s="62"/>
+      <c r="E235" s="64"/>
     </row>
     <row r="236" spans="1:5" s="1" customFormat="1">
-      <c r="A236" s="63"/>
-      <c r="B236" s="63"/>
-      <c r="C236" s="63"/>
-      <c r="D236" s="64"/>
-      <c r="E236" s="66"/>
+      <c r="A236" s="61"/>
+      <c r="B236" s="61"/>
+      <c r="C236" s="61"/>
+      <c r="D236" s="62"/>
+      <c r="E236" s="64"/>
     </row>
     <row r="237" spans="1:5" s="1" customFormat="1">
-      <c r="A237" s="63"/>
-      <c r="B237" s="63"/>
-      <c r="C237" s="63"/>
-      <c r="D237" s="64"/>
-      <c r="E237" s="66"/>
+      <c r="A237" s="61"/>
+      <c r="B237" s="61"/>
+      <c r="C237" s="61"/>
+      <c r="D237" s="62"/>
+      <c r="E237" s="64"/>
     </row>
     <row r="238" spans="1:5" s="1" customFormat="1">
-      <c r="A238" s="63"/>
-      <c r="B238" s="63"/>
-      <c r="C238" s="63"/>
-      <c r="D238" s="64"/>
-      <c r="E238" s="66"/>
+      <c r="A238" s="61"/>
+      <c r="B238" s="61"/>
+      <c r="C238" s="61"/>
+      <c r="D238" s="62"/>
+      <c r="E238" s="64"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>

</xml_diff>

<commit_message>
A lot of fixes.  Hopefully no exceptions anymore.
</commit_message>
<xml_diff>
--- a/Kilroy Equipment List 2016.xlsx
+++ b/Kilroy Equipment List 2016.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="106">
   <si>
     <t>Code Written/Tested</t>
   </si>
@@ -176,24 +176,6 @@
   </si>
   <si>
     <t>leftFrontMotor</t>
-  </si>
-  <si>
-    <t>Left Front Encoder</t>
-  </si>
-  <si>
-    <t>leftFrontEncoder</t>
-  </si>
-  <si>
-    <t>Right Front Encoder</t>
-  </si>
-  <si>
-    <t>rightFrontEncoder</t>
-  </si>
-  <si>
-    <t>12, 13</t>
-  </si>
-  <si>
-    <t>10, 11</t>
   </si>
   <si>
     <t>leftRearEncoder</t>
@@ -1091,8 +1073,8 @@
   <dimension ref="A1:H238"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E63" sqref="E63"/>
+      <pane ySplit="2" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -1162,7 +1144,7 @@
       <c r="A5" s="66"/>
       <c r="B5" s="66"/>
       <c r="C5" s="29" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D5" s="32" t="s">
         <v>43</v>
@@ -1256,26 +1238,26 @@
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="29" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="D14" s="32" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="E14" s="33" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="15" spans="1:8" s="1" customFormat="1">
       <c r="A15" s="52"/>
       <c r="B15" s="52"/>
       <c r="C15" s="26" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D15" s="27" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E15" s="44" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
     <row r="16" spans="1:8" s="1" customFormat="1">
@@ -1386,79 +1368,67 @@
     <row r="27" spans="1:8" s="1" customFormat="1">
       <c r="A27" s="43"/>
       <c r="B27" s="43"/>
-      <c r="C27" s="29" t="s">
-        <v>53</v>
-      </c>
-      <c r="D27" s="32" t="s">
-        <v>54</v>
-      </c>
-      <c r="E27" s="33" t="s">
-        <v>58</v>
-      </c>
+      <c r="C27" s="29"/>
+      <c r="D27" s="32"/>
+      <c r="E27" s="33"/>
     </row>
     <row r="28" spans="1:8" s="1" customFormat="1">
       <c r="A28" s="13"/>
       <c r="B28" s="13"/>
-      <c r="C28" s="23" t="s">
-        <v>55</v>
-      </c>
-      <c r="D28" s="45" t="s">
-        <v>56</v>
-      </c>
-      <c r="E28" s="44" t="s">
-        <v>57</v>
-      </c>
+      <c r="C28" s="23"/>
+      <c r="D28" s="45"/>
+      <c r="E28" s="44"/>
     </row>
     <row r="29" spans="1:8" s="1" customFormat="1">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="29" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D29" s="32" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="E29" s="33" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="30" spans="1:8" s="1" customFormat="1">
       <c r="A30" s="13"/>
       <c r="B30" s="13"/>
       <c r="C30" s="23" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D30" s="45" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="E30" s="44" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="31" spans="1:8" s="1" customFormat="1">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="29" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="D31" s="32" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="E31" s="33" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="32" spans="1:8" s="1" customFormat="1">
       <c r="A32" s="13"/>
       <c r="B32" s="13"/>
       <c r="C32" s="23" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="D32" s="45" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="E32" s="44" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="33" spans="1:5" s="1" customFormat="1">
@@ -1550,23 +1520,23 @@
         <v>6</v>
       </c>
       <c r="C44" s="29" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="D44" s="25" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="E44" s="47" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="45" spans="1:5" s="1" customFormat="1">
       <c r="A45" s="41"/>
       <c r="B45" s="14"/>
       <c r="C45" s="42" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="D45" s="45" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="E45" s="14">
         <v>0</v>
@@ -1605,26 +1575,26 @@
       <c r="A49" s="20"/>
       <c r="B49" s="20"/>
       <c r="C49" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="D49" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="E49" s="47" t="s">
         <v>73</v>
-      </c>
-      <c r="D49" s="25" t="s">
-        <v>71</v>
-      </c>
-      <c r="E49" s="47" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="50" spans="1:8" s="1" customFormat="1">
       <c r="A50" s="8"/>
       <c r="B50" s="8"/>
       <c r="C50" s="26" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="D50" s="27" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="E50" s="28" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="51" spans="1:8" s="1" customFormat="1">
@@ -1663,59 +1633,59 @@
       </c>
       <c r="D55" s="67"/>
       <c r="E55" s="3" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="56" spans="1:8" s="1" customFormat="1">
       <c r="A56" s="20"/>
       <c r="B56" s="20"/>
       <c r="C56" s="46" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="D56" s="25" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="E56" s="33" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
     </row>
     <row r="57" spans="1:8" s="1" customFormat="1">
       <c r="A57" s="8"/>
       <c r="B57" s="8"/>
       <c r="C57" s="26" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="D57" s="27" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="E57" s="28" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="58" spans="1:8" s="1" customFormat="1">
       <c r="A58" s="4"/>
       <c r="B58" s="4"/>
       <c r="C58" s="29" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="D58" s="32" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="E58" s="33" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="59" spans="1:8" s="1" customFormat="1">
       <c r="A59" s="8"/>
       <c r="B59" s="8"/>
       <c r="C59" s="26" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="D59" s="27" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="E59" s="28" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="60" spans="1:8" s="36" customFormat="1" ht="13.15" customHeight="1">
@@ -1784,13 +1754,13 @@
       <c r="A67" s="8"/>
       <c r="B67" s="8"/>
       <c r="C67" s="26" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D67" s="27" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="E67" s="28" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="G67" s="21"/>
     </row>
@@ -1798,13 +1768,13 @@
       <c r="A68" s="4"/>
       <c r="B68" s="4"/>
       <c r="C68" s="29" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D68" s="32" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="E68" s="33" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G68" s="21"/>
     </row>
@@ -1812,13 +1782,13 @@
       <c r="A69" s="8"/>
       <c r="B69" s="8"/>
       <c r="C69" s="23" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="D69" s="45" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="E69" s="44" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="G69" s="21"/>
     </row>
@@ -1826,13 +1796,13 @@
       <c r="A70" s="4"/>
       <c r="B70" s="4"/>
       <c r="C70" s="29" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="D70" s="32" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="E70" s="33" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="G70" s="21"/>
     </row>
@@ -2104,7 +2074,7 @@
         <v>22</v>
       </c>
       <c r="D104" s="27" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="E104" s="44" t="s">
         <v>24</v>
@@ -2127,10 +2097,10 @@
       <c r="A106" s="13"/>
       <c r="B106" s="13"/>
       <c r="C106" s="26" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="D106" s="27" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E106" s="44" t="s">
         <v>20</v>
@@ -2166,7 +2136,7 @@
       <c r="A109" s="4"/>
       <c r="B109" s="4"/>
       <c r="C109" s="29" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D109" s="6" t="s">
         <v>8</v>
@@ -2205,10 +2175,10 @@
       <c r="A112" s="13"/>
       <c r="B112" s="13"/>
       <c r="C112" s="23" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="D112" s="45" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="E112" s="23" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
Added more hardware equipment declarations.  Added equivalent PRINTLN() statements
</commit_message>
<xml_diff>
--- a/Kilroy Equipment List 2016.xlsx
+++ b/Kilroy Equipment List 2016.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="115">
   <si>
     <t>Code Written/Tested</t>
   </si>
@@ -335,6 +335,33 @@
   </si>
   <si>
     <t>catapultSolenoid2</t>
+  </si>
+  <si>
+    <t>Shoot High</t>
+  </si>
+  <si>
+    <t>Shoot Low</t>
+  </si>
+  <si>
+    <t>shootHigh</t>
+  </si>
+  <si>
+    <t>shootLow</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>Victor Motor Controller</t>
+  </si>
+  <si>
+    <t>armMotor</t>
+  </si>
+  <si>
+    <t>PWM 0</t>
   </si>
 </sst>
 </file>
@@ -663,9 +690,6 @@
     <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -704,6 +728,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1073,31 +1100,31 @@
   <dimension ref="A1:H238"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C28" sqref="C28"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" style="61" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" style="61" customWidth="1"/>
-    <col min="3" max="3" width="70.5703125" style="61" customWidth="1"/>
-    <col min="4" max="4" width="21" style="62" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" style="64" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" style="61" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" style="61"/>
-    <col min="8" max="8" width="11.140625" style="61" customWidth="1"/>
-    <col min="9" max="16384" width="8.85546875" style="61"/>
+    <col min="1" max="1" width="14.7109375" style="60" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" style="60" customWidth="1"/>
+    <col min="3" max="3" width="70.5703125" style="60" customWidth="1"/>
+    <col min="4" max="4" width="21" style="61" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" style="63" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" style="60" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" style="60"/>
+    <col min="8" max="8" width="11.140625" style="60" customWidth="1"/>
+    <col min="9" max="16384" width="8.85546875" style="60"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="67" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
     </row>
     <row r="2" spans="1:8" s="1" customFormat="1" ht="25.5">
       <c r="A2" s="13" t="s">
@@ -1119,17 +1146,17 @@
     <row r="3" spans="1:8" s="1" customFormat="1" ht="13.15" customHeight="1">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
-      <c r="C3" s="67" t="s">
+      <c r="C3" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="67"/>
+      <c r="D3" s="66"/>
       <c r="E3" s="3" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="1" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A4" s="65"/>
-      <c r="B4" s="65"/>
+      <c r="A4" s="64"/>
+      <c r="B4" s="64"/>
       <c r="C4" s="30" t="s">
         <v>46</v>
       </c>
@@ -1141,8 +1168,8 @@
       </c>
     </row>
     <row r="5" spans="1:8" s="1" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A5" s="66"/>
-      <c r="B5" s="66"/>
+      <c r="A5" s="65"/>
+      <c r="B5" s="65"/>
       <c r="C5" s="29" t="s">
         <v>86</v>
       </c>
@@ -1182,9 +1209,15 @@
     <row r="8" spans="1:8" s="1" customFormat="1">
       <c r="A8" s="34"/>
       <c r="B8" s="34"/>
-      <c r="C8" s="49"/>
-      <c r="D8" s="56"/>
-      <c r="E8" s="51"/>
+      <c r="C8" s="49" t="s">
+        <v>112</v>
+      </c>
+      <c r="D8" s="69" t="s">
+        <v>113</v>
+      </c>
+      <c r="E8" s="51" t="s">
+        <v>114</v>
+      </c>
       <c r="F8" s="12"/>
       <c r="G8" s="12"/>
       <c r="H8" s="12"/>
@@ -1226,11 +1259,11 @@
     <row r="13" spans="1:8" s="1" customFormat="1" ht="13.15" customHeight="1">
       <c r="A13" s="17"/>
       <c r="B13" s="17"/>
-      <c r="C13" s="69" t="s">
+      <c r="C13" s="68" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="69"/>
-      <c r="E13" s="60" t="s">
+      <c r="D13" s="68"/>
+      <c r="E13" s="59" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1357,10 +1390,10 @@
     <row r="26" spans="1:8" s="1" customFormat="1" ht="13.35" customHeight="1">
       <c r="A26" s="17"/>
       <c r="B26" s="17"/>
-      <c r="C26" s="67" t="s">
+      <c r="C26" s="66" t="s">
         <v>7</v>
       </c>
-      <c r="D26" s="67"/>
+      <c r="D26" s="66"/>
       <c r="E26" s="3" t="s">
         <v>28</v>
       </c>
@@ -1434,16 +1467,28 @@
     <row r="33" spans="1:5" s="1" customFormat="1">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
-      <c r="C33" s="29"/>
-      <c r="D33" s="32"/>
-      <c r="E33" s="33"/>
+      <c r="C33" s="29" t="s">
+        <v>106</v>
+      </c>
+      <c r="D33" s="32" t="s">
+        <v>108</v>
+      </c>
+      <c r="E33" s="33" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="34" spans="1:5" s="1" customFormat="1">
       <c r="A34" s="13"/>
       <c r="B34" s="13"/>
-      <c r="C34" s="23"/>
-      <c r="D34" s="45"/>
-      <c r="E34" s="44"/>
+      <c r="C34" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="D34" s="45" t="s">
+        <v>109</v>
+      </c>
+      <c r="E34" s="44" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="35" spans="1:5" s="1" customFormat="1">
       <c r="A35" s="4"/>
@@ -1457,7 +1502,7 @@
       <c r="B36" s="8"/>
       <c r="C36" s="26"/>
       <c r="D36" s="18"/>
-      <c r="E36" s="57"/>
+      <c r="E36" s="56"/>
     </row>
     <row r="37" spans="1:5" s="1" customFormat="1">
       <c r="A37" s="4"/>
@@ -1476,7 +1521,7 @@
     <row r="39" spans="1:5" s="19" customFormat="1" ht="13.15" customHeight="1">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
-      <c r="C39" s="58"/>
+      <c r="C39" s="57"/>
       <c r="D39" s="32"/>
       <c r="E39" s="33"/>
     </row>
@@ -1504,10 +1549,10 @@
     <row r="43" spans="1:5" s="1" customFormat="1" ht="13.15" customHeight="1">
       <c r="A43" s="17"/>
       <c r="B43" s="17"/>
-      <c r="C43" s="67" t="s">
+      <c r="C43" s="66" t="s">
         <v>9</v>
       </c>
-      <c r="D43" s="67"/>
+      <c r="D43" s="66"/>
       <c r="E43" s="3" t="s">
         <v>10</v>
       </c>
@@ -1563,10 +1608,10 @@
     <row r="48" spans="1:5" s="1" customFormat="1" ht="13.15" customHeight="1">
       <c r="A48" s="17"/>
       <c r="B48" s="17"/>
-      <c r="C48" s="67" t="s">
+      <c r="C48" s="66" t="s">
         <v>11</v>
       </c>
-      <c r="D48" s="67"/>
+      <c r="D48" s="66"/>
       <c r="E48" s="3" t="s">
         <v>12</v>
       </c>
@@ -1628,10 +1673,10 @@
     <row r="55" spans="1:8" s="1" customFormat="1" ht="13.35" customHeight="1">
       <c r="A55" s="17"/>
       <c r="B55" s="17"/>
-      <c r="C55" s="67" t="s">
+      <c r="C55" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="D55" s="67"/>
+      <c r="D55" s="66"/>
       <c r="E55" s="3" t="s">
         <v>100</v>
       </c>
@@ -1700,10 +1745,10 @@
     <row r="61" spans="1:8" s="1" customFormat="1" ht="13.35" customHeight="1">
       <c r="A61" s="17"/>
       <c r="B61" s="17"/>
-      <c r="C61" s="67" t="s">
+      <c r="C61" s="66" t="s">
         <v>30</v>
       </c>
-      <c r="D61" s="67"/>
+      <c r="D61" s="66"/>
       <c r="E61" s="3" t="s">
         <v>29</v>
       </c>
@@ -1741,10 +1786,10 @@
     <row r="66" spans="1:8" s="1" customFormat="1" ht="13.35" customHeight="1">
       <c r="A66" s="17"/>
       <c r="B66" s="17"/>
-      <c r="C66" s="67" t="s">
+      <c r="C66" s="66" t="s">
         <v>14</v>
       </c>
-      <c r="D66" s="67"/>
+      <c r="D66" s="66"/>
       <c r="E66" s="3" t="s">
         <v>15</v>
       </c>
@@ -1809,10 +1854,10 @@
     <row r="71" spans="1:8" s="1" customFormat="1" ht="13.35" customHeight="1">
       <c r="A71" s="17"/>
       <c r="B71" s="17"/>
-      <c r="C71" s="67" t="s">
+      <c r="C71" s="66" t="s">
         <v>16</v>
       </c>
-      <c r="D71" s="67"/>
+      <c r="D71" s="66"/>
       <c r="E71" s="3" t="s">
         <v>17</v>
       </c>
@@ -1897,7 +1942,7 @@
       <c r="B82" s="8"/>
       <c r="C82" s="23"/>
       <c r="D82" s="45"/>
-      <c r="E82" s="59"/>
+      <c r="E82" s="58"/>
       <c r="F82" s="21"/>
     </row>
     <row r="83" spans="1:7" s="1" customFormat="1">
@@ -1970,10 +2015,10 @@
     <row r="92" spans="1:7" s="1" customFormat="1" ht="13.35" customHeight="1">
       <c r="A92" s="17"/>
       <c r="B92" s="17"/>
-      <c r="C92" s="67" t="s">
+      <c r="C92" s="66" t="s">
         <v>18</v>
       </c>
-      <c r="D92" s="67"/>
+      <c r="D92" s="66"/>
       <c r="E92" s="3" t="s">
         <v>17</v>
       </c>
@@ -2059,11 +2104,11 @@
     <row r="103" spans="1:6" s="1" customFormat="1">
       <c r="A103" s="17"/>
       <c r="B103" s="17"/>
-      <c r="C103" s="60" t="s">
+      <c r="C103" s="59" t="s">
         <v>21</v>
       </c>
       <c r="D103" s="22"/>
-      <c r="E103" s="60" t="s">
+      <c r="E103" s="59" t="s">
         <v>26</v>
       </c>
     </row>
@@ -2192,879 +2237,879 @@
       <c r="E113" s="33"/>
     </row>
     <row r="114" spans="1:5" s="1" customFormat="1">
-      <c r="A114" s="61"/>
-      <c r="B114" s="61"/>
-      <c r="C114" s="61"/>
-      <c r="D114" s="62"/>
-      <c r="E114" s="63"/>
+      <c r="A114" s="60"/>
+      <c r="B114" s="60"/>
+      <c r="C114" s="60"/>
+      <c r="D114" s="61"/>
+      <c r="E114" s="62"/>
     </row>
     <row r="115" spans="1:5" s="1" customFormat="1">
-      <c r="A115" s="61"/>
-      <c r="B115" s="61"/>
-      <c r="C115" s="61"/>
-      <c r="D115" s="62"/>
-      <c r="E115" s="63"/>
+      <c r="A115" s="60"/>
+      <c r="B115" s="60"/>
+      <c r="C115" s="60"/>
+      <c r="D115" s="61"/>
+      <c r="E115" s="62"/>
     </row>
     <row r="116" spans="1:5" s="1" customFormat="1">
-      <c r="A116" s="61"/>
-      <c r="B116" s="61"/>
-      <c r="C116" s="61"/>
-      <c r="D116" s="62"/>
-      <c r="E116" s="63"/>
+      <c r="A116" s="60"/>
+      <c r="B116" s="60"/>
+      <c r="C116" s="60"/>
+      <c r="D116" s="61"/>
+      <c r="E116" s="62"/>
     </row>
     <row r="117" spans="1:5" s="1" customFormat="1">
-      <c r="A117" s="61"/>
-      <c r="B117" s="61"/>
-      <c r="C117" s="61"/>
-      <c r="D117" s="62"/>
-      <c r="E117" s="63"/>
+      <c r="A117" s="60"/>
+      <c r="B117" s="60"/>
+      <c r="C117" s="60"/>
+      <c r="D117" s="61"/>
+      <c r="E117" s="62"/>
     </row>
     <row r="118" spans="1:5" s="1" customFormat="1">
-      <c r="A118" s="61"/>
-      <c r="B118" s="61"/>
-      <c r="C118" s="61"/>
-      <c r="D118" s="62"/>
-      <c r="E118" s="63"/>
+      <c r="A118" s="60"/>
+      <c r="B118" s="60"/>
+      <c r="C118" s="60"/>
+      <c r="D118" s="61"/>
+      <c r="E118" s="62"/>
     </row>
     <row r="119" spans="1:5" s="1" customFormat="1">
-      <c r="A119" s="61"/>
-      <c r="B119" s="61"/>
-      <c r="C119" s="61"/>
-      <c r="D119" s="62"/>
-      <c r="E119" s="63"/>
+      <c r="A119" s="60"/>
+      <c r="B119" s="60"/>
+      <c r="C119" s="60"/>
+      <c r="D119" s="61"/>
+      <c r="E119" s="62"/>
     </row>
     <row r="120" spans="1:5" s="1" customFormat="1">
-      <c r="A120" s="61"/>
-      <c r="B120" s="61"/>
-      <c r="C120" s="61"/>
-      <c r="D120" s="62"/>
-      <c r="E120" s="63"/>
+      <c r="A120" s="60"/>
+      <c r="B120" s="60"/>
+      <c r="C120" s="60"/>
+      <c r="D120" s="61"/>
+      <c r="E120" s="62"/>
     </row>
     <row r="121" spans="1:5" s="1" customFormat="1">
-      <c r="A121" s="61"/>
-      <c r="B121" s="61"/>
-      <c r="C121" s="61"/>
-      <c r="D121" s="62"/>
-      <c r="E121" s="63"/>
+      <c r="A121" s="60"/>
+      <c r="B121" s="60"/>
+      <c r="C121" s="60"/>
+      <c r="D121" s="61"/>
+      <c r="E121" s="62"/>
     </row>
     <row r="122" spans="1:5" s="1" customFormat="1">
-      <c r="A122" s="61"/>
-      <c r="B122" s="61"/>
-      <c r="C122" s="61"/>
-      <c r="D122" s="62"/>
-      <c r="E122" s="63"/>
+      <c r="A122" s="60"/>
+      <c r="B122" s="60"/>
+      <c r="C122" s="60"/>
+      <c r="D122" s="61"/>
+      <c r="E122" s="62"/>
     </row>
     <row r="123" spans="1:5" s="1" customFormat="1">
-      <c r="A123" s="61"/>
-      <c r="B123" s="61"/>
-      <c r="C123" s="61"/>
-      <c r="D123" s="62"/>
-      <c r="E123" s="63"/>
+      <c r="A123" s="60"/>
+      <c r="B123" s="60"/>
+      <c r="C123" s="60"/>
+      <c r="D123" s="61"/>
+      <c r="E123" s="62"/>
     </row>
     <row r="124" spans="1:5" s="1" customFormat="1">
-      <c r="A124" s="61"/>
-      <c r="B124" s="61"/>
-      <c r="C124" s="61"/>
-      <c r="D124" s="62"/>
-      <c r="E124" s="63"/>
+      <c r="A124" s="60"/>
+      <c r="B124" s="60"/>
+      <c r="C124" s="60"/>
+      <c r="D124" s="61"/>
+      <c r="E124" s="62"/>
     </row>
     <row r="125" spans="1:5" s="1" customFormat="1">
-      <c r="A125" s="61"/>
-      <c r="B125" s="61"/>
-      <c r="C125" s="61"/>
-      <c r="D125" s="62"/>
-      <c r="E125" s="63"/>
+      <c r="A125" s="60"/>
+      <c r="B125" s="60"/>
+      <c r="C125" s="60"/>
+      <c r="D125" s="61"/>
+      <c r="E125" s="62"/>
     </row>
     <row r="126" spans="1:5" s="1" customFormat="1">
-      <c r="A126" s="61"/>
-      <c r="B126" s="61"/>
-      <c r="C126" s="61"/>
-      <c r="D126" s="62"/>
-      <c r="E126" s="63"/>
+      <c r="A126" s="60"/>
+      <c r="B126" s="60"/>
+      <c r="C126" s="60"/>
+      <c r="D126" s="61"/>
+      <c r="E126" s="62"/>
     </row>
     <row r="127" spans="1:5" s="1" customFormat="1">
-      <c r="A127" s="61"/>
-      <c r="B127" s="61"/>
-      <c r="C127" s="61"/>
-      <c r="D127" s="62"/>
-      <c r="E127" s="63"/>
+      <c r="A127" s="60"/>
+      <c r="B127" s="60"/>
+      <c r="C127" s="60"/>
+      <c r="D127" s="61"/>
+      <c r="E127" s="62"/>
     </row>
     <row r="128" spans="1:5" s="1" customFormat="1">
-      <c r="A128" s="61"/>
-      <c r="B128" s="61"/>
-      <c r="C128" s="61"/>
-      <c r="D128" s="62"/>
-      <c r="E128" s="63"/>
+      <c r="A128" s="60"/>
+      <c r="B128" s="60"/>
+      <c r="C128" s="60"/>
+      <c r="D128" s="61"/>
+      <c r="E128" s="62"/>
     </row>
     <row r="129" spans="1:5" s="1" customFormat="1">
-      <c r="A129" s="61"/>
-      <c r="B129" s="61"/>
-      <c r="C129" s="61"/>
-      <c r="D129" s="62"/>
-      <c r="E129" s="63"/>
+      <c r="A129" s="60"/>
+      <c r="B129" s="60"/>
+      <c r="C129" s="60"/>
+      <c r="D129" s="61"/>
+      <c r="E129" s="62"/>
     </row>
     <row r="130" spans="1:5" s="1" customFormat="1">
-      <c r="A130" s="61"/>
-      <c r="B130" s="61"/>
-      <c r="C130" s="61"/>
-      <c r="D130" s="62"/>
-      <c r="E130" s="63"/>
+      <c r="A130" s="60"/>
+      <c r="B130" s="60"/>
+      <c r="C130" s="60"/>
+      <c r="D130" s="61"/>
+      <c r="E130" s="62"/>
     </row>
     <row r="131" spans="1:5" s="1" customFormat="1">
-      <c r="A131" s="61"/>
-      <c r="B131" s="61"/>
-      <c r="C131" s="61"/>
-      <c r="D131" s="62"/>
-      <c r="E131" s="63"/>
+      <c r="A131" s="60"/>
+      <c r="B131" s="60"/>
+      <c r="C131" s="60"/>
+      <c r="D131" s="61"/>
+      <c r="E131" s="62"/>
     </row>
     <row r="132" spans="1:5" s="1" customFormat="1">
-      <c r="A132" s="61"/>
-      <c r="B132" s="61"/>
-      <c r="C132" s="61"/>
-      <c r="D132" s="62"/>
-      <c r="E132" s="63"/>
+      <c r="A132" s="60"/>
+      <c r="B132" s="60"/>
+      <c r="C132" s="60"/>
+      <c r="D132" s="61"/>
+      <c r="E132" s="62"/>
     </row>
     <row r="133" spans="1:5" s="1" customFormat="1">
-      <c r="A133" s="61"/>
-      <c r="B133" s="61"/>
-      <c r="C133" s="61"/>
-      <c r="D133" s="62"/>
-      <c r="E133" s="63"/>
+      <c r="A133" s="60"/>
+      <c r="B133" s="60"/>
+      <c r="C133" s="60"/>
+      <c r="D133" s="61"/>
+      <c r="E133" s="62"/>
     </row>
     <row r="134" spans="1:5" s="1" customFormat="1">
-      <c r="A134" s="61"/>
-      <c r="B134" s="61"/>
-      <c r="C134" s="61"/>
-      <c r="D134" s="62"/>
-      <c r="E134" s="63"/>
+      <c r="A134" s="60"/>
+      <c r="B134" s="60"/>
+      <c r="C134" s="60"/>
+      <c r="D134" s="61"/>
+      <c r="E134" s="62"/>
     </row>
     <row r="135" spans="1:5" s="1" customFormat="1">
-      <c r="A135" s="61"/>
-      <c r="B135" s="61"/>
-      <c r="C135" s="61"/>
-      <c r="D135" s="62"/>
-      <c r="E135" s="63"/>
+      <c r="A135" s="60"/>
+      <c r="B135" s="60"/>
+      <c r="C135" s="60"/>
+      <c r="D135" s="61"/>
+      <c r="E135" s="62"/>
     </row>
     <row r="136" spans="1:5" s="1" customFormat="1">
-      <c r="A136" s="61"/>
-      <c r="B136" s="61"/>
-      <c r="C136" s="61"/>
-      <c r="D136" s="62"/>
-      <c r="E136" s="63"/>
+      <c r="A136" s="60"/>
+      <c r="B136" s="60"/>
+      <c r="C136" s="60"/>
+      <c r="D136" s="61"/>
+      <c r="E136" s="62"/>
     </row>
     <row r="137" spans="1:5" s="1" customFormat="1">
-      <c r="A137" s="61"/>
-      <c r="B137" s="61"/>
-      <c r="C137" s="61"/>
-      <c r="D137" s="62"/>
-      <c r="E137" s="63"/>
+      <c r="A137" s="60"/>
+      <c r="B137" s="60"/>
+      <c r="C137" s="60"/>
+      <c r="D137" s="61"/>
+      <c r="E137" s="62"/>
     </row>
     <row r="138" spans="1:5" s="1" customFormat="1">
-      <c r="A138" s="61"/>
-      <c r="B138" s="61"/>
-      <c r="C138" s="61"/>
-      <c r="D138" s="62"/>
-      <c r="E138" s="63"/>
+      <c r="A138" s="60"/>
+      <c r="B138" s="60"/>
+      <c r="C138" s="60"/>
+      <c r="D138" s="61"/>
+      <c r="E138" s="62"/>
     </row>
     <row r="139" spans="1:5" s="1" customFormat="1">
-      <c r="A139" s="61"/>
-      <c r="B139" s="61"/>
-      <c r="C139" s="61"/>
-      <c r="D139" s="62"/>
-      <c r="E139" s="63"/>
+      <c r="A139" s="60"/>
+      <c r="B139" s="60"/>
+      <c r="C139" s="60"/>
+      <c r="D139" s="61"/>
+      <c r="E139" s="62"/>
     </row>
     <row r="140" spans="1:5" s="1" customFormat="1">
-      <c r="A140" s="61"/>
-      <c r="B140" s="61"/>
-      <c r="C140" s="61"/>
-      <c r="D140" s="62"/>
-      <c r="E140" s="63"/>
+      <c r="A140" s="60"/>
+      <c r="B140" s="60"/>
+      <c r="C140" s="60"/>
+      <c r="D140" s="61"/>
+      <c r="E140" s="62"/>
     </row>
     <row r="141" spans="1:5" s="1" customFormat="1">
-      <c r="A141" s="61"/>
-      <c r="B141" s="61"/>
-      <c r="C141" s="61"/>
-      <c r="D141" s="62"/>
-      <c r="E141" s="63"/>
+      <c r="A141" s="60"/>
+      <c r="B141" s="60"/>
+      <c r="C141" s="60"/>
+      <c r="D141" s="61"/>
+      <c r="E141" s="62"/>
     </row>
     <row r="142" spans="1:5" s="1" customFormat="1">
-      <c r="A142" s="61"/>
-      <c r="B142" s="61"/>
-      <c r="C142" s="61"/>
-      <c r="D142" s="62"/>
-      <c r="E142" s="63"/>
+      <c r="A142" s="60"/>
+      <c r="B142" s="60"/>
+      <c r="C142" s="60"/>
+      <c r="D142" s="61"/>
+      <c r="E142" s="62"/>
     </row>
     <row r="143" spans="1:5" s="1" customFormat="1">
-      <c r="A143" s="61"/>
-      <c r="B143" s="61"/>
-      <c r="C143" s="61"/>
-      <c r="D143" s="62"/>
-      <c r="E143" s="63"/>
+      <c r="A143" s="60"/>
+      <c r="B143" s="60"/>
+      <c r="C143" s="60"/>
+      <c r="D143" s="61"/>
+      <c r="E143" s="62"/>
     </row>
     <row r="144" spans="1:5" s="1" customFormat="1">
-      <c r="A144" s="61"/>
-      <c r="B144" s="61"/>
-      <c r="C144" s="61"/>
-      <c r="D144" s="62"/>
-      <c r="E144" s="63"/>
+      <c r="A144" s="60"/>
+      <c r="B144" s="60"/>
+      <c r="C144" s="60"/>
+      <c r="D144" s="61"/>
+      <c r="E144" s="62"/>
     </row>
     <row r="145" spans="1:5" s="1" customFormat="1">
-      <c r="A145" s="61"/>
-      <c r="B145" s="61"/>
-      <c r="C145" s="61"/>
-      <c r="D145" s="62"/>
-      <c r="E145" s="63"/>
+      <c r="A145" s="60"/>
+      <c r="B145" s="60"/>
+      <c r="C145" s="60"/>
+      <c r="D145" s="61"/>
+      <c r="E145" s="62"/>
     </row>
     <row r="146" spans="1:5" s="1" customFormat="1">
-      <c r="A146" s="61"/>
-      <c r="B146" s="61"/>
-      <c r="C146" s="61"/>
-      <c r="D146" s="62"/>
-      <c r="E146" s="63"/>
+      <c r="A146" s="60"/>
+      <c r="B146" s="60"/>
+      <c r="C146" s="60"/>
+      <c r="D146" s="61"/>
+      <c r="E146" s="62"/>
     </row>
     <row r="147" spans="1:5" s="1" customFormat="1">
-      <c r="A147" s="61"/>
-      <c r="B147" s="61"/>
-      <c r="C147" s="61"/>
-      <c r="D147" s="62"/>
-      <c r="E147" s="63"/>
+      <c r="A147" s="60"/>
+      <c r="B147" s="60"/>
+      <c r="C147" s="60"/>
+      <c r="D147" s="61"/>
+      <c r="E147" s="62"/>
     </row>
     <row r="148" spans="1:5" s="1" customFormat="1">
-      <c r="A148" s="61"/>
-      <c r="B148" s="61"/>
-      <c r="C148" s="61"/>
-      <c r="D148" s="62"/>
-      <c r="E148" s="63"/>
+      <c r="A148" s="60"/>
+      <c r="B148" s="60"/>
+      <c r="C148" s="60"/>
+      <c r="D148" s="61"/>
+      <c r="E148" s="62"/>
     </row>
     <row r="149" spans="1:5" s="1" customFormat="1">
-      <c r="A149" s="61"/>
-      <c r="B149" s="61"/>
-      <c r="C149" s="61"/>
-      <c r="D149" s="62"/>
-      <c r="E149" s="63"/>
+      <c r="A149" s="60"/>
+      <c r="B149" s="60"/>
+      <c r="C149" s="60"/>
+      <c r="D149" s="61"/>
+      <c r="E149" s="62"/>
     </row>
     <row r="150" spans="1:5" s="1" customFormat="1">
-      <c r="A150" s="61"/>
-      <c r="B150" s="61"/>
-      <c r="C150" s="61"/>
-      <c r="D150" s="62"/>
-      <c r="E150" s="63"/>
+      <c r="A150" s="60"/>
+      <c r="B150" s="60"/>
+      <c r="C150" s="60"/>
+      <c r="D150" s="61"/>
+      <c r="E150" s="62"/>
     </row>
     <row r="151" spans="1:5" s="1" customFormat="1">
-      <c r="A151" s="61"/>
-      <c r="B151" s="61"/>
-      <c r="C151" s="61"/>
-      <c r="D151" s="62"/>
-      <c r="E151" s="63"/>
+      <c r="A151" s="60"/>
+      <c r="B151" s="60"/>
+      <c r="C151" s="60"/>
+      <c r="D151" s="61"/>
+      <c r="E151" s="62"/>
     </row>
     <row r="152" spans="1:5" s="1" customFormat="1">
-      <c r="A152" s="61"/>
-      <c r="B152" s="61"/>
-      <c r="C152" s="61"/>
-      <c r="D152" s="62"/>
-      <c r="E152" s="63"/>
+      <c r="A152" s="60"/>
+      <c r="B152" s="60"/>
+      <c r="C152" s="60"/>
+      <c r="D152" s="61"/>
+      <c r="E152" s="62"/>
     </row>
     <row r="153" spans="1:5" s="1" customFormat="1">
-      <c r="A153" s="61"/>
-      <c r="B153" s="61"/>
-      <c r="C153" s="61"/>
-      <c r="D153" s="62"/>
-      <c r="E153" s="63"/>
+      <c r="A153" s="60"/>
+      <c r="B153" s="60"/>
+      <c r="C153" s="60"/>
+      <c r="D153" s="61"/>
+      <c r="E153" s="62"/>
     </row>
     <row r="154" spans="1:5" s="1" customFormat="1">
-      <c r="A154" s="61"/>
-      <c r="B154" s="61"/>
-      <c r="C154" s="61"/>
-      <c r="D154" s="62"/>
-      <c r="E154" s="63"/>
+      <c r="A154" s="60"/>
+      <c r="B154" s="60"/>
+      <c r="C154" s="60"/>
+      <c r="D154" s="61"/>
+      <c r="E154" s="62"/>
     </row>
     <row r="155" spans="1:5" s="1" customFormat="1">
-      <c r="A155" s="61"/>
-      <c r="B155" s="61"/>
-      <c r="C155" s="61"/>
-      <c r="D155" s="62"/>
-      <c r="E155" s="63"/>
+      <c r="A155" s="60"/>
+      <c r="B155" s="60"/>
+      <c r="C155" s="60"/>
+      <c r="D155" s="61"/>
+      <c r="E155" s="62"/>
     </row>
     <row r="156" spans="1:5" s="1" customFormat="1">
-      <c r="A156" s="61"/>
-      <c r="B156" s="61"/>
-      <c r="C156" s="61"/>
-      <c r="D156" s="62"/>
-      <c r="E156" s="63"/>
+      <c r="A156" s="60"/>
+      <c r="B156" s="60"/>
+      <c r="C156" s="60"/>
+      <c r="D156" s="61"/>
+      <c r="E156" s="62"/>
     </row>
     <row r="157" spans="1:5" s="1" customFormat="1">
-      <c r="A157" s="61"/>
-      <c r="B157" s="61"/>
-      <c r="C157" s="61"/>
-      <c r="D157" s="62"/>
-      <c r="E157" s="63"/>
+      <c r="A157" s="60"/>
+      <c r="B157" s="60"/>
+      <c r="C157" s="60"/>
+      <c r="D157" s="61"/>
+      <c r="E157" s="62"/>
     </row>
     <row r="158" spans="1:5" s="1" customFormat="1">
-      <c r="A158" s="61"/>
-      <c r="B158" s="61"/>
-      <c r="C158" s="61"/>
-      <c r="D158" s="62"/>
-      <c r="E158" s="63"/>
+      <c r="A158" s="60"/>
+      <c r="B158" s="60"/>
+      <c r="C158" s="60"/>
+      <c r="D158" s="61"/>
+      <c r="E158" s="62"/>
     </row>
     <row r="159" spans="1:5" s="1" customFormat="1">
-      <c r="A159" s="61"/>
-      <c r="B159" s="61"/>
-      <c r="C159" s="61"/>
-      <c r="D159" s="62"/>
-      <c r="E159" s="63"/>
+      <c r="A159" s="60"/>
+      <c r="B159" s="60"/>
+      <c r="C159" s="60"/>
+      <c r="D159" s="61"/>
+      <c r="E159" s="62"/>
     </row>
     <row r="160" spans="1:5" s="1" customFormat="1">
-      <c r="A160" s="61"/>
-      <c r="B160" s="61"/>
-      <c r="C160" s="61"/>
-      <c r="D160" s="62"/>
-      <c r="E160" s="63"/>
+      <c r="A160" s="60"/>
+      <c r="B160" s="60"/>
+      <c r="C160" s="60"/>
+      <c r="D160" s="61"/>
+      <c r="E160" s="62"/>
     </row>
     <row r="161" spans="1:5" s="1" customFormat="1">
-      <c r="A161" s="61"/>
-      <c r="B161" s="61"/>
-      <c r="C161" s="61"/>
-      <c r="D161" s="62"/>
-      <c r="E161" s="63"/>
+      <c r="A161" s="60"/>
+      <c r="B161" s="60"/>
+      <c r="C161" s="60"/>
+      <c r="D161" s="61"/>
+      <c r="E161" s="62"/>
     </row>
     <row r="162" spans="1:5" s="1" customFormat="1">
-      <c r="A162" s="61"/>
-      <c r="B162" s="61"/>
-      <c r="C162" s="61"/>
-      <c r="D162" s="62"/>
-      <c r="E162" s="63"/>
+      <c r="A162" s="60"/>
+      <c r="B162" s="60"/>
+      <c r="C162" s="60"/>
+      <c r="D162" s="61"/>
+      <c r="E162" s="62"/>
     </row>
     <row r="163" spans="1:5" s="1" customFormat="1">
-      <c r="A163" s="61"/>
-      <c r="B163" s="61"/>
-      <c r="C163" s="61"/>
-      <c r="D163" s="62"/>
-      <c r="E163" s="63"/>
+      <c r="A163" s="60"/>
+      <c r="B163" s="60"/>
+      <c r="C163" s="60"/>
+      <c r="D163" s="61"/>
+      <c r="E163" s="62"/>
     </row>
     <row r="164" spans="1:5" s="1" customFormat="1">
-      <c r="A164" s="61"/>
-      <c r="B164" s="61"/>
-      <c r="C164" s="61"/>
-      <c r="D164" s="62"/>
-      <c r="E164" s="63"/>
+      <c r="A164" s="60"/>
+      <c r="B164" s="60"/>
+      <c r="C164" s="60"/>
+      <c r="D164" s="61"/>
+      <c r="E164" s="62"/>
     </row>
     <row r="165" spans="1:5" s="1" customFormat="1">
-      <c r="A165" s="61"/>
-      <c r="B165" s="61"/>
-      <c r="C165" s="61"/>
-      <c r="D165" s="62"/>
-      <c r="E165" s="63"/>
+      <c r="A165" s="60"/>
+      <c r="B165" s="60"/>
+      <c r="C165" s="60"/>
+      <c r="D165" s="61"/>
+      <c r="E165" s="62"/>
     </row>
     <row r="166" spans="1:5" s="1" customFormat="1">
-      <c r="A166" s="61"/>
-      <c r="B166" s="61"/>
-      <c r="C166" s="61"/>
-      <c r="D166" s="62"/>
-      <c r="E166" s="63"/>
+      <c r="A166" s="60"/>
+      <c r="B166" s="60"/>
+      <c r="C166" s="60"/>
+      <c r="D166" s="61"/>
+      <c r="E166" s="62"/>
     </row>
     <row r="167" spans="1:5" s="1" customFormat="1">
-      <c r="A167" s="61"/>
-      <c r="B167" s="61"/>
-      <c r="C167" s="61"/>
-      <c r="D167" s="62"/>
-      <c r="E167" s="63"/>
+      <c r="A167" s="60"/>
+      <c r="B167" s="60"/>
+      <c r="C167" s="60"/>
+      <c r="D167" s="61"/>
+      <c r="E167" s="62"/>
     </row>
     <row r="168" spans="1:5" s="1" customFormat="1">
-      <c r="A168" s="61"/>
-      <c r="B168" s="61"/>
-      <c r="C168" s="61"/>
-      <c r="D168" s="62"/>
-      <c r="E168" s="63"/>
+      <c r="A168" s="60"/>
+      <c r="B168" s="60"/>
+      <c r="C168" s="60"/>
+      <c r="D168" s="61"/>
+      <c r="E168" s="62"/>
     </row>
     <row r="169" spans="1:5" s="1" customFormat="1">
-      <c r="A169" s="61"/>
-      <c r="B169" s="61"/>
-      <c r="C169" s="61"/>
-      <c r="D169" s="62"/>
-      <c r="E169" s="63"/>
+      <c r="A169" s="60"/>
+      <c r="B169" s="60"/>
+      <c r="C169" s="60"/>
+      <c r="D169" s="61"/>
+      <c r="E169" s="62"/>
     </row>
     <row r="170" spans="1:5" s="1" customFormat="1">
-      <c r="A170" s="61"/>
-      <c r="B170" s="61"/>
-      <c r="C170" s="61"/>
-      <c r="D170" s="62"/>
-      <c r="E170" s="63"/>
+      <c r="A170" s="60"/>
+      <c r="B170" s="60"/>
+      <c r="C170" s="60"/>
+      <c r="D170" s="61"/>
+      <c r="E170" s="62"/>
     </row>
     <row r="171" spans="1:5" s="1" customFormat="1">
-      <c r="A171" s="61"/>
-      <c r="B171" s="61"/>
-      <c r="C171" s="61"/>
-      <c r="D171" s="62"/>
-      <c r="E171" s="63"/>
+      <c r="A171" s="60"/>
+      <c r="B171" s="60"/>
+      <c r="C171" s="60"/>
+      <c r="D171" s="61"/>
+      <c r="E171" s="62"/>
     </row>
     <row r="172" spans="1:5" s="1" customFormat="1">
-      <c r="A172" s="61"/>
-      <c r="B172" s="61"/>
-      <c r="C172" s="61"/>
-      <c r="D172" s="62"/>
-      <c r="E172" s="63"/>
+      <c r="A172" s="60"/>
+      <c r="B172" s="60"/>
+      <c r="C172" s="60"/>
+      <c r="D172" s="61"/>
+      <c r="E172" s="62"/>
     </row>
     <row r="173" spans="1:5" s="1" customFormat="1">
-      <c r="A173" s="61"/>
-      <c r="B173" s="61"/>
-      <c r="C173" s="61"/>
-      <c r="D173" s="62"/>
-      <c r="E173" s="63"/>
+      <c r="A173" s="60"/>
+      <c r="B173" s="60"/>
+      <c r="C173" s="60"/>
+      <c r="D173" s="61"/>
+      <c r="E173" s="62"/>
     </row>
     <row r="174" spans="1:5" s="1" customFormat="1">
-      <c r="A174" s="61"/>
-      <c r="B174" s="61"/>
-      <c r="C174" s="61"/>
-      <c r="D174" s="62"/>
-      <c r="E174" s="63"/>
+      <c r="A174" s="60"/>
+      <c r="B174" s="60"/>
+      <c r="C174" s="60"/>
+      <c r="D174" s="61"/>
+      <c r="E174" s="62"/>
     </row>
     <row r="175" spans="1:5" s="1" customFormat="1">
-      <c r="A175" s="61"/>
-      <c r="B175" s="61"/>
-      <c r="C175" s="61"/>
-      <c r="D175" s="62"/>
-      <c r="E175" s="63"/>
+      <c r="A175" s="60"/>
+      <c r="B175" s="60"/>
+      <c r="C175" s="60"/>
+      <c r="D175" s="61"/>
+      <c r="E175" s="62"/>
     </row>
     <row r="176" spans="1:5" s="1" customFormat="1">
-      <c r="A176" s="61"/>
-      <c r="B176" s="61"/>
-      <c r="C176" s="61"/>
-      <c r="D176" s="62"/>
-      <c r="E176" s="63"/>
+      <c r="A176" s="60"/>
+      <c r="B176" s="60"/>
+      <c r="C176" s="60"/>
+      <c r="D176" s="61"/>
+      <c r="E176" s="62"/>
     </row>
     <row r="177" spans="1:5" s="1" customFormat="1">
-      <c r="A177" s="61"/>
-      <c r="B177" s="61"/>
-      <c r="C177" s="61"/>
-      <c r="D177" s="62"/>
-      <c r="E177" s="63"/>
+      <c r="A177" s="60"/>
+      <c r="B177" s="60"/>
+      <c r="C177" s="60"/>
+      <c r="D177" s="61"/>
+      <c r="E177" s="62"/>
     </row>
     <row r="178" spans="1:5" s="1" customFormat="1">
-      <c r="A178" s="61"/>
-      <c r="B178" s="61"/>
-      <c r="C178" s="61"/>
-      <c r="D178" s="62"/>
-      <c r="E178" s="63"/>
+      <c r="A178" s="60"/>
+      <c r="B178" s="60"/>
+      <c r="C178" s="60"/>
+      <c r="D178" s="61"/>
+      <c r="E178" s="62"/>
     </row>
     <row r="179" spans="1:5" s="1" customFormat="1">
-      <c r="A179" s="61"/>
-      <c r="B179" s="61"/>
-      <c r="C179" s="61"/>
-      <c r="D179" s="62"/>
-      <c r="E179" s="63"/>
+      <c r="A179" s="60"/>
+      <c r="B179" s="60"/>
+      <c r="C179" s="60"/>
+      <c r="D179" s="61"/>
+      <c r="E179" s="62"/>
     </row>
     <row r="180" spans="1:5" s="1" customFormat="1">
-      <c r="A180" s="61"/>
-      <c r="B180" s="61"/>
-      <c r="C180" s="61"/>
-      <c r="D180" s="62"/>
-      <c r="E180" s="63"/>
+      <c r="A180" s="60"/>
+      <c r="B180" s="60"/>
+      <c r="C180" s="60"/>
+      <c r="D180" s="61"/>
+      <c r="E180" s="62"/>
     </row>
     <row r="181" spans="1:5" s="1" customFormat="1">
-      <c r="A181" s="61"/>
-      <c r="B181" s="61"/>
-      <c r="C181" s="61"/>
-      <c r="D181" s="62"/>
-      <c r="E181" s="63"/>
+      <c r="A181" s="60"/>
+      <c r="B181" s="60"/>
+      <c r="C181" s="60"/>
+      <c r="D181" s="61"/>
+      <c r="E181" s="62"/>
     </row>
     <row r="182" spans="1:5" s="1" customFormat="1">
-      <c r="A182" s="61"/>
-      <c r="B182" s="61"/>
-      <c r="C182" s="61"/>
-      <c r="D182" s="62"/>
-      <c r="E182" s="63"/>
+      <c r="A182" s="60"/>
+      <c r="B182" s="60"/>
+      <c r="C182" s="60"/>
+      <c r="D182" s="61"/>
+      <c r="E182" s="62"/>
     </row>
     <row r="183" spans="1:5" s="1" customFormat="1">
-      <c r="A183" s="61"/>
-      <c r="B183" s="61"/>
-      <c r="C183" s="61"/>
-      <c r="D183" s="62"/>
-      <c r="E183" s="63"/>
+      <c r="A183" s="60"/>
+      <c r="B183" s="60"/>
+      <c r="C183" s="60"/>
+      <c r="D183" s="61"/>
+      <c r="E183" s="62"/>
     </row>
     <row r="184" spans="1:5" s="1" customFormat="1">
-      <c r="A184" s="61"/>
-      <c r="B184" s="61"/>
-      <c r="C184" s="61"/>
-      <c r="D184" s="62"/>
-      <c r="E184" s="63"/>
+      <c r="A184" s="60"/>
+      <c r="B184" s="60"/>
+      <c r="C184" s="60"/>
+      <c r="D184" s="61"/>
+      <c r="E184" s="62"/>
     </row>
     <row r="185" spans="1:5" s="1" customFormat="1">
-      <c r="A185" s="61"/>
-      <c r="B185" s="61"/>
-      <c r="C185" s="61"/>
-      <c r="D185" s="62"/>
-      <c r="E185" s="63"/>
+      <c r="A185" s="60"/>
+      <c r="B185" s="60"/>
+      <c r="C185" s="60"/>
+      <c r="D185" s="61"/>
+      <c r="E185" s="62"/>
     </row>
     <row r="186" spans="1:5" s="1" customFormat="1">
-      <c r="A186" s="61"/>
-      <c r="B186" s="61"/>
-      <c r="C186" s="61"/>
-      <c r="D186" s="62"/>
-      <c r="E186" s="63"/>
+      <c r="A186" s="60"/>
+      <c r="B186" s="60"/>
+      <c r="C186" s="60"/>
+      <c r="D186" s="61"/>
+      <c r="E186" s="62"/>
     </row>
     <row r="187" spans="1:5" s="1" customFormat="1">
-      <c r="A187" s="61"/>
-      <c r="B187" s="61"/>
-      <c r="C187" s="61"/>
-      <c r="D187" s="62"/>
-      <c r="E187" s="63"/>
+      <c r="A187" s="60"/>
+      <c r="B187" s="60"/>
+      <c r="C187" s="60"/>
+      <c r="D187" s="61"/>
+      <c r="E187" s="62"/>
     </row>
     <row r="188" spans="1:5" s="1" customFormat="1">
-      <c r="A188" s="61"/>
-      <c r="B188" s="61"/>
-      <c r="C188" s="61"/>
-      <c r="D188" s="62"/>
-      <c r="E188" s="63"/>
+      <c r="A188" s="60"/>
+      <c r="B188" s="60"/>
+      <c r="C188" s="60"/>
+      <c r="D188" s="61"/>
+      <c r="E188" s="62"/>
     </row>
     <row r="189" spans="1:5" s="1" customFormat="1">
-      <c r="A189" s="61"/>
-      <c r="B189" s="61"/>
-      <c r="C189" s="61"/>
-      <c r="D189" s="62"/>
-      <c r="E189" s="63"/>
+      <c r="A189" s="60"/>
+      <c r="B189" s="60"/>
+      <c r="C189" s="60"/>
+      <c r="D189" s="61"/>
+      <c r="E189" s="62"/>
     </row>
     <row r="190" spans="1:5" s="1" customFormat="1">
-      <c r="A190" s="61"/>
-      <c r="B190" s="61"/>
-      <c r="C190" s="61"/>
-      <c r="D190" s="62"/>
-      <c r="E190" s="63"/>
+      <c r="A190" s="60"/>
+      <c r="B190" s="60"/>
+      <c r="C190" s="60"/>
+      <c r="D190" s="61"/>
+      <c r="E190" s="62"/>
     </row>
     <row r="191" spans="1:5" s="1" customFormat="1">
-      <c r="A191" s="61"/>
-      <c r="B191" s="61"/>
-      <c r="C191" s="61"/>
-      <c r="D191" s="62"/>
-      <c r="E191" s="63"/>
+      <c r="A191" s="60"/>
+      <c r="B191" s="60"/>
+      <c r="C191" s="60"/>
+      <c r="D191" s="61"/>
+      <c r="E191" s="62"/>
     </row>
     <row r="192" spans="1:5" s="1" customFormat="1">
-      <c r="A192" s="61"/>
-      <c r="B192" s="61"/>
-      <c r="C192" s="61"/>
-      <c r="D192" s="62"/>
-      <c r="E192" s="63"/>
+      <c r="A192" s="60"/>
+      <c r="B192" s="60"/>
+      <c r="C192" s="60"/>
+      <c r="D192" s="61"/>
+      <c r="E192" s="62"/>
     </row>
     <row r="193" spans="1:5" s="1" customFormat="1">
-      <c r="A193" s="61"/>
-      <c r="B193" s="61"/>
-      <c r="C193" s="61"/>
-      <c r="D193" s="62"/>
-      <c r="E193" s="63"/>
+      <c r="A193" s="60"/>
+      <c r="B193" s="60"/>
+      <c r="C193" s="60"/>
+      <c r="D193" s="61"/>
+      <c r="E193" s="62"/>
     </row>
     <row r="194" spans="1:5" s="1" customFormat="1">
-      <c r="A194" s="61"/>
-      <c r="B194" s="61"/>
-      <c r="C194" s="61"/>
-      <c r="D194" s="62"/>
-      <c r="E194" s="64"/>
+      <c r="A194" s="60"/>
+      <c r="B194" s="60"/>
+      <c r="C194" s="60"/>
+      <c r="D194" s="61"/>
+      <c r="E194" s="63"/>
     </row>
     <row r="195" spans="1:5" s="1" customFormat="1">
-      <c r="A195" s="61"/>
-      <c r="B195" s="61"/>
-      <c r="C195" s="61"/>
-      <c r="D195" s="62"/>
-      <c r="E195" s="64"/>
+      <c r="A195" s="60"/>
+      <c r="B195" s="60"/>
+      <c r="C195" s="60"/>
+      <c r="D195" s="61"/>
+      <c r="E195" s="63"/>
     </row>
     <row r="196" spans="1:5" s="1" customFormat="1">
-      <c r="A196" s="61"/>
-      <c r="B196" s="61"/>
-      <c r="C196" s="61"/>
-      <c r="D196" s="62"/>
-      <c r="E196" s="64"/>
+      <c r="A196" s="60"/>
+      <c r="B196" s="60"/>
+      <c r="C196" s="60"/>
+      <c r="D196" s="61"/>
+      <c r="E196" s="63"/>
     </row>
     <row r="197" spans="1:5" s="1" customFormat="1">
-      <c r="A197" s="61"/>
-      <c r="B197" s="61"/>
-      <c r="C197" s="61"/>
-      <c r="D197" s="62"/>
-      <c r="E197" s="64"/>
+      <c r="A197" s="60"/>
+      <c r="B197" s="60"/>
+      <c r="C197" s="60"/>
+      <c r="D197" s="61"/>
+      <c r="E197" s="63"/>
     </row>
     <row r="198" spans="1:5" s="1" customFormat="1">
-      <c r="A198" s="61"/>
-      <c r="B198" s="61"/>
-      <c r="C198" s="61"/>
-      <c r="D198" s="62"/>
-      <c r="E198" s="64"/>
+      <c r="A198" s="60"/>
+      <c r="B198" s="60"/>
+      <c r="C198" s="60"/>
+      <c r="D198" s="61"/>
+      <c r="E198" s="63"/>
     </row>
     <row r="199" spans="1:5" s="1" customFormat="1">
-      <c r="A199" s="61"/>
-      <c r="B199" s="61"/>
-      <c r="C199" s="61"/>
-      <c r="D199" s="62"/>
-      <c r="E199" s="64"/>
+      <c r="A199" s="60"/>
+      <c r="B199" s="60"/>
+      <c r="C199" s="60"/>
+      <c r="D199" s="61"/>
+      <c r="E199" s="63"/>
     </row>
     <row r="200" spans="1:5" s="1" customFormat="1">
-      <c r="A200" s="61"/>
-      <c r="B200" s="61"/>
-      <c r="C200" s="61"/>
-      <c r="D200" s="62"/>
-      <c r="E200" s="64"/>
+      <c r="A200" s="60"/>
+      <c r="B200" s="60"/>
+      <c r="C200" s="60"/>
+      <c r="D200" s="61"/>
+      <c r="E200" s="63"/>
     </row>
     <row r="201" spans="1:5" s="1" customFormat="1">
-      <c r="A201" s="61"/>
-      <c r="B201" s="61"/>
-      <c r="C201" s="61"/>
-      <c r="D201" s="62"/>
-      <c r="E201" s="64"/>
+      <c r="A201" s="60"/>
+      <c r="B201" s="60"/>
+      <c r="C201" s="60"/>
+      <c r="D201" s="61"/>
+      <c r="E201" s="63"/>
     </row>
     <row r="202" spans="1:5" s="1" customFormat="1">
-      <c r="A202" s="61"/>
-      <c r="B202" s="61"/>
-      <c r="C202" s="61"/>
-      <c r="D202" s="62"/>
-      <c r="E202" s="64"/>
+      <c r="A202" s="60"/>
+      <c r="B202" s="60"/>
+      <c r="C202" s="60"/>
+      <c r="D202" s="61"/>
+      <c r="E202" s="63"/>
     </row>
     <row r="203" spans="1:5" s="1" customFormat="1">
-      <c r="A203" s="61"/>
-      <c r="B203" s="61"/>
-      <c r="C203" s="61"/>
-      <c r="D203" s="62"/>
-      <c r="E203" s="64"/>
+      <c r="A203" s="60"/>
+      <c r="B203" s="60"/>
+      <c r="C203" s="60"/>
+      <c r="D203" s="61"/>
+      <c r="E203" s="63"/>
     </row>
     <row r="204" spans="1:5" s="1" customFormat="1">
-      <c r="A204" s="61"/>
-      <c r="B204" s="61"/>
-      <c r="C204" s="61"/>
-      <c r="D204" s="62"/>
-      <c r="E204" s="64"/>
+      <c r="A204" s="60"/>
+      <c r="B204" s="60"/>
+      <c r="C204" s="60"/>
+      <c r="D204" s="61"/>
+      <c r="E204" s="63"/>
     </row>
     <row r="205" spans="1:5" s="1" customFormat="1">
-      <c r="A205" s="61"/>
-      <c r="B205" s="61"/>
-      <c r="C205" s="61"/>
-      <c r="D205" s="62"/>
-      <c r="E205" s="64"/>
+      <c r="A205" s="60"/>
+      <c r="B205" s="60"/>
+      <c r="C205" s="60"/>
+      <c r="D205" s="61"/>
+      <c r="E205" s="63"/>
     </row>
     <row r="206" spans="1:5" s="1" customFormat="1">
-      <c r="A206" s="61"/>
-      <c r="B206" s="61"/>
-      <c r="C206" s="61"/>
-      <c r="D206" s="62"/>
-      <c r="E206" s="64"/>
+      <c r="A206" s="60"/>
+      <c r="B206" s="60"/>
+      <c r="C206" s="60"/>
+      <c r="D206" s="61"/>
+      <c r="E206" s="63"/>
     </row>
     <row r="207" spans="1:5" s="1" customFormat="1">
-      <c r="A207" s="61"/>
-      <c r="B207" s="61"/>
-      <c r="C207" s="61"/>
-      <c r="D207" s="62"/>
-      <c r="E207" s="64"/>
+      <c r="A207" s="60"/>
+      <c r="B207" s="60"/>
+      <c r="C207" s="60"/>
+      <c r="D207" s="61"/>
+      <c r="E207" s="63"/>
     </row>
     <row r="208" spans="1:5" s="1" customFormat="1">
-      <c r="A208" s="61"/>
-      <c r="B208" s="61"/>
-      <c r="C208" s="61"/>
-      <c r="D208" s="62"/>
-      <c r="E208" s="64"/>
+      <c r="A208" s="60"/>
+      <c r="B208" s="60"/>
+      <c r="C208" s="60"/>
+      <c r="D208" s="61"/>
+      <c r="E208" s="63"/>
     </row>
     <row r="209" spans="1:5" s="1" customFormat="1">
-      <c r="A209" s="61"/>
-      <c r="B209" s="61"/>
-      <c r="C209" s="61"/>
-      <c r="D209" s="62"/>
-      <c r="E209" s="64"/>
+      <c r="A209" s="60"/>
+      <c r="B209" s="60"/>
+      <c r="C209" s="60"/>
+      <c r="D209" s="61"/>
+      <c r="E209" s="63"/>
     </row>
     <row r="210" spans="1:5" s="1" customFormat="1">
-      <c r="A210" s="61"/>
-      <c r="B210" s="61"/>
-      <c r="C210" s="61"/>
-      <c r="D210" s="62"/>
-      <c r="E210" s="64"/>
+      <c r="A210" s="60"/>
+      <c r="B210" s="60"/>
+      <c r="C210" s="60"/>
+      <c r="D210" s="61"/>
+      <c r="E210" s="63"/>
     </row>
     <row r="211" spans="1:5" s="1" customFormat="1">
-      <c r="A211" s="61"/>
-      <c r="B211" s="61"/>
-      <c r="C211" s="61"/>
-      <c r="D211" s="62"/>
-      <c r="E211" s="64"/>
+      <c r="A211" s="60"/>
+      <c r="B211" s="60"/>
+      <c r="C211" s="60"/>
+      <c r="D211" s="61"/>
+      <c r="E211" s="63"/>
     </row>
     <row r="212" spans="1:5" s="1" customFormat="1">
-      <c r="A212" s="61"/>
-      <c r="B212" s="61"/>
-      <c r="C212" s="61"/>
-      <c r="D212" s="62"/>
-      <c r="E212" s="64"/>
+      <c r="A212" s="60"/>
+      <c r="B212" s="60"/>
+      <c r="C212" s="60"/>
+      <c r="D212" s="61"/>
+      <c r="E212" s="63"/>
     </row>
     <row r="213" spans="1:5" s="1" customFormat="1">
-      <c r="A213" s="61"/>
-      <c r="B213" s="61"/>
-      <c r="C213" s="61"/>
-      <c r="D213" s="62"/>
-      <c r="E213" s="64"/>
+      <c r="A213" s="60"/>
+      <c r="B213" s="60"/>
+      <c r="C213" s="60"/>
+      <c r="D213" s="61"/>
+      <c r="E213" s="63"/>
     </row>
     <row r="214" spans="1:5" s="1" customFormat="1">
-      <c r="A214" s="61"/>
-      <c r="B214" s="61"/>
-      <c r="C214" s="61"/>
-      <c r="D214" s="62"/>
-      <c r="E214" s="64"/>
+      <c r="A214" s="60"/>
+      <c r="B214" s="60"/>
+      <c r="C214" s="60"/>
+      <c r="D214" s="61"/>
+      <c r="E214" s="63"/>
     </row>
     <row r="215" spans="1:5" s="1" customFormat="1">
-      <c r="A215" s="61"/>
-      <c r="B215" s="61"/>
-      <c r="C215" s="61"/>
-      <c r="D215" s="62"/>
-      <c r="E215" s="64"/>
+      <c r="A215" s="60"/>
+      <c r="B215" s="60"/>
+      <c r="C215" s="60"/>
+      <c r="D215" s="61"/>
+      <c r="E215" s="63"/>
     </row>
     <row r="216" spans="1:5" s="1" customFormat="1">
-      <c r="A216" s="61"/>
-      <c r="B216" s="61"/>
-      <c r="C216" s="61"/>
-      <c r="D216" s="62"/>
-      <c r="E216" s="64"/>
+      <c r="A216" s="60"/>
+      <c r="B216" s="60"/>
+      <c r="C216" s="60"/>
+      <c r="D216" s="61"/>
+      <c r="E216" s="63"/>
     </row>
     <row r="217" spans="1:5" s="1" customFormat="1">
-      <c r="A217" s="61"/>
-      <c r="B217" s="61"/>
-      <c r="C217" s="61"/>
-      <c r="D217" s="62"/>
-      <c r="E217" s="64"/>
+      <c r="A217" s="60"/>
+      <c r="B217" s="60"/>
+      <c r="C217" s="60"/>
+      <c r="D217" s="61"/>
+      <c r="E217" s="63"/>
     </row>
     <row r="218" spans="1:5" s="1" customFormat="1">
-      <c r="A218" s="61"/>
-      <c r="B218" s="61"/>
-      <c r="C218" s="61"/>
-      <c r="D218" s="62"/>
-      <c r="E218" s="64"/>
+      <c r="A218" s="60"/>
+      <c r="B218" s="60"/>
+      <c r="C218" s="60"/>
+      <c r="D218" s="61"/>
+      <c r="E218" s="63"/>
     </row>
     <row r="219" spans="1:5" s="1" customFormat="1">
-      <c r="A219" s="61"/>
-      <c r="B219" s="61"/>
-      <c r="C219" s="61"/>
-      <c r="D219" s="62"/>
-      <c r="E219" s="64"/>
+      <c r="A219" s="60"/>
+      <c r="B219" s="60"/>
+      <c r="C219" s="60"/>
+      <c r="D219" s="61"/>
+      <c r="E219" s="63"/>
     </row>
     <row r="220" spans="1:5" s="1" customFormat="1">
-      <c r="A220" s="61"/>
-      <c r="B220" s="61"/>
-      <c r="C220" s="61"/>
-      <c r="D220" s="62"/>
-      <c r="E220" s="64"/>
+      <c r="A220" s="60"/>
+      <c r="B220" s="60"/>
+      <c r="C220" s="60"/>
+      <c r="D220" s="61"/>
+      <c r="E220" s="63"/>
     </row>
     <row r="221" spans="1:5" s="1" customFormat="1">
-      <c r="A221" s="61"/>
-      <c r="B221" s="61"/>
-      <c r="C221" s="61"/>
-      <c r="D221" s="62"/>
-      <c r="E221" s="64"/>
+      <c r="A221" s="60"/>
+      <c r="B221" s="60"/>
+      <c r="C221" s="60"/>
+      <c r="D221" s="61"/>
+      <c r="E221" s="63"/>
     </row>
     <row r="222" spans="1:5" s="1" customFormat="1">
-      <c r="A222" s="61"/>
-      <c r="B222" s="61"/>
-      <c r="C222" s="61"/>
-      <c r="D222" s="62"/>
-      <c r="E222" s="64"/>
+      <c r="A222" s="60"/>
+      <c r="B222" s="60"/>
+      <c r="C222" s="60"/>
+      <c r="D222" s="61"/>
+      <c r="E222" s="63"/>
     </row>
     <row r="223" spans="1:5" s="1" customFormat="1">
-      <c r="A223" s="61"/>
-      <c r="B223" s="61"/>
-      <c r="C223" s="61"/>
-      <c r="D223" s="62"/>
-      <c r="E223" s="64"/>
+      <c r="A223" s="60"/>
+      <c r="B223" s="60"/>
+      <c r="C223" s="60"/>
+      <c r="D223" s="61"/>
+      <c r="E223" s="63"/>
     </row>
     <row r="224" spans="1:5" s="1" customFormat="1">
-      <c r="A224" s="61"/>
-      <c r="B224" s="61"/>
-      <c r="C224" s="61"/>
-      <c r="D224" s="62"/>
-      <c r="E224" s="64"/>
+      <c r="A224" s="60"/>
+      <c r="B224" s="60"/>
+      <c r="C224" s="60"/>
+      <c r="D224" s="61"/>
+      <c r="E224" s="63"/>
     </row>
     <row r="225" spans="1:5" s="1" customFormat="1">
-      <c r="A225" s="61"/>
-      <c r="B225" s="61"/>
-      <c r="C225" s="61"/>
-      <c r="D225" s="62"/>
-      <c r="E225" s="64"/>
+      <c r="A225" s="60"/>
+      <c r="B225" s="60"/>
+      <c r="C225" s="60"/>
+      <c r="D225" s="61"/>
+      <c r="E225" s="63"/>
     </row>
     <row r="226" spans="1:5" s="1" customFormat="1">
-      <c r="A226" s="61"/>
-      <c r="B226" s="61"/>
-      <c r="C226" s="61"/>
-      <c r="D226" s="62"/>
-      <c r="E226" s="64"/>
+      <c r="A226" s="60"/>
+      <c r="B226" s="60"/>
+      <c r="C226" s="60"/>
+      <c r="D226" s="61"/>
+      <c r="E226" s="63"/>
     </row>
     <row r="227" spans="1:5" s="1" customFormat="1">
-      <c r="A227" s="61"/>
-      <c r="B227" s="61"/>
-      <c r="C227" s="61"/>
-      <c r="D227" s="62"/>
-      <c r="E227" s="64"/>
+      <c r="A227" s="60"/>
+      <c r="B227" s="60"/>
+      <c r="C227" s="60"/>
+      <c r="D227" s="61"/>
+      <c r="E227" s="63"/>
     </row>
     <row r="228" spans="1:5" s="1" customFormat="1">
-      <c r="A228" s="61"/>
-      <c r="B228" s="61"/>
-      <c r="C228" s="61"/>
-      <c r="D228" s="62"/>
-      <c r="E228" s="64"/>
+      <c r="A228" s="60"/>
+      <c r="B228" s="60"/>
+      <c r="C228" s="60"/>
+      <c r="D228" s="61"/>
+      <c r="E228" s="63"/>
     </row>
     <row r="229" spans="1:5" s="1" customFormat="1">
-      <c r="A229" s="61"/>
-      <c r="B229" s="61"/>
-      <c r="C229" s="61"/>
-      <c r="D229" s="62"/>
-      <c r="E229" s="64"/>
+      <c r="A229" s="60"/>
+      <c r="B229" s="60"/>
+      <c r="C229" s="60"/>
+      <c r="D229" s="61"/>
+      <c r="E229" s="63"/>
     </row>
     <row r="230" spans="1:5" s="1" customFormat="1">
-      <c r="A230" s="61"/>
-      <c r="B230" s="61"/>
-      <c r="C230" s="61"/>
-      <c r="D230" s="62"/>
-      <c r="E230" s="64"/>
+      <c r="A230" s="60"/>
+      <c r="B230" s="60"/>
+      <c r="C230" s="60"/>
+      <c r="D230" s="61"/>
+      <c r="E230" s="63"/>
     </row>
     <row r="231" spans="1:5" s="1" customFormat="1">
-      <c r="A231" s="61"/>
-      <c r="B231" s="61"/>
-      <c r="C231" s="61"/>
-      <c r="D231" s="62"/>
-      <c r="E231" s="64"/>
+      <c r="A231" s="60"/>
+      <c r="B231" s="60"/>
+      <c r="C231" s="60"/>
+      <c r="D231" s="61"/>
+      <c r="E231" s="63"/>
     </row>
     <row r="232" spans="1:5" s="1" customFormat="1">
-      <c r="A232" s="61"/>
-      <c r="B232" s="61"/>
-      <c r="C232" s="61"/>
-      <c r="D232" s="62"/>
-      <c r="E232" s="64"/>
+      <c r="A232" s="60"/>
+      <c r="B232" s="60"/>
+      <c r="C232" s="60"/>
+      <c r="D232" s="61"/>
+      <c r="E232" s="63"/>
     </row>
     <row r="233" spans="1:5" s="1" customFormat="1">
-      <c r="A233" s="61"/>
-      <c r="B233" s="61"/>
-      <c r="C233" s="61"/>
-      <c r="D233" s="62"/>
-      <c r="E233" s="64"/>
+      <c r="A233" s="60"/>
+      <c r="B233" s="60"/>
+      <c r="C233" s="60"/>
+      <c r="D233" s="61"/>
+      <c r="E233" s="63"/>
     </row>
     <row r="234" spans="1:5" s="1" customFormat="1">
-      <c r="A234" s="61"/>
-      <c r="B234" s="61"/>
-      <c r="C234" s="61"/>
-      <c r="D234" s="62"/>
-      <c r="E234" s="64"/>
+      <c r="A234" s="60"/>
+      <c r="B234" s="60"/>
+      <c r="C234" s="60"/>
+      <c r="D234" s="61"/>
+      <c r="E234" s="63"/>
     </row>
     <row r="235" spans="1:5" s="1" customFormat="1">
-      <c r="A235" s="61"/>
-      <c r="B235" s="61"/>
-      <c r="C235" s="61"/>
-      <c r="D235" s="62"/>
-      <c r="E235" s="64"/>
+      <c r="A235" s="60"/>
+      <c r="B235" s="60"/>
+      <c r="C235" s="60"/>
+      <c r="D235" s="61"/>
+      <c r="E235" s="63"/>
     </row>
     <row r="236" spans="1:5" s="1" customFormat="1">
-      <c r="A236" s="61"/>
-      <c r="B236" s="61"/>
-      <c r="C236" s="61"/>
-      <c r="D236" s="62"/>
-      <c r="E236" s="64"/>
+      <c r="A236" s="60"/>
+      <c r="B236" s="60"/>
+      <c r="C236" s="60"/>
+      <c r="D236" s="61"/>
+      <c r="E236" s="63"/>
     </row>
     <row r="237" spans="1:5" s="1" customFormat="1">
-      <c r="A237" s="61"/>
-      <c r="B237" s="61"/>
-      <c r="C237" s="61"/>
-      <c r="D237" s="62"/>
-      <c r="E237" s="64"/>
+      <c r="A237" s="60"/>
+      <c r="B237" s="60"/>
+      <c r="C237" s="60"/>
+      <c r="D237" s="61"/>
+      <c r="E237" s="63"/>
     </row>
     <row r="238" spans="1:5" s="1" customFormat="1">
-      <c r="A238" s="61"/>
-      <c r="B238" s="61"/>
-      <c r="C238" s="61"/>
-      <c r="D238" s="62"/>
-      <c r="E238" s="64"/>
+      <c r="A238" s="60"/>
+      <c r="B238" s="60"/>
+      <c r="C238" s="60"/>
+      <c r="D238" s="61"/>
+      <c r="E238" s="63"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>

</xml_diff>

<commit_message>
changed shootHigh to port 8 from 6
</commit_message>
<xml_diff>
--- a/Kilroy Equipment List 2016.xlsx
+++ b/Kilroy Equipment List 2016.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="116">
   <si>
     <t>Code Written/Tested</t>
   </si>
@@ -362,6 +362,9 @@
   </si>
   <si>
     <t>4, 5</t>
+  </si>
+  <si>
+    <t>8</t>
   </si>
 </sst>
 </file>
@@ -1100,8 +1103,8 @@
   <dimension ref="A1:H238"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F37" sqref="F37"/>
+      <pane ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -1474,7 +1477,7 @@
         <v>106</v>
       </c>
       <c r="E33" s="33" t="s">
-        <v>87</v>
+        <v>115</v>
       </c>
     </row>
     <row r="34" spans="1:5" s="1" customFormat="1">

</xml_diff>

<commit_message>
Added ManipulatorArm class and Victors for intake motors in Hardware. Also updated Equipment list.
</commit_message>
<xml_diff>
--- a/Kilroy Equipment List 2016.xlsx
+++ b/Kilroy Equipment List 2016.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="132">
   <si>
     <t>Code Written/Tested</t>
   </si>
@@ -151,18 +151,9 @@
     <t>leftRearMotor</t>
   </si>
   <si>
-    <t>Right Rear Motor Controller</t>
-  </si>
-  <si>
-    <t>Right Front Motor Controller</t>
-  </si>
-  <si>
     <t>rightFrontMotor</t>
   </si>
   <si>
-    <t>Left Front Motor Controller</t>
-  </si>
-  <si>
     <t>leftFrontMotor</t>
   </si>
   <si>
@@ -265,9 +256,6 @@
     <t>errorMessage</t>
   </si>
   <si>
-    <t>Left Rear Motor Controller</t>
-  </si>
-  <si>
     <t>6</t>
   </si>
   <si>
@@ -331,9 +319,6 @@
     <t>shootLow</t>
   </si>
   <si>
-    <t>Victor Motor Controller</t>
-  </si>
-  <si>
     <t>armMotor</t>
   </si>
   <si>
@@ -382,13 +367,52 @@
     <t>Take Lit image</t>
   </si>
   <si>
-    <t>6+7</t>
-  </si>
-  <si>
     <t>Take unlit image</t>
   </si>
   <si>
-    <t>10+11</t>
+    <t>starboardArmIntakeMotor</t>
+  </si>
+  <si>
+    <t>PWM 6</t>
+  </si>
+  <si>
+    <t>portArmIntakeMotor</t>
+  </si>
+  <si>
+    <t>PWM 5</t>
+  </si>
+  <si>
+    <t>Left Operator 6+7</t>
+  </si>
+  <si>
+    <t>Left Operator10+11</t>
+  </si>
+  <si>
+    <t>Right Driver 3</t>
+  </si>
+  <si>
+    <t>Right Driver 2</t>
+  </si>
+  <si>
+    <t>Arm Motor Controller (Victor)</t>
+  </si>
+  <si>
+    <t>Starboard Intake motor (Victor)</t>
+  </si>
+  <si>
+    <t>Port Intake Motor (Victor)</t>
+  </si>
+  <si>
+    <t>Left Front Motor Controller (Talon)</t>
+  </si>
+  <si>
+    <t>Right Front Motor Controller (Talon)</t>
+  </si>
+  <si>
+    <t>Left Rear Motor Controller (Talon)</t>
+  </si>
+  <si>
+    <t>Right Rear Motor Controller (Talon)</t>
   </si>
 </sst>
 </file>
@@ -1127,8 +1151,8 @@
   <dimension ref="A1:H238"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E75" sqref="E75"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -1185,76 +1209,82 @@
       <c r="A4" s="64"/>
       <c r="B4" s="64"/>
       <c r="C4" s="30" t="s">
-        <v>44</v>
+        <v>131</v>
       </c>
       <c r="D4" s="31" t="s">
         <v>42</v>
       </c>
       <c r="E4" s="50" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="1" customFormat="1" ht="12.75" customHeight="1">
       <c r="A5" s="65"/>
       <c r="B5" s="65"/>
       <c r="C5" s="29" t="s">
-        <v>82</v>
+        <v>130</v>
       </c>
       <c r="D5" s="32" t="s">
         <v>43</v>
       </c>
       <c r="E5" s="33" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="1" customFormat="1" ht="12.75" customHeight="1">
       <c r="A6" s="8"/>
       <c r="B6" s="8"/>
       <c r="C6" s="26" t="s">
-        <v>45</v>
+        <v>129</v>
       </c>
       <c r="D6" s="27" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E6" s="28" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="35" customFormat="1">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="29" t="s">
-        <v>47</v>
+        <v>128</v>
       </c>
       <c r="D7" s="32" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E7" s="33" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="1" customFormat="1">
       <c r="A8" s="34"/>
       <c r="B8" s="34"/>
       <c r="C8" s="49" t="s">
-        <v>104</v>
+        <v>125</v>
       </c>
       <c r="D8" s="66" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="E8" s="51" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="F8" s="12"/>
       <c r="G8" s="12"/>
       <c r="H8" s="12"/>
     </row>
-    <row r="9" spans="1:8" s="1" customFormat="1">
+    <row r="9" spans="1:8" s="1" customFormat="1" ht="25.5">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
-      <c r="C9" s="29"/>
-      <c r="D9" s="32"/>
-      <c r="E9" s="33"/>
+      <c r="C9" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="D9" s="32" t="s">
+        <v>117</v>
+      </c>
+      <c r="E9" s="33" t="s">
+        <v>118</v>
+      </c>
       <c r="F9" s="12"/>
       <c r="G9" s="12"/>
       <c r="H9" s="12"/>
@@ -1262,9 +1292,15 @@
     <row r="10" spans="1:8" s="1" customFormat="1">
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
-      <c r="C10" s="26"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="28"/>
+      <c r="C10" s="26" t="s">
+        <v>127</v>
+      </c>
+      <c r="D10" s="27" t="s">
+        <v>119</v>
+      </c>
+      <c r="E10" s="28" t="s">
+        <v>120</v>
+      </c>
       <c r="F10" s="12"/>
       <c r="G10" s="12"/>
       <c r="H10" s="12"/>
@@ -1298,26 +1334,26 @@
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="29" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D14" s="32" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E14" s="33" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="15" spans="1:8" s="1" customFormat="1">
       <c r="A15" s="52"/>
       <c r="B15" s="52"/>
       <c r="C15" s="26" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D15" s="27" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E15" s="44" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:8" s="1" customFormat="1">
@@ -1443,91 +1479,91 @@
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="29" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D29" s="32" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E29" s="33" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30" spans="1:8" s="1" customFormat="1">
       <c r="A30" s="13"/>
       <c r="B30" s="13"/>
       <c r="C30" s="23" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D30" s="45" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E30" s="44" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="31" spans="1:8" s="1" customFormat="1">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="29" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D31" s="32" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E31" s="33" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="32" spans="1:8" s="1" customFormat="1">
       <c r="A32" s="13"/>
       <c r="B32" s="13"/>
       <c r="C32" s="23" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D32" s="45" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E32" s="44" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="33" spans="1:5" s="1" customFormat="1">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="29" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D33" s="32" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E33" s="33" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="34" spans="1:5" s="1" customFormat="1">
       <c r="A34" s="13"/>
       <c r="B34" s="13"/>
       <c r="C34" s="23" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D34" s="45" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="E34" s="44" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
     <row r="35" spans="1:5" s="1" customFormat="1">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="29" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="D35" s="32" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="E35" s="33" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
     </row>
     <row r="36" spans="1:5" s="1" customFormat="1">
@@ -1605,10 +1641,10 @@
       <c r="A45" s="41"/>
       <c r="B45" s="14"/>
       <c r="C45" s="42" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D45" s="45" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E45" s="14">
         <v>0</v>
@@ -1647,26 +1683,26 @@
       <c r="A49" s="20"/>
       <c r="B49" s="20"/>
       <c r="C49" s="46" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D49" s="25" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E49" s="47" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="50" spans="1:8" s="1" customFormat="1">
       <c r="A50" s="8"/>
       <c r="B50" s="8"/>
       <c r="C50" s="26" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D50" s="27" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="E50" s="28" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="51" spans="1:8" s="1" customFormat="1">
@@ -1705,59 +1741,59 @@
       </c>
       <c r="D55" s="67"/>
       <c r="E55" s="3" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="56" spans="1:8" s="1" customFormat="1">
       <c r="A56" s="20"/>
       <c r="B56" s="20"/>
       <c r="C56" s="46" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D56" s="25" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E56" s="33" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="57" spans="1:8" s="1" customFormat="1">
       <c r="A57" s="8"/>
       <c r="B57" s="8"/>
       <c r="C57" s="26" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D57" s="27" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E57" s="28" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="58" spans="1:8" s="1" customFormat="1">
       <c r="A58" s="4"/>
       <c r="B58" s="4"/>
       <c r="C58" s="29" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D58" s="32" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E58" s="33" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="59" spans="1:8" s="1" customFormat="1">
       <c r="A59" s="8"/>
       <c r="B59" s="8"/>
       <c r="C59" s="26" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D59" s="27" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E59" s="28" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="60" spans="1:8" s="36" customFormat="1" ht="13.15" customHeight="1">
@@ -1826,13 +1862,13 @@
       <c r="A67" s="8"/>
       <c r="B67" s="8"/>
       <c r="C67" s="26" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D67" s="27" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E67" s="28" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="G67" s="21"/>
     </row>
@@ -1840,13 +1876,13 @@
       <c r="A68" s="4"/>
       <c r="B68" s="4"/>
       <c r="C68" s="29" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D68" s="32" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E68" s="33" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="G68" s="21"/>
     </row>
@@ -1854,13 +1890,13 @@
       <c r="A69" s="8"/>
       <c r="B69" s="8"/>
       <c r="C69" s="23" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D69" s="45" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E69" s="44" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G69" s="21"/>
     </row>
@@ -1868,13 +1904,13 @@
       <c r="A70" s="4"/>
       <c r="B70" s="4"/>
       <c r="C70" s="29" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D70" s="32" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E70" s="33" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="G70" s="21"/>
     </row>
@@ -1894,33 +1930,33 @@
       <c r="A72" s="8"/>
       <c r="B72" s="8"/>
       <c r="C72" s="24" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="D72" s="27" t="s">
-        <v>119</v>
-      </c>
-      <c r="E72" s="26">
-        <v>3</v>
+        <v>114</v>
+      </c>
+      <c r="E72" s="26" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="73" spans="1:8" s="36" customFormat="1" ht="25.5">
       <c r="A73" s="4"/>
       <c r="B73" s="4"/>
       <c r="C73" s="29" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D73" s="32" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="E73" s="33" t="s">
-        <v>76</v>
+        <v>124</v>
       </c>
     </row>
     <row r="74" spans="1:8" s="1" customFormat="1">
       <c r="A74" s="48"/>
       <c r="B74" s="48"/>
       <c r="C74" s="23" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="D74" s="23"/>
       <c r="E74" s="23" t="s">
@@ -1931,11 +1967,11 @@
       <c r="A75" s="4"/>
       <c r="B75" s="4"/>
       <c r="C75" s="33" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="D75" s="32"/>
       <c r="E75" s="33" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="76" spans="1:8" s="1" customFormat="1">
@@ -2164,7 +2200,7 @@
         <v>22</v>
       </c>
       <c r="D104" s="27" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E104" s="44" t="s">
         <v>24</v>
@@ -2187,10 +2223,10 @@
       <c r="A106" s="13"/>
       <c r="B106" s="13"/>
       <c r="C106" s="26" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D106" s="27" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E106" s="44" t="s">
         <v>20</v>
@@ -2226,7 +2262,7 @@
       <c r="A109" s="4"/>
       <c r="B109" s="4"/>
       <c r="C109" s="29" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D109" s="6" t="s">
         <v>8</v>
@@ -2265,10 +2301,10 @@
       <c r="A112" s="13"/>
       <c r="B112" s="13"/>
       <c r="C112" s="23" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D112" s="45" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E112" s="23" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
Added prints statements for the two new victors in teleop
</commit_message>
<xml_diff>
--- a/Kilroy Equipment List 2016.xlsx
+++ b/Kilroy Equipment List 2016.xlsx
@@ -397,9 +397,6 @@
     <t>Arm Motor Controller (Victor)</t>
   </si>
   <si>
-    <t>Starboard Intake motor (Victor)</t>
-  </si>
-  <si>
     <t>Port Intake Motor (Victor)</t>
   </si>
   <si>
@@ -413,6 +410,9 @@
   </si>
   <si>
     <t>Right Rear Motor Controller (Talon)</t>
+  </si>
+  <si>
+    <t>Starboard Intake Motor (Victor)</t>
   </si>
 </sst>
 </file>
@@ -1152,7 +1152,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
+      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -1209,7 +1209,7 @@
       <c r="A4" s="64"/>
       <c r="B4" s="64"/>
       <c r="C4" s="30" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D4" s="31" t="s">
         <v>42</v>
@@ -1222,7 +1222,7 @@
       <c r="A5" s="65"/>
       <c r="B5" s="65"/>
       <c r="C5" s="29" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D5" s="32" t="s">
         <v>43</v>
@@ -1235,7 +1235,7 @@
       <c r="A6" s="8"/>
       <c r="B6" s="8"/>
       <c r="C6" s="26" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D6" s="27" t="s">
         <v>44</v>
@@ -1248,7 +1248,7 @@
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="29" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D7" s="32" t="s">
         <v>45</v>
@@ -1276,8 +1276,8 @@
     <row r="9" spans="1:8" s="1" customFormat="1" ht="25.5">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
-      <c r="C9" s="29" t="s">
-        <v>126</v>
+      <c r="C9" s="57" t="s">
+        <v>131</v>
       </c>
       <c r="D9" s="32" t="s">
         <v>117</v>
@@ -1293,7 +1293,7 @@
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="C10" s="26" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D10" s="27" t="s">
         <v>119</v>

</xml_diff>

<commit_message>
Lots of changes.  This is going to be fun to merge...
</commit_message>
<xml_diff>
--- a/Kilroy Equipment List 2016.xlsx
+++ b/Kilroy Equipment List 2016.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="137">
   <si>
     <t>Code Written/Tested</t>
   </si>
@@ -376,9 +376,6 @@
     <t>PWM 6</t>
   </si>
   <si>
-    <t>portArmIntakeMotor</t>
-  </si>
-  <si>
     <t>PWM 5</t>
   </si>
   <si>
@@ -397,9 +394,6 @@
     <t>Arm Motor Controller (Victor)</t>
   </si>
   <si>
-    <t>Port Intake Motor (Victor)</t>
-  </si>
-  <si>
     <t>Left Front Motor Controller (Talon)</t>
   </si>
   <si>
@@ -413,6 +407,27 @@
   </si>
   <si>
     <t>Starboard Intake Motor (Victor)</t>
+  </si>
+  <si>
+    <t>NOT ADDED YET</t>
+  </si>
+  <si>
+    <t>Arm Red light sensor</t>
+  </si>
+  <si>
+    <t>Arm potentiometer</t>
+  </si>
+  <si>
+    <t>armPositionPot</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>Intake Motor (Victor)</t>
+  </si>
+  <si>
+    <t>armIntakeMotor</t>
   </si>
 </sst>
 </file>
@@ -574,7 +589,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -627,9 +642,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -782,6 +794,21 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1152,30 +1179,30 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
+      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" style="60" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" style="60" customWidth="1"/>
-    <col min="3" max="3" width="70.5703125" style="60" customWidth="1"/>
-    <col min="4" max="4" width="21" style="61" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" style="63" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" style="60" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" style="60"/>
-    <col min="8" max="8" width="11.140625" style="60" customWidth="1"/>
-    <col min="9" max="16384" width="8.85546875" style="60"/>
+    <col min="1" max="1" width="14.7109375" style="59" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" style="59" customWidth="1"/>
+    <col min="3" max="3" width="70.5703125" style="59" customWidth="1"/>
+    <col min="4" max="4" width="21" style="60" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" style="62" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" style="59" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" style="59"/>
+    <col min="8" max="8" width="11.140625" style="59" customWidth="1"/>
+    <col min="9" max="16384" width="8.85546875" style="59"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="67" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
     </row>
     <row r="2" spans="1:8" s="1" customFormat="1" ht="25.5">
       <c r="A2" s="13" t="s">
@@ -1184,89 +1211,89 @@
       <c r="B2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="38" t="s">
+      <c r="C2" s="37" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="39" t="s">
+      <c r="E2" s="38" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="1" customFormat="1" ht="13.15" customHeight="1">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
-      <c r="C3" s="67" t="s">
+      <c r="C3" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="67"/>
+      <c r="D3" s="66"/>
       <c r="E3" s="3" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="1" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A4" s="64"/>
-      <c r="B4" s="64"/>
-      <c r="C4" s="30" t="s">
-        <v>130</v>
-      </c>
-      <c r="D4" s="31" t="s">
+      <c r="A4" s="63"/>
+      <c r="B4" s="63"/>
+      <c r="C4" s="29" t="s">
+        <v>128</v>
+      </c>
+      <c r="D4" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="E4" s="50" t="s">
+      <c r="E4" s="49" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="1" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A5" s="65"/>
-      <c r="B5" s="65"/>
-      <c r="C5" s="29" t="s">
-        <v>129</v>
-      </c>
-      <c r="D5" s="32" t="s">
+      <c r="A5" s="64"/>
+      <c r="B5" s="64"/>
+      <c r="C5" s="28" t="s">
+        <v>127</v>
+      </c>
+      <c r="D5" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="E5" s="33" t="s">
+      <c r="E5" s="32" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="1" customFormat="1" ht="12.75" customHeight="1">
       <c r="A6" s="8"/>
       <c r="B6" s="8"/>
-      <c r="C6" s="26" t="s">
-        <v>128</v>
-      </c>
-      <c r="D6" s="27" t="s">
+      <c r="C6" s="25" t="s">
+        <v>126</v>
+      </c>
+      <c r="D6" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="E6" s="28" t="s">
+      <c r="E6" s="27" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="35" customFormat="1">
+    <row r="7" spans="1:8" s="34" customFormat="1">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
-      <c r="C7" s="29" t="s">
-        <v>127</v>
-      </c>
-      <c r="D7" s="32" t="s">
+      <c r="C7" s="28" t="s">
+        <v>125</v>
+      </c>
+      <c r="D7" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="E7" s="33" t="s">
+      <c r="E7" s="32" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="1" customFormat="1">
-      <c r="A8" s="34"/>
-      <c r="B8" s="34"/>
-      <c r="C8" s="49" t="s">
-        <v>125</v>
-      </c>
-      <c r="D8" s="66" t="s">
+      <c r="A8" s="33"/>
+      <c r="B8" s="33"/>
+      <c r="C8" s="48" t="s">
+        <v>124</v>
+      </c>
+      <c r="D8" s="65" t="s">
         <v>100</v>
       </c>
-      <c r="E8" s="51" t="s">
+      <c r="E8" s="50" t="s">
         <v>101</v>
       </c>
       <c r="F8" s="12"/>
@@ -1276,13 +1303,13 @@
     <row r="9" spans="1:8" s="1" customFormat="1" ht="25.5">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
-      <c r="C9" s="57" t="s">
-        <v>131</v>
-      </c>
-      <c r="D9" s="32" t="s">
+      <c r="C9" s="73" t="s">
+        <v>129</v>
+      </c>
+      <c r="D9" s="70" t="s">
         <v>117</v>
       </c>
-      <c r="E9" s="33" t="s">
+      <c r="E9" s="71" t="s">
         <v>118</v>
       </c>
       <c r="F9" s="12"/>
@@ -1292,14 +1319,14 @@
     <row r="10" spans="1:8" s="1" customFormat="1">
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
-      <c r="C10" s="26" t="s">
-        <v>126</v>
-      </c>
-      <c r="D10" s="27" t="s">
+      <c r="C10" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="D10" s="26" t="s">
+        <v>136</v>
+      </c>
+      <c r="E10" s="27" t="s">
         <v>119</v>
-      </c>
-      <c r="E10" s="28" t="s">
-        <v>120</v>
       </c>
       <c r="F10" s="12"/>
       <c r="G10" s="12"/>
@@ -1322,46 +1349,46 @@
     <row r="13" spans="1:8" s="1" customFormat="1" ht="13.15" customHeight="1">
       <c r="A13" s="17"/>
       <c r="B13" s="17"/>
-      <c r="C13" s="69" t="s">
+      <c r="C13" s="68" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="69"/>
-      <c r="E13" s="59" t="s">
+      <c r="D13" s="68"/>
+      <c r="E13" s="58" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:8" s="1" customFormat="1">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
-      <c r="C14" s="29" t="s">
+      <c r="C14" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="D14" s="32" t="s">
+      <c r="D14" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="E14" s="33" t="s">
+      <c r="E14" s="32" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="15" spans="1:8" s="1" customFormat="1">
-      <c r="A15" s="52"/>
-      <c r="B15" s="52"/>
-      <c r="C15" s="26" t="s">
+      <c r="A15" s="51"/>
+      <c r="B15" s="51"/>
+      <c r="C15" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="D15" s="27" t="s">
+      <c r="D15" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="E15" s="44" t="s">
+      <c r="E15" s="43" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:8" s="1" customFormat="1">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
-      <c r="C16" s="29"/>
-      <c r="D16" s="32"/>
-      <c r="E16" s="33"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="31"/>
+      <c r="E16" s="32"/>
       <c r="F16" s="12"/>
       <c r="G16" s="12"/>
       <c r="H16" s="12"/>
@@ -1369,16 +1396,16 @@
     <row r="17" spans="1:8" s="1" customFormat="1">
       <c r="A17" s="8"/>
       <c r="B17" s="8"/>
-      <c r="C17" s="26"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="28"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="27"/>
       <c r="F17" s="12"/>
       <c r="G17" s="12"/>
       <c r="H17" s="12"/>
     </row>
     <row r="18" spans="1:8" s="1" customFormat="1">
-      <c r="A18" s="43"/>
-      <c r="B18" s="43"/>
+      <c r="A18" s="42"/>
+      <c r="B18" s="42"/>
       <c r="C18" s="5"/>
       <c r="D18" s="6"/>
       <c r="E18" s="7"/>
@@ -1453,146 +1480,150 @@
     <row r="26" spans="1:8" s="1" customFormat="1" ht="13.35" customHeight="1">
       <c r="A26" s="17"/>
       <c r="B26" s="17"/>
-      <c r="C26" s="67" t="s">
+      <c r="C26" s="66" t="s">
         <v>7</v>
       </c>
-      <c r="D26" s="67"/>
+      <c r="D26" s="66"/>
       <c r="E26" s="3" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="27" spans="1:8" s="1" customFormat="1">
-      <c r="A27" s="43"/>
-      <c r="B27" s="43"/>
-      <c r="C27" s="29"/>
-      <c r="D27" s="32"/>
-      <c r="E27" s="33"/>
+      <c r="A27" s="42"/>
+      <c r="B27" s="42"/>
+      <c r="C27" s="28"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="32"/>
     </row>
     <row r="28" spans="1:8" s="1" customFormat="1">
       <c r="A28" s="13"/>
       <c r="B28" s="13"/>
-      <c r="C28" s="23"/>
-      <c r="D28" s="45"/>
-      <c r="E28" s="44"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="44"/>
+      <c r="E28" s="43"/>
     </row>
     <row r="29" spans="1:8" s="1" customFormat="1">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
-      <c r="C29" s="29" t="s">
+      <c r="C29" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="D29" s="32" t="s">
+      <c r="D29" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="E29" s="33" t="s">
+      <c r="E29" s="32" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="30" spans="1:8" s="1" customFormat="1">
       <c r="A30" s="13"/>
       <c r="B30" s="13"/>
-      <c r="C30" s="23" t="s">
+      <c r="C30" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="D30" s="45" t="s">
+      <c r="D30" s="44" t="s">
         <v>49</v>
       </c>
-      <c r="E30" s="44" t="s">
+      <c r="E30" s="43" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="31" spans="1:8" s="1" customFormat="1">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
-      <c r="C31" s="29" t="s">
+      <c r="C31" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="D31" s="32" t="s">
+      <c r="D31" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="E31" s="33" t="s">
+      <c r="E31" s="32" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="32" spans="1:8" s="1" customFormat="1">
       <c r="A32" s="13"/>
       <c r="B32" s="13"/>
-      <c r="C32" s="23" t="s">
+      <c r="C32" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="D32" s="45" t="s">
+      <c r="D32" s="44" t="s">
         <v>84</v>
       </c>
-      <c r="E32" s="44" t="s">
+      <c r="E32" s="43" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="33" spans="1:5" s="1" customFormat="1">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
-      <c r="C33" s="29" t="s">
+      <c r="C33" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="D33" s="32" t="s">
+      <c r="D33" s="31" t="s">
         <v>98</v>
       </c>
-      <c r="E33" s="33" t="s">
+      <c r="E33" s="32" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="34" spans="1:5" s="1" customFormat="1">
       <c r="A34" s="13"/>
       <c r="B34" s="13"/>
-      <c r="C34" s="23" t="s">
+      <c r="C34" s="22" t="s">
         <v>97</v>
       </c>
-      <c r="D34" s="45" t="s">
+      <c r="D34" s="44" t="s">
         <v>99</v>
       </c>
-      <c r="E34" s="44" t="s">
+      <c r="E34" s="43" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="35" spans="1:5" s="1" customFormat="1">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
-      <c r="C35" s="29" t="s">
+      <c r="C35" s="69" t="s">
         <v>103</v>
       </c>
-      <c r="D35" s="32" t="s">
+      <c r="D35" s="70" t="s">
         <v>104</v>
       </c>
-      <c r="E35" s="33" t="s">
+      <c r="E35" s="71" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="36" spans="1:5" s="1" customFormat="1">
       <c r="A36" s="8"/>
       <c r="B36" s="8"/>
-      <c r="C36" s="26"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="56"/>
+      <c r="C36" s="25" t="s">
+        <v>131</v>
+      </c>
+      <c r="D36" s="72" t="s">
+        <v>130</v>
+      </c>
+      <c r="E36" s="55"/>
     </row>
     <row r="37" spans="1:5" s="1" customFormat="1">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
-      <c r="C37" s="29"/>
-      <c r="D37" s="32"/>
-      <c r="E37" s="33"/>
+      <c r="C37" s="28"/>
+      <c r="D37" s="31"/>
+      <c r="E37" s="32"/>
     </row>
     <row r="38" spans="1:5" s="1" customFormat="1" ht="13.35" customHeight="1">
       <c r="A38" s="13"/>
       <c r="B38" s="13"/>
-      <c r="C38" s="23"/>
-      <c r="D38" s="45"/>
-      <c r="E38" s="44"/>
-    </row>
-    <row r="39" spans="1:5" s="19" customFormat="1" ht="13.15" customHeight="1">
+      <c r="C38" s="22"/>
+      <c r="D38" s="44"/>
+      <c r="E38" s="43"/>
+    </row>
+    <row r="39" spans="1:5" s="18" customFormat="1" ht="13.15" customHeight="1">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
-      <c r="C39" s="57"/>
-      <c r="D39" s="32"/>
-      <c r="E39" s="33"/>
+      <c r="C39" s="56"/>
+      <c r="D39" s="31"/>
+      <c r="E39" s="32"/>
     </row>
     <row r="40" spans="1:5" s="1" customFormat="1" ht="13.15" customHeight="1">
       <c r="A40" s="8"/>
@@ -1601,49 +1632,49 @@
       <c r="D40" s="10"/>
       <c r="E40" s="11"/>
     </row>
-    <row r="41" spans="1:5" s="19" customFormat="1" ht="13.15" customHeight="1">
+    <row r="41" spans="1:5" s="18" customFormat="1" ht="13.15" customHeight="1">
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
       <c r="C41" s="5"/>
       <c r="D41" s="6"/>
       <c r="E41" s="7"/>
     </row>
-    <row r="42" spans="1:5" s="19" customFormat="1" ht="13.15" customHeight="1">
+    <row r="42" spans="1:5" s="18" customFormat="1" ht="13.15" customHeight="1">
       <c r="A42" s="13"/>
       <c r="B42" s="13"/>
-      <c r="C42" s="23"/>
-      <c r="D42" s="45"/>
-      <c r="E42" s="44"/>
+      <c r="C42" s="22"/>
+      <c r="D42" s="44"/>
+      <c r="E42" s="43"/>
     </row>
     <row r="43" spans="1:5" s="1" customFormat="1" ht="13.15" customHeight="1">
       <c r="A43" s="17"/>
       <c r="B43" s="17"/>
-      <c r="C43" s="67" t="s">
+      <c r="C43" s="66" t="s">
         <v>9</v>
       </c>
-      <c r="D43" s="67"/>
+      <c r="D43" s="66"/>
       <c r="E43" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="44" spans="1:5" s="1" customFormat="1">
-      <c r="A44" s="40" t="s">
+      <c r="A44" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="B44" s="40" t="s">
+      <c r="B44" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="C44" s="29"/>
-      <c r="D44" s="25"/>
-      <c r="E44" s="47"/>
+      <c r="C44" s="28"/>
+      <c r="D44" s="24"/>
+      <c r="E44" s="46"/>
     </row>
     <row r="45" spans="1:5" s="1" customFormat="1">
-      <c r="A45" s="41"/>
+      <c r="A45" s="40"/>
       <c r="B45" s="14"/>
-      <c r="C45" s="42" t="s">
+      <c r="C45" s="41" t="s">
         <v>81</v>
       </c>
-      <c r="D45" s="45" t="s">
+      <c r="D45" s="44" t="s">
         <v>82</v>
       </c>
       <c r="E45" s="14">
@@ -1671,147 +1702,153 @@
     <row r="48" spans="1:5" s="1" customFormat="1" ht="13.15" customHeight="1">
       <c r="A48" s="17"/>
       <c r="B48" s="17"/>
-      <c r="C48" s="67" t="s">
+      <c r="C48" s="66" t="s">
         <v>11</v>
       </c>
-      <c r="D48" s="67"/>
+      <c r="D48" s="66"/>
       <c r="E48" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="49" spans="1:8" s="19" customFormat="1" ht="13.15" customHeight="1">
-      <c r="A49" s="20"/>
-      <c r="B49" s="20"/>
-      <c r="C49" s="46" t="s">
+    <row r="49" spans="1:8" s="18" customFormat="1" ht="13.15" customHeight="1">
+      <c r="A49" s="19"/>
+      <c r="B49" s="19"/>
+      <c r="C49" s="45" t="s">
         <v>60</v>
       </c>
-      <c r="D49" s="25" t="s">
+      <c r="D49" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="E49" s="47" t="s">
+      <c r="E49" s="46" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="50" spans="1:8" s="1" customFormat="1">
       <c r="A50" s="8"/>
       <c r="B50" s="8"/>
-      <c r="C50" s="26" t="s">
+      <c r="C50" s="25" t="s">
         <v>86</v>
       </c>
-      <c r="D50" s="27" t="s">
+      <c r="D50" s="26" t="s">
         <v>87</v>
       </c>
-      <c r="E50" s="28" t="s">
+      <c r="E50" s="27" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="51" spans="1:8" s="1" customFormat="1">
       <c r="A51" s="4"/>
       <c r="B51" s="4"/>
-      <c r="C51" s="29"/>
-      <c r="D51" s="32"/>
-      <c r="E51" s="33"/>
+      <c r="C51" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="D51" s="31" t="s">
+        <v>133</v>
+      </c>
+      <c r="E51" s="32" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="52" spans="1:8" s="1" customFormat="1">
       <c r="A52" s="8"/>
       <c r="B52" s="8"/>
-      <c r="C52" s="26"/>
-      <c r="D52" s="27"/>
-      <c r="E52" s="28"/>
+      <c r="C52" s="25"/>
+      <c r="D52" s="26"/>
+      <c r="E52" s="27"/>
     </row>
     <row r="53" spans="1:8" s="1" customFormat="1">
       <c r="A53" s="4"/>
       <c r="B53" s="4"/>
-      <c r="C53" s="29"/>
-      <c r="D53" s="32"/>
-      <c r="E53" s="33"/>
+      <c r="C53" s="28"/>
+      <c r="D53" s="31"/>
+      <c r="E53" s="32"/>
     </row>
     <row r="54" spans="1:8" s="1" customFormat="1">
       <c r="A54" s="8"/>
       <c r="B54" s="8"/>
-      <c r="C54" s="26"/>
-      <c r="D54" s="27"/>
-      <c r="E54" s="28"/>
+      <c r="C54" s="25"/>
+      <c r="D54" s="26"/>
+      <c r="E54" s="27"/>
     </row>
     <row r="55" spans="1:8" s="1" customFormat="1" ht="13.35" customHeight="1">
       <c r="A55" s="17"/>
       <c r="B55" s="17"/>
-      <c r="C55" s="67" t="s">
+      <c r="C55" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="D55" s="67"/>
+      <c r="D55" s="66"/>
       <c r="E55" s="3" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="56" spans="1:8" s="1" customFormat="1">
-      <c r="A56" s="20"/>
-      <c r="B56" s="20"/>
-      <c r="C56" s="46" t="s">
+      <c r="A56" s="19"/>
+      <c r="B56" s="19"/>
+      <c r="C56" s="45" t="s">
         <v>88</v>
       </c>
-      <c r="D56" s="25" t="s">
+      <c r="D56" s="24" t="s">
         <v>89</v>
       </c>
-      <c r="E56" s="33" t="s">
+      <c r="E56" s="32" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="57" spans="1:8" s="1" customFormat="1">
       <c r="A57" s="8"/>
       <c r="B57" s="8"/>
-      <c r="C57" s="26" t="s">
+      <c r="C57" s="25" t="s">
         <v>92</v>
       </c>
-      <c r="D57" s="27" t="s">
+      <c r="D57" s="26" t="s">
         <v>93</v>
       </c>
-      <c r="E57" s="28" t="s">
+      <c r="E57" s="27" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="58" spans="1:8" s="1" customFormat="1">
       <c r="A58" s="4"/>
       <c r="B58" s="4"/>
-      <c r="C58" s="29" t="s">
+      <c r="C58" s="28" t="s">
         <v>92</v>
       </c>
-      <c r="D58" s="32" t="s">
+      <c r="D58" s="31" t="s">
         <v>94</v>
       </c>
-      <c r="E58" s="33" t="s">
+      <c r="E58" s="32" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="59" spans="1:8" s="1" customFormat="1">
       <c r="A59" s="8"/>
       <c r="B59" s="8"/>
-      <c r="C59" s="26" t="s">
+      <c r="C59" s="25" t="s">
         <v>92</v>
       </c>
-      <c r="D59" s="27" t="s">
+      <c r="D59" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="E59" s="28" t="s">
+      <c r="E59" s="27" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="60" spans="1:8" s="36" customFormat="1" ht="13.15" customHeight="1">
+    <row r="60" spans="1:8" s="35" customFormat="1" ht="13.15" customHeight="1">
       <c r="A60" s="4"/>
       <c r="B60" s="4"/>
       <c r="C60" s="5"/>
       <c r="D60" s="6"/>
       <c r="E60" s="7"/>
-      <c r="G60" s="37"/>
-      <c r="H60" s="37"/>
+      <c r="G60" s="36"/>
+      <c r="H60" s="36"/>
     </row>
     <row r="61" spans="1:8" s="1" customFormat="1" ht="13.35" customHeight="1">
       <c r="A61" s="17"/>
       <c r="B61" s="17"/>
-      <c r="C61" s="67" t="s">
+      <c r="C61" s="66" t="s">
         <v>30</v>
       </c>
-      <c r="D61" s="67"/>
+      <c r="D61" s="66"/>
       <c r="E61" s="3" t="s">
         <v>29</v>
       </c>
@@ -1837,278 +1874,278 @@
       <c r="D64" s="10"/>
       <c r="E64" s="11"/>
     </row>
-    <row r="65" spans="1:8" s="36" customFormat="1" ht="13.15" customHeight="1">
+    <row r="65" spans="1:8" s="35" customFormat="1" ht="13.15" customHeight="1">
       <c r="A65" s="4"/>
       <c r="B65" s="4"/>
       <c r="C65" s="5"/>
       <c r="D65" s="6"/>
       <c r="E65" s="7"/>
-      <c r="G65" s="37"/>
-      <c r="H65" s="37"/>
+      <c r="G65" s="36"/>
+      <c r="H65" s="36"/>
     </row>
     <row r="66" spans="1:8" s="1" customFormat="1" ht="13.35" customHeight="1">
       <c r="A66" s="17"/>
       <c r="B66" s="17"/>
-      <c r="C66" s="67" t="s">
+      <c r="C66" s="66" t="s">
         <v>14</v>
       </c>
-      <c r="D66" s="67"/>
+      <c r="D66" s="66"/>
       <c r="E66" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G66" s="21"/>
+      <c r="G66" s="20"/>
     </row>
     <row r="67" spans="1:8" s="1" customFormat="1">
       <c r="A67" s="8"/>
       <c r="B67" s="8"/>
-      <c r="C67" s="26" t="s">
+      <c r="C67" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="D67" s="27" t="s">
+      <c r="D67" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="E67" s="28" t="s">
+      <c r="E67" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="G67" s="21"/>
+      <c r="G67" s="20"/>
     </row>
     <row r="68" spans="1:8" s="1" customFormat="1">
       <c r="A68" s="4"/>
       <c r="B68" s="4"/>
-      <c r="C68" s="29" t="s">
+      <c r="C68" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="D68" s="32" t="s">
+      <c r="D68" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="E68" s="33" t="s">
+      <c r="E68" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="G68" s="21"/>
+      <c r="G68" s="20"/>
     </row>
     <row r="69" spans="1:8" s="1" customFormat="1">
       <c r="A69" s="8"/>
       <c r="B69" s="8"/>
-      <c r="C69" s="23" t="s">
+      <c r="C69" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="D69" s="45" t="s">
+      <c r="D69" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="E69" s="44" t="s">
+      <c r="E69" s="43" t="s">
         <v>73</v>
       </c>
-      <c r="G69" s="21"/>
+      <c r="G69" s="20"/>
     </row>
     <row r="70" spans="1:8" s="1" customFormat="1">
       <c r="A70" s="4"/>
       <c r="B70" s="4"/>
-      <c r="C70" s="29" t="s">
+      <c r="C70" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="D70" s="32" t="s">
+      <c r="D70" s="31" t="s">
         <v>75</v>
       </c>
-      <c r="E70" s="33" t="s">
+      <c r="E70" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="G70" s="21"/>
+      <c r="G70" s="20"/>
     </row>
     <row r="71" spans="1:8" s="1" customFormat="1" ht="13.35" customHeight="1">
       <c r="A71" s="17"/>
       <c r="B71" s="17"/>
-      <c r="C71" s="67" t="s">
+      <c r="C71" s="66" t="s">
         <v>16</v>
       </c>
-      <c r="D71" s="67"/>
+      <c r="D71" s="66"/>
       <c r="E71" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G71" s="21"/>
+      <c r="G71" s="20"/>
     </row>
     <row r="72" spans="1:8" s="1" customFormat="1" ht="25.5">
       <c r="A72" s="8"/>
       <c r="B72" s="8"/>
-      <c r="C72" s="24" t="s">
+      <c r="C72" s="23" t="s">
         <v>111</v>
       </c>
-      <c r="D72" s="27" t="s">
+      <c r="D72" s="26" t="s">
         <v>114</v>
       </c>
-      <c r="E72" s="26" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" s="36" customFormat="1" ht="25.5">
+      <c r="E72" s="25" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" s="35" customFormat="1" ht="25.5">
       <c r="A73" s="4"/>
       <c r="B73" s="4"/>
-      <c r="C73" s="29" t="s">
+      <c r="C73" s="28" t="s">
         <v>112</v>
       </c>
-      <c r="D73" s="32" t="s">
+      <c r="D73" s="31" t="s">
         <v>113</v>
       </c>
-      <c r="E73" s="33" t="s">
-        <v>124</v>
+      <c r="E73" s="32" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="74" spans="1:8" s="1" customFormat="1">
-      <c r="A74" s="48"/>
-      <c r="B74" s="48"/>
-      <c r="C74" s="23" t="s">
+      <c r="A74" s="47"/>
+      <c r="B74" s="47"/>
+      <c r="C74" s="22" t="s">
         <v>115</v>
       </c>
-      <c r="D74" s="23"/>
-      <c r="E74" s="23" t="s">
-        <v>121</v>
+      <c r="D74" s="22"/>
+      <c r="E74" s="22" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="75" spans="1:8" s="1" customFormat="1">
       <c r="A75" s="4"/>
       <c r="B75" s="4"/>
-      <c r="C75" s="33" t="s">
+      <c r="C75" s="32" t="s">
         <v>116</v>
       </c>
-      <c r="D75" s="32"/>
-      <c r="E75" s="33" t="s">
-        <v>122</v>
+      <c r="D75" s="31"/>
+      <c r="E75" s="32" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="76" spans="1:8" s="1" customFormat="1">
       <c r="A76" s="8"/>
       <c r="B76" s="8"/>
-      <c r="C76" s="53"/>
-      <c r="D76" s="54"/>
-      <c r="E76" s="55"/>
+      <c r="C76" s="52"/>
+      <c r="D76" s="53"/>
+      <c r="E76" s="54"/>
     </row>
     <row r="77" spans="1:8" s="1" customFormat="1">
       <c r="A77" s="4"/>
       <c r="B77" s="4"/>
-      <c r="C77" s="29"/>
-      <c r="D77" s="32"/>
-      <c r="E77" s="33"/>
+      <c r="C77" s="28"/>
+      <c r="D77" s="31"/>
+      <c r="E77" s="32"/>
     </row>
     <row r="78" spans="1:8" s="1" customFormat="1" ht="13.15" customHeight="1">
       <c r="A78" s="13"/>
       <c r="B78" s="8"/>
-      <c r="C78" s="30"/>
-      <c r="D78" s="45"/>
-      <c r="E78" s="44"/>
-      <c r="F78" s="21"/>
+      <c r="C78" s="29"/>
+      <c r="D78" s="44"/>
+      <c r="E78" s="43"/>
+      <c r="F78" s="20"/>
     </row>
     <row r="79" spans="1:8" s="1" customFormat="1">
       <c r="A79" s="4"/>
       <c r="B79" s="4"/>
-      <c r="C79" s="29"/>
-      <c r="D79" s="32"/>
-      <c r="E79" s="33"/>
+      <c r="C79" s="28"/>
+      <c r="D79" s="31"/>
+      <c r="E79" s="32"/>
     </row>
     <row r="80" spans="1:8" s="1" customFormat="1" ht="13.15" customHeight="1">
       <c r="A80" s="13"/>
       <c r="B80" s="8"/>
-      <c r="C80" s="23"/>
-      <c r="D80" s="45"/>
-      <c r="E80" s="44"/>
-      <c r="F80" s="21"/>
+      <c r="C80" s="22"/>
+      <c r="D80" s="44"/>
+      <c r="E80" s="43"/>
+      <c r="F80" s="20"/>
     </row>
     <row r="81" spans="1:7" s="1" customFormat="1">
       <c r="A81" s="4"/>
       <c r="B81" s="4"/>
-      <c r="C81" s="29"/>
-      <c r="D81" s="32"/>
-      <c r="E81" s="33"/>
+      <c r="C81" s="28"/>
+      <c r="D81" s="31"/>
+      <c r="E81" s="32"/>
     </row>
     <row r="82" spans="1:7" s="1" customFormat="1" ht="12.75" customHeight="1">
       <c r="A82" s="13"/>
       <c r="B82" s="8"/>
-      <c r="C82" s="23"/>
-      <c r="D82" s="45"/>
-      <c r="E82" s="58"/>
-      <c r="F82" s="21"/>
+      <c r="C82" s="22"/>
+      <c r="D82" s="44"/>
+      <c r="E82" s="57"/>
+      <c r="F82" s="20"/>
     </row>
     <row r="83" spans="1:7" s="1" customFormat="1">
       <c r="A83" s="4"/>
       <c r="B83" s="4"/>
-      <c r="C83" s="29"/>
-      <c r="D83" s="32"/>
-      <c r="E83" s="44"/>
+      <c r="C83" s="28"/>
+      <c r="D83" s="31"/>
+      <c r="E83" s="43"/>
     </row>
     <row r="84" spans="1:7" s="1" customFormat="1" ht="13.15" customHeight="1">
       <c r="A84" s="13"/>
       <c r="B84" s="8"/>
-      <c r="C84" s="23"/>
-      <c r="D84" s="45"/>
-      <c r="E84" s="44"/>
-      <c r="F84" s="21"/>
+      <c r="C84" s="22"/>
+      <c r="D84" s="44"/>
+      <c r="E84" s="43"/>
+      <c r="F84" s="20"/>
     </row>
     <row r="85" spans="1:7" s="1" customFormat="1">
       <c r="A85" s="4"/>
       <c r="B85" s="4"/>
-      <c r="C85" s="29"/>
+      <c r="C85" s="28"/>
       <c r="D85" s="6"/>
-      <c r="E85" s="33"/>
+      <c r="E85" s="32"/>
     </row>
     <row r="86" spans="1:7" s="1" customFormat="1" ht="13.15" customHeight="1">
       <c r="A86" s="13"/>
       <c r="B86" s="8"/>
-      <c r="C86" s="23"/>
-      <c r="D86" s="45"/>
-      <c r="E86" s="44"/>
-      <c r="F86" s="21"/>
+      <c r="C86" s="22"/>
+      <c r="D86" s="44"/>
+      <c r="E86" s="43"/>
+      <c r="F86" s="20"/>
     </row>
     <row r="87" spans="1:7" s="1" customFormat="1">
       <c r="A87" s="4"/>
       <c r="B87" s="4"/>
-      <c r="C87" s="29"/>
-      <c r="D87" s="32"/>
-      <c r="E87" s="33"/>
+      <c r="C87" s="28"/>
+      <c r="D87" s="31"/>
+      <c r="E87" s="32"/>
     </row>
     <row r="88" spans="1:7" s="1" customFormat="1" ht="12.75" customHeight="1">
       <c r="A88" s="13"/>
       <c r="B88" s="8"/>
-      <c r="C88" s="23"/>
+      <c r="C88" s="22"/>
       <c r="D88" s="15"/>
-      <c r="E88" s="44"/>
-      <c r="F88" s="21"/>
+      <c r="E88" s="43"/>
+      <c r="F88" s="20"/>
     </row>
     <row r="89" spans="1:7" s="1" customFormat="1" ht="13.5" customHeight="1">
       <c r="A89" s="4"/>
       <c r="B89" s="4"/>
-      <c r="C89" s="29"/>
-      <c r="D89" s="32"/>
-      <c r="E89" s="33"/>
+      <c r="C89" s="28"/>
+      <c r="D89" s="31"/>
+      <c r="E89" s="32"/>
     </row>
     <row r="90" spans="1:7" s="1" customFormat="1" ht="13.15" customHeight="1">
       <c r="A90" s="13"/>
       <c r="B90" s="8"/>
-      <c r="C90" s="23"/>
-      <c r="D90" s="45"/>
-      <c r="E90" s="44"/>
-      <c r="F90" s="21"/>
+      <c r="C90" s="22"/>
+      <c r="D90" s="44"/>
+      <c r="E90" s="43"/>
+      <c r="F90" s="20"/>
     </row>
     <row r="91" spans="1:7" s="1" customFormat="1">
       <c r="A91" s="4"/>
       <c r="B91" s="4"/>
-      <c r="C91" s="29"/>
-      <c r="D91" s="32"/>
-      <c r="E91" s="33"/>
+      <c r="C91" s="28"/>
+      <c r="D91" s="31"/>
+      <c r="E91" s="32"/>
     </row>
     <row r="92" spans="1:7" s="1" customFormat="1" ht="13.35" customHeight="1">
       <c r="A92" s="17"/>
       <c r="B92" s="17"/>
-      <c r="C92" s="67" t="s">
+      <c r="C92" s="66" t="s">
         <v>18</v>
       </c>
-      <c r="D92" s="67"/>
+      <c r="D92" s="66"/>
       <c r="E92" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G92" s="21"/>
+      <c r="G92" s="20"/>
     </row>
     <row r="93" spans="1:7" s="1" customFormat="1">
       <c r="A93" s="8"/>
       <c r="B93" s="8"/>
-      <c r="C93" s="24" t="s">
+      <c r="C93" s="23" t="s">
         <v>23</v>
       </c>
       <c r="D93" s="10" t="s">
@@ -2128,7 +2165,7 @@
     <row r="95" spans="1:7" s="1" customFormat="1">
       <c r="A95" s="8"/>
       <c r="B95" s="8"/>
-      <c r="C95" s="23"/>
+      <c r="C95" s="22"/>
       <c r="D95" s="15"/>
       <c r="E95" s="16"/>
     </row>
@@ -2142,7 +2179,7 @@
     <row r="97" spans="1:6" s="1" customFormat="1" ht="13.35" customHeight="1">
       <c r="A97" s="8"/>
       <c r="B97" s="8"/>
-      <c r="C97" s="21"/>
+      <c r="C97" s="20"/>
       <c r="D97" s="15"/>
       <c r="E97" s="16"/>
     </row>
@@ -2166,7 +2203,7 @@
       <c r="C100" s="5"/>
       <c r="D100" s="6"/>
       <c r="E100" s="7"/>
-      <c r="F100" s="21"/>
+      <c r="F100" s="20"/>
     </row>
     <row r="101" spans="1:6" s="1" customFormat="1">
       <c r="A101" s="13"/>
@@ -2185,11 +2222,11 @@
     <row r="103" spans="1:6" s="1" customFormat="1">
       <c r="A103" s="17"/>
       <c r="B103" s="17"/>
-      <c r="C103" s="59" t="s">
+      <c r="C103" s="58" t="s">
         <v>21</v>
       </c>
-      <c r="D103" s="22"/>
-      <c r="E103" s="59" t="s">
+      <c r="D103" s="21"/>
+      <c r="E103" s="58" t="s">
         <v>26</v>
       </c>
     </row>
@@ -2199,10 +2236,10 @@
       <c r="C104" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D104" s="27" t="s">
+      <c r="D104" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="E104" s="44" t="s">
+      <c r="E104" s="43" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2215,40 +2252,40 @@
       <c r="D105" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E105" s="33" t="s">
+      <c r="E105" s="32" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="106" spans="1:6" s="1" customFormat="1">
       <c r="A106" s="13"/>
       <c r="B106" s="13"/>
-      <c r="C106" s="26" t="s">
+      <c r="C106" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="D106" s="27" t="s">
+      <c r="D106" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="E106" s="44" t="s">
+      <c r="E106" s="43" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="107" spans="1:6" s="1" customFormat="1">
       <c r="A107" s="4"/>
       <c r="B107" s="4"/>
-      <c r="C107" s="29" t="s">
+      <c r="C107" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="D107" s="32" t="s">
+      <c r="D107" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="E107" s="33" t="s">
+      <c r="E107" s="32" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="108" spans="1:6" s="1" customFormat="1">
       <c r="A108" s="13"/>
       <c r="B108" s="13"/>
-      <c r="C108" s="23" t="s">
+      <c r="C108" s="22" t="s">
         <v>31</v>
       </c>
       <c r="D108" s="15" t="s">
@@ -2261,936 +2298,936 @@
     <row r="109" spans="1:6" s="1" customFormat="1">
       <c r="A109" s="4"/>
       <c r="B109" s="4"/>
-      <c r="C109" s="29" t="s">
+      <c r="C109" s="28" t="s">
         <v>76</v>
       </c>
       <c r="D109" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E109" s="33" t="s">
+      <c r="E109" s="32" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="110" spans="1:6" s="1" customFormat="1">
       <c r="A110" s="13"/>
       <c r="B110" s="13"/>
-      <c r="C110" s="23" t="s">
+      <c r="C110" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="D110" s="45" t="s">
+      <c r="D110" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="E110" s="23" t="s">
+      <c r="E110" s="22" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="111" spans="1:6" s="1" customFormat="1">
       <c r="A111" s="4"/>
       <c r="B111" s="4"/>
-      <c r="C111" s="29" t="s">
+      <c r="C111" s="28" t="s">
         <v>35</v>
       </c>
       <c r="D111" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E111" s="33" t="s">
+      <c r="E111" s="32" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="112" spans="1:6" s="1" customFormat="1">
       <c r="A112" s="13"/>
       <c r="B112" s="13"/>
-      <c r="C112" s="23" t="s">
+      <c r="C112" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="D112" s="45" t="s">
+      <c r="D112" s="44" t="s">
         <v>78</v>
       </c>
-      <c r="E112" s="23" t="s">
+      <c r="E112" s="22" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="113" spans="1:5" s="1" customFormat="1">
       <c r="A113" s="4"/>
       <c r="B113" s="4"/>
-      <c r="C113" s="29"/>
-      <c r="D113" s="32"/>
-      <c r="E113" s="33"/>
+      <c r="C113" s="28"/>
+      <c r="D113" s="31"/>
+      <c r="E113" s="32"/>
     </row>
     <row r="114" spans="1:5" s="1" customFormat="1">
-      <c r="A114" s="60"/>
-      <c r="B114" s="60"/>
-      <c r="C114" s="60"/>
-      <c r="D114" s="61"/>
-      <c r="E114" s="62"/>
+      <c r="A114" s="59"/>
+      <c r="B114" s="59"/>
+      <c r="C114" s="59"/>
+      <c r="D114" s="60"/>
+      <c r="E114" s="61"/>
     </row>
     <row r="115" spans="1:5" s="1" customFormat="1">
-      <c r="A115" s="60"/>
-      <c r="B115" s="60"/>
-      <c r="C115" s="60"/>
-      <c r="D115" s="61"/>
-      <c r="E115" s="62"/>
+      <c r="A115" s="59"/>
+      <c r="B115" s="59"/>
+      <c r="C115" s="59"/>
+      <c r="D115" s="60"/>
+      <c r="E115" s="61"/>
     </row>
     <row r="116" spans="1:5" s="1" customFormat="1">
-      <c r="A116" s="60"/>
-      <c r="B116" s="60"/>
-      <c r="C116" s="60"/>
-      <c r="D116" s="61"/>
-      <c r="E116" s="62"/>
+      <c r="A116" s="59"/>
+      <c r="B116" s="59"/>
+      <c r="C116" s="59"/>
+      <c r="D116" s="60"/>
+      <c r="E116" s="61"/>
     </row>
     <row r="117" spans="1:5" s="1" customFormat="1">
-      <c r="A117" s="60"/>
-      <c r="B117" s="60"/>
-      <c r="C117" s="60"/>
-      <c r="D117" s="61"/>
-      <c r="E117" s="62"/>
+      <c r="A117" s="59"/>
+      <c r="B117" s="59"/>
+      <c r="C117" s="59"/>
+      <c r="D117" s="60"/>
+      <c r="E117" s="61"/>
     </row>
     <row r="118" spans="1:5" s="1" customFormat="1">
-      <c r="A118" s="60"/>
-      <c r="B118" s="60"/>
-      <c r="C118" s="60"/>
-      <c r="D118" s="61"/>
-      <c r="E118" s="62"/>
+      <c r="A118" s="59"/>
+      <c r="B118" s="59"/>
+      <c r="C118" s="59"/>
+      <c r="D118" s="60"/>
+      <c r="E118" s="61"/>
     </row>
     <row r="119" spans="1:5" s="1" customFormat="1">
-      <c r="A119" s="60"/>
-      <c r="B119" s="60"/>
-      <c r="C119" s="60"/>
-      <c r="D119" s="61"/>
-      <c r="E119" s="62"/>
+      <c r="A119" s="59"/>
+      <c r="B119" s="59"/>
+      <c r="C119" s="59"/>
+      <c r="D119" s="60"/>
+      <c r="E119" s="61"/>
     </row>
     <row r="120" spans="1:5" s="1" customFormat="1">
-      <c r="A120" s="60"/>
-      <c r="B120" s="60"/>
-      <c r="C120" s="60"/>
-      <c r="D120" s="61"/>
-      <c r="E120" s="62"/>
+      <c r="A120" s="59"/>
+      <c r="B120" s="59"/>
+      <c r="C120" s="59"/>
+      <c r="D120" s="60"/>
+      <c r="E120" s="61"/>
     </row>
     <row r="121" spans="1:5" s="1" customFormat="1">
-      <c r="A121" s="60"/>
-      <c r="B121" s="60"/>
-      <c r="C121" s="60"/>
-      <c r="D121" s="61"/>
-      <c r="E121" s="62"/>
+      <c r="A121" s="59"/>
+      <c r="B121" s="59"/>
+      <c r="C121" s="59"/>
+      <c r="D121" s="60"/>
+      <c r="E121" s="61"/>
     </row>
     <row r="122" spans="1:5" s="1" customFormat="1">
-      <c r="A122" s="60"/>
-      <c r="B122" s="60"/>
-      <c r="C122" s="60"/>
-      <c r="D122" s="61"/>
-      <c r="E122" s="62"/>
+      <c r="A122" s="59"/>
+      <c r="B122" s="59"/>
+      <c r="C122" s="59"/>
+      <c r="D122" s="60"/>
+      <c r="E122" s="61"/>
     </row>
     <row r="123" spans="1:5" s="1" customFormat="1">
-      <c r="A123" s="60"/>
-      <c r="B123" s="60"/>
-      <c r="C123" s="60"/>
-      <c r="D123" s="61"/>
-      <c r="E123" s="62"/>
+      <c r="A123" s="59"/>
+      <c r="B123" s="59"/>
+      <c r="C123" s="59"/>
+      <c r="D123" s="60"/>
+      <c r="E123" s="61"/>
     </row>
     <row r="124" spans="1:5" s="1" customFormat="1">
-      <c r="A124" s="60"/>
-      <c r="B124" s="60"/>
-      <c r="C124" s="60"/>
-      <c r="D124" s="61"/>
-      <c r="E124" s="62"/>
+      <c r="A124" s="59"/>
+      <c r="B124" s="59"/>
+      <c r="C124" s="59"/>
+      <c r="D124" s="60"/>
+      <c r="E124" s="61"/>
     </row>
     <row r="125" spans="1:5" s="1" customFormat="1">
-      <c r="A125" s="60"/>
-      <c r="B125" s="60"/>
-      <c r="C125" s="60"/>
-      <c r="D125" s="61"/>
-      <c r="E125" s="62"/>
+      <c r="A125" s="59"/>
+      <c r="B125" s="59"/>
+      <c r="C125" s="59"/>
+      <c r="D125" s="60"/>
+      <c r="E125" s="61"/>
     </row>
     <row r="126" spans="1:5" s="1" customFormat="1">
-      <c r="A126" s="60"/>
-      <c r="B126" s="60"/>
-      <c r="C126" s="60"/>
-      <c r="D126" s="61"/>
-      <c r="E126" s="62"/>
+      <c r="A126" s="59"/>
+      <c r="B126" s="59"/>
+      <c r="C126" s="59"/>
+      <c r="D126" s="60"/>
+      <c r="E126" s="61"/>
     </row>
     <row r="127" spans="1:5" s="1" customFormat="1">
-      <c r="A127" s="60"/>
-      <c r="B127" s="60"/>
-      <c r="C127" s="60"/>
-      <c r="D127" s="61"/>
-      <c r="E127" s="62"/>
+      <c r="A127" s="59"/>
+      <c r="B127" s="59"/>
+      <c r="C127" s="59"/>
+      <c r="D127" s="60"/>
+      <c r="E127" s="61"/>
     </row>
     <row r="128" spans="1:5" s="1" customFormat="1">
-      <c r="A128" s="60"/>
-      <c r="B128" s="60"/>
-      <c r="C128" s="60"/>
-      <c r="D128" s="61"/>
-      <c r="E128" s="62"/>
+      <c r="A128" s="59"/>
+      <c r="B128" s="59"/>
+      <c r="C128" s="59"/>
+      <c r="D128" s="60"/>
+      <c r="E128" s="61"/>
     </row>
     <row r="129" spans="1:5" s="1" customFormat="1">
-      <c r="A129" s="60"/>
-      <c r="B129" s="60"/>
-      <c r="C129" s="60"/>
-      <c r="D129" s="61"/>
-      <c r="E129" s="62"/>
+      <c r="A129" s="59"/>
+      <c r="B129" s="59"/>
+      <c r="C129" s="59"/>
+      <c r="D129" s="60"/>
+      <c r="E129" s="61"/>
     </row>
     <row r="130" spans="1:5" s="1" customFormat="1">
-      <c r="A130" s="60"/>
-      <c r="B130" s="60"/>
-      <c r="C130" s="60"/>
-      <c r="D130" s="61"/>
-      <c r="E130" s="62"/>
+      <c r="A130" s="59"/>
+      <c r="B130" s="59"/>
+      <c r="C130" s="59"/>
+      <c r="D130" s="60"/>
+      <c r="E130" s="61"/>
     </row>
     <row r="131" spans="1:5" s="1" customFormat="1">
-      <c r="A131" s="60"/>
-      <c r="B131" s="60"/>
-      <c r="C131" s="60"/>
-      <c r="D131" s="61"/>
-      <c r="E131" s="62"/>
+      <c r="A131" s="59"/>
+      <c r="B131" s="59"/>
+      <c r="C131" s="59"/>
+      <c r="D131" s="60"/>
+      <c r="E131" s="61"/>
     </row>
     <row r="132" spans="1:5" s="1" customFormat="1">
-      <c r="A132" s="60"/>
-      <c r="B132" s="60"/>
-      <c r="C132" s="60"/>
-      <c r="D132" s="61"/>
-      <c r="E132" s="62"/>
+      <c r="A132" s="59"/>
+      <c r="B132" s="59"/>
+      <c r="C132" s="59"/>
+      <c r="D132" s="60"/>
+      <c r="E132" s="61"/>
     </row>
     <row r="133" spans="1:5" s="1" customFormat="1">
-      <c r="A133" s="60"/>
-      <c r="B133" s="60"/>
-      <c r="C133" s="60"/>
-      <c r="D133" s="61"/>
-      <c r="E133" s="62"/>
+      <c r="A133" s="59"/>
+      <c r="B133" s="59"/>
+      <c r="C133" s="59"/>
+      <c r="D133" s="60"/>
+      <c r="E133" s="61"/>
     </row>
     <row r="134" spans="1:5" s="1" customFormat="1">
-      <c r="A134" s="60"/>
-      <c r="B134" s="60"/>
-      <c r="C134" s="60"/>
-      <c r="D134" s="61"/>
-      <c r="E134" s="62"/>
+      <c r="A134" s="59"/>
+      <c r="B134" s="59"/>
+      <c r="C134" s="59"/>
+      <c r="D134" s="60"/>
+      <c r="E134" s="61"/>
     </row>
     <row r="135" spans="1:5" s="1" customFormat="1">
-      <c r="A135" s="60"/>
-      <c r="B135" s="60"/>
-      <c r="C135" s="60"/>
-      <c r="D135" s="61"/>
-      <c r="E135" s="62"/>
+      <c r="A135" s="59"/>
+      <c r="B135" s="59"/>
+      <c r="C135" s="59"/>
+      <c r="D135" s="60"/>
+      <c r="E135" s="61"/>
     </row>
     <row r="136" spans="1:5" s="1" customFormat="1">
-      <c r="A136" s="60"/>
-      <c r="B136" s="60"/>
-      <c r="C136" s="60"/>
-      <c r="D136" s="61"/>
-      <c r="E136" s="62"/>
+      <c r="A136" s="59"/>
+      <c r="B136" s="59"/>
+      <c r="C136" s="59"/>
+      <c r="D136" s="60"/>
+      <c r="E136" s="61"/>
     </row>
     <row r="137" spans="1:5" s="1" customFormat="1">
-      <c r="A137" s="60"/>
-      <c r="B137" s="60"/>
-      <c r="C137" s="60"/>
-      <c r="D137" s="61"/>
-      <c r="E137" s="62"/>
+      <c r="A137" s="59"/>
+      <c r="B137" s="59"/>
+      <c r="C137" s="59"/>
+      <c r="D137" s="60"/>
+      <c r="E137" s="61"/>
     </row>
     <row r="138" spans="1:5" s="1" customFormat="1">
-      <c r="A138" s="60"/>
-      <c r="B138" s="60"/>
-      <c r="C138" s="60"/>
-      <c r="D138" s="61"/>
-      <c r="E138" s="62"/>
+      <c r="A138" s="59"/>
+      <c r="B138" s="59"/>
+      <c r="C138" s="59"/>
+      <c r="D138" s="60"/>
+      <c r="E138" s="61"/>
     </row>
     <row r="139" spans="1:5" s="1" customFormat="1">
-      <c r="A139" s="60"/>
-      <c r="B139" s="60"/>
-      <c r="C139" s="60"/>
-      <c r="D139" s="61"/>
-      <c r="E139" s="62"/>
+      <c r="A139" s="59"/>
+      <c r="B139" s="59"/>
+      <c r="C139" s="59"/>
+      <c r="D139" s="60"/>
+      <c r="E139" s="61"/>
     </row>
     <row r="140" spans="1:5" s="1" customFormat="1">
-      <c r="A140" s="60"/>
-      <c r="B140" s="60"/>
-      <c r="C140" s="60"/>
-      <c r="D140" s="61"/>
-      <c r="E140" s="62"/>
+      <c r="A140" s="59"/>
+      <c r="B140" s="59"/>
+      <c r="C140" s="59"/>
+      <c r="D140" s="60"/>
+      <c r="E140" s="61"/>
     </row>
     <row r="141" spans="1:5" s="1" customFormat="1">
-      <c r="A141" s="60"/>
-      <c r="B141" s="60"/>
-      <c r="C141" s="60"/>
-      <c r="D141" s="61"/>
-      <c r="E141" s="62"/>
+      <c r="A141" s="59"/>
+      <c r="B141" s="59"/>
+      <c r="C141" s="59"/>
+      <c r="D141" s="60"/>
+      <c r="E141" s="61"/>
     </row>
     <row r="142" spans="1:5" s="1" customFormat="1">
-      <c r="A142" s="60"/>
-      <c r="B142" s="60"/>
-      <c r="C142" s="60"/>
-      <c r="D142" s="61"/>
-      <c r="E142" s="62"/>
+      <c r="A142" s="59"/>
+      <c r="B142" s="59"/>
+      <c r="C142" s="59"/>
+      <c r="D142" s="60"/>
+      <c r="E142" s="61"/>
     </row>
     <row r="143" spans="1:5" s="1" customFormat="1">
-      <c r="A143" s="60"/>
-      <c r="B143" s="60"/>
-      <c r="C143" s="60"/>
-      <c r="D143" s="61"/>
-      <c r="E143" s="62"/>
+      <c r="A143" s="59"/>
+      <c r="B143" s="59"/>
+      <c r="C143" s="59"/>
+      <c r="D143" s="60"/>
+      <c r="E143" s="61"/>
     </row>
     <row r="144" spans="1:5" s="1" customFormat="1">
-      <c r="A144" s="60"/>
-      <c r="B144" s="60"/>
-      <c r="C144" s="60"/>
-      <c r="D144" s="61"/>
-      <c r="E144" s="62"/>
+      <c r="A144" s="59"/>
+      <c r="B144" s="59"/>
+      <c r="C144" s="59"/>
+      <c r="D144" s="60"/>
+      <c r="E144" s="61"/>
     </row>
     <row r="145" spans="1:5" s="1" customFormat="1">
-      <c r="A145" s="60"/>
-      <c r="B145" s="60"/>
-      <c r="C145" s="60"/>
-      <c r="D145" s="61"/>
-      <c r="E145" s="62"/>
+      <c r="A145" s="59"/>
+      <c r="B145" s="59"/>
+      <c r="C145" s="59"/>
+      <c r="D145" s="60"/>
+      <c r="E145" s="61"/>
     </row>
     <row r="146" spans="1:5" s="1" customFormat="1">
-      <c r="A146" s="60"/>
-      <c r="B146" s="60"/>
-      <c r="C146" s="60"/>
-      <c r="D146" s="61"/>
-      <c r="E146" s="62"/>
+      <c r="A146" s="59"/>
+      <c r="B146" s="59"/>
+      <c r="C146" s="59"/>
+      <c r="D146" s="60"/>
+      <c r="E146" s="61"/>
     </row>
     <row r="147" spans="1:5" s="1" customFormat="1">
-      <c r="A147" s="60"/>
-      <c r="B147" s="60"/>
-      <c r="C147" s="60"/>
-      <c r="D147" s="61"/>
-      <c r="E147" s="62"/>
+      <c r="A147" s="59"/>
+      <c r="B147" s="59"/>
+      <c r="C147" s="59"/>
+      <c r="D147" s="60"/>
+      <c r="E147" s="61"/>
     </row>
     <row r="148" spans="1:5" s="1" customFormat="1">
-      <c r="A148" s="60"/>
-      <c r="B148" s="60"/>
-      <c r="C148" s="60"/>
-      <c r="D148" s="61"/>
-      <c r="E148" s="62"/>
+      <c r="A148" s="59"/>
+      <c r="B148" s="59"/>
+      <c r="C148" s="59"/>
+      <c r="D148" s="60"/>
+      <c r="E148" s="61"/>
     </row>
     <row r="149" spans="1:5" s="1" customFormat="1">
-      <c r="A149" s="60"/>
-      <c r="B149" s="60"/>
-      <c r="C149" s="60"/>
-      <c r="D149" s="61"/>
-      <c r="E149" s="62"/>
+      <c r="A149" s="59"/>
+      <c r="B149" s="59"/>
+      <c r="C149" s="59"/>
+      <c r="D149" s="60"/>
+      <c r="E149" s="61"/>
     </row>
     <row r="150" spans="1:5" s="1" customFormat="1">
-      <c r="A150" s="60"/>
-      <c r="B150" s="60"/>
-      <c r="C150" s="60"/>
-      <c r="D150" s="61"/>
-      <c r="E150" s="62"/>
+      <c r="A150" s="59"/>
+      <c r="B150" s="59"/>
+      <c r="C150" s="59"/>
+      <c r="D150" s="60"/>
+      <c r="E150" s="61"/>
     </row>
     <row r="151" spans="1:5" s="1" customFormat="1">
-      <c r="A151" s="60"/>
-      <c r="B151" s="60"/>
-      <c r="C151" s="60"/>
-      <c r="D151" s="61"/>
-      <c r="E151" s="62"/>
+      <c r="A151" s="59"/>
+      <c r="B151" s="59"/>
+      <c r="C151" s="59"/>
+      <c r="D151" s="60"/>
+      <c r="E151" s="61"/>
     </row>
     <row r="152" spans="1:5" s="1" customFormat="1">
-      <c r="A152" s="60"/>
-      <c r="B152" s="60"/>
-      <c r="C152" s="60"/>
-      <c r="D152" s="61"/>
-      <c r="E152" s="62"/>
+      <c r="A152" s="59"/>
+      <c r="B152" s="59"/>
+      <c r="C152" s="59"/>
+      <c r="D152" s="60"/>
+      <c r="E152" s="61"/>
     </row>
     <row r="153" spans="1:5" s="1" customFormat="1">
-      <c r="A153" s="60"/>
-      <c r="B153" s="60"/>
-      <c r="C153" s="60"/>
-      <c r="D153" s="61"/>
-      <c r="E153" s="62"/>
+      <c r="A153" s="59"/>
+      <c r="B153" s="59"/>
+      <c r="C153" s="59"/>
+      <c r="D153" s="60"/>
+      <c r="E153" s="61"/>
     </row>
     <row r="154" spans="1:5" s="1" customFormat="1">
-      <c r="A154" s="60"/>
-      <c r="B154" s="60"/>
-      <c r="C154" s="60"/>
-      <c r="D154" s="61"/>
-      <c r="E154" s="62"/>
+      <c r="A154" s="59"/>
+      <c r="B154" s="59"/>
+      <c r="C154" s="59"/>
+      <c r="D154" s="60"/>
+      <c r="E154" s="61"/>
     </row>
     <row r="155" spans="1:5" s="1" customFormat="1">
-      <c r="A155" s="60"/>
-      <c r="B155" s="60"/>
-      <c r="C155" s="60"/>
-      <c r="D155" s="61"/>
-      <c r="E155" s="62"/>
+      <c r="A155" s="59"/>
+      <c r="B155" s="59"/>
+      <c r="C155" s="59"/>
+      <c r="D155" s="60"/>
+      <c r="E155" s="61"/>
     </row>
     <row r="156" spans="1:5" s="1" customFormat="1">
-      <c r="A156" s="60"/>
-      <c r="B156" s="60"/>
-      <c r="C156" s="60"/>
-      <c r="D156" s="61"/>
-      <c r="E156" s="62"/>
+      <c r="A156" s="59"/>
+      <c r="B156" s="59"/>
+      <c r="C156" s="59"/>
+      <c r="D156" s="60"/>
+      <c r="E156" s="61"/>
     </row>
     <row r="157" spans="1:5" s="1" customFormat="1">
-      <c r="A157" s="60"/>
-      <c r="B157" s="60"/>
-      <c r="C157" s="60"/>
-      <c r="D157" s="61"/>
-      <c r="E157" s="62"/>
+      <c r="A157" s="59"/>
+      <c r="B157" s="59"/>
+      <c r="C157" s="59"/>
+      <c r="D157" s="60"/>
+      <c r="E157" s="61"/>
     </row>
     <row r="158" spans="1:5" s="1" customFormat="1">
-      <c r="A158" s="60"/>
-      <c r="B158" s="60"/>
-      <c r="C158" s="60"/>
-      <c r="D158" s="61"/>
-      <c r="E158" s="62"/>
+      <c r="A158" s="59"/>
+      <c r="B158" s="59"/>
+      <c r="C158" s="59"/>
+      <c r="D158" s="60"/>
+      <c r="E158" s="61"/>
     </row>
     <row r="159" spans="1:5" s="1" customFormat="1">
-      <c r="A159" s="60"/>
-      <c r="B159" s="60"/>
-      <c r="C159" s="60"/>
-      <c r="D159" s="61"/>
-      <c r="E159" s="62"/>
+      <c r="A159" s="59"/>
+      <c r="B159" s="59"/>
+      <c r="C159" s="59"/>
+      <c r="D159" s="60"/>
+      <c r="E159" s="61"/>
     </row>
     <row r="160" spans="1:5" s="1" customFormat="1">
-      <c r="A160" s="60"/>
-      <c r="B160" s="60"/>
-      <c r="C160" s="60"/>
-      <c r="D160" s="61"/>
-      <c r="E160" s="62"/>
+      <c r="A160" s="59"/>
+      <c r="B160" s="59"/>
+      <c r="C160" s="59"/>
+      <c r="D160" s="60"/>
+      <c r="E160" s="61"/>
     </row>
     <row r="161" spans="1:5" s="1" customFormat="1">
-      <c r="A161" s="60"/>
-      <c r="B161" s="60"/>
-      <c r="C161" s="60"/>
-      <c r="D161" s="61"/>
-      <c r="E161" s="62"/>
+      <c r="A161" s="59"/>
+      <c r="B161" s="59"/>
+      <c r="C161" s="59"/>
+      <c r="D161" s="60"/>
+      <c r="E161" s="61"/>
     </row>
     <row r="162" spans="1:5" s="1" customFormat="1">
-      <c r="A162" s="60"/>
-      <c r="B162" s="60"/>
-      <c r="C162" s="60"/>
-      <c r="D162" s="61"/>
-      <c r="E162" s="62"/>
+      <c r="A162" s="59"/>
+      <c r="B162" s="59"/>
+      <c r="C162" s="59"/>
+      <c r="D162" s="60"/>
+      <c r="E162" s="61"/>
     </row>
     <row r="163" spans="1:5" s="1" customFormat="1">
-      <c r="A163" s="60"/>
-      <c r="B163" s="60"/>
-      <c r="C163" s="60"/>
-      <c r="D163" s="61"/>
-      <c r="E163" s="62"/>
+      <c r="A163" s="59"/>
+      <c r="B163" s="59"/>
+      <c r="C163" s="59"/>
+      <c r="D163" s="60"/>
+      <c r="E163" s="61"/>
     </row>
     <row r="164" spans="1:5" s="1" customFormat="1">
-      <c r="A164" s="60"/>
-      <c r="B164" s="60"/>
-      <c r="C164" s="60"/>
-      <c r="D164" s="61"/>
-      <c r="E164" s="62"/>
+      <c r="A164" s="59"/>
+      <c r="B164" s="59"/>
+      <c r="C164" s="59"/>
+      <c r="D164" s="60"/>
+      <c r="E164" s="61"/>
     </row>
     <row r="165" spans="1:5" s="1" customFormat="1">
-      <c r="A165" s="60"/>
-      <c r="B165" s="60"/>
-      <c r="C165" s="60"/>
-      <c r="D165" s="61"/>
-      <c r="E165" s="62"/>
+      <c r="A165" s="59"/>
+      <c r="B165" s="59"/>
+      <c r="C165" s="59"/>
+      <c r="D165" s="60"/>
+      <c r="E165" s="61"/>
     </row>
     <row r="166" spans="1:5" s="1" customFormat="1">
-      <c r="A166" s="60"/>
-      <c r="B166" s="60"/>
-      <c r="C166" s="60"/>
-      <c r="D166" s="61"/>
-      <c r="E166" s="62"/>
+      <c r="A166" s="59"/>
+      <c r="B166" s="59"/>
+      <c r="C166" s="59"/>
+      <c r="D166" s="60"/>
+      <c r="E166" s="61"/>
     </row>
     <row r="167" spans="1:5" s="1" customFormat="1">
-      <c r="A167" s="60"/>
-      <c r="B167" s="60"/>
-      <c r="C167" s="60"/>
-      <c r="D167" s="61"/>
-      <c r="E167" s="62"/>
+      <c r="A167" s="59"/>
+      <c r="B167" s="59"/>
+      <c r="C167" s="59"/>
+      <c r="D167" s="60"/>
+      <c r="E167" s="61"/>
     </row>
     <row r="168" spans="1:5" s="1" customFormat="1">
-      <c r="A168" s="60"/>
-      <c r="B168" s="60"/>
-      <c r="C168" s="60"/>
-      <c r="D168" s="61"/>
-      <c r="E168" s="62"/>
+      <c r="A168" s="59"/>
+      <c r="B168" s="59"/>
+      <c r="C168" s="59"/>
+      <c r="D168" s="60"/>
+      <c r="E168" s="61"/>
     </row>
     <row r="169" spans="1:5" s="1" customFormat="1">
-      <c r="A169" s="60"/>
-      <c r="B169" s="60"/>
-      <c r="C169" s="60"/>
-      <c r="D169" s="61"/>
-      <c r="E169" s="62"/>
+      <c r="A169" s="59"/>
+      <c r="B169" s="59"/>
+      <c r="C169" s="59"/>
+      <c r="D169" s="60"/>
+      <c r="E169" s="61"/>
     </row>
     <row r="170" spans="1:5" s="1" customFormat="1">
-      <c r="A170" s="60"/>
-      <c r="B170" s="60"/>
-      <c r="C170" s="60"/>
-      <c r="D170" s="61"/>
-      <c r="E170" s="62"/>
+      <c r="A170" s="59"/>
+      <c r="B170" s="59"/>
+      <c r="C170" s="59"/>
+      <c r="D170" s="60"/>
+      <c r="E170" s="61"/>
     </row>
     <row r="171" spans="1:5" s="1" customFormat="1">
-      <c r="A171" s="60"/>
-      <c r="B171" s="60"/>
-      <c r="C171" s="60"/>
-      <c r="D171" s="61"/>
-      <c r="E171" s="62"/>
+      <c r="A171" s="59"/>
+      <c r="B171" s="59"/>
+      <c r="C171" s="59"/>
+      <c r="D171" s="60"/>
+      <c r="E171" s="61"/>
     </row>
     <row r="172" spans="1:5" s="1" customFormat="1">
-      <c r="A172" s="60"/>
-      <c r="B172" s="60"/>
-      <c r="C172" s="60"/>
-      <c r="D172" s="61"/>
-      <c r="E172" s="62"/>
+      <c r="A172" s="59"/>
+      <c r="B172" s="59"/>
+      <c r="C172" s="59"/>
+      <c r="D172" s="60"/>
+      <c r="E172" s="61"/>
     </row>
     <row r="173" spans="1:5" s="1" customFormat="1">
-      <c r="A173" s="60"/>
-      <c r="B173" s="60"/>
-      <c r="C173" s="60"/>
-      <c r="D173" s="61"/>
-      <c r="E173" s="62"/>
+      <c r="A173" s="59"/>
+      <c r="B173" s="59"/>
+      <c r="C173" s="59"/>
+      <c r="D173" s="60"/>
+      <c r="E173" s="61"/>
     </row>
     <row r="174" spans="1:5" s="1" customFormat="1">
-      <c r="A174" s="60"/>
-      <c r="B174" s="60"/>
-      <c r="C174" s="60"/>
-      <c r="D174" s="61"/>
-      <c r="E174" s="62"/>
+      <c r="A174" s="59"/>
+      <c r="B174" s="59"/>
+      <c r="C174" s="59"/>
+      <c r="D174" s="60"/>
+      <c r="E174" s="61"/>
     </row>
     <row r="175" spans="1:5" s="1" customFormat="1">
-      <c r="A175" s="60"/>
-      <c r="B175" s="60"/>
-      <c r="C175" s="60"/>
-      <c r="D175" s="61"/>
-      <c r="E175" s="62"/>
+      <c r="A175" s="59"/>
+      <c r="B175" s="59"/>
+      <c r="C175" s="59"/>
+      <c r="D175" s="60"/>
+      <c r="E175" s="61"/>
     </row>
     <row r="176" spans="1:5" s="1" customFormat="1">
-      <c r="A176" s="60"/>
-      <c r="B176" s="60"/>
-      <c r="C176" s="60"/>
-      <c r="D176" s="61"/>
-      <c r="E176" s="62"/>
+      <c r="A176" s="59"/>
+      <c r="B176" s="59"/>
+      <c r="C176" s="59"/>
+      <c r="D176" s="60"/>
+      <c r="E176" s="61"/>
     </row>
     <row r="177" spans="1:5" s="1" customFormat="1">
-      <c r="A177" s="60"/>
-      <c r="B177" s="60"/>
-      <c r="C177" s="60"/>
-      <c r="D177" s="61"/>
-      <c r="E177" s="62"/>
+      <c r="A177" s="59"/>
+      <c r="B177" s="59"/>
+      <c r="C177" s="59"/>
+      <c r="D177" s="60"/>
+      <c r="E177" s="61"/>
     </row>
     <row r="178" spans="1:5" s="1" customFormat="1">
-      <c r="A178" s="60"/>
-      <c r="B178" s="60"/>
-      <c r="C178" s="60"/>
-      <c r="D178" s="61"/>
-      <c r="E178" s="62"/>
+      <c r="A178" s="59"/>
+      <c r="B178" s="59"/>
+      <c r="C178" s="59"/>
+      <c r="D178" s="60"/>
+      <c r="E178" s="61"/>
     </row>
     <row r="179" spans="1:5" s="1" customFormat="1">
-      <c r="A179" s="60"/>
-      <c r="B179" s="60"/>
-      <c r="C179" s="60"/>
-      <c r="D179" s="61"/>
-      <c r="E179" s="62"/>
+      <c r="A179" s="59"/>
+      <c r="B179" s="59"/>
+      <c r="C179" s="59"/>
+      <c r="D179" s="60"/>
+      <c r="E179" s="61"/>
     </row>
     <row r="180" spans="1:5" s="1" customFormat="1">
-      <c r="A180" s="60"/>
-      <c r="B180" s="60"/>
-      <c r="C180" s="60"/>
-      <c r="D180" s="61"/>
-      <c r="E180" s="62"/>
+      <c r="A180" s="59"/>
+      <c r="B180" s="59"/>
+      <c r="C180" s="59"/>
+      <c r="D180" s="60"/>
+      <c r="E180" s="61"/>
     </row>
     <row r="181" spans="1:5" s="1" customFormat="1">
-      <c r="A181" s="60"/>
-      <c r="B181" s="60"/>
-      <c r="C181" s="60"/>
-      <c r="D181" s="61"/>
-      <c r="E181" s="62"/>
+      <c r="A181" s="59"/>
+      <c r="B181" s="59"/>
+      <c r="C181" s="59"/>
+      <c r="D181" s="60"/>
+      <c r="E181" s="61"/>
     </row>
     <row r="182" spans="1:5" s="1" customFormat="1">
-      <c r="A182" s="60"/>
-      <c r="B182" s="60"/>
-      <c r="C182" s="60"/>
-      <c r="D182" s="61"/>
-      <c r="E182" s="62"/>
+      <c r="A182" s="59"/>
+      <c r="B182" s="59"/>
+      <c r="C182" s="59"/>
+      <c r="D182" s="60"/>
+      <c r="E182" s="61"/>
     </row>
     <row r="183" spans="1:5" s="1" customFormat="1">
-      <c r="A183" s="60"/>
-      <c r="B183" s="60"/>
-      <c r="C183" s="60"/>
-      <c r="D183" s="61"/>
-      <c r="E183" s="62"/>
+      <c r="A183" s="59"/>
+      <c r="B183" s="59"/>
+      <c r="C183" s="59"/>
+      <c r="D183" s="60"/>
+      <c r="E183" s="61"/>
     </row>
     <row r="184" spans="1:5" s="1" customFormat="1">
-      <c r="A184" s="60"/>
-      <c r="B184" s="60"/>
-      <c r="C184" s="60"/>
-      <c r="D184" s="61"/>
-      <c r="E184" s="62"/>
+      <c r="A184" s="59"/>
+      <c r="B184" s="59"/>
+      <c r="C184" s="59"/>
+      <c r="D184" s="60"/>
+      <c r="E184" s="61"/>
     </row>
     <row r="185" spans="1:5" s="1" customFormat="1">
-      <c r="A185" s="60"/>
-      <c r="B185" s="60"/>
-      <c r="C185" s="60"/>
-      <c r="D185" s="61"/>
-      <c r="E185" s="62"/>
+      <c r="A185" s="59"/>
+      <c r="B185" s="59"/>
+      <c r="C185" s="59"/>
+      <c r="D185" s="60"/>
+      <c r="E185" s="61"/>
     </row>
     <row r="186" spans="1:5" s="1" customFormat="1">
-      <c r="A186" s="60"/>
-      <c r="B186" s="60"/>
-      <c r="C186" s="60"/>
-      <c r="D186" s="61"/>
-      <c r="E186" s="62"/>
+      <c r="A186" s="59"/>
+      <c r="B186" s="59"/>
+      <c r="C186" s="59"/>
+      <c r="D186" s="60"/>
+      <c r="E186" s="61"/>
     </row>
     <row r="187" spans="1:5" s="1" customFormat="1">
-      <c r="A187" s="60"/>
-      <c r="B187" s="60"/>
-      <c r="C187" s="60"/>
-      <c r="D187" s="61"/>
-      <c r="E187" s="62"/>
+      <c r="A187" s="59"/>
+      <c r="B187" s="59"/>
+      <c r="C187" s="59"/>
+      <c r="D187" s="60"/>
+      <c r="E187" s="61"/>
     </row>
     <row r="188" spans="1:5" s="1" customFormat="1">
-      <c r="A188" s="60"/>
-      <c r="B188" s="60"/>
-      <c r="C188" s="60"/>
-      <c r="D188" s="61"/>
-      <c r="E188" s="62"/>
+      <c r="A188" s="59"/>
+      <c r="B188" s="59"/>
+      <c r="C188" s="59"/>
+      <c r="D188" s="60"/>
+      <c r="E188" s="61"/>
     </row>
     <row r="189" spans="1:5" s="1" customFormat="1">
-      <c r="A189" s="60"/>
-      <c r="B189" s="60"/>
-      <c r="C189" s="60"/>
-      <c r="D189" s="61"/>
-      <c r="E189" s="62"/>
+      <c r="A189" s="59"/>
+      <c r="B189" s="59"/>
+      <c r="C189" s="59"/>
+      <c r="D189" s="60"/>
+      <c r="E189" s="61"/>
     </row>
     <row r="190" spans="1:5" s="1" customFormat="1">
-      <c r="A190" s="60"/>
-      <c r="B190" s="60"/>
-      <c r="C190" s="60"/>
-      <c r="D190" s="61"/>
-      <c r="E190" s="62"/>
+      <c r="A190" s="59"/>
+      <c r="B190" s="59"/>
+      <c r="C190" s="59"/>
+      <c r="D190" s="60"/>
+      <c r="E190" s="61"/>
     </row>
     <row r="191" spans="1:5" s="1" customFormat="1">
-      <c r="A191" s="60"/>
-      <c r="B191" s="60"/>
-      <c r="C191" s="60"/>
-      <c r="D191" s="61"/>
-      <c r="E191" s="62"/>
+      <c r="A191" s="59"/>
+      <c r="B191" s="59"/>
+      <c r="C191" s="59"/>
+      <c r="D191" s="60"/>
+      <c r="E191" s="61"/>
     </row>
     <row r="192" spans="1:5" s="1" customFormat="1">
-      <c r="A192" s="60"/>
-      <c r="B192" s="60"/>
-      <c r="C192" s="60"/>
-      <c r="D192" s="61"/>
-      <c r="E192" s="62"/>
+      <c r="A192" s="59"/>
+      <c r="B192" s="59"/>
+      <c r="C192" s="59"/>
+      <c r="D192" s="60"/>
+      <c r="E192" s="61"/>
     </row>
     <row r="193" spans="1:5" s="1" customFormat="1">
-      <c r="A193" s="60"/>
-      <c r="B193" s="60"/>
-      <c r="C193" s="60"/>
-      <c r="D193" s="61"/>
-      <c r="E193" s="62"/>
+      <c r="A193" s="59"/>
+      <c r="B193" s="59"/>
+      <c r="C193" s="59"/>
+      <c r="D193" s="60"/>
+      <c r="E193" s="61"/>
     </row>
     <row r="194" spans="1:5" s="1" customFormat="1">
-      <c r="A194" s="60"/>
-      <c r="B194" s="60"/>
-      <c r="C194" s="60"/>
-      <c r="D194" s="61"/>
-      <c r="E194" s="63"/>
+      <c r="A194" s="59"/>
+      <c r="B194" s="59"/>
+      <c r="C194" s="59"/>
+      <c r="D194" s="60"/>
+      <c r="E194" s="62"/>
     </row>
     <row r="195" spans="1:5" s="1" customFormat="1">
-      <c r="A195" s="60"/>
-      <c r="B195" s="60"/>
-      <c r="C195" s="60"/>
-      <c r="D195" s="61"/>
-      <c r="E195" s="63"/>
+      <c r="A195" s="59"/>
+      <c r="B195" s="59"/>
+      <c r="C195" s="59"/>
+      <c r="D195" s="60"/>
+      <c r="E195" s="62"/>
     </row>
     <row r="196" spans="1:5" s="1" customFormat="1">
-      <c r="A196" s="60"/>
-      <c r="B196" s="60"/>
-      <c r="C196" s="60"/>
-      <c r="D196" s="61"/>
-      <c r="E196" s="63"/>
+      <c r="A196" s="59"/>
+      <c r="B196" s="59"/>
+      <c r="C196" s="59"/>
+      <c r="D196" s="60"/>
+      <c r="E196" s="62"/>
     </row>
     <row r="197" spans="1:5" s="1" customFormat="1">
-      <c r="A197" s="60"/>
-      <c r="B197" s="60"/>
-      <c r="C197" s="60"/>
-      <c r="D197" s="61"/>
-      <c r="E197" s="63"/>
+      <c r="A197" s="59"/>
+      <c r="B197" s="59"/>
+      <c r="C197" s="59"/>
+      <c r="D197" s="60"/>
+      <c r="E197" s="62"/>
     </row>
     <row r="198" spans="1:5" s="1" customFormat="1">
-      <c r="A198" s="60"/>
-      <c r="B198" s="60"/>
-      <c r="C198" s="60"/>
-      <c r="D198" s="61"/>
-      <c r="E198" s="63"/>
+      <c r="A198" s="59"/>
+      <c r="B198" s="59"/>
+      <c r="C198" s="59"/>
+      <c r="D198" s="60"/>
+      <c r="E198" s="62"/>
     </row>
     <row r="199" spans="1:5" s="1" customFormat="1">
-      <c r="A199" s="60"/>
-      <c r="B199" s="60"/>
-      <c r="C199" s="60"/>
-      <c r="D199" s="61"/>
-      <c r="E199" s="63"/>
+      <c r="A199" s="59"/>
+      <c r="B199" s="59"/>
+      <c r="C199" s="59"/>
+      <c r="D199" s="60"/>
+      <c r="E199" s="62"/>
     </row>
     <row r="200" spans="1:5" s="1" customFormat="1">
-      <c r="A200" s="60"/>
-      <c r="B200" s="60"/>
-      <c r="C200" s="60"/>
-      <c r="D200" s="61"/>
-      <c r="E200" s="63"/>
+      <c r="A200" s="59"/>
+      <c r="B200" s="59"/>
+      <c r="C200" s="59"/>
+      <c r="D200" s="60"/>
+      <c r="E200" s="62"/>
     </row>
     <row r="201" spans="1:5" s="1" customFormat="1">
-      <c r="A201" s="60"/>
-      <c r="B201" s="60"/>
-      <c r="C201" s="60"/>
-      <c r="D201" s="61"/>
-      <c r="E201" s="63"/>
+      <c r="A201" s="59"/>
+      <c r="B201" s="59"/>
+      <c r="C201" s="59"/>
+      <c r="D201" s="60"/>
+      <c r="E201" s="62"/>
     </row>
     <row r="202" spans="1:5" s="1" customFormat="1">
-      <c r="A202" s="60"/>
-      <c r="B202" s="60"/>
-      <c r="C202" s="60"/>
-      <c r="D202" s="61"/>
-      <c r="E202" s="63"/>
+      <c r="A202" s="59"/>
+      <c r="B202" s="59"/>
+      <c r="C202" s="59"/>
+      <c r="D202" s="60"/>
+      <c r="E202" s="62"/>
     </row>
     <row r="203" spans="1:5" s="1" customFormat="1">
-      <c r="A203" s="60"/>
-      <c r="B203" s="60"/>
-      <c r="C203" s="60"/>
-      <c r="D203" s="61"/>
-      <c r="E203" s="63"/>
+      <c r="A203" s="59"/>
+      <c r="B203" s="59"/>
+      <c r="C203" s="59"/>
+      <c r="D203" s="60"/>
+      <c r="E203" s="62"/>
     </row>
     <row r="204" spans="1:5" s="1" customFormat="1">
-      <c r="A204" s="60"/>
-      <c r="B204" s="60"/>
-      <c r="C204" s="60"/>
-      <c r="D204" s="61"/>
-      <c r="E204" s="63"/>
+      <c r="A204" s="59"/>
+      <c r="B204" s="59"/>
+      <c r="C204" s="59"/>
+      <c r="D204" s="60"/>
+      <c r="E204" s="62"/>
     </row>
     <row r="205" spans="1:5" s="1" customFormat="1">
-      <c r="A205" s="60"/>
-      <c r="B205" s="60"/>
-      <c r="C205" s="60"/>
-      <c r="D205" s="61"/>
-      <c r="E205" s="63"/>
+      <c r="A205" s="59"/>
+      <c r="B205" s="59"/>
+      <c r="C205" s="59"/>
+      <c r="D205" s="60"/>
+      <c r="E205" s="62"/>
     </row>
     <row r="206" spans="1:5" s="1" customFormat="1">
-      <c r="A206" s="60"/>
-      <c r="B206" s="60"/>
-      <c r="C206" s="60"/>
-      <c r="D206" s="61"/>
-      <c r="E206" s="63"/>
+      <c r="A206" s="59"/>
+      <c r="B206" s="59"/>
+      <c r="C206" s="59"/>
+      <c r="D206" s="60"/>
+      <c r="E206" s="62"/>
     </row>
     <row r="207" spans="1:5" s="1" customFormat="1">
-      <c r="A207" s="60"/>
-      <c r="B207" s="60"/>
-      <c r="C207" s="60"/>
-      <c r="D207" s="61"/>
-      <c r="E207" s="63"/>
+      <c r="A207" s="59"/>
+      <c r="B207" s="59"/>
+      <c r="C207" s="59"/>
+      <c r="D207" s="60"/>
+      <c r="E207" s="62"/>
     </row>
     <row r="208" spans="1:5" s="1" customFormat="1">
-      <c r="A208" s="60"/>
-      <c r="B208" s="60"/>
-      <c r="C208" s="60"/>
-      <c r="D208" s="61"/>
-      <c r="E208" s="63"/>
+      <c r="A208" s="59"/>
+      <c r="B208" s="59"/>
+      <c r="C208" s="59"/>
+      <c r="D208" s="60"/>
+      <c r="E208" s="62"/>
     </row>
     <row r="209" spans="1:5" s="1" customFormat="1">
-      <c r="A209" s="60"/>
-      <c r="B209" s="60"/>
-      <c r="C209" s="60"/>
-      <c r="D209" s="61"/>
-      <c r="E209" s="63"/>
+      <c r="A209" s="59"/>
+      <c r="B209" s="59"/>
+      <c r="C209" s="59"/>
+      <c r="D209" s="60"/>
+      <c r="E209" s="62"/>
     </row>
     <row r="210" spans="1:5" s="1" customFormat="1">
-      <c r="A210" s="60"/>
-      <c r="B210" s="60"/>
-      <c r="C210" s="60"/>
-      <c r="D210" s="61"/>
-      <c r="E210" s="63"/>
+      <c r="A210" s="59"/>
+      <c r="B210" s="59"/>
+      <c r="C210" s="59"/>
+      <c r="D210" s="60"/>
+      <c r="E210" s="62"/>
     </row>
     <row r="211" spans="1:5" s="1" customFormat="1">
-      <c r="A211" s="60"/>
-      <c r="B211" s="60"/>
-      <c r="C211" s="60"/>
-      <c r="D211" s="61"/>
-      <c r="E211" s="63"/>
+      <c r="A211" s="59"/>
+      <c r="B211" s="59"/>
+      <c r="C211" s="59"/>
+      <c r="D211" s="60"/>
+      <c r="E211" s="62"/>
     </row>
     <row r="212" spans="1:5" s="1" customFormat="1">
-      <c r="A212" s="60"/>
-      <c r="B212" s="60"/>
-      <c r="C212" s="60"/>
-      <c r="D212" s="61"/>
-      <c r="E212" s="63"/>
+      <c r="A212" s="59"/>
+      <c r="B212" s="59"/>
+      <c r="C212" s="59"/>
+      <c r="D212" s="60"/>
+      <c r="E212" s="62"/>
     </row>
     <row r="213" spans="1:5" s="1" customFormat="1">
-      <c r="A213" s="60"/>
-      <c r="B213" s="60"/>
-      <c r="C213" s="60"/>
-      <c r="D213" s="61"/>
-      <c r="E213" s="63"/>
+      <c r="A213" s="59"/>
+      <c r="B213" s="59"/>
+      <c r="C213" s="59"/>
+      <c r="D213" s="60"/>
+      <c r="E213" s="62"/>
     </row>
     <row r="214" spans="1:5" s="1" customFormat="1">
-      <c r="A214" s="60"/>
-      <c r="B214" s="60"/>
-      <c r="C214" s="60"/>
-      <c r="D214" s="61"/>
-      <c r="E214" s="63"/>
+      <c r="A214" s="59"/>
+      <c r="B214" s="59"/>
+      <c r="C214" s="59"/>
+      <c r="D214" s="60"/>
+      <c r="E214" s="62"/>
     </row>
     <row r="215" spans="1:5" s="1" customFormat="1">
-      <c r="A215" s="60"/>
-      <c r="B215" s="60"/>
-      <c r="C215" s="60"/>
-      <c r="D215" s="61"/>
-      <c r="E215" s="63"/>
+      <c r="A215" s="59"/>
+      <c r="B215" s="59"/>
+      <c r="C215" s="59"/>
+      <c r="D215" s="60"/>
+      <c r="E215" s="62"/>
     </row>
     <row r="216" spans="1:5" s="1" customFormat="1">
-      <c r="A216" s="60"/>
-      <c r="B216" s="60"/>
-      <c r="C216" s="60"/>
-      <c r="D216" s="61"/>
-      <c r="E216" s="63"/>
+      <c r="A216" s="59"/>
+      <c r="B216" s="59"/>
+      <c r="C216" s="59"/>
+      <c r="D216" s="60"/>
+      <c r="E216" s="62"/>
     </row>
     <row r="217" spans="1:5" s="1" customFormat="1">
-      <c r="A217" s="60"/>
-      <c r="B217" s="60"/>
-      <c r="C217" s="60"/>
-      <c r="D217" s="61"/>
-      <c r="E217" s="63"/>
+      <c r="A217" s="59"/>
+      <c r="B217" s="59"/>
+      <c r="C217" s="59"/>
+      <c r="D217" s="60"/>
+      <c r="E217" s="62"/>
     </row>
     <row r="218" spans="1:5" s="1" customFormat="1">
-      <c r="A218" s="60"/>
-      <c r="B218" s="60"/>
-      <c r="C218" s="60"/>
-      <c r="D218" s="61"/>
-      <c r="E218" s="63"/>
+      <c r="A218" s="59"/>
+      <c r="B218" s="59"/>
+      <c r="C218" s="59"/>
+      <c r="D218" s="60"/>
+      <c r="E218" s="62"/>
     </row>
     <row r="219" spans="1:5" s="1" customFormat="1">
-      <c r="A219" s="60"/>
-      <c r="B219" s="60"/>
-      <c r="C219" s="60"/>
-      <c r="D219" s="61"/>
-      <c r="E219" s="63"/>
+      <c r="A219" s="59"/>
+      <c r="B219" s="59"/>
+      <c r="C219" s="59"/>
+      <c r="D219" s="60"/>
+      <c r="E219" s="62"/>
     </row>
     <row r="220" spans="1:5" s="1" customFormat="1">
-      <c r="A220" s="60"/>
-      <c r="B220" s="60"/>
-      <c r="C220" s="60"/>
-      <c r="D220" s="61"/>
-      <c r="E220" s="63"/>
+      <c r="A220" s="59"/>
+      <c r="B220" s="59"/>
+      <c r="C220" s="59"/>
+      <c r="D220" s="60"/>
+      <c r="E220" s="62"/>
     </row>
     <row r="221" spans="1:5" s="1" customFormat="1">
-      <c r="A221" s="60"/>
-      <c r="B221" s="60"/>
-      <c r="C221" s="60"/>
-      <c r="D221" s="61"/>
-      <c r="E221" s="63"/>
+      <c r="A221" s="59"/>
+      <c r="B221" s="59"/>
+      <c r="C221" s="59"/>
+      <c r="D221" s="60"/>
+      <c r="E221" s="62"/>
     </row>
     <row r="222" spans="1:5" s="1" customFormat="1">
-      <c r="A222" s="60"/>
-      <c r="B222" s="60"/>
-      <c r="C222" s="60"/>
-      <c r="D222" s="61"/>
-      <c r="E222" s="63"/>
+      <c r="A222" s="59"/>
+      <c r="B222" s="59"/>
+      <c r="C222" s="59"/>
+      <c r="D222" s="60"/>
+      <c r="E222" s="62"/>
     </row>
     <row r="223" spans="1:5" s="1" customFormat="1">
-      <c r="A223" s="60"/>
-      <c r="B223" s="60"/>
-      <c r="C223" s="60"/>
-      <c r="D223" s="61"/>
-      <c r="E223" s="63"/>
+      <c r="A223" s="59"/>
+      <c r="B223" s="59"/>
+      <c r="C223" s="59"/>
+      <c r="D223" s="60"/>
+      <c r="E223" s="62"/>
     </row>
     <row r="224" spans="1:5" s="1" customFormat="1">
-      <c r="A224" s="60"/>
-      <c r="B224" s="60"/>
-      <c r="C224" s="60"/>
-      <c r="D224" s="61"/>
-      <c r="E224" s="63"/>
+      <c r="A224" s="59"/>
+      <c r="B224" s="59"/>
+      <c r="C224" s="59"/>
+      <c r="D224" s="60"/>
+      <c r="E224" s="62"/>
     </row>
     <row r="225" spans="1:5" s="1" customFormat="1">
-      <c r="A225" s="60"/>
-      <c r="B225" s="60"/>
-      <c r="C225" s="60"/>
-      <c r="D225" s="61"/>
-      <c r="E225" s="63"/>
+      <c r="A225" s="59"/>
+      <c r="B225" s="59"/>
+      <c r="C225" s="59"/>
+      <c r="D225" s="60"/>
+      <c r="E225" s="62"/>
     </row>
     <row r="226" spans="1:5" s="1" customFormat="1">
-      <c r="A226" s="60"/>
-      <c r="B226" s="60"/>
-      <c r="C226" s="60"/>
-      <c r="D226" s="61"/>
-      <c r="E226" s="63"/>
+      <c r="A226" s="59"/>
+      <c r="B226" s="59"/>
+      <c r="C226" s="59"/>
+      <c r="D226" s="60"/>
+      <c r="E226" s="62"/>
     </row>
     <row r="227" spans="1:5" s="1" customFormat="1">
-      <c r="A227" s="60"/>
-      <c r="B227" s="60"/>
-      <c r="C227" s="60"/>
-      <c r="D227" s="61"/>
-      <c r="E227" s="63"/>
+      <c r="A227" s="59"/>
+      <c r="B227" s="59"/>
+      <c r="C227" s="59"/>
+      <c r="D227" s="60"/>
+      <c r="E227" s="62"/>
     </row>
     <row r="228" spans="1:5" s="1" customFormat="1">
-      <c r="A228" s="60"/>
-      <c r="B228" s="60"/>
-      <c r="C228" s="60"/>
-      <c r="D228" s="61"/>
-      <c r="E228" s="63"/>
+      <c r="A228" s="59"/>
+      <c r="B228" s="59"/>
+      <c r="C228" s="59"/>
+      <c r="D228" s="60"/>
+      <c r="E228" s="62"/>
     </row>
     <row r="229" spans="1:5" s="1" customFormat="1">
-      <c r="A229" s="60"/>
-      <c r="B229" s="60"/>
-      <c r="C229" s="60"/>
-      <c r="D229" s="61"/>
-      <c r="E229" s="63"/>
+      <c r="A229" s="59"/>
+      <c r="B229" s="59"/>
+      <c r="C229" s="59"/>
+      <c r="D229" s="60"/>
+      <c r="E229" s="62"/>
     </row>
     <row r="230" spans="1:5" s="1" customFormat="1">
-      <c r="A230" s="60"/>
-      <c r="B230" s="60"/>
-      <c r="C230" s="60"/>
-      <c r="D230" s="61"/>
-      <c r="E230" s="63"/>
+      <c r="A230" s="59"/>
+      <c r="B230" s="59"/>
+      <c r="C230" s="59"/>
+      <c r="D230" s="60"/>
+      <c r="E230" s="62"/>
     </row>
     <row r="231" spans="1:5" s="1" customFormat="1">
-      <c r="A231" s="60"/>
-      <c r="B231" s="60"/>
-      <c r="C231" s="60"/>
-      <c r="D231" s="61"/>
-      <c r="E231" s="63"/>
+      <c r="A231" s="59"/>
+      <c r="B231" s="59"/>
+      <c r="C231" s="59"/>
+      <c r="D231" s="60"/>
+      <c r="E231" s="62"/>
     </row>
     <row r="232" spans="1:5" s="1" customFormat="1">
-      <c r="A232" s="60"/>
-      <c r="B232" s="60"/>
-      <c r="C232" s="60"/>
-      <c r="D232" s="61"/>
-      <c r="E232" s="63"/>
+      <c r="A232" s="59"/>
+      <c r="B232" s="59"/>
+      <c r="C232" s="59"/>
+      <c r="D232" s="60"/>
+      <c r="E232" s="62"/>
     </row>
     <row r="233" spans="1:5" s="1" customFormat="1">
-      <c r="A233" s="60"/>
-      <c r="B233" s="60"/>
-      <c r="C233" s="60"/>
-      <c r="D233" s="61"/>
-      <c r="E233" s="63"/>
+      <c r="A233" s="59"/>
+      <c r="B233" s="59"/>
+      <c r="C233" s="59"/>
+      <c r="D233" s="60"/>
+      <c r="E233" s="62"/>
     </row>
     <row r="234" spans="1:5" s="1" customFormat="1">
-      <c r="A234" s="60"/>
-      <c r="B234" s="60"/>
-      <c r="C234" s="60"/>
-      <c r="D234" s="61"/>
-      <c r="E234" s="63"/>
+      <c r="A234" s="59"/>
+      <c r="B234" s="59"/>
+      <c r="C234" s="59"/>
+      <c r="D234" s="60"/>
+      <c r="E234" s="62"/>
     </row>
     <row r="235" spans="1:5" s="1" customFormat="1">
-      <c r="A235" s="60"/>
-      <c r="B235" s="60"/>
-      <c r="C235" s="60"/>
-      <c r="D235" s="61"/>
-      <c r="E235" s="63"/>
+      <c r="A235" s="59"/>
+      <c r="B235" s="59"/>
+      <c r="C235" s="59"/>
+      <c r="D235" s="60"/>
+      <c r="E235" s="62"/>
     </row>
     <row r="236" spans="1:5" s="1" customFormat="1">
-      <c r="A236" s="60"/>
-      <c r="B236" s="60"/>
-      <c r="C236" s="60"/>
-      <c r="D236" s="61"/>
-      <c r="E236" s="63"/>
+      <c r="A236" s="59"/>
+      <c r="B236" s="59"/>
+      <c r="C236" s="59"/>
+      <c r="D236" s="60"/>
+      <c r="E236" s="62"/>
     </row>
     <row r="237" spans="1:5" s="1" customFormat="1">
-      <c r="A237" s="60"/>
-      <c r="B237" s="60"/>
-      <c r="C237" s="60"/>
-      <c r="D237" s="61"/>
-      <c r="E237" s="63"/>
+      <c r="A237" s="59"/>
+      <c r="B237" s="59"/>
+      <c r="C237" s="59"/>
+      <c r="D237" s="60"/>
+      <c r="E237" s="62"/>
     </row>
     <row r="238" spans="1:5" s="1" customFormat="1">
-      <c r="A238" s="60"/>
-      <c r="B238" s="60"/>
-      <c r="C238" s="60"/>
-      <c r="D238" s="61"/>
-      <c r="E238" s="63"/>
+      <c r="A238" s="59"/>
+      <c r="B238" s="59"/>
+      <c r="C238" s="59"/>
+      <c r="D238" s="60"/>
+      <c r="E238" s="62"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>

</xml_diff>

<commit_message>
Added the code to run the smart dashboard from disabledInit()
</commit_message>
<xml_diff>
--- a/Kilroy Equipment List 2016.xlsx
+++ b/Kilroy Equipment List 2016.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="10590" windowHeight="5790"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="14745" windowHeight="4860"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -13,11 +13,12 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$E$102</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="134">
   <si>
     <t>Code Written/Tested</t>
   </si>
@@ -413,6 +414,12 @@
   </si>
   <si>
     <t>Starboard Intake Motor (Victor)</t>
+  </si>
+  <si>
+    <t>armPot</t>
+  </si>
+  <si>
+    <t>Manipulator Arm Potentiometer - (range 360)</t>
   </si>
 </sst>
 </file>
@@ -1150,9 +1157,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H238"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -1708,9 +1715,15 @@
     <row r="51" spans="1:8" s="1" customFormat="1">
       <c r="A51" s="4"/>
       <c r="B51" s="4"/>
-      <c r="C51" s="29"/>
-      <c r="D51" s="32"/>
-      <c r="E51" s="33"/>
+      <c r="C51" s="57" t="s">
+        <v>133</v>
+      </c>
+      <c r="D51" s="32" t="s">
+        <v>132</v>
+      </c>
+      <c r="E51" s="33" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="52" spans="1:8" s="1" customFormat="1">
       <c r="A52" s="8"/>

</xml_diff>

<commit_message>
Fixed the equipment list.
</commit_message>
<xml_diff>
--- a/Kilroy Equipment List 2016.xlsx
+++ b/Kilroy Equipment List 2016.xlsx
@@ -1,3 +1,436 @@
+
+<file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+  <workbookPr/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="10590" windowHeight="5790"/>
+  </bookViews>
+  <sheets>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+  </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$E$102</definedName>
+  </definedNames>
+  <calcPr calcId="125725"/>
+</workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="137">
+  <si>
+    <t>Code Written/Tested</t>
+  </si>
+  <si>
+    <t>Part Wired</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Name in Code</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>Speed Controllers</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Digital Inputs (see also IR sensors)</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>Relays</t>
+  </si>
+  <si>
+    <t>Relay Port</t>
+  </si>
+  <si>
+    <t>Analog Inputs/Outputs</t>
+  </si>
+  <si>
+    <t>Analog Port</t>
+  </si>
+  <si>
+    <t>Double Solenoids</t>
+  </si>
+  <si>
+    <t>Joysticks</t>
+  </si>
+  <si>
+    <t>USB Port</t>
+  </si>
+  <si>
+    <t>Operator Controls</t>
+  </si>
+  <si>
+    <t>Button</t>
+  </si>
+  <si>
+    <t>Driver Station</t>
+  </si>
+  <si>
+    <t>driverStation</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Miscellaneous</t>
+  </si>
+  <si>
+    <t>Axis Camera</t>
+  </si>
+  <si>
+    <t>The entire driver station.</t>
+  </si>
+  <si>
+    <t>10.3.39.11</t>
+  </si>
+  <si>
+    <t>IR Sensor/Red Light Sensors (see also Digital Inputs)</t>
+  </si>
+  <si>
+    <t>IP Address</t>
+  </si>
+  <si>
+    <t>Classmate/Toshiba</t>
+  </si>
+  <si>
+    <t>DIO Port</t>
+  </si>
+  <si>
+    <t>CAN Port</t>
+  </si>
+  <si>
+    <t>PDB (Power Distribution Board)</t>
+  </si>
+  <si>
+    <t>roboRIO</t>
+  </si>
+  <si>
+    <t>roboRIO-339.local</t>
+  </si>
+  <si>
+    <t>dns</t>
+  </si>
+  <si>
+    <t>10.3.39.1</t>
+  </si>
+  <si>
+    <t>Kilroy-Laptops</t>
+  </si>
+  <si>
+    <t>Transmission</t>
+  </si>
+  <si>
+    <t>transmission</t>
+  </si>
+  <si>
+    <t>Timer</t>
+  </si>
+  <si>
+    <t>kilroyTimer</t>
+  </si>
+  <si>
+    <t>Kilroy Equipment List (2016)</t>
+  </si>
+  <si>
+    <t>PWM Port / CAN ID</t>
+  </si>
+  <si>
+    <t>rightRearMotor</t>
+  </si>
+  <si>
+    <t>leftRearMotor</t>
+  </si>
+  <si>
+    <t>rightFrontMotor</t>
+  </si>
+  <si>
+    <t>leftFrontMotor</t>
+  </si>
+  <si>
+    <t>leftRearEncoder</t>
+  </si>
+  <si>
+    <t>0, 1</t>
+  </si>
+  <si>
+    <t>Left Rear Encoder</t>
+  </si>
+  <si>
+    <t>rightRearEncoder</t>
+  </si>
+  <si>
+    <t>2, 3</t>
+  </si>
+  <si>
+    <t>Right Rear Encoder</t>
+  </si>
+  <si>
+    <t>USB Camera</t>
+  </si>
+  <si>
+    <t>cameraServer(cam0)</t>
+  </si>
+  <si>
+    <t>axisCamera</t>
+  </si>
+  <si>
+    <t>Disable Autonomous Switch</t>
+  </si>
+  <si>
+    <t>autonomousEnabled</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>delayPot</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Delay Potentiometer - (range 270)</t>
+  </si>
+  <si>
+    <t>Left Front IR sensor</t>
+  </si>
+  <si>
+    <t>leftIR</t>
+  </si>
+  <si>
+    <t>Right Front IR sensor</t>
+  </si>
+  <si>
+    <t>rightIR</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>Left drivers joystick</t>
+  </si>
+  <si>
+    <t>leftDriver</t>
+  </si>
+  <si>
+    <t>Right drivers joystick</t>
+  </si>
+  <si>
+    <t>rightDriver</t>
+  </si>
+  <si>
+    <t>Left Operators joystick</t>
+  </si>
+  <si>
+    <t>leftOperator</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>Right Operator's joystick</t>
+  </si>
+  <si>
+    <t>rightOperator</t>
+  </si>
+  <si>
+    <t>Open Mesh</t>
+  </si>
+  <si>
+    <t>Error Message</t>
+  </si>
+  <si>
+    <t>errorMessage</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>Ring Light Relay</t>
+  </si>
+  <si>
+    <t>ringLightRelay</t>
+  </si>
+  <si>
+    <t>Six Position Switch</t>
+  </si>
+  <si>
+    <t>sixPositionDial</t>
+  </si>
+  <si>
+    <t>14,15,16,17,18,21</t>
+  </si>
+  <si>
+    <t>Transducer - (range 130)</t>
+  </si>
+  <si>
+    <t>transducer</t>
+  </si>
+  <si>
+    <t>Double Solenoid</t>
+  </si>
+  <si>
+    <t>cameraSolenoid</t>
+  </si>
+  <si>
+    <t>PCM Port</t>
+  </si>
+  <si>
+    <t>3,4</t>
+  </si>
+  <si>
+    <t>Single Solenoid</t>
+  </si>
+  <si>
+    <t>catapultSolenoid0</t>
+  </si>
+  <si>
+    <t>catapultSolenoid1</t>
+  </si>
+  <si>
+    <t>catapultSolenoid2</t>
+  </si>
+  <si>
+    <t>Shoot High</t>
+  </si>
+  <si>
+    <t>Shoot Low</t>
+  </si>
+  <si>
+    <t>shootHigh</t>
+  </si>
+  <si>
+    <t>shootLow</t>
+  </si>
+  <si>
+    <t>armMotor</t>
+  </si>
+  <si>
+    <t>PWM 0</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>Arm Encoder</t>
+  </si>
+  <si>
+    <t>armEncoder</t>
+  </si>
+  <si>
+    <t>4, 5</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>PWM 2</t>
+  </si>
+  <si>
+    <t>PWM 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> PWM 1</t>
+  </si>
+  <si>
+    <t>PWM 4</t>
+  </si>
+  <si>
+    <t>Upshift button</t>
+  </si>
+  <si>
+    <t>Downshift button</t>
+  </si>
+  <si>
+    <t>GEAR_DOWNSHIFT_JOYSTICK_BUTTON</t>
+  </si>
+  <si>
+    <t>GEAR_UPSHIFT_JOYSTICK_BUTTON</t>
+  </si>
+  <si>
+    <t>Take Lit image</t>
+  </si>
+  <si>
+    <t>Take unlit image</t>
+  </si>
+  <si>
+    <t>starboardArmIntakeMotor</t>
+  </si>
+  <si>
+    <t>PWM 6</t>
+  </si>
+  <si>
+    <t>PWM 5</t>
+  </si>
+  <si>
+    <t>Left Operator 6+7</t>
+  </si>
+  <si>
+    <t>Left Operator10+11</t>
+  </si>
+  <si>
+    <t>Right Driver 3</t>
+  </si>
+  <si>
+    <t>Right Driver 2</t>
+  </si>
+  <si>
+    <t>Arm Motor Controller (Victor)</t>
+  </si>
+  <si>
+    <t>Left Front Motor Controller (Talon)</t>
+  </si>
+  <si>
+    <t>Right Front Motor Controller (Talon)</t>
+  </si>
+  <si>
+    <t>Left Rear Motor Controller (Talon)</t>
+  </si>
+  <si>
+    <t>Right Rear Motor Controller (Talon)</t>
+  </si>
+  <si>
+    <t>Starboard Intake Motor (Victor)</t>
+  </si>
+  <si>
+    <t>NOT ADDED YET</t>
+  </si>
+  <si>
+    <t>Arm Red light sensor</t>
+  </si>
+  <si>
+    <t>Arm potentiometer</t>
+  </si>
+  <si>
+    <t>armPositionPot</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>Intake Motor (Victor)</t>
+  </si>
+  <si>
+    <t>armIntakeMotor</t>
+  </si>
+</sst>
+</file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
@@ -394,6 +827,352 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults>
+    <a:spDef>
+      <a:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="1" cy="1"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </a:spPr>
+      <a:bodyPr vertOverflow="clip" wrap="square" lIns="18288" tIns="0" rIns="0" bIns="0" upright="1"/>
+      <a:lstStyle/>
+    </a:spDef>
+    <a:lnDef>
+      <a:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="1" cy="1"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </a:spPr>
+      <a:bodyPr vertOverflow="clip" wrap="square" lIns="18288" tIns="0" rIns="0" bIns="0" upright="1"/>
+      <a:lstStyle/>
+    </a:lnDef>
+  </a:objectDefaults>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H238"/>

</xml_diff>

<commit_message>
Did some testing on Auto. Fixed arm down code. Fixed armPot Stuff.
</commit_message>
<xml_diff>
--- a/Kilroy Equipment List 2016.xlsx
+++ b/Kilroy Equipment List 2016.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4506"/>
   <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2520" windowWidth="10590" windowHeight="5790"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="136">
   <si>
     <t>Code Written/Tested</t>
   </si>
@@ -419,9 +419,6 @@
   </si>
   <si>
     <t>armPositionPot</t>
-  </si>
-  <si>
-    <t>4</t>
   </si>
   <si>
     <t>Intake Motor (Victor)</t>
@@ -786,6 +783,21 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -794,21 +806,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1178,8 +1175,8 @@
   <dimension ref="A1:H238"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
+      <pane ySplit="2" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -1196,13 +1193,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1">
-      <c r="A1" s="67" t="s">
+      <c r="A1" s="72" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="67"/>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
     </row>
     <row r="2" spans="1:8" s="1" customFormat="1" ht="25.5">
       <c r="A2" s="13" t="s">
@@ -1224,10 +1221,10 @@
     <row r="3" spans="1:8" s="1" customFormat="1" ht="13.15" customHeight="1">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
-      <c r="C3" s="66" t="s">
+      <c r="C3" s="71" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="66"/>
+      <c r="D3" s="71"/>
       <c r="E3" s="3" t="s">
         <v>41</v>
       </c>
@@ -1303,13 +1300,13 @@
     <row r="9" spans="1:8" s="1" customFormat="1" ht="25.5">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
-      <c r="C9" s="73" t="s">
+      <c r="C9" s="70" t="s">
         <v>129</v>
       </c>
-      <c r="D9" s="70" t="s">
+      <c r="D9" s="67" t="s">
         <v>117</v>
       </c>
-      <c r="E9" s="71" t="s">
+      <c r="E9" s="68" t="s">
         <v>118</v>
       </c>
       <c r="F9" s="12"/>
@@ -1320,10 +1317,10 @@
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="C10" s="25" t="s">
+        <v>134</v>
+      </c>
+      <c r="D10" s="26" t="s">
         <v>135</v>
-      </c>
-      <c r="D10" s="26" t="s">
-        <v>136</v>
       </c>
       <c r="E10" s="27" t="s">
         <v>119</v>
@@ -1349,10 +1346,10 @@
     <row r="13" spans="1:8" s="1" customFormat="1" ht="13.15" customHeight="1">
       <c r="A13" s="17"/>
       <c r="B13" s="17"/>
-      <c r="C13" s="68" t="s">
+      <c r="C13" s="73" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="68"/>
+      <c r="D13" s="73"/>
       <c r="E13" s="58" t="s">
         <v>28</v>
       </c>
@@ -1480,10 +1477,10 @@
     <row r="26" spans="1:8" s="1" customFormat="1" ht="13.35" customHeight="1">
       <c r="A26" s="17"/>
       <c r="B26" s="17"/>
-      <c r="C26" s="66" t="s">
+      <c r="C26" s="71" t="s">
         <v>7</v>
       </c>
-      <c r="D26" s="66"/>
+      <c r="D26" s="71"/>
       <c r="E26" s="3" t="s">
         <v>28</v>
       </c>
@@ -1583,13 +1580,13 @@
     <row r="35" spans="1:5" s="1" customFormat="1">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
-      <c r="C35" s="69" t="s">
+      <c r="C35" s="66" t="s">
         <v>103</v>
       </c>
-      <c r="D35" s="70" t="s">
+      <c r="D35" s="67" t="s">
         <v>104</v>
       </c>
-      <c r="E35" s="71" t="s">
+      <c r="E35" s="68" t="s">
         <v>105</v>
       </c>
     </row>
@@ -1599,7 +1596,7 @@
       <c r="C36" s="25" t="s">
         <v>131</v>
       </c>
-      <c r="D36" s="72" t="s">
+      <c r="D36" s="69" t="s">
         <v>130</v>
       </c>
       <c r="E36" s="55"/>
@@ -1649,10 +1646,10 @@
     <row r="43" spans="1:5" s="1" customFormat="1" ht="13.15" customHeight="1">
       <c r="A43" s="17"/>
       <c r="B43" s="17"/>
-      <c r="C43" s="66" t="s">
+      <c r="C43" s="71" t="s">
         <v>9</v>
       </c>
-      <c r="D43" s="66"/>
+      <c r="D43" s="71"/>
       <c r="E43" s="3" t="s">
         <v>10</v>
       </c>
@@ -1702,10 +1699,10 @@
     <row r="48" spans="1:5" s="1" customFormat="1" ht="13.15" customHeight="1">
       <c r="A48" s="17"/>
       <c r="B48" s="17"/>
-      <c r="C48" s="66" t="s">
+      <c r="C48" s="71" t="s">
         <v>11</v>
       </c>
-      <c r="D48" s="66"/>
+      <c r="D48" s="71"/>
       <c r="E48" s="3" t="s">
         <v>12</v>
       </c>
@@ -1746,7 +1743,7 @@
         <v>133</v>
       </c>
       <c r="E51" s="32" t="s">
-        <v>134</v>
+        <v>59</v>
       </c>
     </row>
     <row r="52" spans="1:8" s="1" customFormat="1">
@@ -1773,10 +1770,10 @@
     <row r="55" spans="1:8" s="1" customFormat="1" ht="13.35" customHeight="1">
       <c r="A55" s="17"/>
       <c r="B55" s="17"/>
-      <c r="C55" s="66" t="s">
+      <c r="C55" s="71" t="s">
         <v>13</v>
       </c>
-      <c r="D55" s="66"/>
+      <c r="D55" s="71"/>
       <c r="E55" s="3" t="s">
         <v>90</v>
       </c>
@@ -1845,10 +1842,10 @@
     <row r="61" spans="1:8" s="1" customFormat="1" ht="13.35" customHeight="1">
       <c r="A61" s="17"/>
       <c r="B61" s="17"/>
-      <c r="C61" s="66" t="s">
+      <c r="C61" s="71" t="s">
         <v>30</v>
       </c>
-      <c r="D61" s="66"/>
+      <c r="D61" s="71"/>
       <c r="E61" s="3" t="s">
         <v>29</v>
       </c>
@@ -1886,10 +1883,10 @@
     <row r="66" spans="1:8" s="1" customFormat="1" ht="13.35" customHeight="1">
       <c r="A66" s="17"/>
       <c r="B66" s="17"/>
-      <c r="C66" s="66" t="s">
+      <c r="C66" s="71" t="s">
         <v>14</v>
       </c>
-      <c r="D66" s="66"/>
+      <c r="D66" s="71"/>
       <c r="E66" s="3" t="s">
         <v>15</v>
       </c>
@@ -1954,10 +1951,10 @@
     <row r="71" spans="1:8" s="1" customFormat="1" ht="13.35" customHeight="1">
       <c r="A71" s="17"/>
       <c r="B71" s="17"/>
-      <c r="C71" s="66" t="s">
+      <c r="C71" s="71" t="s">
         <v>16</v>
       </c>
-      <c r="D71" s="66"/>
+      <c r="D71" s="71"/>
       <c r="E71" s="3" t="s">
         <v>17</v>
       </c>
@@ -2133,10 +2130,10 @@
     <row r="92" spans="1:7" s="1" customFormat="1" ht="13.35" customHeight="1">
       <c r="A92" s="17"/>
       <c r="B92" s="17"/>
-      <c r="C92" s="66" t="s">
+      <c r="C92" s="71" t="s">
         <v>18</v>
       </c>
-      <c r="D92" s="66"/>
+      <c r="D92" s="71"/>
       <c r="E92" s="3" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
Moved ports to match Kam's request
</commit_message>
<xml_diff>
--- a/Kilroy Equipment List 2016.xlsx
+++ b/Kilroy Equipment List 2016.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2520" windowWidth="10590" windowHeight="5790"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="134">
   <si>
     <t>Code Written/Tested</t>
   </si>
@@ -160,18 +160,12 @@
     <t>leftRearEncoder</t>
   </si>
   <si>
-    <t>0, 1</t>
-  </si>
-  <si>
     <t>Left Rear Encoder</t>
   </si>
   <si>
     <t>rightRearEncoder</t>
   </si>
   <si>
-    <t>2, 3</t>
-  </si>
-  <si>
     <t>Right Rear Encoder</t>
   </si>
   <si>
@@ -256,12 +250,6 @@
     <t>errorMessage</t>
   </si>
   <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>22</t>
-  </si>
-  <si>
     <t>Ring Light Relay</t>
   </si>
   <si>
@@ -409,12 +397,6 @@
     <t>Starboard Intake Motor (Victor)</t>
   </si>
   <si>
-    <t>NOT ADDED YET</t>
-  </si>
-  <si>
-    <t>Arm Red light sensor</t>
-  </si>
-  <si>
     <t>Arm potentiometer</t>
   </si>
   <si>
@@ -425,6 +407,18 @@
   </si>
   <si>
     <t>armIntakeMotor</t>
+  </si>
+  <si>
+    <t>Arm IR sensor</t>
+  </si>
+  <si>
+    <t>3, 4</t>
+  </si>
+  <si>
+    <t>5, 6</t>
+  </si>
+  <si>
+    <t>armIR</t>
   </si>
 </sst>
 </file>
@@ -1175,15 +1169,15 @@
   <dimension ref="A1:H238"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E51" sqref="E51"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="14.7109375" style="59" customWidth="1"/>
     <col min="2" max="2" width="14.5703125" style="59" customWidth="1"/>
-    <col min="3" max="3" width="70.5703125" style="59" customWidth="1"/>
+    <col min="3" max="3" width="50.7109375" style="59" customWidth="1"/>
     <col min="4" max="4" width="21" style="60" customWidth="1"/>
     <col min="5" max="5" width="18.140625" style="62" customWidth="1"/>
     <col min="6" max="6" width="20.28515625" style="59" customWidth="1"/>
@@ -1233,65 +1227,65 @@
       <c r="A4" s="63"/>
       <c r="B4" s="63"/>
       <c r="C4" s="29" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="D4" s="30" t="s">
         <v>42</v>
       </c>
       <c r="E4" s="49" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="1" customFormat="1" ht="12.75" customHeight="1">
       <c r="A5" s="64"/>
       <c r="B5" s="64"/>
       <c r="C5" s="28" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>43</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="1" customFormat="1" ht="12.75" customHeight="1">
       <c r="A6" s="8"/>
       <c r="B6" s="8"/>
       <c r="C6" s="25" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="D6" s="26" t="s">
         <v>44</v>
       </c>
       <c r="E6" s="27" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="34" customFormat="1">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="28" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>45</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="1" customFormat="1">
       <c r="A8" s="33"/>
       <c r="B8" s="33"/>
       <c r="C8" s="48" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="D8" s="65" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E8" s="50" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F8" s="12"/>
       <c r="G8" s="12"/>
@@ -1301,13 +1295,13 @@
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="70" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D9" s="67" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E9" s="68" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="F9" s="12"/>
       <c r="G9" s="12"/>
@@ -1317,13 +1311,13 @@
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="C10" s="25" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="D10" s="26" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="E10" s="27" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="F10" s="12"/>
       <c r="G10" s="12"/>
@@ -1358,34 +1352,40 @@
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="28" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D14" s="31" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:8" s="1" customFormat="1">
       <c r="A15" s="51"/>
       <c r="B15" s="51"/>
       <c r="C15" s="25" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D15" s="26" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E15" s="43" t="s">
-        <v>80</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:8" s="1" customFormat="1">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
-      <c r="C16" s="28"/>
-      <c r="D16" s="31"/>
-      <c r="E16" s="32"/>
+      <c r="C16" s="28" t="s">
+        <v>130</v>
+      </c>
+      <c r="D16" s="31" t="s">
+        <v>133</v>
+      </c>
+      <c r="E16" s="32" t="s">
+        <v>71</v>
+      </c>
       <c r="F16" s="12"/>
       <c r="G16" s="12"/>
       <c r="H16" s="12"/>
@@ -1503,102 +1503,98 @@
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="28" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D29" s="31" t="s">
         <v>46</v>
       </c>
       <c r="E29" s="32" t="s">
-        <v>47</v>
+        <v>132</v>
       </c>
     </row>
     <row r="30" spans="1:8" s="1" customFormat="1">
       <c r="A30" s="13"/>
       <c r="B30" s="13"/>
       <c r="C30" s="22" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D30" s="44" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E30" s="43" t="s">
-        <v>50</v>
+        <v>131</v>
       </c>
     </row>
     <row r="31" spans="1:8" s="1" customFormat="1">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="D31" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="E31" s="32" t="s">
         <v>55</v>
-      </c>
-      <c r="D31" s="31" t="s">
-        <v>56</v>
-      </c>
-      <c r="E31" s="32" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="32" spans="1:8" s="1" customFormat="1">
       <c r="A32" s="13"/>
       <c r="B32" s="13"/>
       <c r="C32" s="22" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D32" s="44" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E32" s="43" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="33" spans="1:5" s="1" customFormat="1">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="28" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D33" s="31" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E33" s="32" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="34" spans="1:5" s="1" customFormat="1">
       <c r="A34" s="13"/>
       <c r="B34" s="13"/>
       <c r="C34" s="22" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D34" s="44" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E34" s="43" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="35" spans="1:5" s="1" customFormat="1">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="66" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D35" s="67" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="E35" s="68" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="36" spans="1:5" s="1" customFormat="1">
       <c r="A36" s="8"/>
       <c r="B36" s="8"/>
-      <c r="C36" s="25" t="s">
-        <v>131</v>
-      </c>
-      <c r="D36" s="69" t="s">
-        <v>130</v>
-      </c>
+      <c r="C36" s="25"/>
+      <c r="D36" s="69"/>
       <c r="E36" s="55"/>
     </row>
     <row r="37" spans="1:5" s="1" customFormat="1">
@@ -1669,10 +1665,10 @@
       <c r="A45" s="40"/>
       <c r="B45" s="14"/>
       <c r="C45" s="41" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D45" s="44" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E45" s="14">
         <v>0</v>
@@ -1711,39 +1707,39 @@
       <c r="A49" s="19"/>
       <c r="B49" s="19"/>
       <c r="C49" s="45" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D49" s="24" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E49" s="46" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="50" spans="1:8" s="1" customFormat="1">
       <c r="A50" s="8"/>
       <c r="B50" s="8"/>
       <c r="C50" s="25" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D50" s="26" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E50" s="27" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="51" spans="1:8" s="1" customFormat="1">
       <c r="A51" s="4"/>
       <c r="B51" s="4"/>
       <c r="C51" s="28" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="D51" s="31" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="E51" s="32" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="52" spans="1:8" s="1" customFormat="1">
@@ -1775,59 +1771,59 @@
       </c>
       <c r="D55" s="71"/>
       <c r="E55" s="3" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="56" spans="1:8" s="1" customFormat="1">
       <c r="A56" s="19"/>
       <c r="B56" s="19"/>
       <c r="C56" s="45" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D56" s="24" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E56" s="32" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="57" spans="1:8" s="1" customFormat="1">
       <c r="A57" s="8"/>
       <c r="B57" s="8"/>
       <c r="C57" s="25" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D57" s="26" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E57" s="27" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="58" spans="1:8" s="1" customFormat="1">
       <c r="A58" s="4"/>
       <c r="B58" s="4"/>
       <c r="C58" s="28" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D58" s="31" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E58" s="32" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="59" spans="1:8" s="1" customFormat="1">
       <c r="A59" s="8"/>
       <c r="B59" s="8"/>
       <c r="C59" s="25" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D59" s="26" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E59" s="27" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="60" spans="1:8" s="35" customFormat="1" ht="13.15" customHeight="1">
@@ -1896,13 +1892,13 @@
       <c r="A67" s="8"/>
       <c r="B67" s="8"/>
       <c r="C67" s="25" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D67" s="26" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E67" s="27" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G67" s="20"/>
     </row>
@@ -1910,13 +1906,13 @@
       <c r="A68" s="4"/>
       <c r="B68" s="4"/>
       <c r="C68" s="28" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D68" s="31" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E68" s="32" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G68" s="20"/>
     </row>
@@ -1924,13 +1920,13 @@
       <c r="A69" s="8"/>
       <c r="B69" s="8"/>
       <c r="C69" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="D69" s="44" t="s">
+        <v>70</v>
+      </c>
+      <c r="E69" s="43" t="s">
         <v>71</v>
-      </c>
-      <c r="D69" s="44" t="s">
-        <v>72</v>
-      </c>
-      <c r="E69" s="43" t="s">
-        <v>73</v>
       </c>
       <c r="G69" s="20"/>
     </row>
@@ -1938,13 +1934,13 @@
       <c r="A70" s="4"/>
       <c r="B70" s="4"/>
       <c r="C70" s="28" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D70" s="31" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E70" s="32" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G70" s="20"/>
     </row>
@@ -1964,48 +1960,48 @@
       <c r="A72" s="8"/>
       <c r="B72" s="8"/>
       <c r="C72" s="23" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D72" s="26" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="E72" s="25" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="73" spans="1:8" s="35" customFormat="1" ht="25.5">
       <c r="A73" s="4"/>
       <c r="B73" s="4"/>
       <c r="C73" s="28" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D73" s="31" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="E73" s="32" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="74" spans="1:8" s="1" customFormat="1">
       <c r="A74" s="47"/>
       <c r="B74" s="47"/>
       <c r="C74" s="22" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D74" s="22"/>
       <c r="E74" s="22" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="75" spans="1:8" s="1" customFormat="1">
       <c r="A75" s="4"/>
       <c r="B75" s="4"/>
       <c r="C75" s="32" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="D75" s="31"/>
       <c r="E75" s="32" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="76" spans="1:8" s="1" customFormat="1">
@@ -2234,7 +2230,7 @@
         <v>22</v>
       </c>
       <c r="D104" s="26" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E104" s="43" t="s">
         <v>24</v>
@@ -2257,10 +2253,10 @@
       <c r="A106" s="13"/>
       <c r="B106" s="13"/>
       <c r="C106" s="25" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D106" s="26" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E106" s="43" t="s">
         <v>20</v>
@@ -2296,7 +2292,7 @@
       <c r="A109" s="4"/>
       <c r="B109" s="4"/>
       <c r="C109" s="28" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D109" s="6" t="s">
         <v>8</v>
@@ -2335,10 +2331,10 @@
       <c r="A112" s="13"/>
       <c r="B112" s="13"/>
       <c r="C112" s="22" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D112" s="44" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E112" s="22" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
Switched the ports on the armPot and the delayPot since they were backwards; also fixed the max value for the armPot from 360 to 270.
</commit_message>
<xml_diff>
--- a/Kilroy Equipment List 2016.xlsx
+++ b/Kilroy Equipment List 2016.xlsx
@@ -1169,8 +1169,8 @@
   <dimension ref="A1:H238"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C1:C1048576"/>
+      <pane ySplit="2" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -1713,7 +1713,7 @@
         <v>56</v>
       </c>
       <c r="E49" s="46" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
     </row>
     <row r="50" spans="1:8" s="1" customFormat="1">
@@ -1739,7 +1739,7 @@
         <v>127</v>
       </c>
       <c r="E51" s="32" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
     </row>
     <row r="52" spans="1:8" s="1" customFormat="1">

</xml_diff>

<commit_message>
Changed something in Kilroy Equipment, don't remember what.
</commit_message>
<xml_diff>
--- a/Kilroy Equipment List 2016.xlsx
+++ b/Kilroy Equipment List 2016.xlsx
@@ -265,9 +265,6 @@
     <t>14,15,16,17,18,21</t>
   </si>
   <si>
-    <t>Transducer - (range 130)</t>
-  </si>
-  <si>
     <t>transducer</t>
   </si>
   <si>
@@ -419,6 +416,9 @@
   </si>
   <si>
     <t>armIR</t>
+  </si>
+  <si>
+    <t>Transducer - (range 200)</t>
   </si>
 </sst>
 </file>
@@ -1169,8 +1169,8 @@
   <dimension ref="A1:H238"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E52" sqref="E52"/>
+      <pane ySplit="2" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -1227,65 +1227,65 @@
       <c r="A4" s="63"/>
       <c r="B4" s="63"/>
       <c r="C4" s="29" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D4" s="30" t="s">
         <v>42</v>
       </c>
       <c r="E4" s="49" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="1" customFormat="1" ht="12.75" customHeight="1">
       <c r="A5" s="64"/>
       <c r="B5" s="64"/>
       <c r="C5" s="28" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>43</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="1" customFormat="1" ht="12.75" customHeight="1">
       <c r="A6" s="8"/>
       <c r="B6" s="8"/>
       <c r="C6" s="25" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D6" s="26" t="s">
         <v>44</v>
       </c>
       <c r="E6" s="27" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="34" customFormat="1">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="28" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>45</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="1" customFormat="1">
       <c r="A8" s="33"/>
       <c r="B8" s="33"/>
       <c r="C8" s="48" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D8" s="65" t="s">
+        <v>95</v>
+      </c>
+      <c r="E8" s="50" t="s">
         <v>96</v>
-      </c>
-      <c r="E8" s="50" t="s">
-        <v>97</v>
       </c>
       <c r="F8" s="12"/>
       <c r="G8" s="12"/>
@@ -1295,13 +1295,13 @@
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="70" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D9" s="67" t="s">
+        <v>112</v>
+      </c>
+      <c r="E9" s="68" t="s">
         <v>113</v>
-      </c>
-      <c r="E9" s="68" t="s">
-        <v>114</v>
       </c>
       <c r="F9" s="12"/>
       <c r="G9" s="12"/>
@@ -1311,13 +1311,13 @@
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="C10" s="25" t="s">
+        <v>127</v>
+      </c>
+      <c r="D10" s="26" t="s">
         <v>128</v>
       </c>
-      <c r="D10" s="26" t="s">
-        <v>129</v>
-      </c>
       <c r="E10" s="27" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F10" s="12"/>
       <c r="G10" s="12"/>
@@ -1378,10 +1378,10 @@
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="28" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E16" s="32" t="s">
         <v>71</v>
@@ -1509,7 +1509,7 @@
         <v>46</v>
       </c>
       <c r="E29" s="32" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="30" spans="1:8" s="1" customFormat="1">
@@ -1522,7 +1522,7 @@
         <v>48</v>
       </c>
       <c r="E30" s="43" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="31" spans="1:8" s="1" customFormat="1">
@@ -1555,39 +1555,39 @@
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="28" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D33" s="31" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E33" s="32" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="34" spans="1:5" s="1" customFormat="1">
       <c r="A34" s="13"/>
       <c r="B34" s="13"/>
       <c r="C34" s="22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D34" s="44" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E34" s="43" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="35" spans="1:5" s="1" customFormat="1">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="66" t="s">
+        <v>98</v>
+      </c>
+      <c r="D35" s="67" t="s">
         <v>99</v>
       </c>
-      <c r="D35" s="67" t="s">
+      <c r="E35" s="68" t="s">
         <v>100</v>
-      </c>
-      <c r="E35" s="68" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="36" spans="1:5" s="1" customFormat="1">
@@ -1720,10 +1720,10 @@
       <c r="A50" s="8"/>
       <c r="B50" s="8"/>
       <c r="C50" s="25" t="s">
+        <v>133</v>
+      </c>
+      <c r="D50" s="26" t="s">
         <v>82</v>
-      </c>
-      <c r="D50" s="26" t="s">
-        <v>83</v>
       </c>
       <c r="E50" s="27" t="s">
         <v>71</v>
@@ -1733,10 +1733,10 @@
       <c r="A51" s="4"/>
       <c r="B51" s="4"/>
       <c r="C51" s="28" t="s">
+        <v>125</v>
+      </c>
+      <c r="D51" s="31" t="s">
         <v>126</v>
-      </c>
-      <c r="D51" s="31" t="s">
-        <v>127</v>
       </c>
       <c r="E51" s="32" t="s">
         <v>64</v>
@@ -1771,30 +1771,30 @@
       </c>
       <c r="D55" s="71"/>
       <c r="E55" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="56" spans="1:8" s="1" customFormat="1">
       <c r="A56" s="19"/>
       <c r="B56" s="19"/>
       <c r="C56" s="45" t="s">
+        <v>83</v>
+      </c>
+      <c r="D56" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="D56" s="24" t="s">
-        <v>85</v>
-      </c>
       <c r="E56" s="32" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="57" spans="1:8" s="1" customFormat="1">
       <c r="A57" s="8"/>
       <c r="B57" s="8"/>
       <c r="C57" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="D57" s="26" t="s">
         <v>88</v>
-      </c>
-      <c r="D57" s="26" t="s">
-        <v>89</v>
       </c>
       <c r="E57" s="27" t="s">
         <v>63</v>
@@ -1804,10 +1804,10 @@
       <c r="A58" s="4"/>
       <c r="B58" s="4"/>
       <c r="C58" s="28" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D58" s="31" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E58" s="32" t="s">
         <v>57</v>
@@ -1817,10 +1817,10 @@
       <c r="A59" s="8"/>
       <c r="B59" s="8"/>
       <c r="C59" s="25" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D59" s="26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E59" s="27" t="s">
         <v>71</v>
@@ -1960,48 +1960,48 @@
       <c r="A72" s="8"/>
       <c r="B72" s="8"/>
       <c r="C72" s="23" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D72" s="26" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E72" s="25" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="73" spans="1:8" s="35" customFormat="1" ht="25.5">
       <c r="A73" s="4"/>
       <c r="B73" s="4"/>
       <c r="C73" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="D73" s="31" t="s">
         <v>108</v>
       </c>
-      <c r="D73" s="31" t="s">
-        <v>109</v>
-      </c>
       <c r="E73" s="32" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="74" spans="1:8" s="1" customFormat="1">
       <c r="A74" s="47"/>
       <c r="B74" s="47"/>
       <c r="C74" s="22" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D74" s="22"/>
       <c r="E74" s="22" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="75" spans="1:8" s="1" customFormat="1">
       <c r="A75" s="4"/>
       <c r="B75" s="4"/>
       <c r="C75" s="32" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D75" s="31"/>
       <c r="E75" s="32" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="76" spans="1:8" s="1" customFormat="1">

</xml_diff>

<commit_message>
cleaned up some code in teleop
</commit_message>
<xml_diff>
--- a/Kilroy Equipment List 2016.xlsx
+++ b/Kilroy Equipment List 2016.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="151">
   <si>
     <t>Code Written/Tested</t>
   </si>
@@ -419,6 +419,57 @@
   </si>
   <si>
     <t>Transducer - (range 200)</t>
+  </si>
+  <si>
+    <t>Right Operator 4</t>
+  </si>
+  <si>
+    <t>Pick up ball button - until IR sensor stops it</t>
+  </si>
+  <si>
+    <t>Right Operator 5</t>
+  </si>
+  <si>
+    <t>Push out ball from pickup mechanism</t>
+  </si>
+  <si>
+    <t>Bring up - bring down Axis camera</t>
+  </si>
+  <si>
+    <t>cameraToggleButton</t>
+  </si>
+  <si>
+    <t>Left Operator 2</t>
+  </si>
+  <si>
+    <t>Right Operator Y</t>
+  </si>
+  <si>
+    <t>Move arm up/down</t>
+  </si>
+  <si>
+    <t>Align by camera</t>
+  </si>
+  <si>
+    <t>Fire the ball</t>
+  </si>
+  <si>
+    <t>Cancel Fire</t>
+  </si>
+  <si>
+    <t>Left operator trigger</t>
+  </si>
+  <si>
+    <t>Right operator Trigger</t>
+  </si>
+  <si>
+    <t>Left Operator 3</t>
+  </si>
+  <si>
+    <t>Fire override (no matter what)</t>
+  </si>
+  <si>
+    <t>Left Operator 4 + trigger</t>
   </si>
 </sst>
 </file>
@@ -580,7 +631,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -735,22 +786,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1169,31 +1208,31 @@
   <dimension ref="A1:H238"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C50" sqref="C50"/>
+      <pane ySplit="2" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E83" sqref="E83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" style="59" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" style="59" customWidth="1"/>
-    <col min="3" max="3" width="50.7109375" style="59" customWidth="1"/>
-    <col min="4" max="4" width="21" style="60" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" style="62" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" style="59" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" style="59"/>
-    <col min="8" max="8" width="11.140625" style="59" customWidth="1"/>
-    <col min="9" max="16384" width="8.85546875" style="59"/>
+    <col min="1" max="1" width="14.7109375" style="55" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" style="55" customWidth="1"/>
+    <col min="3" max="3" width="50.7109375" style="55" customWidth="1"/>
+    <col min="4" max="4" width="21" style="56" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" style="58" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" style="55" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" style="55"/>
+    <col min="8" max="8" width="11.140625" style="55" customWidth="1"/>
+    <col min="9" max="16384" width="8.85546875" style="55"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1">
-      <c r="A1" s="72" t="s">
+      <c r="A1" s="68" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="72"/>
-      <c r="C1" s="72"/>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72"/>
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
     </row>
     <row r="2" spans="1:8" s="1" customFormat="1" ht="25.5">
       <c r="A2" s="13" t="s">
@@ -1215,17 +1254,17 @@
     <row r="3" spans="1:8" s="1" customFormat="1" ht="13.15" customHeight="1">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
-      <c r="C3" s="71" t="s">
+      <c r="C3" s="67" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="71"/>
+      <c r="D3" s="67"/>
       <c r="E3" s="3" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="1" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A4" s="63"/>
-      <c r="B4" s="63"/>
+      <c r="A4" s="59"/>
+      <c r="B4" s="59"/>
       <c r="C4" s="29" t="s">
         <v>123</v>
       </c>
@@ -1237,8 +1276,8 @@
       </c>
     </row>
     <row r="5" spans="1:8" s="1" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A5" s="64"/>
-      <c r="B5" s="64"/>
+      <c r="A5" s="60"/>
+      <c r="B5" s="60"/>
       <c r="C5" s="28" t="s">
         <v>122</v>
       </c>
@@ -1281,7 +1320,7 @@
       <c r="C8" s="48" t="s">
         <v>119</v>
       </c>
-      <c r="D8" s="65" t="s">
+      <c r="D8" s="61" t="s">
         <v>95</v>
       </c>
       <c r="E8" s="50" t="s">
@@ -1294,13 +1333,13 @@
     <row r="9" spans="1:8" s="1" customFormat="1" ht="25.5">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
-      <c r="C9" s="70" t="s">
+      <c r="C9" s="66" t="s">
         <v>124</v>
       </c>
-      <c r="D9" s="67" t="s">
+      <c r="D9" s="63" t="s">
         <v>112</v>
       </c>
-      <c r="E9" s="68" t="s">
+      <c r="E9" s="64" t="s">
         <v>113</v>
       </c>
       <c r="F9" s="12"/>
@@ -1340,11 +1379,11 @@
     <row r="13" spans="1:8" s="1" customFormat="1" ht="13.15" customHeight="1">
       <c r="A13" s="17"/>
       <c r="B13" s="17"/>
-      <c r="C13" s="73" t="s">
+      <c r="C13" s="69" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="73"/>
-      <c r="E13" s="58" t="s">
+      <c r="D13" s="69"/>
+      <c r="E13" s="54" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1477,10 +1516,10 @@
     <row r="26" spans="1:8" s="1" customFormat="1" ht="13.35" customHeight="1">
       <c r="A26" s="17"/>
       <c r="B26" s="17"/>
-      <c r="C26" s="71" t="s">
+      <c r="C26" s="67" t="s">
         <v>7</v>
       </c>
-      <c r="D26" s="71"/>
+      <c r="D26" s="67"/>
       <c r="E26" s="3" t="s">
         <v>28</v>
       </c>
@@ -1580,13 +1619,13 @@
     <row r="35" spans="1:5" s="1" customFormat="1">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
-      <c r="C35" s="66" t="s">
+      <c r="C35" s="62" t="s">
         <v>98</v>
       </c>
-      <c r="D35" s="67" t="s">
+      <c r="D35" s="63" t="s">
         <v>99</v>
       </c>
-      <c r="E35" s="68" t="s">
+      <c r="E35" s="64" t="s">
         <v>100</v>
       </c>
     </row>
@@ -1594,8 +1633,8 @@
       <c r="A36" s="8"/>
       <c r="B36" s="8"/>
       <c r="C36" s="25"/>
-      <c r="D36" s="69"/>
-      <c r="E36" s="55"/>
+      <c r="D36" s="65"/>
+      <c r="E36" s="52"/>
     </row>
     <row r="37" spans="1:5" s="1" customFormat="1">
       <c r="A37" s="4"/>
@@ -1614,7 +1653,7 @@
     <row r="39" spans="1:5" s="18" customFormat="1" ht="13.15" customHeight="1">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
-      <c r="C39" s="56"/>
+      <c r="C39" s="53"/>
       <c r="D39" s="31"/>
       <c r="E39" s="32"/>
     </row>
@@ -1642,10 +1681,10 @@
     <row r="43" spans="1:5" s="1" customFormat="1" ht="13.15" customHeight="1">
       <c r="A43" s="17"/>
       <c r="B43" s="17"/>
-      <c r="C43" s="71" t="s">
+      <c r="C43" s="67" t="s">
         <v>9</v>
       </c>
-      <c r="D43" s="71"/>
+      <c r="D43" s="67"/>
       <c r="E43" s="3" t="s">
         <v>10</v>
       </c>
@@ -1695,10 +1734,10 @@
     <row r="48" spans="1:5" s="1" customFormat="1" ht="13.15" customHeight="1">
       <c r="A48" s="17"/>
       <c r="B48" s="17"/>
-      <c r="C48" s="71" t="s">
+      <c r="C48" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="D48" s="71"/>
+      <c r="D48" s="67"/>
       <c r="E48" s="3" t="s">
         <v>12</v>
       </c>
@@ -1766,10 +1805,10 @@
     <row r="55" spans="1:8" s="1" customFormat="1" ht="13.35" customHeight="1">
       <c r="A55" s="17"/>
       <c r="B55" s="17"/>
-      <c r="C55" s="71" t="s">
+      <c r="C55" s="67" t="s">
         <v>13</v>
       </c>
-      <c r="D55" s="71"/>
+      <c r="D55" s="67"/>
       <c r="E55" s="3" t="s">
         <v>85</v>
       </c>
@@ -1838,10 +1877,10 @@
     <row r="61" spans="1:8" s="1" customFormat="1" ht="13.35" customHeight="1">
       <c r="A61" s="17"/>
       <c r="B61" s="17"/>
-      <c r="C61" s="71" t="s">
+      <c r="C61" s="67" t="s">
         <v>30</v>
       </c>
-      <c r="D61" s="71"/>
+      <c r="D61" s="67"/>
       <c r="E61" s="3" t="s">
         <v>29</v>
       </c>
@@ -1879,10 +1918,10 @@
     <row r="66" spans="1:8" s="1" customFormat="1" ht="13.35" customHeight="1">
       <c r="A66" s="17"/>
       <c r="B66" s="17"/>
-      <c r="C66" s="71" t="s">
+      <c r="C66" s="67" t="s">
         <v>14</v>
       </c>
-      <c r="D66" s="71"/>
+      <c r="D66" s="67"/>
       <c r="E66" s="3" t="s">
         <v>15</v>
       </c>
@@ -1947,10 +1986,10 @@
     <row r="71" spans="1:8" s="1" customFormat="1" ht="13.35" customHeight="1">
       <c r="A71" s="17"/>
       <c r="B71" s="17"/>
-      <c r="C71" s="71" t="s">
+      <c r="C71" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="D71" s="71"/>
+      <c r="D71" s="67"/>
       <c r="E71" s="3" t="s">
         <v>17</v>
       </c>
@@ -2005,63 +2044,97 @@
       </c>
     </row>
     <row r="76" spans="1:8" s="1" customFormat="1">
-      <c r="A76" s="8"/>
-      <c r="B76" s="8"/>
-      <c r="C76" s="52"/>
-      <c r="D76" s="53"/>
-      <c r="E76" s="54"/>
+      <c r="A76" s="10"/>
+      <c r="B76" s="10"/>
+      <c r="C76" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="D76" s="10"/>
+      <c r="E76" s="27" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="77" spans="1:8" s="1" customFormat="1">
       <c r="A77" s="4"/>
       <c r="B77" s="4"/>
-      <c r="C77" s="28"/>
+      <c r="C77" s="28" t="s">
+        <v>137</v>
+      </c>
       <c r="D77" s="31"/>
-      <c r="E77" s="32"/>
+      <c r="E77" s="32" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="78" spans="1:8" s="1" customFormat="1" ht="13.15" customHeight="1">
       <c r="A78" s="13"/>
       <c r="B78" s="8"/>
-      <c r="C78" s="29"/>
-      <c r="D78" s="44"/>
-      <c r="E78" s="43"/>
+      <c r="C78" s="29" t="s">
+        <v>138</v>
+      </c>
+      <c r="D78" s="44" t="s">
+        <v>139</v>
+      </c>
+      <c r="E78" s="43" t="s">
+        <v>140</v>
+      </c>
       <c r="F78" s="20"/>
     </row>
     <row r="79" spans="1:8" s="1" customFormat="1">
       <c r="A79" s="4"/>
       <c r="B79" s="4"/>
-      <c r="C79" s="28"/>
+      <c r="C79" s="28" t="s">
+        <v>142</v>
+      </c>
       <c r="D79" s="31"/>
-      <c r="E79" s="32"/>
+      <c r="E79" s="32" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="80" spans="1:8" s="1" customFormat="1" ht="13.15" customHeight="1">
       <c r="A80" s="13"/>
       <c r="B80" s="8"/>
-      <c r="C80" s="22"/>
+      <c r="C80" s="22" t="s">
+        <v>143</v>
+      </c>
       <c r="D80" s="44"/>
-      <c r="E80" s="43"/>
+      <c r="E80" s="43" t="s">
+        <v>147</v>
+      </c>
       <c r="F80" s="20"/>
     </row>
     <row r="81" spans="1:7" s="1" customFormat="1">
       <c r="A81" s="4"/>
       <c r="B81" s="4"/>
-      <c r="C81" s="28"/>
+      <c r="C81" s="28" t="s">
+        <v>144</v>
+      </c>
       <c r="D81" s="31"/>
-      <c r="E81" s="32"/>
+      <c r="E81" s="32" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="82" spans="1:7" s="1" customFormat="1" ht="12.75" customHeight="1">
       <c r="A82" s="13"/>
       <c r="B82" s="8"/>
-      <c r="C82" s="22"/>
+      <c r="C82" s="22" t="s">
+        <v>145</v>
+      </c>
       <c r="D82" s="44"/>
-      <c r="E82" s="57"/>
+      <c r="E82" s="23" t="s">
+        <v>148</v>
+      </c>
       <c r="F82" s="20"/>
     </row>
-    <row r="83" spans="1:7" s="1" customFormat="1">
+    <row r="83" spans="1:7" s="1" customFormat="1" ht="25.5">
       <c r="A83" s="4"/>
       <c r="B83" s="4"/>
-      <c r="C83" s="28"/>
+      <c r="C83" s="28" t="s">
+        <v>149</v>
+      </c>
       <c r="D83" s="31"/>
-      <c r="E83" s="43"/>
+      <c r="E83" s="32" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="84" spans="1:7" s="1" customFormat="1" ht="13.15" customHeight="1">
       <c r="A84" s="13"/>
@@ -2126,10 +2199,10 @@
     <row r="92" spans="1:7" s="1" customFormat="1" ht="13.35" customHeight="1">
       <c r="A92" s="17"/>
       <c r="B92" s="17"/>
-      <c r="C92" s="71" t="s">
+      <c r="C92" s="67" t="s">
         <v>18</v>
       </c>
-      <c r="D92" s="71"/>
+      <c r="D92" s="67"/>
       <c r="E92" s="3" t="s">
         <v>17</v>
       </c>
@@ -2215,11 +2288,11 @@
     <row r="103" spans="1:6" s="1" customFormat="1">
       <c r="A103" s="17"/>
       <c r="B103" s="17"/>
-      <c r="C103" s="58" t="s">
+      <c r="C103" s="54" t="s">
         <v>21</v>
       </c>
       <c r="D103" s="21"/>
-      <c r="E103" s="58" t="s">
+      <c r="E103" s="54" t="s">
         <v>26</v>
       </c>
     </row>
@@ -2348,879 +2421,879 @@
       <c r="E113" s="32"/>
     </row>
     <row r="114" spans="1:5" s="1" customFormat="1">
-      <c r="A114" s="59"/>
-      <c r="B114" s="59"/>
-      <c r="C114" s="59"/>
-      <c r="D114" s="60"/>
-      <c r="E114" s="61"/>
+      <c r="A114" s="55"/>
+      <c r="B114" s="55"/>
+      <c r="C114" s="55"/>
+      <c r="D114" s="56"/>
+      <c r="E114" s="57"/>
     </row>
     <row r="115" spans="1:5" s="1" customFormat="1">
-      <c r="A115" s="59"/>
-      <c r="B115" s="59"/>
-      <c r="C115" s="59"/>
-      <c r="D115" s="60"/>
-      <c r="E115" s="61"/>
+      <c r="A115" s="55"/>
+      <c r="B115" s="55"/>
+      <c r="C115" s="55"/>
+      <c r="D115" s="56"/>
+      <c r="E115" s="57"/>
     </row>
     <row r="116" spans="1:5" s="1" customFormat="1">
-      <c r="A116" s="59"/>
-      <c r="B116" s="59"/>
-      <c r="C116" s="59"/>
-      <c r="D116" s="60"/>
-      <c r="E116" s="61"/>
+      <c r="A116" s="55"/>
+      <c r="B116" s="55"/>
+      <c r="C116" s="55"/>
+      <c r="D116" s="56"/>
+      <c r="E116" s="57"/>
     </row>
     <row r="117" spans="1:5" s="1" customFormat="1">
-      <c r="A117" s="59"/>
-      <c r="B117" s="59"/>
-      <c r="C117" s="59"/>
-      <c r="D117" s="60"/>
-      <c r="E117" s="61"/>
+      <c r="A117" s="55"/>
+      <c r="B117" s="55"/>
+      <c r="C117" s="55"/>
+      <c r="D117" s="56"/>
+      <c r="E117" s="57"/>
     </row>
     <row r="118" spans="1:5" s="1" customFormat="1">
-      <c r="A118" s="59"/>
-      <c r="B118" s="59"/>
-      <c r="C118" s="59"/>
-      <c r="D118" s="60"/>
-      <c r="E118" s="61"/>
+      <c r="A118" s="55"/>
+      <c r="B118" s="55"/>
+      <c r="C118" s="55"/>
+      <c r="D118" s="56"/>
+      <c r="E118" s="57"/>
     </row>
     <row r="119" spans="1:5" s="1" customFormat="1">
-      <c r="A119" s="59"/>
-      <c r="B119" s="59"/>
-      <c r="C119" s="59"/>
-      <c r="D119" s="60"/>
-      <c r="E119" s="61"/>
+      <c r="A119" s="55"/>
+      <c r="B119" s="55"/>
+      <c r="C119" s="55"/>
+      <c r="D119" s="56"/>
+      <c r="E119" s="57"/>
     </row>
     <row r="120" spans="1:5" s="1" customFormat="1">
-      <c r="A120" s="59"/>
-      <c r="B120" s="59"/>
-      <c r="C120" s="59"/>
-      <c r="D120" s="60"/>
-      <c r="E120" s="61"/>
+      <c r="A120" s="55"/>
+      <c r="B120" s="55"/>
+      <c r="C120" s="55"/>
+      <c r="D120" s="56"/>
+      <c r="E120" s="57"/>
     </row>
     <row r="121" spans="1:5" s="1" customFormat="1">
-      <c r="A121" s="59"/>
-      <c r="B121" s="59"/>
-      <c r="C121" s="59"/>
-      <c r="D121" s="60"/>
-      <c r="E121" s="61"/>
+      <c r="A121" s="55"/>
+      <c r="B121" s="55"/>
+      <c r="C121" s="55"/>
+      <c r="D121" s="56"/>
+      <c r="E121" s="57"/>
     </row>
     <row r="122" spans="1:5" s="1" customFormat="1">
-      <c r="A122" s="59"/>
-      <c r="B122" s="59"/>
-      <c r="C122" s="59"/>
-      <c r="D122" s="60"/>
-      <c r="E122" s="61"/>
+      <c r="A122" s="55"/>
+      <c r="B122" s="55"/>
+      <c r="C122" s="55"/>
+      <c r="D122" s="56"/>
+      <c r="E122" s="57"/>
     </row>
     <row r="123" spans="1:5" s="1" customFormat="1">
-      <c r="A123" s="59"/>
-      <c r="B123" s="59"/>
-      <c r="C123" s="59"/>
-      <c r="D123" s="60"/>
-      <c r="E123" s="61"/>
+      <c r="A123" s="55"/>
+      <c r="B123" s="55"/>
+      <c r="C123" s="55"/>
+      <c r="D123" s="56"/>
+      <c r="E123" s="57"/>
     </row>
     <row r="124" spans="1:5" s="1" customFormat="1">
-      <c r="A124" s="59"/>
-      <c r="B124" s="59"/>
-      <c r="C124" s="59"/>
-      <c r="D124" s="60"/>
-      <c r="E124" s="61"/>
+      <c r="A124" s="55"/>
+      <c r="B124" s="55"/>
+      <c r="C124" s="55"/>
+      <c r="D124" s="56"/>
+      <c r="E124" s="57"/>
     </row>
     <row r="125" spans="1:5" s="1" customFormat="1">
-      <c r="A125" s="59"/>
-      <c r="B125" s="59"/>
-      <c r="C125" s="59"/>
-      <c r="D125" s="60"/>
-      <c r="E125" s="61"/>
+      <c r="A125" s="55"/>
+      <c r="B125" s="55"/>
+      <c r="C125" s="55"/>
+      <c r="D125" s="56"/>
+      <c r="E125" s="57"/>
     </row>
     <row r="126" spans="1:5" s="1" customFormat="1">
-      <c r="A126" s="59"/>
-      <c r="B126" s="59"/>
-      <c r="C126" s="59"/>
-      <c r="D126" s="60"/>
-      <c r="E126" s="61"/>
+      <c r="A126" s="55"/>
+      <c r="B126" s="55"/>
+      <c r="C126" s="55"/>
+      <c r="D126" s="56"/>
+      <c r="E126" s="57"/>
     </row>
     <row r="127" spans="1:5" s="1" customFormat="1">
-      <c r="A127" s="59"/>
-      <c r="B127" s="59"/>
-      <c r="C127" s="59"/>
-      <c r="D127" s="60"/>
-      <c r="E127" s="61"/>
+      <c r="A127" s="55"/>
+      <c r="B127" s="55"/>
+      <c r="C127" s="55"/>
+      <c r="D127" s="56"/>
+      <c r="E127" s="57"/>
     </row>
     <row r="128" spans="1:5" s="1" customFormat="1">
-      <c r="A128" s="59"/>
-      <c r="B128" s="59"/>
-      <c r="C128" s="59"/>
-      <c r="D128" s="60"/>
-      <c r="E128" s="61"/>
+      <c r="A128" s="55"/>
+      <c r="B128" s="55"/>
+      <c r="C128" s="55"/>
+      <c r="D128" s="56"/>
+      <c r="E128" s="57"/>
     </row>
     <row r="129" spans="1:5" s="1" customFormat="1">
-      <c r="A129" s="59"/>
-      <c r="B129" s="59"/>
-      <c r="C129" s="59"/>
-      <c r="D129" s="60"/>
-      <c r="E129" s="61"/>
+      <c r="A129" s="55"/>
+      <c r="B129" s="55"/>
+      <c r="C129" s="55"/>
+      <c r="D129" s="56"/>
+      <c r="E129" s="57"/>
     </row>
     <row r="130" spans="1:5" s="1" customFormat="1">
-      <c r="A130" s="59"/>
-      <c r="B130" s="59"/>
-      <c r="C130" s="59"/>
-      <c r="D130" s="60"/>
-      <c r="E130" s="61"/>
+      <c r="A130" s="55"/>
+      <c r="B130" s="55"/>
+      <c r="C130" s="55"/>
+      <c r="D130" s="56"/>
+      <c r="E130" s="57"/>
     </row>
     <row r="131" spans="1:5" s="1" customFormat="1">
-      <c r="A131" s="59"/>
-      <c r="B131" s="59"/>
-      <c r="C131" s="59"/>
-      <c r="D131" s="60"/>
-      <c r="E131" s="61"/>
+      <c r="A131" s="55"/>
+      <c r="B131" s="55"/>
+      <c r="C131" s="55"/>
+      <c r="D131" s="56"/>
+      <c r="E131" s="57"/>
     </row>
     <row r="132" spans="1:5" s="1" customFormat="1">
-      <c r="A132" s="59"/>
-      <c r="B132" s="59"/>
-      <c r="C132" s="59"/>
-      <c r="D132" s="60"/>
-      <c r="E132" s="61"/>
+      <c r="A132" s="55"/>
+      <c r="B132" s="55"/>
+      <c r="C132" s="55"/>
+      <c r="D132" s="56"/>
+      <c r="E132" s="57"/>
     </row>
     <row r="133" spans="1:5" s="1" customFormat="1">
-      <c r="A133" s="59"/>
-      <c r="B133" s="59"/>
-      <c r="C133" s="59"/>
-      <c r="D133" s="60"/>
-      <c r="E133" s="61"/>
+      <c r="A133" s="55"/>
+      <c r="B133" s="55"/>
+      <c r="C133" s="55"/>
+      <c r="D133" s="56"/>
+      <c r="E133" s="57"/>
     </row>
     <row r="134" spans="1:5" s="1" customFormat="1">
-      <c r="A134" s="59"/>
-      <c r="B134" s="59"/>
-      <c r="C134" s="59"/>
-      <c r="D134" s="60"/>
-      <c r="E134" s="61"/>
+      <c r="A134" s="55"/>
+      <c r="B134" s="55"/>
+      <c r="C134" s="55"/>
+      <c r="D134" s="56"/>
+      <c r="E134" s="57"/>
     </row>
     <row r="135" spans="1:5" s="1" customFormat="1">
-      <c r="A135" s="59"/>
-      <c r="B135" s="59"/>
-      <c r="C135" s="59"/>
-      <c r="D135" s="60"/>
-      <c r="E135" s="61"/>
+      <c r="A135" s="55"/>
+      <c r="B135" s="55"/>
+      <c r="C135" s="55"/>
+      <c r="D135" s="56"/>
+      <c r="E135" s="57"/>
     </row>
     <row r="136" spans="1:5" s="1" customFormat="1">
-      <c r="A136" s="59"/>
-      <c r="B136" s="59"/>
-      <c r="C136" s="59"/>
-      <c r="D136" s="60"/>
-      <c r="E136" s="61"/>
+      <c r="A136" s="55"/>
+      <c r="B136" s="55"/>
+      <c r="C136" s="55"/>
+      <c r="D136" s="56"/>
+      <c r="E136" s="57"/>
     </row>
     <row r="137" spans="1:5" s="1" customFormat="1">
-      <c r="A137" s="59"/>
-      <c r="B137" s="59"/>
-      <c r="C137" s="59"/>
-      <c r="D137" s="60"/>
-      <c r="E137" s="61"/>
+      <c r="A137" s="55"/>
+      <c r="B137" s="55"/>
+      <c r="C137" s="55"/>
+      <c r="D137" s="56"/>
+      <c r="E137" s="57"/>
     </row>
     <row r="138" spans="1:5" s="1" customFormat="1">
-      <c r="A138" s="59"/>
-      <c r="B138" s="59"/>
-      <c r="C138" s="59"/>
-      <c r="D138" s="60"/>
-      <c r="E138" s="61"/>
+      <c r="A138" s="55"/>
+      <c r="B138" s="55"/>
+      <c r="C138" s="55"/>
+      <c r="D138" s="56"/>
+      <c r="E138" s="57"/>
     </row>
     <row r="139" spans="1:5" s="1" customFormat="1">
-      <c r="A139" s="59"/>
-      <c r="B139" s="59"/>
-      <c r="C139" s="59"/>
-      <c r="D139" s="60"/>
-      <c r="E139" s="61"/>
+      <c r="A139" s="55"/>
+      <c r="B139" s="55"/>
+      <c r="C139" s="55"/>
+      <c r="D139" s="56"/>
+      <c r="E139" s="57"/>
     </row>
     <row r="140" spans="1:5" s="1" customFormat="1">
-      <c r="A140" s="59"/>
-      <c r="B140" s="59"/>
-      <c r="C140" s="59"/>
-      <c r="D140" s="60"/>
-      <c r="E140" s="61"/>
+      <c r="A140" s="55"/>
+      <c r="B140" s="55"/>
+      <c r="C140" s="55"/>
+      <c r="D140" s="56"/>
+      <c r="E140" s="57"/>
     </row>
     <row r="141" spans="1:5" s="1" customFormat="1">
-      <c r="A141" s="59"/>
-      <c r="B141" s="59"/>
-      <c r="C141" s="59"/>
-      <c r="D141" s="60"/>
-      <c r="E141" s="61"/>
+      <c r="A141" s="55"/>
+      <c r="B141" s="55"/>
+      <c r="C141" s="55"/>
+      <c r="D141" s="56"/>
+      <c r="E141" s="57"/>
     </row>
     <row r="142" spans="1:5" s="1" customFormat="1">
-      <c r="A142" s="59"/>
-      <c r="B142" s="59"/>
-      <c r="C142" s="59"/>
-      <c r="D142" s="60"/>
-      <c r="E142" s="61"/>
+      <c r="A142" s="55"/>
+      <c r="B142" s="55"/>
+      <c r="C142" s="55"/>
+      <c r="D142" s="56"/>
+      <c r="E142" s="57"/>
     </row>
     <row r="143" spans="1:5" s="1" customFormat="1">
-      <c r="A143" s="59"/>
-      <c r="B143" s="59"/>
-      <c r="C143" s="59"/>
-      <c r="D143" s="60"/>
-      <c r="E143" s="61"/>
+      <c r="A143" s="55"/>
+      <c r="B143" s="55"/>
+      <c r="C143" s="55"/>
+      <c r="D143" s="56"/>
+      <c r="E143" s="57"/>
     </row>
     <row r="144" spans="1:5" s="1" customFormat="1">
-      <c r="A144" s="59"/>
-      <c r="B144" s="59"/>
-      <c r="C144" s="59"/>
-      <c r="D144" s="60"/>
-      <c r="E144" s="61"/>
+      <c r="A144" s="55"/>
+      <c r="B144" s="55"/>
+      <c r="C144" s="55"/>
+      <c r="D144" s="56"/>
+      <c r="E144" s="57"/>
     </row>
     <row r="145" spans="1:5" s="1" customFormat="1">
-      <c r="A145" s="59"/>
-      <c r="B145" s="59"/>
-      <c r="C145" s="59"/>
-      <c r="D145" s="60"/>
-      <c r="E145" s="61"/>
+      <c r="A145" s="55"/>
+      <c r="B145" s="55"/>
+      <c r="C145" s="55"/>
+      <c r="D145" s="56"/>
+      <c r="E145" s="57"/>
     </row>
     <row r="146" spans="1:5" s="1" customFormat="1">
-      <c r="A146" s="59"/>
-      <c r="B146" s="59"/>
-      <c r="C146" s="59"/>
-      <c r="D146" s="60"/>
-      <c r="E146" s="61"/>
+      <c r="A146" s="55"/>
+      <c r="B146" s="55"/>
+      <c r="C146" s="55"/>
+      <c r="D146" s="56"/>
+      <c r="E146" s="57"/>
     </row>
     <row r="147" spans="1:5" s="1" customFormat="1">
-      <c r="A147" s="59"/>
-      <c r="B147" s="59"/>
-      <c r="C147" s="59"/>
-      <c r="D147" s="60"/>
-      <c r="E147" s="61"/>
+      <c r="A147" s="55"/>
+      <c r="B147" s="55"/>
+      <c r="C147" s="55"/>
+      <c r="D147" s="56"/>
+      <c r="E147" s="57"/>
     </row>
     <row r="148" spans="1:5" s="1" customFormat="1">
-      <c r="A148" s="59"/>
-      <c r="B148" s="59"/>
-      <c r="C148" s="59"/>
-      <c r="D148" s="60"/>
-      <c r="E148" s="61"/>
+      <c r="A148" s="55"/>
+      <c r="B148" s="55"/>
+      <c r="C148" s="55"/>
+      <c r="D148" s="56"/>
+      <c r="E148" s="57"/>
     </row>
     <row r="149" spans="1:5" s="1" customFormat="1">
-      <c r="A149" s="59"/>
-      <c r="B149" s="59"/>
-      <c r="C149" s="59"/>
-      <c r="D149" s="60"/>
-      <c r="E149" s="61"/>
+      <c r="A149" s="55"/>
+      <c r="B149" s="55"/>
+      <c r="C149" s="55"/>
+      <c r="D149" s="56"/>
+      <c r="E149" s="57"/>
     </row>
     <row r="150" spans="1:5" s="1" customFormat="1">
-      <c r="A150" s="59"/>
-      <c r="B150" s="59"/>
-      <c r="C150" s="59"/>
-      <c r="D150" s="60"/>
-      <c r="E150" s="61"/>
+      <c r="A150" s="55"/>
+      <c r="B150" s="55"/>
+      <c r="C150" s="55"/>
+      <c r="D150" s="56"/>
+      <c r="E150" s="57"/>
     </row>
     <row r="151" spans="1:5" s="1" customFormat="1">
-      <c r="A151" s="59"/>
-      <c r="B151" s="59"/>
-      <c r="C151" s="59"/>
-      <c r="D151" s="60"/>
-      <c r="E151" s="61"/>
+      <c r="A151" s="55"/>
+      <c r="B151" s="55"/>
+      <c r="C151" s="55"/>
+      <c r="D151" s="56"/>
+      <c r="E151" s="57"/>
     </row>
     <row r="152" spans="1:5" s="1" customFormat="1">
-      <c r="A152" s="59"/>
-      <c r="B152" s="59"/>
-      <c r="C152" s="59"/>
-      <c r="D152" s="60"/>
-      <c r="E152" s="61"/>
+      <c r="A152" s="55"/>
+      <c r="B152" s="55"/>
+      <c r="C152" s="55"/>
+      <c r="D152" s="56"/>
+      <c r="E152" s="57"/>
     </row>
     <row r="153" spans="1:5" s="1" customFormat="1">
-      <c r="A153" s="59"/>
-      <c r="B153" s="59"/>
-      <c r="C153" s="59"/>
-      <c r="D153" s="60"/>
-      <c r="E153" s="61"/>
+      <c r="A153" s="55"/>
+      <c r="B153" s="55"/>
+      <c r="C153" s="55"/>
+      <c r="D153" s="56"/>
+      <c r="E153" s="57"/>
     </row>
     <row r="154" spans="1:5" s="1" customFormat="1">
-      <c r="A154" s="59"/>
-      <c r="B154" s="59"/>
-      <c r="C154" s="59"/>
-      <c r="D154" s="60"/>
-      <c r="E154" s="61"/>
+      <c r="A154" s="55"/>
+      <c r="B154" s="55"/>
+      <c r="C154" s="55"/>
+      <c r="D154" s="56"/>
+      <c r="E154" s="57"/>
     </row>
     <row r="155" spans="1:5" s="1" customFormat="1">
-      <c r="A155" s="59"/>
-      <c r="B155" s="59"/>
-      <c r="C155" s="59"/>
-      <c r="D155" s="60"/>
-      <c r="E155" s="61"/>
+      <c r="A155" s="55"/>
+      <c r="B155" s="55"/>
+      <c r="C155" s="55"/>
+      <c r="D155" s="56"/>
+      <c r="E155" s="57"/>
     </row>
     <row r="156" spans="1:5" s="1" customFormat="1">
-      <c r="A156" s="59"/>
-      <c r="B156" s="59"/>
-      <c r="C156" s="59"/>
-      <c r="D156" s="60"/>
-      <c r="E156" s="61"/>
+      <c r="A156" s="55"/>
+      <c r="B156" s="55"/>
+      <c r="C156" s="55"/>
+      <c r="D156" s="56"/>
+      <c r="E156" s="57"/>
     </row>
     <row r="157" spans="1:5" s="1" customFormat="1">
-      <c r="A157" s="59"/>
-      <c r="B157" s="59"/>
-      <c r="C157" s="59"/>
-      <c r="D157" s="60"/>
-      <c r="E157" s="61"/>
+      <c r="A157" s="55"/>
+      <c r="B157" s="55"/>
+      <c r="C157" s="55"/>
+      <c r="D157" s="56"/>
+      <c r="E157" s="57"/>
     </row>
     <row r="158" spans="1:5" s="1" customFormat="1">
-      <c r="A158" s="59"/>
-      <c r="B158" s="59"/>
-      <c r="C158" s="59"/>
-      <c r="D158" s="60"/>
-      <c r="E158" s="61"/>
+      <c r="A158" s="55"/>
+      <c r="B158" s="55"/>
+      <c r="C158" s="55"/>
+      <c r="D158" s="56"/>
+      <c r="E158" s="57"/>
     </row>
     <row r="159" spans="1:5" s="1" customFormat="1">
-      <c r="A159" s="59"/>
-      <c r="B159" s="59"/>
-      <c r="C159" s="59"/>
-      <c r="D159" s="60"/>
-      <c r="E159" s="61"/>
+      <c r="A159" s="55"/>
+      <c r="B159" s="55"/>
+      <c r="C159" s="55"/>
+      <c r="D159" s="56"/>
+      <c r="E159" s="57"/>
     </row>
     <row r="160" spans="1:5" s="1" customFormat="1">
-      <c r="A160" s="59"/>
-      <c r="B160" s="59"/>
-      <c r="C160" s="59"/>
-      <c r="D160" s="60"/>
-      <c r="E160" s="61"/>
+      <c r="A160" s="55"/>
+      <c r="B160" s="55"/>
+      <c r="C160" s="55"/>
+      <c r="D160" s="56"/>
+      <c r="E160" s="57"/>
     </row>
     <row r="161" spans="1:5" s="1" customFormat="1">
-      <c r="A161" s="59"/>
-      <c r="B161" s="59"/>
-      <c r="C161" s="59"/>
-      <c r="D161" s="60"/>
-      <c r="E161" s="61"/>
+      <c r="A161" s="55"/>
+      <c r="B161" s="55"/>
+      <c r="C161" s="55"/>
+      <c r="D161" s="56"/>
+      <c r="E161" s="57"/>
     </row>
     <row r="162" spans="1:5" s="1" customFormat="1">
-      <c r="A162" s="59"/>
-      <c r="B162" s="59"/>
-      <c r="C162" s="59"/>
-      <c r="D162" s="60"/>
-      <c r="E162" s="61"/>
+      <c r="A162" s="55"/>
+      <c r="B162" s="55"/>
+      <c r="C162" s="55"/>
+      <c r="D162" s="56"/>
+      <c r="E162" s="57"/>
     </row>
     <row r="163" spans="1:5" s="1" customFormat="1">
-      <c r="A163" s="59"/>
-      <c r="B163" s="59"/>
-      <c r="C163" s="59"/>
-      <c r="D163" s="60"/>
-      <c r="E163" s="61"/>
+      <c r="A163" s="55"/>
+      <c r="B163" s="55"/>
+      <c r="C163" s="55"/>
+      <c r="D163" s="56"/>
+      <c r="E163" s="57"/>
     </row>
     <row r="164" spans="1:5" s="1" customFormat="1">
-      <c r="A164" s="59"/>
-      <c r="B164" s="59"/>
-      <c r="C164" s="59"/>
-      <c r="D164" s="60"/>
-      <c r="E164" s="61"/>
+      <c r="A164" s="55"/>
+      <c r="B164" s="55"/>
+      <c r="C164" s="55"/>
+      <c r="D164" s="56"/>
+      <c r="E164" s="57"/>
     </row>
     <row r="165" spans="1:5" s="1" customFormat="1">
-      <c r="A165" s="59"/>
-      <c r="B165" s="59"/>
-      <c r="C165" s="59"/>
-      <c r="D165" s="60"/>
-      <c r="E165" s="61"/>
+      <c r="A165" s="55"/>
+      <c r="B165" s="55"/>
+      <c r="C165" s="55"/>
+      <c r="D165" s="56"/>
+      <c r="E165" s="57"/>
     </row>
     <row r="166" spans="1:5" s="1" customFormat="1">
-      <c r="A166" s="59"/>
-      <c r="B166" s="59"/>
-      <c r="C166" s="59"/>
-      <c r="D166" s="60"/>
-      <c r="E166" s="61"/>
+      <c r="A166" s="55"/>
+      <c r="B166" s="55"/>
+      <c r="C166" s="55"/>
+      <c r="D166" s="56"/>
+      <c r="E166" s="57"/>
     </row>
     <row r="167" spans="1:5" s="1" customFormat="1">
-      <c r="A167" s="59"/>
-      <c r="B167" s="59"/>
-      <c r="C167" s="59"/>
-      <c r="D167" s="60"/>
-      <c r="E167" s="61"/>
+      <c r="A167" s="55"/>
+      <c r="B167" s="55"/>
+      <c r="C167" s="55"/>
+      <c r="D167" s="56"/>
+      <c r="E167" s="57"/>
     </row>
     <row r="168" spans="1:5" s="1" customFormat="1">
-      <c r="A168" s="59"/>
-      <c r="B168" s="59"/>
-      <c r="C168" s="59"/>
-      <c r="D168" s="60"/>
-      <c r="E168" s="61"/>
+      <c r="A168" s="55"/>
+      <c r="B168" s="55"/>
+      <c r="C168" s="55"/>
+      <c r="D168" s="56"/>
+      <c r="E168" s="57"/>
     </row>
     <row r="169" spans="1:5" s="1" customFormat="1">
-      <c r="A169" s="59"/>
-      <c r="B169" s="59"/>
-      <c r="C169" s="59"/>
-      <c r="D169" s="60"/>
-      <c r="E169" s="61"/>
+      <c r="A169" s="55"/>
+      <c r="B169" s="55"/>
+      <c r="C169" s="55"/>
+      <c r="D169" s="56"/>
+      <c r="E169" s="57"/>
     </row>
     <row r="170" spans="1:5" s="1" customFormat="1">
-      <c r="A170" s="59"/>
-      <c r="B170" s="59"/>
-      <c r="C170" s="59"/>
-      <c r="D170" s="60"/>
-      <c r="E170" s="61"/>
+      <c r="A170" s="55"/>
+      <c r="B170" s="55"/>
+      <c r="C170" s="55"/>
+      <c r="D170" s="56"/>
+      <c r="E170" s="57"/>
     </row>
     <row r="171" spans="1:5" s="1" customFormat="1">
-      <c r="A171" s="59"/>
-      <c r="B171" s="59"/>
-      <c r="C171" s="59"/>
-      <c r="D171" s="60"/>
-      <c r="E171" s="61"/>
+      <c r="A171" s="55"/>
+      <c r="B171" s="55"/>
+      <c r="C171" s="55"/>
+      <c r="D171" s="56"/>
+      <c r="E171" s="57"/>
     </row>
     <row r="172" spans="1:5" s="1" customFormat="1">
-      <c r="A172" s="59"/>
-      <c r="B172" s="59"/>
-      <c r="C172" s="59"/>
-      <c r="D172" s="60"/>
-      <c r="E172" s="61"/>
+      <c r="A172" s="55"/>
+      <c r="B172" s="55"/>
+      <c r="C172" s="55"/>
+      <c r="D172" s="56"/>
+      <c r="E172" s="57"/>
     </row>
     <row r="173" spans="1:5" s="1" customFormat="1">
-      <c r="A173" s="59"/>
-      <c r="B173" s="59"/>
-      <c r="C173" s="59"/>
-      <c r="D173" s="60"/>
-      <c r="E173" s="61"/>
+      <c r="A173" s="55"/>
+      <c r="B173" s="55"/>
+      <c r="C173" s="55"/>
+      <c r="D173" s="56"/>
+      <c r="E173" s="57"/>
     </row>
     <row r="174" spans="1:5" s="1" customFormat="1">
-      <c r="A174" s="59"/>
-      <c r="B174" s="59"/>
-      <c r="C174" s="59"/>
-      <c r="D174" s="60"/>
-      <c r="E174" s="61"/>
+      <c r="A174" s="55"/>
+      <c r="B174" s="55"/>
+      <c r="C174" s="55"/>
+      <c r="D174" s="56"/>
+      <c r="E174" s="57"/>
     </row>
     <row r="175" spans="1:5" s="1" customFormat="1">
-      <c r="A175" s="59"/>
-      <c r="B175" s="59"/>
-      <c r="C175" s="59"/>
-      <c r="D175" s="60"/>
-      <c r="E175" s="61"/>
+      <c r="A175" s="55"/>
+      <c r="B175" s="55"/>
+      <c r="C175" s="55"/>
+      <c r="D175" s="56"/>
+      <c r="E175" s="57"/>
     </row>
     <row r="176" spans="1:5" s="1" customFormat="1">
-      <c r="A176" s="59"/>
-      <c r="B176" s="59"/>
-      <c r="C176" s="59"/>
-      <c r="D176" s="60"/>
-      <c r="E176" s="61"/>
+      <c r="A176" s="55"/>
+      <c r="B176" s="55"/>
+      <c r="C176" s="55"/>
+      <c r="D176" s="56"/>
+      <c r="E176" s="57"/>
     </row>
     <row r="177" spans="1:5" s="1" customFormat="1">
-      <c r="A177" s="59"/>
-      <c r="B177" s="59"/>
-      <c r="C177" s="59"/>
-      <c r="D177" s="60"/>
-      <c r="E177" s="61"/>
+      <c r="A177" s="55"/>
+      <c r="B177" s="55"/>
+      <c r="C177" s="55"/>
+      <c r="D177" s="56"/>
+      <c r="E177" s="57"/>
     </row>
     <row r="178" spans="1:5" s="1" customFormat="1">
-      <c r="A178" s="59"/>
-      <c r="B178" s="59"/>
-      <c r="C178" s="59"/>
-      <c r="D178" s="60"/>
-      <c r="E178" s="61"/>
+      <c r="A178" s="55"/>
+      <c r="B178" s="55"/>
+      <c r="C178" s="55"/>
+      <c r="D178" s="56"/>
+      <c r="E178" s="57"/>
     </row>
     <row r="179" spans="1:5" s="1" customFormat="1">
-      <c r="A179" s="59"/>
-      <c r="B179" s="59"/>
-      <c r="C179" s="59"/>
-      <c r="D179" s="60"/>
-      <c r="E179" s="61"/>
+      <c r="A179" s="55"/>
+      <c r="B179" s="55"/>
+      <c r="C179" s="55"/>
+      <c r="D179" s="56"/>
+      <c r="E179" s="57"/>
     </row>
     <row r="180" spans="1:5" s="1" customFormat="1">
-      <c r="A180" s="59"/>
-      <c r="B180" s="59"/>
-      <c r="C180" s="59"/>
-      <c r="D180" s="60"/>
-      <c r="E180" s="61"/>
+      <c r="A180" s="55"/>
+      <c r="B180" s="55"/>
+      <c r="C180" s="55"/>
+      <c r="D180" s="56"/>
+      <c r="E180" s="57"/>
     </row>
     <row r="181" spans="1:5" s="1" customFormat="1">
-      <c r="A181" s="59"/>
-      <c r="B181" s="59"/>
-      <c r="C181" s="59"/>
-      <c r="D181" s="60"/>
-      <c r="E181" s="61"/>
+      <c r="A181" s="55"/>
+      <c r="B181" s="55"/>
+      <c r="C181" s="55"/>
+      <c r="D181" s="56"/>
+      <c r="E181" s="57"/>
     </row>
     <row r="182" spans="1:5" s="1" customFormat="1">
-      <c r="A182" s="59"/>
-      <c r="B182" s="59"/>
-      <c r="C182" s="59"/>
-      <c r="D182" s="60"/>
-      <c r="E182" s="61"/>
+      <c r="A182" s="55"/>
+      <c r="B182" s="55"/>
+      <c r="C182" s="55"/>
+      <c r="D182" s="56"/>
+      <c r="E182" s="57"/>
     </row>
     <row r="183" spans="1:5" s="1" customFormat="1">
-      <c r="A183" s="59"/>
-      <c r="B183" s="59"/>
-      <c r="C183" s="59"/>
-      <c r="D183" s="60"/>
-      <c r="E183" s="61"/>
+      <c r="A183" s="55"/>
+      <c r="B183" s="55"/>
+      <c r="C183" s="55"/>
+      <c r="D183" s="56"/>
+      <c r="E183" s="57"/>
     </row>
     <row r="184" spans="1:5" s="1" customFormat="1">
-      <c r="A184" s="59"/>
-      <c r="B184" s="59"/>
-      <c r="C184" s="59"/>
-      <c r="D184" s="60"/>
-      <c r="E184" s="61"/>
+      <c r="A184" s="55"/>
+      <c r="B184" s="55"/>
+      <c r="C184" s="55"/>
+      <c r="D184" s="56"/>
+      <c r="E184" s="57"/>
     </row>
     <row r="185" spans="1:5" s="1" customFormat="1">
-      <c r="A185" s="59"/>
-      <c r="B185" s="59"/>
-      <c r="C185" s="59"/>
-      <c r="D185" s="60"/>
-      <c r="E185" s="61"/>
+      <c r="A185" s="55"/>
+      <c r="B185" s="55"/>
+      <c r="C185" s="55"/>
+      <c r="D185" s="56"/>
+      <c r="E185" s="57"/>
     </row>
     <row r="186" spans="1:5" s="1" customFormat="1">
-      <c r="A186" s="59"/>
-      <c r="B186" s="59"/>
-      <c r="C186" s="59"/>
-      <c r="D186" s="60"/>
-      <c r="E186" s="61"/>
+      <c r="A186" s="55"/>
+      <c r="B186" s="55"/>
+      <c r="C186" s="55"/>
+      <c r="D186" s="56"/>
+      <c r="E186" s="57"/>
     </row>
     <row r="187" spans="1:5" s="1" customFormat="1">
-      <c r="A187" s="59"/>
-      <c r="B187" s="59"/>
-      <c r="C187" s="59"/>
-      <c r="D187" s="60"/>
-      <c r="E187" s="61"/>
+      <c r="A187" s="55"/>
+      <c r="B187" s="55"/>
+      <c r="C187" s="55"/>
+      <c r="D187" s="56"/>
+      <c r="E187" s="57"/>
     </row>
     <row r="188" spans="1:5" s="1" customFormat="1">
-      <c r="A188" s="59"/>
-      <c r="B188" s="59"/>
-      <c r="C188" s="59"/>
-      <c r="D188" s="60"/>
-      <c r="E188" s="61"/>
+      <c r="A188" s="55"/>
+      <c r="B188" s="55"/>
+      <c r="C188" s="55"/>
+      <c r="D188" s="56"/>
+      <c r="E188" s="57"/>
     </row>
     <row r="189" spans="1:5" s="1" customFormat="1">
-      <c r="A189" s="59"/>
-      <c r="B189" s="59"/>
-      <c r="C189" s="59"/>
-      <c r="D189" s="60"/>
-      <c r="E189" s="61"/>
+      <c r="A189" s="55"/>
+      <c r="B189" s="55"/>
+      <c r="C189" s="55"/>
+      <c r="D189" s="56"/>
+      <c r="E189" s="57"/>
     </row>
     <row r="190" spans="1:5" s="1" customFormat="1">
-      <c r="A190" s="59"/>
-      <c r="B190" s="59"/>
-      <c r="C190" s="59"/>
-      <c r="D190" s="60"/>
-      <c r="E190" s="61"/>
+      <c r="A190" s="55"/>
+      <c r="B190" s="55"/>
+      <c r="C190" s="55"/>
+      <c r="D190" s="56"/>
+      <c r="E190" s="57"/>
     </row>
     <row r="191" spans="1:5" s="1" customFormat="1">
-      <c r="A191" s="59"/>
-      <c r="B191" s="59"/>
-      <c r="C191" s="59"/>
-      <c r="D191" s="60"/>
-      <c r="E191" s="61"/>
+      <c r="A191" s="55"/>
+      <c r="B191" s="55"/>
+      <c r="C191" s="55"/>
+      <c r="D191" s="56"/>
+      <c r="E191" s="57"/>
     </row>
     <row r="192" spans="1:5" s="1" customFormat="1">
-      <c r="A192" s="59"/>
-      <c r="B192" s="59"/>
-      <c r="C192" s="59"/>
-      <c r="D192" s="60"/>
-      <c r="E192" s="61"/>
+      <c r="A192" s="55"/>
+      <c r="B192" s="55"/>
+      <c r="C192" s="55"/>
+      <c r="D192" s="56"/>
+      <c r="E192" s="57"/>
     </row>
     <row r="193" spans="1:5" s="1" customFormat="1">
-      <c r="A193" s="59"/>
-      <c r="B193" s="59"/>
-      <c r="C193" s="59"/>
-      <c r="D193" s="60"/>
-      <c r="E193" s="61"/>
+      <c r="A193" s="55"/>
+      <c r="B193" s="55"/>
+      <c r="C193" s="55"/>
+      <c r="D193" s="56"/>
+      <c r="E193" s="57"/>
     </row>
     <row r="194" spans="1:5" s="1" customFormat="1">
-      <c r="A194" s="59"/>
-      <c r="B194" s="59"/>
-      <c r="C194" s="59"/>
-      <c r="D194" s="60"/>
-      <c r="E194" s="62"/>
+      <c r="A194" s="55"/>
+      <c r="B194" s="55"/>
+      <c r="C194" s="55"/>
+      <c r="D194" s="56"/>
+      <c r="E194" s="58"/>
     </row>
     <row r="195" spans="1:5" s="1" customFormat="1">
-      <c r="A195" s="59"/>
-      <c r="B195" s="59"/>
-      <c r="C195" s="59"/>
-      <c r="D195" s="60"/>
-      <c r="E195" s="62"/>
+      <c r="A195" s="55"/>
+      <c r="B195" s="55"/>
+      <c r="C195" s="55"/>
+      <c r="D195" s="56"/>
+      <c r="E195" s="58"/>
     </row>
     <row r="196" spans="1:5" s="1" customFormat="1">
-      <c r="A196" s="59"/>
-      <c r="B196" s="59"/>
-      <c r="C196" s="59"/>
-      <c r="D196" s="60"/>
-      <c r="E196" s="62"/>
+      <c r="A196" s="55"/>
+      <c r="B196" s="55"/>
+      <c r="C196" s="55"/>
+      <c r="D196" s="56"/>
+      <c r="E196" s="58"/>
     </row>
     <row r="197" spans="1:5" s="1" customFormat="1">
-      <c r="A197" s="59"/>
-      <c r="B197" s="59"/>
-      <c r="C197" s="59"/>
-      <c r="D197" s="60"/>
-      <c r="E197" s="62"/>
+      <c r="A197" s="55"/>
+      <c r="B197" s="55"/>
+      <c r="C197" s="55"/>
+      <c r="D197" s="56"/>
+      <c r="E197" s="58"/>
     </row>
     <row r="198" spans="1:5" s="1" customFormat="1">
-      <c r="A198" s="59"/>
-      <c r="B198" s="59"/>
-      <c r="C198" s="59"/>
-      <c r="D198" s="60"/>
-      <c r="E198" s="62"/>
+      <c r="A198" s="55"/>
+      <c r="B198" s="55"/>
+      <c r="C198" s="55"/>
+      <c r="D198" s="56"/>
+      <c r="E198" s="58"/>
     </row>
     <row r="199" spans="1:5" s="1" customFormat="1">
-      <c r="A199" s="59"/>
-      <c r="B199" s="59"/>
-      <c r="C199" s="59"/>
-      <c r="D199" s="60"/>
-      <c r="E199" s="62"/>
+      <c r="A199" s="55"/>
+      <c r="B199" s="55"/>
+      <c r="C199" s="55"/>
+      <c r="D199" s="56"/>
+      <c r="E199" s="58"/>
     </row>
     <row r="200" spans="1:5" s="1" customFormat="1">
-      <c r="A200" s="59"/>
-      <c r="B200" s="59"/>
-      <c r="C200" s="59"/>
-      <c r="D200" s="60"/>
-      <c r="E200" s="62"/>
+      <c r="A200" s="55"/>
+      <c r="B200" s="55"/>
+      <c r="C200" s="55"/>
+      <c r="D200" s="56"/>
+      <c r="E200" s="58"/>
     </row>
     <row r="201" spans="1:5" s="1" customFormat="1">
-      <c r="A201" s="59"/>
-      <c r="B201" s="59"/>
-      <c r="C201" s="59"/>
-      <c r="D201" s="60"/>
-      <c r="E201" s="62"/>
+      <c r="A201" s="55"/>
+      <c r="B201" s="55"/>
+      <c r="C201" s="55"/>
+      <c r="D201" s="56"/>
+      <c r="E201" s="58"/>
     </row>
     <row r="202" spans="1:5" s="1" customFormat="1">
-      <c r="A202" s="59"/>
-      <c r="B202" s="59"/>
-      <c r="C202" s="59"/>
-      <c r="D202" s="60"/>
-      <c r="E202" s="62"/>
+      <c r="A202" s="55"/>
+      <c r="B202" s="55"/>
+      <c r="C202" s="55"/>
+      <c r="D202" s="56"/>
+      <c r="E202" s="58"/>
     </row>
     <row r="203" spans="1:5" s="1" customFormat="1">
-      <c r="A203" s="59"/>
-      <c r="B203" s="59"/>
-      <c r="C203" s="59"/>
-      <c r="D203" s="60"/>
-      <c r="E203" s="62"/>
+      <c r="A203" s="55"/>
+      <c r="B203" s="55"/>
+      <c r="C203" s="55"/>
+      <c r="D203" s="56"/>
+      <c r="E203" s="58"/>
     </row>
     <row r="204" spans="1:5" s="1" customFormat="1">
-      <c r="A204" s="59"/>
-      <c r="B204" s="59"/>
-      <c r="C204" s="59"/>
-      <c r="D204" s="60"/>
-      <c r="E204" s="62"/>
+      <c r="A204" s="55"/>
+      <c r="B204" s="55"/>
+      <c r="C204" s="55"/>
+      <c r="D204" s="56"/>
+      <c r="E204" s="58"/>
     </row>
     <row r="205" spans="1:5" s="1" customFormat="1">
-      <c r="A205" s="59"/>
-      <c r="B205" s="59"/>
-      <c r="C205" s="59"/>
-      <c r="D205" s="60"/>
-      <c r="E205" s="62"/>
+      <c r="A205" s="55"/>
+      <c r="B205" s="55"/>
+      <c r="C205" s="55"/>
+      <c r="D205" s="56"/>
+      <c r="E205" s="58"/>
     </row>
     <row r="206" spans="1:5" s="1" customFormat="1">
-      <c r="A206" s="59"/>
-      <c r="B206" s="59"/>
-      <c r="C206" s="59"/>
-      <c r="D206" s="60"/>
-      <c r="E206" s="62"/>
+      <c r="A206" s="55"/>
+      <c r="B206" s="55"/>
+      <c r="C206" s="55"/>
+      <c r="D206" s="56"/>
+      <c r="E206" s="58"/>
     </row>
     <row r="207" spans="1:5" s="1" customFormat="1">
-      <c r="A207" s="59"/>
-      <c r="B207" s="59"/>
-      <c r="C207" s="59"/>
-      <c r="D207" s="60"/>
-      <c r="E207" s="62"/>
+      <c r="A207" s="55"/>
+      <c r="B207" s="55"/>
+      <c r="C207" s="55"/>
+      <c r="D207" s="56"/>
+      <c r="E207" s="58"/>
     </row>
     <row r="208" spans="1:5" s="1" customFormat="1">
-      <c r="A208" s="59"/>
-      <c r="B208" s="59"/>
-      <c r="C208" s="59"/>
-      <c r="D208" s="60"/>
-      <c r="E208" s="62"/>
+      <c r="A208" s="55"/>
+      <c r="B208" s="55"/>
+      <c r="C208" s="55"/>
+      <c r="D208" s="56"/>
+      <c r="E208" s="58"/>
     </row>
     <row r="209" spans="1:5" s="1" customFormat="1">
-      <c r="A209" s="59"/>
-      <c r="B209" s="59"/>
-      <c r="C209" s="59"/>
-      <c r="D209" s="60"/>
-      <c r="E209" s="62"/>
+      <c r="A209" s="55"/>
+      <c r="B209" s="55"/>
+      <c r="C209" s="55"/>
+      <c r="D209" s="56"/>
+      <c r="E209" s="58"/>
     </row>
     <row r="210" spans="1:5" s="1" customFormat="1">
-      <c r="A210" s="59"/>
-      <c r="B210" s="59"/>
-      <c r="C210" s="59"/>
-      <c r="D210" s="60"/>
-      <c r="E210" s="62"/>
+      <c r="A210" s="55"/>
+      <c r="B210" s="55"/>
+      <c r="C210" s="55"/>
+      <c r="D210" s="56"/>
+      <c r="E210" s="58"/>
     </row>
     <row r="211" spans="1:5" s="1" customFormat="1">
-      <c r="A211" s="59"/>
-      <c r="B211" s="59"/>
-      <c r="C211" s="59"/>
-      <c r="D211" s="60"/>
-      <c r="E211" s="62"/>
+      <c r="A211" s="55"/>
+      <c r="B211" s="55"/>
+      <c r="C211" s="55"/>
+      <c r="D211" s="56"/>
+      <c r="E211" s="58"/>
     </row>
     <row r="212" spans="1:5" s="1" customFormat="1">
-      <c r="A212" s="59"/>
-      <c r="B212" s="59"/>
-      <c r="C212" s="59"/>
-      <c r="D212" s="60"/>
-      <c r="E212" s="62"/>
+      <c r="A212" s="55"/>
+      <c r="B212" s="55"/>
+      <c r="C212" s="55"/>
+      <c r="D212" s="56"/>
+      <c r="E212" s="58"/>
     </row>
     <row r="213" spans="1:5" s="1" customFormat="1">
-      <c r="A213" s="59"/>
-      <c r="B213" s="59"/>
-      <c r="C213" s="59"/>
-      <c r="D213" s="60"/>
-      <c r="E213" s="62"/>
+      <c r="A213" s="55"/>
+      <c r="B213" s="55"/>
+      <c r="C213" s="55"/>
+      <c r="D213" s="56"/>
+      <c r="E213" s="58"/>
     </row>
     <row r="214" spans="1:5" s="1" customFormat="1">
-      <c r="A214" s="59"/>
-      <c r="B214" s="59"/>
-      <c r="C214" s="59"/>
-      <c r="D214" s="60"/>
-      <c r="E214" s="62"/>
+      <c r="A214" s="55"/>
+      <c r="B214" s="55"/>
+      <c r="C214" s="55"/>
+      <c r="D214" s="56"/>
+      <c r="E214" s="58"/>
     </row>
     <row r="215" spans="1:5" s="1" customFormat="1">
-      <c r="A215" s="59"/>
-      <c r="B215" s="59"/>
-      <c r="C215" s="59"/>
-      <c r="D215" s="60"/>
-      <c r="E215" s="62"/>
+      <c r="A215" s="55"/>
+      <c r="B215" s="55"/>
+      <c r="C215" s="55"/>
+      <c r="D215" s="56"/>
+      <c r="E215" s="58"/>
     </row>
     <row r="216" spans="1:5" s="1" customFormat="1">
-      <c r="A216" s="59"/>
-      <c r="B216" s="59"/>
-      <c r="C216" s="59"/>
-      <c r="D216" s="60"/>
-      <c r="E216" s="62"/>
+      <c r="A216" s="55"/>
+      <c r="B216" s="55"/>
+      <c r="C216" s="55"/>
+      <c r="D216" s="56"/>
+      <c r="E216" s="58"/>
     </row>
     <row r="217" spans="1:5" s="1" customFormat="1">
-      <c r="A217" s="59"/>
-      <c r="B217" s="59"/>
-      <c r="C217" s="59"/>
-      <c r="D217" s="60"/>
-      <c r="E217" s="62"/>
+      <c r="A217" s="55"/>
+      <c r="B217" s="55"/>
+      <c r="C217" s="55"/>
+      <c r="D217" s="56"/>
+      <c r="E217" s="58"/>
     </row>
     <row r="218" spans="1:5" s="1" customFormat="1">
-      <c r="A218" s="59"/>
-      <c r="B218" s="59"/>
-      <c r="C218" s="59"/>
-      <c r="D218" s="60"/>
-      <c r="E218" s="62"/>
+      <c r="A218" s="55"/>
+      <c r="B218" s="55"/>
+      <c r="C218" s="55"/>
+      <c r="D218" s="56"/>
+      <c r="E218" s="58"/>
     </row>
     <row r="219" spans="1:5" s="1" customFormat="1">
-      <c r="A219" s="59"/>
-      <c r="B219" s="59"/>
-      <c r="C219" s="59"/>
-      <c r="D219" s="60"/>
-      <c r="E219" s="62"/>
+      <c r="A219" s="55"/>
+      <c r="B219" s="55"/>
+      <c r="C219" s="55"/>
+      <c r="D219" s="56"/>
+      <c r="E219" s="58"/>
     </row>
     <row r="220" spans="1:5" s="1" customFormat="1">
-      <c r="A220" s="59"/>
-      <c r="B220" s="59"/>
-      <c r="C220" s="59"/>
-      <c r="D220" s="60"/>
-      <c r="E220" s="62"/>
+      <c r="A220" s="55"/>
+      <c r="B220" s="55"/>
+      <c r="C220" s="55"/>
+      <c r="D220" s="56"/>
+      <c r="E220" s="58"/>
     </row>
     <row r="221" spans="1:5" s="1" customFormat="1">
-      <c r="A221" s="59"/>
-      <c r="B221" s="59"/>
-      <c r="C221" s="59"/>
-      <c r="D221" s="60"/>
-      <c r="E221" s="62"/>
+      <c r="A221" s="55"/>
+      <c r="B221" s="55"/>
+      <c r="C221" s="55"/>
+      <c r="D221" s="56"/>
+      <c r="E221" s="58"/>
     </row>
     <row r="222" spans="1:5" s="1" customFormat="1">
-      <c r="A222" s="59"/>
-      <c r="B222" s="59"/>
-      <c r="C222" s="59"/>
-      <c r="D222" s="60"/>
-      <c r="E222" s="62"/>
+      <c r="A222" s="55"/>
+      <c r="B222" s="55"/>
+      <c r="C222" s="55"/>
+      <c r="D222" s="56"/>
+      <c r="E222" s="58"/>
     </row>
     <row r="223" spans="1:5" s="1" customFormat="1">
-      <c r="A223" s="59"/>
-      <c r="B223" s="59"/>
-      <c r="C223" s="59"/>
-      <c r="D223" s="60"/>
-      <c r="E223" s="62"/>
+      <c r="A223" s="55"/>
+      <c r="B223" s="55"/>
+      <c r="C223" s="55"/>
+      <c r="D223" s="56"/>
+      <c r="E223" s="58"/>
     </row>
     <row r="224" spans="1:5" s="1" customFormat="1">
-      <c r="A224" s="59"/>
-      <c r="B224" s="59"/>
-      <c r="C224" s="59"/>
-      <c r="D224" s="60"/>
-      <c r="E224" s="62"/>
+      <c r="A224" s="55"/>
+      <c r="B224" s="55"/>
+      <c r="C224" s="55"/>
+      <c r="D224" s="56"/>
+      <c r="E224" s="58"/>
     </row>
     <row r="225" spans="1:5" s="1" customFormat="1">
-      <c r="A225" s="59"/>
-      <c r="B225" s="59"/>
-      <c r="C225" s="59"/>
-      <c r="D225" s="60"/>
-      <c r="E225" s="62"/>
+      <c r="A225" s="55"/>
+      <c r="B225" s="55"/>
+      <c r="C225" s="55"/>
+      <c r="D225" s="56"/>
+      <c r="E225" s="58"/>
     </row>
     <row r="226" spans="1:5" s="1" customFormat="1">
-      <c r="A226" s="59"/>
-      <c r="B226" s="59"/>
-      <c r="C226" s="59"/>
-      <c r="D226" s="60"/>
-      <c r="E226" s="62"/>
+      <c r="A226" s="55"/>
+      <c r="B226" s="55"/>
+      <c r="C226" s="55"/>
+      <c r="D226" s="56"/>
+      <c r="E226" s="58"/>
     </row>
     <row r="227" spans="1:5" s="1" customFormat="1">
-      <c r="A227" s="59"/>
-      <c r="B227" s="59"/>
-      <c r="C227" s="59"/>
-      <c r="D227" s="60"/>
-      <c r="E227" s="62"/>
+      <c r="A227" s="55"/>
+      <c r="B227" s="55"/>
+      <c r="C227" s="55"/>
+      <c r="D227" s="56"/>
+      <c r="E227" s="58"/>
     </row>
     <row r="228" spans="1:5" s="1" customFormat="1">
-      <c r="A228" s="59"/>
-      <c r="B228" s="59"/>
-      <c r="C228" s="59"/>
-      <c r="D228" s="60"/>
-      <c r="E228" s="62"/>
+      <c r="A228" s="55"/>
+      <c r="B228" s="55"/>
+      <c r="C228" s="55"/>
+      <c r="D228" s="56"/>
+      <c r="E228" s="58"/>
     </row>
     <row r="229" spans="1:5" s="1" customFormat="1">
-      <c r="A229" s="59"/>
-      <c r="B229" s="59"/>
-      <c r="C229" s="59"/>
-      <c r="D229" s="60"/>
-      <c r="E229" s="62"/>
+      <c r="A229" s="55"/>
+      <c r="B229" s="55"/>
+      <c r="C229" s="55"/>
+      <c r="D229" s="56"/>
+      <c r="E229" s="58"/>
     </row>
     <row r="230" spans="1:5" s="1" customFormat="1">
-      <c r="A230" s="59"/>
-      <c r="B230" s="59"/>
-      <c r="C230" s="59"/>
-      <c r="D230" s="60"/>
-      <c r="E230" s="62"/>
+      <c r="A230" s="55"/>
+      <c r="B230" s="55"/>
+      <c r="C230" s="55"/>
+      <c r="D230" s="56"/>
+      <c r="E230" s="58"/>
     </row>
     <row r="231" spans="1:5" s="1" customFormat="1">
-      <c r="A231" s="59"/>
-      <c r="B231" s="59"/>
-      <c r="C231" s="59"/>
-      <c r="D231" s="60"/>
-      <c r="E231" s="62"/>
+      <c r="A231" s="55"/>
+      <c r="B231" s="55"/>
+      <c r="C231" s="55"/>
+      <c r="D231" s="56"/>
+      <c r="E231" s="58"/>
     </row>
     <row r="232" spans="1:5" s="1" customFormat="1">
-      <c r="A232" s="59"/>
-      <c r="B232" s="59"/>
-      <c r="C232" s="59"/>
-      <c r="D232" s="60"/>
-      <c r="E232" s="62"/>
+      <c r="A232" s="55"/>
+      <c r="B232" s="55"/>
+      <c r="C232" s="55"/>
+      <c r="D232" s="56"/>
+      <c r="E232" s="58"/>
     </row>
     <row r="233" spans="1:5" s="1" customFormat="1">
-      <c r="A233" s="59"/>
-      <c r="B233" s="59"/>
-      <c r="C233" s="59"/>
-      <c r="D233" s="60"/>
-      <c r="E233" s="62"/>
+      <c r="A233" s="55"/>
+      <c r="B233" s="55"/>
+      <c r="C233" s="55"/>
+      <c r="D233" s="56"/>
+      <c r="E233" s="58"/>
     </row>
     <row r="234" spans="1:5" s="1" customFormat="1">
-      <c r="A234" s="59"/>
-      <c r="B234" s="59"/>
-      <c r="C234" s="59"/>
-      <c r="D234" s="60"/>
-      <c r="E234" s="62"/>
+      <c r="A234" s="55"/>
+      <c r="B234" s="55"/>
+      <c r="C234" s="55"/>
+      <c r="D234" s="56"/>
+      <c r="E234" s="58"/>
     </row>
     <row r="235" spans="1:5" s="1" customFormat="1">
-      <c r="A235" s="59"/>
-      <c r="B235" s="59"/>
-      <c r="C235" s="59"/>
-      <c r="D235" s="60"/>
-      <c r="E235" s="62"/>
+      <c r="A235" s="55"/>
+      <c r="B235" s="55"/>
+      <c r="C235" s="55"/>
+      <c r="D235" s="56"/>
+      <c r="E235" s="58"/>
     </row>
     <row r="236" spans="1:5" s="1" customFormat="1">
-      <c r="A236" s="59"/>
-      <c r="B236" s="59"/>
-      <c r="C236" s="59"/>
-      <c r="D236" s="60"/>
-      <c r="E236" s="62"/>
+      <c r="A236" s="55"/>
+      <c r="B236" s="55"/>
+      <c r="C236" s="55"/>
+      <c r="D236" s="56"/>
+      <c r="E236" s="58"/>
     </row>
     <row r="237" spans="1:5" s="1" customFormat="1">
-      <c r="A237" s="59"/>
-      <c r="B237" s="59"/>
-      <c r="C237" s="59"/>
-      <c r="D237" s="60"/>
-      <c r="E237" s="62"/>
+      <c r="A237" s="55"/>
+      <c r="B237" s="55"/>
+      <c r="C237" s="55"/>
+      <c r="D237" s="56"/>
+      <c r="E237" s="58"/>
     </row>
     <row r="238" spans="1:5" s="1" customFormat="1">
-      <c r="A238" s="59"/>
-      <c r="B238" s="59"/>
-      <c r="C238" s="59"/>
-      <c r="D238" s="60"/>
-      <c r="E238" s="62"/>
+      <c r="A238" s="55"/>
+      <c r="B238" s="55"/>
+      <c r="C238" s="55"/>
+      <c r="D238" s="56"/>
+      <c r="E238" s="58"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>

</xml_diff>

<commit_message>
Added to Guidance IR ball sensor checked joystick buttons, etc.
</commit_message>
<xml_diff>
--- a/Kilroy Equipment List 2016.xlsx
+++ b/Kilroy Equipment List 2016.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4506"/>
   <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2520" windowWidth="10590" windowHeight="5790"/>
@@ -397,9 +397,6 @@
     <t>Arm potentiometer</t>
   </si>
   <si>
-    <t>armPositionPot</t>
-  </si>
-  <si>
     <t>Intake Motor (Victor)</t>
   </si>
   <si>
@@ -470,6 +467,9 @@
   </si>
   <si>
     <t>Left Operator 4 + trigger</t>
+  </si>
+  <si>
+    <t>armPot</t>
   </si>
 </sst>
 </file>
@@ -1208,8 +1208,8 @@
   <dimension ref="A1:H238"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E83" sqref="E83"/>
+      <pane ySplit="2" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -1350,10 +1350,10 @@
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="C10" s="25" t="s">
+        <v>126</v>
+      </c>
+      <c r="D10" s="26" t="s">
         <v>127</v>
-      </c>
-      <c r="D10" s="26" t="s">
-        <v>128</v>
       </c>
       <c r="E10" s="27" t="s">
         <v>114</v>
@@ -1417,10 +1417,10 @@
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="28" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E16" s="32" t="s">
         <v>71</v>
@@ -1548,7 +1548,7 @@
         <v>46</v>
       </c>
       <c r="E29" s="32" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="30" spans="1:8" s="1" customFormat="1">
@@ -1561,7 +1561,7 @@
         <v>48</v>
       </c>
       <c r="E30" s="43" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="31" spans="1:8" s="1" customFormat="1">
@@ -1759,7 +1759,7 @@
       <c r="A50" s="8"/>
       <c r="B50" s="8"/>
       <c r="C50" s="25" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D50" s="26" t="s">
         <v>82</v>
@@ -1775,7 +1775,7 @@
         <v>125</v>
       </c>
       <c r="D51" s="31" t="s">
-        <v>126</v>
+        <v>150</v>
       </c>
       <c r="E51" s="32" t="s">
         <v>64</v>
@@ -2047,35 +2047,35 @@
       <c r="A76" s="10"/>
       <c r="B76" s="10"/>
       <c r="C76" s="25" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D76" s="10"/>
       <c r="E76" s="27" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="77" spans="1:8" s="1" customFormat="1">
       <c r="A77" s="4"/>
       <c r="B77" s="4"/>
       <c r="C77" s="28" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D77" s="31"/>
       <c r="E77" s="32" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="78" spans="1:8" s="1" customFormat="1" ht="13.15" customHeight="1">
       <c r="A78" s="13"/>
       <c r="B78" s="8"/>
       <c r="C78" s="29" t="s">
+        <v>137</v>
+      </c>
+      <c r="D78" s="44" t="s">
         <v>138</v>
       </c>
-      <c r="D78" s="44" t="s">
+      <c r="E78" s="43" t="s">
         <v>139</v>
-      </c>
-      <c r="E78" s="43" t="s">
-        <v>140</v>
       </c>
       <c r="F78" s="20"/>
     </row>
@@ -2083,22 +2083,22 @@
       <c r="A79" s="4"/>
       <c r="B79" s="4"/>
       <c r="C79" s="28" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D79" s="31"/>
       <c r="E79" s="32" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="80" spans="1:8" s="1" customFormat="1" ht="13.15" customHeight="1">
       <c r="A80" s="13"/>
       <c r="B80" s="8"/>
       <c r="C80" s="22" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D80" s="44"/>
       <c r="E80" s="43" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F80" s="20"/>
     </row>
@@ -2106,22 +2106,22 @@
       <c r="A81" s="4"/>
       <c r="B81" s="4"/>
       <c r="C81" s="28" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D81" s="31"/>
       <c r="E81" s="32" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="82" spans="1:7" s="1" customFormat="1" ht="12.75" customHeight="1">
       <c r="A82" s="13"/>
       <c r="B82" s="8"/>
       <c r="C82" s="22" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D82" s="44"/>
       <c r="E82" s="23" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F82" s="20"/>
     </row>
@@ -2129,11 +2129,11 @@
       <c r="A83" s="4"/>
       <c r="B83" s="4"/>
       <c r="C83" s="28" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D83" s="31"/>
       <c r="E83" s="32" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="84" spans="1:7" s="1" customFormat="1" ht="13.15" customHeight="1">

</xml_diff>

<commit_message>
Reverted Kilroy Equipment list spreadsheet so it is readable.
</commit_message>
<xml_diff>
--- a/Kilroy Equipment List 2016.xlsx
+++ b/Kilroy Equipment List 2016.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2520" windowWidth="10590" windowHeight="5790"/>
@@ -397,6 +397,9 @@
     <t>Arm potentiometer</t>
   </si>
   <si>
+    <t>armPositionPot</t>
+  </si>
+  <si>
     <t>Intake Motor (Victor)</t>
   </si>
   <si>
@@ -467,9 +470,6 @@
   </si>
   <si>
     <t>Left Operator 4 + trigger</t>
-  </si>
-  <si>
-    <t>armPot</t>
   </si>
 </sst>
 </file>
@@ -1208,8 +1208,8 @@
   <dimension ref="A1:H238"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D51" sqref="D51"/>
+      <pane ySplit="2" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E83" sqref="E83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -1350,10 +1350,10 @@
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="C10" s="25" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D10" s="26" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E10" s="27" t="s">
         <v>114</v>
@@ -1417,10 +1417,10 @@
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="28" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E16" s="32" t="s">
         <v>71</v>
@@ -1548,7 +1548,7 @@
         <v>46</v>
       </c>
       <c r="E29" s="32" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="30" spans="1:8" s="1" customFormat="1">
@@ -1561,7 +1561,7 @@
         <v>48</v>
       </c>
       <c r="E30" s="43" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="31" spans="1:8" s="1" customFormat="1">
@@ -1759,7 +1759,7 @@
       <c r="A50" s="8"/>
       <c r="B50" s="8"/>
       <c r="C50" s="25" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D50" s="26" t="s">
         <v>82</v>
@@ -1775,7 +1775,7 @@
         <v>125</v>
       </c>
       <c r="D51" s="31" t="s">
-        <v>150</v>
+        <v>126</v>
       </c>
       <c r="E51" s="32" t="s">
         <v>64</v>
@@ -2047,35 +2047,35 @@
       <c r="A76" s="10"/>
       <c r="B76" s="10"/>
       <c r="C76" s="25" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D76" s="10"/>
       <c r="E76" s="27" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="77" spans="1:8" s="1" customFormat="1">
       <c r="A77" s="4"/>
       <c r="B77" s="4"/>
       <c r="C77" s="28" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D77" s="31"/>
       <c r="E77" s="32" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="78" spans="1:8" s="1" customFormat="1" ht="13.15" customHeight="1">
       <c r="A78" s="13"/>
       <c r="B78" s="8"/>
       <c r="C78" s="29" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D78" s="44" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E78" s="43" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="F78" s="20"/>
     </row>
@@ -2083,22 +2083,22 @@
       <c r="A79" s="4"/>
       <c r="B79" s="4"/>
       <c r="C79" s="28" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D79" s="31"/>
       <c r="E79" s="32" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="80" spans="1:8" s="1" customFormat="1" ht="13.15" customHeight="1">
       <c r="A80" s="13"/>
       <c r="B80" s="8"/>
       <c r="C80" s="22" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D80" s="44"/>
       <c r="E80" s="43" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="F80" s="20"/>
     </row>
@@ -2106,22 +2106,22 @@
       <c r="A81" s="4"/>
       <c r="B81" s="4"/>
       <c r="C81" s="28" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D81" s="31"/>
       <c r="E81" s="32" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="82" spans="1:7" s="1" customFormat="1" ht="12.75" customHeight="1">
       <c r="A82" s="13"/>
       <c r="B82" s="8"/>
       <c r="C82" s="22" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D82" s="44"/>
       <c r="E82" s="23" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="F82" s="20"/>
     </row>
@@ -2129,11 +2129,11 @@
       <c r="A83" s="4"/>
       <c r="B83" s="4"/>
       <c r="C83" s="28" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D83" s="31"/>
       <c r="E83" s="32" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="84" spans="1:7" s="1" customFormat="1" ht="13.15" customHeight="1">

</xml_diff>

<commit_message>
Added override buttons to equipment list.
</commit_message>
<xml_diff>
--- a/Kilroy Equipment List 2016.xlsx
+++ b/Kilroy Equipment List 2016.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="155">
   <si>
     <t>Code Written/Tested</t>
   </si>
@@ -470,6 +470,18 @@
   </si>
   <si>
     <t>Left Operator 4 + trigger</t>
+  </si>
+  <si>
+    <t>Pull in ball override</t>
+  </si>
+  <si>
+    <t>Right Operator 3</t>
+  </si>
+  <si>
+    <t>move arm override</t>
+  </si>
+  <si>
+    <t>Right Operator 2</t>
   </si>
 </sst>
 </file>
@@ -1208,8 +1220,8 @@
   <dimension ref="A1:H238"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E83" sqref="E83"/>
+      <pane ySplit="2" topLeftCell="A69" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E85" sqref="E85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -2139,17 +2151,25 @@
     <row r="84" spans="1:7" s="1" customFormat="1" ht="13.15" customHeight="1">
       <c r="A84" s="13"/>
       <c r="B84" s="8"/>
-      <c r="C84" s="22"/>
+      <c r="C84" s="22" t="s">
+        <v>151</v>
+      </c>
       <c r="D84" s="44"/>
-      <c r="E84" s="43"/>
+      <c r="E84" s="43" t="s">
+        <v>152</v>
+      </c>
       <c r="F84" s="20"/>
     </row>
     <row r="85" spans="1:7" s="1" customFormat="1">
       <c r="A85" s="4"/>
       <c r="B85" s="4"/>
-      <c r="C85" s="28"/>
+      <c r="C85" s="28" t="s">
+        <v>153</v>
+      </c>
       <c r="D85" s="6"/>
-      <c r="E85" s="32"/>
+      <c r="E85" s="32" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="86" spans="1:7" s="1" customFormat="1" ht="13.15" customHeight="1">
       <c r="A86" s="13"/>

</xml_diff>